<commit_message>
Checked for missing Fmsy and Total Biomass data and ran mechanism model including these two (didn't run past thorny skate due to missing data)
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,17 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="GAM_Summary_Fproxy_AvgCondStrat" sheetId="1" r:id="rId1"/>
+    <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
+    <sheet name="Mechanism GAMs" sheetId="3" r:id="rId2"/>
+    <sheet name="MechanismSummaryTable" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="633" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="802" uniqueCount="132">
   <si>
     <t>Species</t>
   </si>
@@ -350,12 +352,78 @@
   <si>
     <t>AvgTempFall</t>
   </si>
+  <si>
+    <t>Plot wasn't produced</t>
+  </si>
+  <si>
+    <t>Average Temp Winter 2020</t>
+  </si>
+  <si>
+    <t>AvgTempWinter</t>
+  </si>
+  <si>
+    <t>Peak condition at -0.5</t>
+  </si>
+  <si>
+    <t>Possible peak around 0.75</t>
+  </si>
+  <si>
+    <t>GAM p-values for Environmental Variables</t>
+  </si>
+  <si>
+    <t>Local Density</t>
+  </si>
+  <si>
+    <t>Zooplankton</t>
+  </si>
+  <si>
+    <t>Temperature Anomaly</t>
+  </si>
+  <si>
+    <t>Average Stomach Fullness Strata Lag</t>
+  </si>
+  <si>
+    <t>Local Biomass Strata</t>
+  </si>
+  <si>
+    <t>Local Abundance Strata</t>
+  </si>
+  <si>
+    <t>Zooplankton Biomass Anomaly</t>
+  </si>
+  <si>
+    <t>Copepod Small/Large Ratio</t>
+  </si>
+  <si>
+    <t>Total Copepods Millions</t>
+  </si>
+  <si>
+    <t>Average Temp Spring</t>
+  </si>
+  <si>
+    <t>Average Temp Summer</t>
+  </si>
+  <si>
+    <t>Average Temp Fall</t>
+  </si>
+  <si>
+    <t>At least 1 stock with &lt;20 years of data</t>
+  </si>
+  <si>
+    <t>Unit or all stocks &lt;20 years of data</t>
+  </si>
+  <si>
+    <t>form.cond &lt;- formula(AvgRelCondStrata ~ s(AvgBottomTempStrata, k=10) +s(AvgExpcatchwtStrata, k=10) +s(TotalBiomass, k=10) +s(Fproxy, k=10) +s(CopepodSmallLarge, k=10) +s(AvgTempFall, k=10), data=condSPP)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -490,8 +558,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="33">
+  <fills count="39">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -671,8 +752,44 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFDDEBF7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFE699"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -787,6 +904,353 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="dotted">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="dotted">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="dotted">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="dotted">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -832,8 +1296,190 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="35" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1198,10 +1844,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M339"/>
+  <dimension ref="A1:M371"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A309" workbookViewId="0">
-      <selection activeCell="F312" sqref="F312"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D351" sqref="D351"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1213,6 +1859,12 @@
       <c r="A1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" s="62" t="s">
+        <v>128</v>
+      </c>
+      <c r="G1" s="61" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1361,7 +2013,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B9">
@@ -1464,7 +2116,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="A14" s="61" t="s">
         <v>17</v>
       </c>
       <c r="B14">
@@ -1507,7 +2159,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="A16" s="62" t="s">
         <v>19</v>
       </c>
       <c r="B16">
@@ -1527,7 +2179,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="A17" s="62" t="s">
         <v>20</v>
       </c>
       <c r="B17">
@@ -1696,7 +2348,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
+      <c r="A25" s="61" t="s">
         <v>28</v>
       </c>
       <c r="B25">
@@ -1841,7 +2493,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
+      <c r="A34" s="62" t="s">
         <v>11</v>
       </c>
       <c r="B34">
@@ -1861,7 +2513,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
+      <c r="A35" s="61" t="s">
         <v>12</v>
       </c>
       <c r="B35">
@@ -1964,7 +2616,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A40" t="s">
+      <c r="A40" s="61" t="s">
         <v>17</v>
       </c>
       <c r="B40">
@@ -2007,7 +2659,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A42" t="s">
+      <c r="A42" s="62" t="s">
         <v>19</v>
       </c>
       <c r="B42">
@@ -2027,7 +2679,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A43" t="s">
+      <c r="A43" s="62" t="s">
         <v>20</v>
       </c>
       <c r="B43">
@@ -2047,7 +2699,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A44" t="s">
+      <c r="A44" s="62" t="s">
         <v>21</v>
       </c>
       <c r="B44">
@@ -2193,7 +2845,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A51" t="s">
+      <c r="A51" s="61" t="s">
         <v>28</v>
       </c>
       <c r="B51">
@@ -7137,6 +7789,9 @@
       <c r="F219">
         <v>510</v>
       </c>
+      <c r="G219" t="s">
+        <v>110</v>
+      </c>
       <c r="H219" t="s">
         <v>61</v>
       </c>
@@ -10382,6 +11037,24 @@
       </c>
     </row>
     <row r="310" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A310" t="s">
+        <v>0</v>
+      </c>
+      <c r="B310" t="s">
+        <v>109</v>
+      </c>
+      <c r="C310" t="s">
+        <v>2</v>
+      </c>
+      <c r="D310" t="s">
+        <v>3</v>
+      </c>
+      <c r="E310" t="s">
+        <v>4</v>
+      </c>
+      <c r="F310" t="s">
+        <v>5</v>
+      </c>
       <c r="H310" t="s">
         <v>0</v>
       </c>
@@ -10402,6 +11075,24 @@
       </c>
     </row>
     <row r="311" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A311" t="s">
+        <v>6</v>
+      </c>
+      <c r="B311">
+        <v>1E-3</v>
+      </c>
+      <c r="C311">
+        <v>0.02</v>
+      </c>
+      <c r="D311">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E311">
+        <v>23.393000000000001</v>
+      </c>
+      <c r="F311">
+        <v>917</v>
+      </c>
       <c r="H311" t="s">
         <v>6</v>
       </c>
@@ -10422,6 +11113,24 @@
       </c>
     </row>
     <row r="312" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A312" t="s">
+        <v>7</v>
+      </c>
+      <c r="B312">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="C312">
+        <v>0</v>
+      </c>
+      <c r="D312">
+        <v>0</v>
+      </c>
+      <c r="E312">
+        <v>20.327999999999999</v>
+      </c>
+      <c r="F312">
+        <v>1591</v>
+      </c>
       <c r="H312" t="s">
         <v>7</v>
       </c>
@@ -10442,6 +11151,24 @@
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A313" t="s">
+        <v>8</v>
+      </c>
+      <c r="B313">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="C313">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D313">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E313">
+        <v>28.539000000000001</v>
+      </c>
+      <c r="F313">
+        <v>881</v>
+      </c>
       <c r="H313" t="s">
         <v>8</v>
       </c>
@@ -10462,6 +11189,24 @@
       </c>
     </row>
     <row r="314" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A314" t="s">
+        <v>9</v>
+      </c>
+      <c r="B314">
+        <v>0.08</v>
+      </c>
+      <c r="C314">
+        <v>2E-3</v>
+      </c>
+      <c r="D314">
+        <v>2E-3</v>
+      </c>
+      <c r="E314">
+        <v>62.173999999999999</v>
+      </c>
+      <c r="F314">
+        <v>1652</v>
+      </c>
       <c r="H314" t="s">
         <v>9</v>
       </c>
@@ -10482,6 +11227,24 @@
       </c>
     </row>
     <row r="315" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A315" t="s">
+        <v>10</v>
+      </c>
+      <c r="B315">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="C315">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D315">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E315">
+        <v>49.307000000000002</v>
+      </c>
+      <c r="F315">
+        <v>548</v>
+      </c>
       <c r="H315" t="s">
         <v>10</v>
       </c>
@@ -10502,6 +11265,24 @@
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A316" t="s">
+        <v>41</v>
+      </c>
+      <c r="B316">
+        <v>0</v>
+      </c>
+      <c r="C316">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="D316">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="E316">
+        <v>87.027000000000001</v>
+      </c>
+      <c r="F316">
+        <v>1177</v>
+      </c>
       <c r="H316" t="s">
         <v>41</v>
       </c>
@@ -10522,6 +11303,24 @@
       </c>
     </row>
     <row r="317" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A317" t="s">
+        <v>11</v>
+      </c>
+      <c r="B317">
+        <v>0</v>
+      </c>
+      <c r="C317">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D317">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E317">
+        <v>54.828000000000003</v>
+      </c>
+      <c r="F317">
+        <v>2329</v>
+      </c>
       <c r="H317" t="s">
         <v>11</v>
       </c>
@@ -10542,6 +11341,24 @@
       </c>
     </row>
     <row r="318" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A318" t="s">
+        <v>12</v>
+      </c>
+      <c r="B318">
+        <v>0.69299999999999995</v>
+      </c>
+      <c r="C318">
+        <v>0</v>
+      </c>
+      <c r="D318">
+        <v>0</v>
+      </c>
+      <c r="E318">
+        <v>16.474</v>
+      </c>
+      <c r="F318">
+        <v>954</v>
+      </c>
       <c r="H318" t="s">
         <v>12</v>
       </c>
@@ -10562,6 +11379,24 @@
       </c>
     </row>
     <row r="319" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A319" t="s">
+        <v>13</v>
+      </c>
+      <c r="B319">
+        <v>0</v>
+      </c>
+      <c r="C319">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D319">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E319">
+        <v>15.022</v>
+      </c>
+      <c r="F319">
+        <v>1180</v>
+      </c>
       <c r="H319" t="s">
         <v>13</v>
       </c>
@@ -10582,6 +11417,24 @@
       </c>
     </row>
     <row r="320" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A320" t="s">
+        <v>14</v>
+      </c>
+      <c r="B320">
+        <v>0.66600000000000004</v>
+      </c>
+      <c r="C320">
+        <v>0</v>
+      </c>
+      <c r="D320">
+        <v>0</v>
+      </c>
+      <c r="E320">
+        <v>25.187000000000001</v>
+      </c>
+      <c r="F320">
+        <v>597</v>
+      </c>
       <c r="H320" t="s">
         <v>14</v>
       </c>
@@ -10601,7 +11454,25 @@
         <v>710</v>
       </c>
     </row>
-    <row r="321" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A321" t="s">
+        <v>15</v>
+      </c>
+      <c r="B321">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C321">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D321">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E321">
+        <v>17.475000000000001</v>
+      </c>
+      <c r="F321">
+        <v>1041</v>
+      </c>
       <c r="H321" t="s">
         <v>15</v>
       </c>
@@ -10621,7 +11492,25 @@
         <v>1324</v>
       </c>
     </row>
-    <row r="322" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A322" t="s">
+        <v>16</v>
+      </c>
+      <c r="B322">
+        <v>0</v>
+      </c>
+      <c r="C322">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D322">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E322">
+        <v>59.515000000000001</v>
+      </c>
+      <c r="F322">
+        <v>1793</v>
+      </c>
       <c r="H322" t="s">
         <v>16</v>
       </c>
@@ -10641,7 +11530,25 @@
         <v>4195</v>
       </c>
     </row>
-    <row r="323" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A323" t="s">
+        <v>42</v>
+      </c>
+      <c r="B323">
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="C323">
+        <v>1E-3</v>
+      </c>
+      <c r="D323">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="E323">
+        <v>26.393000000000001</v>
+      </c>
+      <c r="F323">
+        <v>1621</v>
+      </c>
       <c r="H323" t="s">
         <v>42</v>
       </c>
@@ -10661,7 +11568,25 @@
         <v>1693</v>
       </c>
     </row>
-    <row r="324" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A324" t="s">
+        <v>17</v>
+      </c>
+      <c r="B324">
+        <v>0.02</v>
+      </c>
+      <c r="C324">
+        <v>1.2E-2</v>
+      </c>
+      <c r="D324">
+        <v>0.02</v>
+      </c>
+      <c r="E324">
+        <v>23.841000000000001</v>
+      </c>
+      <c r="F324">
+        <v>958</v>
+      </c>
       <c r="H324" t="s">
         <v>17</v>
       </c>
@@ -10681,7 +11606,25 @@
         <v>1222</v>
       </c>
     </row>
-    <row r="325" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A325" t="s">
+        <v>18</v>
+      </c>
+      <c r="B325">
+        <v>1E-3</v>
+      </c>
+      <c r="C325">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D325">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E325">
+        <v>13.972</v>
+      </c>
+      <c r="F325">
+        <v>1465</v>
+      </c>
       <c r="H325" t="s">
         <v>18</v>
       </c>
@@ -10701,7 +11644,25 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="326" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A326" t="s">
+        <v>43</v>
+      </c>
+      <c r="B326">
+        <v>0</v>
+      </c>
+      <c r="C326">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D326">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E326">
+        <v>71.477999999999994</v>
+      </c>
+      <c r="F326">
+        <v>1680</v>
+      </c>
       <c r="H326" t="s">
         <v>43</v>
       </c>
@@ -10721,7 +11682,25 @@
         <v>1831</v>
       </c>
     </row>
-    <row r="327" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A327" t="s">
+        <v>19</v>
+      </c>
+      <c r="B327">
+        <v>0</v>
+      </c>
+      <c r="C327">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D327">
+        <v>3.9E-2</v>
+      </c>
+      <c r="E327">
+        <v>57.759</v>
+      </c>
+      <c r="F327">
+        <v>945</v>
+      </c>
       <c r="H327" t="s">
         <v>19</v>
       </c>
@@ -10741,7 +11720,25 @@
         <v>3817</v>
       </c>
     </row>
-    <row r="328" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A328" t="s">
+        <v>20</v>
+      </c>
+      <c r="B328">
+        <v>2E-3</v>
+      </c>
+      <c r="C328">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D328">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E328">
+        <v>12.904999999999999</v>
+      </c>
+      <c r="F328">
+        <v>1194</v>
+      </c>
       <c r="H328" t="s">
         <v>20</v>
       </c>
@@ -10761,7 +11758,25 @@
         <v>3408</v>
       </c>
     </row>
-    <row r="329" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A329" t="s">
+        <v>44</v>
+      </c>
+      <c r="B329">
+        <v>1.6E-2</v>
+      </c>
+      <c r="C329">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D329">
+        <v>0.02</v>
+      </c>
+      <c r="E329">
+        <v>29.981999999999999</v>
+      </c>
+      <c r="F329">
+        <v>853</v>
+      </c>
       <c r="H329" t="s">
         <v>44</v>
       </c>
@@ -10781,7 +11796,25 @@
         <v>1090</v>
       </c>
     </row>
-    <row r="330" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A330" t="s">
+        <v>21</v>
+      </c>
+      <c r="B330">
+        <v>0</v>
+      </c>
+      <c r="C330">
+        <v>0.04</v>
+      </c>
+      <c r="D330">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="E330">
+        <v>84.358000000000004</v>
+      </c>
+      <c r="F330">
+        <v>1412</v>
+      </c>
       <c r="H330" t="s">
         <v>21</v>
       </c>
@@ -10801,7 +11834,25 @@
         <v>3004</v>
       </c>
     </row>
-    <row r="331" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A331" t="s">
+        <v>22</v>
+      </c>
+      <c r="B331">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="C331">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D331">
+        <v>2.4E-2</v>
+      </c>
+      <c r="E331">
+        <v>24.507000000000001</v>
+      </c>
+      <c r="F331">
+        <v>489</v>
+      </c>
       <c r="H331" t="s">
         <v>22</v>
       </c>
@@ -10821,7 +11872,25 @@
         <v>535</v>
       </c>
     </row>
-    <row r="332" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A332" t="s">
+        <v>23</v>
+      </c>
+      <c r="B332">
+        <v>0</v>
+      </c>
+      <c r="C332">
+        <v>2.3E-2</v>
+      </c>
+      <c r="D332">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E332">
+        <v>153.708</v>
+      </c>
+      <c r="F332">
+        <v>2491</v>
+      </c>
       <c r="H332" t="s">
         <v>23</v>
       </c>
@@ -10841,7 +11910,25 @@
         <v>2738</v>
       </c>
     </row>
-    <row r="333" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A333" t="s">
+        <v>24</v>
+      </c>
+      <c r="B333">
+        <v>0.29199999999999998</v>
+      </c>
+      <c r="C333">
+        <v>0</v>
+      </c>
+      <c r="D333">
+        <v>0</v>
+      </c>
+      <c r="E333">
+        <v>19.399999999999999</v>
+      </c>
+      <c r="F333">
+        <v>856</v>
+      </c>
       <c r="H333" t="s">
         <v>24</v>
       </c>
@@ -10861,7 +11948,25 @@
         <v>867</v>
       </c>
     </row>
-    <row r="334" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A334" t="s">
+        <v>25</v>
+      </c>
+      <c r="B334">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="C334">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D334">
+        <v>0.01</v>
+      </c>
+      <c r="E334">
+        <v>55.82</v>
+      </c>
+      <c r="F334">
+        <v>704</v>
+      </c>
       <c r="H334" t="s">
         <v>25</v>
       </c>
@@ -10881,7 +11986,28 @@
         <v>777</v>
       </c>
     </row>
-    <row r="335" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A335" t="s">
+        <v>45</v>
+      </c>
+      <c r="B335">
+        <v>0</v>
+      </c>
+      <c r="C335">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D335">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E335">
+        <v>63.42</v>
+      </c>
+      <c r="F335">
+        <v>857</v>
+      </c>
+      <c r="G335" t="s">
+        <v>48</v>
+      </c>
       <c r="H335" t="s">
         <v>45</v>
       </c>
@@ -10901,7 +12027,25 @@
         <v>858</v>
       </c>
     </row>
-    <row r="336" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A336" t="s">
+        <v>26</v>
+      </c>
+      <c r="B336">
+        <v>1E-3</v>
+      </c>
+      <c r="C336">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D336">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="E336">
+        <v>15.478999999999999</v>
+      </c>
+      <c r="F336">
+        <v>803</v>
+      </c>
       <c r="H336" t="s">
         <v>26</v>
       </c>
@@ -10921,7 +12065,25 @@
         <v>1052</v>
       </c>
     </row>
-    <row r="337" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A337" t="s">
+        <v>46</v>
+      </c>
+      <c r="B337">
+        <v>0.624</v>
+      </c>
+      <c r="C337">
+        <v>0</v>
+      </c>
+      <c r="D337">
+        <v>0</v>
+      </c>
+      <c r="E337">
+        <v>79.507999999999996</v>
+      </c>
+      <c r="F337">
+        <v>477</v>
+      </c>
       <c r="H337" t="s">
         <v>46</v>
       </c>
@@ -10941,7 +12103,25 @@
         <v>554</v>
       </c>
     </row>
-    <row r="338" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A338" t="s">
+        <v>27</v>
+      </c>
+      <c r="B338">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C338">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D338">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E338">
+        <v>34.764000000000003</v>
+      </c>
+      <c r="F338">
+        <v>631</v>
+      </c>
       <c r="H338" t="s">
         <v>27</v>
       </c>
@@ -10961,7 +12141,25 @@
         <v>705</v>
       </c>
     </row>
-    <row r="339" spans="8:13" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A339" t="s">
+        <v>28</v>
+      </c>
+      <c r="B339">
+        <v>0</v>
+      </c>
+      <c r="C339">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D339">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E339">
+        <v>53.372</v>
+      </c>
+      <c r="F339">
+        <v>1385</v>
+      </c>
       <c r="H339" t="s">
         <v>28</v>
       </c>
@@ -10979,6 +12177,617 @@
       </c>
       <c r="M339">
         <v>3147</v>
+      </c>
+    </row>
+    <row r="341" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A341" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="342" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A342" t="s">
+        <v>0</v>
+      </c>
+      <c r="B342" t="s">
+        <v>112</v>
+      </c>
+      <c r="C342" t="s">
+        <v>2</v>
+      </c>
+      <c r="D342" t="s">
+        <v>3</v>
+      </c>
+      <c r="E342" t="s">
+        <v>4</v>
+      </c>
+      <c r="F342" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="343" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A343" t="s">
+        <v>6</v>
+      </c>
+      <c r="B343">
+        <v>1E-3</v>
+      </c>
+      <c r="C343">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D343">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E343">
+        <v>22.885000000000002</v>
+      </c>
+      <c r="F343">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="344" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A344" t="s">
+        <v>7</v>
+      </c>
+      <c r="B344">
+        <v>1E-3</v>
+      </c>
+      <c r="C344">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="D344">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E344">
+        <v>20.254999999999999</v>
+      </c>
+      <c r="F344">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="345" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A345" t="s">
+        <v>8</v>
+      </c>
+      <c r="B345">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C345">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D345">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E345">
+        <v>28.390999999999998</v>
+      </c>
+      <c r="F345">
+        <v>772</v>
+      </c>
+    </row>
+    <row r="346" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A346" t="s">
+        <v>9</v>
+      </c>
+      <c r="B346">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C346">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D346">
+        <v>0.01</v>
+      </c>
+      <c r="E346">
+        <v>61.853000000000002</v>
+      </c>
+      <c r="F346">
+        <v>1473</v>
+      </c>
+    </row>
+    <row r="347" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A347" t="s">
+        <v>10</v>
+      </c>
+      <c r="B347">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="C347">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="D347">
+        <v>2.3E-2</v>
+      </c>
+      <c r="E347">
+        <v>48.901000000000003</v>
+      </c>
+      <c r="F347">
+        <v>442</v>
+      </c>
+    </row>
+    <row r="348" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A348" t="s">
+        <v>41</v>
+      </c>
+      <c r="B348">
+        <v>0</v>
+      </c>
+      <c r="C348">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D348">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="E348">
+        <v>90.183000000000007</v>
+      </c>
+      <c r="F348">
+        <v>972</v>
+      </c>
+      <c r="G348" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="349" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A349" t="s">
+        <v>11</v>
+      </c>
+      <c r="B349">
+        <v>0</v>
+      </c>
+      <c r="C349">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D349">
+        <v>0.02</v>
+      </c>
+      <c r="E349">
+        <v>54.712000000000003</v>
+      </c>
+      <c r="F349">
+        <v>2008</v>
+      </c>
+    </row>
+    <row r="350" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A350" t="s">
+        <v>12</v>
+      </c>
+      <c r="B350">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C350">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D350">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="E350">
+        <v>16.14</v>
+      </c>
+      <c r="F350">
+        <v>792</v>
+      </c>
+    </row>
+    <row r="351" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A351" t="s">
+        <v>13</v>
+      </c>
+      <c r="B351">
+        <v>0</v>
+      </c>
+      <c r="C351">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D351">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E351">
+        <v>15.78</v>
+      </c>
+      <c r="F351">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="352" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A352" t="s">
+        <v>14</v>
+      </c>
+      <c r="B352">
+        <v>1</v>
+      </c>
+      <c r="C352">
+        <v>0</v>
+      </c>
+      <c r="D352">
+        <v>0</v>
+      </c>
+      <c r="E352">
+        <v>24.568000000000001</v>
+      </c>
+      <c r="F352">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="353" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A353" t="s">
+        <v>15</v>
+      </c>
+      <c r="B353">
+        <v>1E-3</v>
+      </c>
+      <c r="C353">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D353">
+        <v>0.03</v>
+      </c>
+      <c r="E353">
+        <v>17.577000000000002</v>
+      </c>
+      <c r="F353">
+        <v>820</v>
+      </c>
+    </row>
+    <row r="354" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A354" t="s">
+        <v>16</v>
+      </c>
+      <c r="B354">
+        <v>0</v>
+      </c>
+      <c r="C354">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D354">
+        <v>1.9E-2</v>
+      </c>
+      <c r="E354">
+        <v>62.203000000000003</v>
+      </c>
+      <c r="F354">
+        <v>1488</v>
+      </c>
+    </row>
+    <row r="355" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A355" t="s">
+        <v>42</v>
+      </c>
+      <c r="B355">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="C355">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D355">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E355">
+        <v>26.263000000000002</v>
+      </c>
+      <c r="F355">
+        <v>1504</v>
+      </c>
+    </row>
+    <row r="356" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A356" t="s">
+        <v>17</v>
+      </c>
+      <c r="B356">
+        <v>0</v>
+      </c>
+      <c r="C356">
+        <v>2.4E-2</v>
+      </c>
+      <c r="D356">
+        <v>0.03</v>
+      </c>
+      <c r="E356">
+        <v>25.218</v>
+      </c>
+      <c r="F356">
+        <v>782</v>
+      </c>
+    </row>
+    <row r="357" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A357" t="s">
+        <v>18</v>
+      </c>
+      <c r="B357">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="C357">
+        <v>0</v>
+      </c>
+      <c r="D357">
+        <v>0</v>
+      </c>
+      <c r="E357">
+        <v>13.949</v>
+      </c>
+      <c r="F357">
+        <v>1381</v>
+      </c>
+    </row>
+    <row r="358" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A358" t="s">
+        <v>43</v>
+      </c>
+      <c r="B358">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C358">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="D358">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="E358">
+        <v>71.382000000000005</v>
+      </c>
+      <c r="F358">
+        <v>1499</v>
+      </c>
+    </row>
+    <row r="359" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A359" t="s">
+        <v>19</v>
+      </c>
+      <c r="B359">
+        <v>0</v>
+      </c>
+      <c r="C359">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="D359">
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="E359">
+        <v>55.494999999999997</v>
+      </c>
+      <c r="F359">
+        <v>817</v>
+      </c>
+      <c r="G359" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="360" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A360" t="s">
+        <v>20</v>
+      </c>
+      <c r="B360">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C360">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="D360">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="E360">
+        <v>13.103</v>
+      </c>
+      <c r="F360">
+        <v>1033</v>
+      </c>
+    </row>
+    <row r="361" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A361" t="s">
+        <v>44</v>
+      </c>
+      <c r="B361">
+        <v>0</v>
+      </c>
+      <c r="C361">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D361">
+        <v>0.04</v>
+      </c>
+      <c r="E361">
+        <v>32.497999999999998</v>
+      </c>
+      <c r="F361">
+        <v>699</v>
+      </c>
+    </row>
+    <row r="362" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A362" t="s">
+        <v>21</v>
+      </c>
+      <c r="B362">
+        <v>0</v>
+      </c>
+      <c r="C362">
+        <v>0.02</v>
+      </c>
+      <c r="D362">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="E362">
+        <v>87.542000000000002</v>
+      </c>
+      <c r="F362">
+        <v>1288</v>
+      </c>
+    </row>
+    <row r="363" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A363" t="s">
+        <v>22</v>
+      </c>
+      <c r="B363">
+        <v>0.24</v>
+      </c>
+      <c r="C363">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D363">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="E363">
+        <v>23.725999999999999</v>
+      </c>
+      <c r="F363">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="364" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A364" t="s">
+        <v>23</v>
+      </c>
+      <c r="B364">
+        <v>0</v>
+      </c>
+      <c r="C364">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="D364">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="E364">
+        <v>156.83699999999999</v>
+      </c>
+      <c r="F364">
+        <v>2268</v>
+      </c>
+    </row>
+    <row r="365" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A365" t="s">
+        <v>24</v>
+      </c>
+      <c r="B365">
+        <v>0</v>
+      </c>
+      <c r="C365">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="D365">
+        <v>3.1E-2</v>
+      </c>
+      <c r="E365">
+        <v>18.861999999999998</v>
+      </c>
+      <c r="F365">
+        <v>816</v>
+      </c>
+    </row>
+    <row r="366" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A366" t="s">
+        <v>25</v>
+      </c>
+      <c r="B366">
+        <v>1E-3</v>
+      </c>
+      <c r="C366">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="D366">
+        <v>0.02</v>
+      </c>
+      <c r="E366">
+        <v>54.966999999999999</v>
+      </c>
+      <c r="F366">
+        <v>657</v>
+      </c>
+    </row>
+    <row r="367" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A367" t="s">
+        <v>45</v>
+      </c>
+      <c r="B367">
+        <v>0</v>
+      </c>
+      <c r="C367">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="D367">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="E367">
+        <v>64.676000000000002</v>
+      </c>
+      <c r="F367">
+        <v>827</v>
+      </c>
+    </row>
+    <row r="368" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A368" t="s">
+        <v>26</v>
+      </c>
+      <c r="B368">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C368">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D368">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="E368">
+        <v>16.079999999999998</v>
+      </c>
+      <c r="F368">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="369" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A369" t="s">
+        <v>46</v>
+      </c>
+      <c r="B369">
+        <v>0.41099999999999998</v>
+      </c>
+      <c r="C369">
+        <v>0</v>
+      </c>
+      <c r="D369">
+        <v>0</v>
+      </c>
+      <c r="E369">
+        <v>78.387</v>
+      </c>
+      <c r="F369">
+        <v>451</v>
+      </c>
+    </row>
+    <row r="370" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A370" t="s">
+        <v>27</v>
+      </c>
+      <c r="B370">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="C370">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D370">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="E370">
+        <v>34.905000000000001</v>
+      </c>
+      <c r="F370">
+        <v>512</v>
+      </c>
+    </row>
+    <row r="371" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A371" t="s">
+        <v>28</v>
+      </c>
+      <c r="B371">
+        <v>0.128</v>
+      </c>
+      <c r="C371">
+        <v>1E-3</v>
+      </c>
+      <c r="D371">
+        <v>2E-3</v>
+      </c>
+      <c r="E371">
+        <v>56.68</v>
+      </c>
+      <c r="F371">
+        <v>1114</v>
       </c>
     </row>
   </sheetData>
@@ -11011,4 +12820,1486 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AA33"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="5" max="5" width="9.6328125" customWidth="1"/>
+    <col min="6" max="6" width="10.7265625" customWidth="1"/>
+    <col min="7" max="7" width="10.26953125" customWidth="1"/>
+    <col min="15" max="15" width="15.54296875" customWidth="1"/>
+    <col min="19" max="19" width="9.90625" customWidth="1"/>
+    <col min="20" max="20" width="11.08984375" customWidth="1"/>
+    <col min="21" max="21" width="9.6328125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="O1">
+        <v>2019</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A2" s="1"/>
+      <c r="B2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="6"/>
+      <c r="O2" s="1"/>
+      <c r="P2" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3"/>
+      <c r="T2" s="3"/>
+      <c r="U2" s="3"/>
+      <c r="V2" s="3"/>
+      <c r="W2" s="3"/>
+      <c r="X2" s="3"/>
+      <c r="Y2" s="4"/>
+      <c r="Z2" s="5"/>
+      <c r="AA2" s="6"/>
+    </row>
+    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="D3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="E3" s="9"/>
+      <c r="F3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="G3" s="10"/>
+      <c r="H3" s="9"/>
+      <c r="I3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="J3" s="10"/>
+      <c r="K3" s="9"/>
+      <c r="L3" s="11"/>
+      <c r="M3" s="12"/>
+      <c r="O3" s="1"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="59" t="s">
+        <v>119</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>116</v>
+      </c>
+      <c r="S3" s="9"/>
+      <c r="T3" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="U3" s="10"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="X3" s="10"/>
+      <c r="Y3" s="9"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="12"/>
+    </row>
+    <row r="4" spans="1:27" ht="39.5" x14ac:dyDescent="0.35">
+      <c r="A4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4" s="60"/>
+      <c r="D4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="E4" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="F4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="G4" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="H4" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="I4" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="J4" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="K4" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="L4" s="18"/>
+      <c r="M4" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="O4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="P4" s="14" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q4" s="60"/>
+      <c r="R4" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="S4" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="T4" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="U4" s="17" t="s">
+        <v>123</v>
+      </c>
+      <c r="V4" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="W4" s="16" t="s">
+        <v>125</v>
+      </c>
+      <c r="X4" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y4" s="15" t="s">
+        <v>127</v>
+      </c>
+      <c r="Z4" s="18"/>
+      <c r="AA4" s="14" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" s="46"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="49"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="51"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
+      <c r="J5" s="51"/>
+      <c r="K5" s="49"/>
+      <c r="L5" s="52"/>
+      <c r="M5" s="46"/>
+      <c r="O5" s="19" t="s">
+        <v>42</v>
+      </c>
+      <c r="P5" s="20">
+        <v>0.16</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="R5" s="22">
+        <v>0</v>
+      </c>
+      <c r="S5" s="23"/>
+      <c r="T5" s="24">
+        <v>1E-3</v>
+      </c>
+      <c r="U5" s="25"/>
+      <c r="V5" s="23"/>
+      <c r="W5" s="26">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="23"/>
+      <c r="Z5" s="5"/>
+      <c r="AA5" s="27">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="53"/>
+      <c r="C6" s="54"/>
+      <c r="D6" s="55"/>
+      <c r="E6" s="56"/>
+      <c r="F6" s="57"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="56"/>
+      <c r="I6" s="57"/>
+      <c r="J6" s="58"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="52"/>
+      <c r="M6" s="53"/>
+      <c r="O6" s="28" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="29">
+        <v>2E-3</v>
+      </c>
+      <c r="Q6" s="30">
+        <v>3.9E-2</v>
+      </c>
+      <c r="R6" s="31">
+        <v>0.54300000000000004</v>
+      </c>
+      <c r="S6" s="32"/>
+      <c r="T6" s="33">
+        <v>1E-3</v>
+      </c>
+      <c r="U6" s="34"/>
+      <c r="V6" s="32"/>
+      <c r="W6" s="33">
+        <v>0</v>
+      </c>
+      <c r="X6" s="34"/>
+      <c r="Y6" s="32"/>
+      <c r="Z6" s="5"/>
+      <c r="AA6" s="35">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="53"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="55"/>
+      <c r="E7" s="56"/>
+      <c r="F7" s="57"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="56"/>
+      <c r="I7" s="57"/>
+      <c r="J7" s="58"/>
+      <c r="K7" s="56"/>
+      <c r="L7" s="52"/>
+      <c r="M7" s="53"/>
+      <c r="O7" s="28" t="s">
+        <v>18</v>
+      </c>
+      <c r="P7" s="29">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="Q7" s="30">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="R7" s="31">
+        <v>0.11</v>
+      </c>
+      <c r="S7" s="32"/>
+      <c r="T7" s="33">
+        <v>0</v>
+      </c>
+      <c r="U7" s="34"/>
+      <c r="V7" s="32"/>
+      <c r="W7" s="36"/>
+      <c r="X7" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="32"/>
+      <c r="Z7" s="5"/>
+      <c r="AA7" s="29">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A8" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="53"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
+      <c r="E8" s="56"/>
+      <c r="F8" s="57"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="56"/>
+      <c r="I8" s="57"/>
+      <c r="J8" s="58"/>
+      <c r="K8" s="56"/>
+      <c r="L8" s="52"/>
+      <c r="M8" s="53"/>
+      <c r="O8" s="28" t="s">
+        <v>43</v>
+      </c>
+      <c r="P8" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="39">
+        <v>0.13</v>
+      </c>
+      <c r="R8" s="31">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="S8" s="32"/>
+      <c r="T8" s="33">
+        <v>0</v>
+      </c>
+      <c r="U8" s="34"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="36"/>
+      <c r="X8" s="34"/>
+      <c r="Y8" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="5"/>
+      <c r="AA8" s="29">
+        <v>0.17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="53"/>
+      <c r="C9" s="54"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="56"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="58"/>
+      <c r="H9" s="56"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
+      <c r="K9" s="56"/>
+      <c r="L9" s="52"/>
+      <c r="M9" s="53"/>
+      <c r="O9" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="P9" s="35">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="Q9" s="39">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="R9" s="31">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="S9" s="32"/>
+      <c r="T9" s="36"/>
+      <c r="U9" s="41">
+        <v>0.04</v>
+      </c>
+      <c r="V9" s="32"/>
+      <c r="W9" s="36">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="X9" s="34"/>
+      <c r="Y9" s="32"/>
+      <c r="Z9" s="5"/>
+      <c r="AA9" s="29">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A10" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="53"/>
+      <c r="C10" s="54"/>
+      <c r="D10" s="55"/>
+      <c r="E10" s="56"/>
+      <c r="F10" s="57"/>
+      <c r="G10" s="58"/>
+      <c r="H10" s="56"/>
+      <c r="I10" s="57"/>
+      <c r="J10" s="58"/>
+      <c r="K10" s="56"/>
+      <c r="L10" s="52"/>
+      <c r="M10" s="53"/>
+      <c r="O10" s="28" t="s">
+        <v>24</v>
+      </c>
+      <c r="P10" s="29">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Q10" s="39">
+        <v>0.38</v>
+      </c>
+      <c r="R10" s="42">
+        <v>1E-3</v>
+      </c>
+      <c r="S10" s="32"/>
+      <c r="T10" s="36"/>
+      <c r="U10" s="41">
+        <v>2E-3</v>
+      </c>
+      <c r="V10" s="32"/>
+      <c r="W10" s="36">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="X10" s="34"/>
+      <c r="Y10" s="32"/>
+      <c r="Z10" s="5"/>
+      <c r="AA10" s="29">
+        <v>0.23799999999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A11" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="53"/>
+      <c r="C11" s="54"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="56"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="58"/>
+      <c r="H11" s="56"/>
+      <c r="I11" s="57"/>
+      <c r="J11" s="58"/>
+      <c r="K11" s="56"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="53"/>
+      <c r="O11" s="28" t="s">
+        <v>20</v>
+      </c>
+      <c r="P11" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="39">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="R11" s="42">
+        <v>0</v>
+      </c>
+      <c r="S11" s="32"/>
+      <c r="T11" s="36"/>
+      <c r="U11" s="37">
+        <v>0</v>
+      </c>
+      <c r="V11" s="32"/>
+      <c r="W11" s="36"/>
+      <c r="X11" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="32"/>
+      <c r="Z11" s="5"/>
+      <c r="AA11" s="29">
+        <v>0.191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="B12" s="53"/>
+      <c r="C12" s="54"/>
+      <c r="D12" s="55"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="57"/>
+      <c r="G12" s="58"/>
+      <c r="H12" s="56"/>
+      <c r="I12" s="57"/>
+      <c r="J12" s="58"/>
+      <c r="K12" s="56"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="53"/>
+      <c r="O12" s="28" t="s">
+        <v>44</v>
+      </c>
+      <c r="P12" s="35">
+        <v>0.187</v>
+      </c>
+      <c r="Q12" s="30">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="R12" s="31">
+        <v>0.621</v>
+      </c>
+      <c r="S12" s="32"/>
+      <c r="T12" s="36"/>
+      <c r="U12" s="41">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="V12" s="32"/>
+      <c r="W12" s="36"/>
+      <c r="X12" s="41">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y12" s="32"/>
+      <c r="Z12" s="5"/>
+      <c r="AA12" s="29">
+        <v>0.113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B13" s="53"/>
+      <c r="C13" s="54"/>
+      <c r="D13" s="55"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="58"/>
+      <c r="H13" s="56"/>
+      <c r="I13" s="57"/>
+      <c r="J13" s="58"/>
+      <c r="K13" s="56"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="53"/>
+      <c r="O13" s="28" t="s">
+        <v>7</v>
+      </c>
+      <c r="P13" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="39">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="R13" s="42">
+        <v>0</v>
+      </c>
+      <c r="S13" s="32"/>
+      <c r="T13" s="36"/>
+      <c r="U13" s="34"/>
+      <c r="V13" s="40">
+        <v>0</v>
+      </c>
+      <c r="W13" s="36"/>
+      <c r="X13" s="41">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="Y13" s="32"/>
+      <c r="Z13" s="5"/>
+      <c r="AA13" s="35">
+        <v>9.6000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A14" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="53"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="56"/>
+      <c r="F14" s="57"/>
+      <c r="G14" s="58"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="57"/>
+      <c r="J14" s="58"/>
+      <c r="K14" s="56"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="53"/>
+      <c r="O14" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="P14" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q14" s="30">
+        <v>2E-3</v>
+      </c>
+      <c r="R14" s="31">
+        <v>0.47699999999999998</v>
+      </c>
+      <c r="S14" s="32"/>
+      <c r="T14" s="36"/>
+      <c r="U14" s="34"/>
+      <c r="V14" s="32">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="W14" s="36"/>
+      <c r="X14" s="41">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="Y14" s="32"/>
+      <c r="Z14" s="5"/>
+      <c r="AA14" s="29">
+        <v>0.154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A15" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="53"/>
+      <c r="C15" s="54"/>
+      <c r="D15" s="55"/>
+      <c r="E15" s="56"/>
+      <c r="F15" s="57"/>
+      <c r="G15" s="58"/>
+      <c r="H15" s="56"/>
+      <c r="I15" s="57"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="56"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="53"/>
+      <c r="O15" s="28" t="s">
+        <v>45</v>
+      </c>
+      <c r="P15" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q15" s="43">
+        <v>0</v>
+      </c>
+      <c r="R15" s="31">
+        <v>0.66400000000000003</v>
+      </c>
+      <c r="S15" s="32"/>
+      <c r="T15" s="36"/>
+      <c r="U15" s="34"/>
+      <c r="V15" s="40">
+        <v>0</v>
+      </c>
+      <c r="W15" s="36"/>
+      <c r="X15" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="32"/>
+      <c r="Z15" s="5"/>
+      <c r="AA15" s="29">
+        <v>0.42099999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A16" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="53"/>
+      <c r="C16" s="54"/>
+      <c r="D16" s="55"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="57"/>
+      <c r="G16" s="58"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="57"/>
+      <c r="J16" s="58"/>
+      <c r="K16" s="56"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="53"/>
+      <c r="O16" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="P16" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="30">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="R16" s="31">
+        <v>0.307</v>
+      </c>
+      <c r="S16" s="32"/>
+      <c r="T16" s="36"/>
+      <c r="U16" s="34"/>
+      <c r="V16" s="40">
+        <v>0</v>
+      </c>
+      <c r="W16" s="33">
+        <v>0</v>
+      </c>
+      <c r="X16" s="34"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="5"/>
+      <c r="AA16" s="29">
+        <v>0.252</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="B17" s="53"/>
+      <c r="C17" s="54"/>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="58"/>
+      <c r="H17" s="56"/>
+      <c r="I17" s="57"/>
+      <c r="J17" s="58"/>
+      <c r="K17" s="56"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="53"/>
+      <c r="O17" s="28" t="s">
+        <v>22</v>
+      </c>
+      <c r="P17" s="35">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="Q17" s="39"/>
+      <c r="R17" s="31">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="S17" s="32"/>
+      <c r="T17" s="36"/>
+      <c r="U17" s="34"/>
+      <c r="V17" s="44">
+        <v>0.01</v>
+      </c>
+      <c r="W17" s="45">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="X17" s="34"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="5"/>
+      <c r="AA17" s="29">
+        <v>0.125</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="53"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="55"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="57"/>
+      <c r="G18" s="58"/>
+      <c r="H18" s="56"/>
+      <c r="I18" s="57"/>
+      <c r="J18" s="58"/>
+      <c r="K18" s="56"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="53"/>
+      <c r="O18" s="28" t="s">
+        <v>10</v>
+      </c>
+      <c r="P18" s="35">
+        <v>0.753</v>
+      </c>
+      <c r="Q18" s="39">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="R18" s="42">
+        <v>0</v>
+      </c>
+      <c r="S18" s="32"/>
+      <c r="T18" s="36"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="32">
+        <v>9.4E-2</v>
+      </c>
+      <c r="W18" s="36"/>
+      <c r="X18" s="34"/>
+      <c r="Y18" s="32">
+        <v>0.25800000000000001</v>
+      </c>
+      <c r="Z18" s="5"/>
+      <c r="AA18" s="29">
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" s="53"/>
+      <c r="C19" s="54"/>
+      <c r="D19" s="55"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="58"/>
+      <c r="K19" s="56"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="53"/>
+      <c r="O19" s="28" t="s">
+        <v>16</v>
+      </c>
+      <c r="P19" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q19" s="30">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="R19" s="31"/>
+      <c r="S19" s="44">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="T19" s="33">
+        <v>0</v>
+      </c>
+      <c r="U19" s="34"/>
+      <c r="V19" s="32"/>
+      <c r="W19" s="36"/>
+      <c r="X19" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="5"/>
+      <c r="AA19" s="29">
+        <v>0.21199999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="53"/>
+      <c r="C20" s="54"/>
+      <c r="D20" s="55"/>
+      <c r="E20" s="56"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="56"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="58"/>
+      <c r="K20" s="56"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="53"/>
+      <c r="O20" s="28" t="s">
+        <v>26</v>
+      </c>
+      <c r="P20" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q20" s="39">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="R20" s="31"/>
+      <c r="S20" s="32">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="T20" s="45">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="U20" s="34"/>
+      <c r="V20" s="32"/>
+      <c r="W20" s="36"/>
+      <c r="X20" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="5"/>
+      <c r="AA20" s="29">
+        <v>0.38500000000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A21" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="B21" s="53"/>
+      <c r="C21" s="54"/>
+      <c r="D21" s="55"/>
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="56"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="58"/>
+      <c r="K21" s="56"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="53"/>
+      <c r="O21" s="28" t="s">
+        <v>41</v>
+      </c>
+      <c r="P21" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q21" s="39"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="32">
+        <v>0.158</v>
+      </c>
+      <c r="T21" s="33">
+        <v>0</v>
+      </c>
+      <c r="U21" s="34"/>
+      <c r="V21" s="32"/>
+      <c r="W21" s="36"/>
+      <c r="X21" s="34"/>
+      <c r="Y21" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="5"/>
+      <c r="AA21" s="35">
+        <v>9.2999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A22" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="B22" s="53"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="55"/>
+      <c r="E22" s="56"/>
+      <c r="F22" s="57"/>
+      <c r="G22" s="58"/>
+      <c r="H22" s="56"/>
+      <c r="I22" s="57"/>
+      <c r="J22" s="58"/>
+      <c r="K22" s="56"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="53"/>
+      <c r="O22" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="P22" s="35">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="Q22" s="39">
+        <v>0.996</v>
+      </c>
+      <c r="R22" s="31"/>
+      <c r="S22" s="32">
+        <v>0.161</v>
+      </c>
+      <c r="T22" s="36"/>
+      <c r="U22" s="37">
+        <v>0</v>
+      </c>
+      <c r="V22" s="32"/>
+      <c r="W22" s="36"/>
+      <c r="X22" s="34"/>
+      <c r="Y22" s="32">
+        <v>0.25900000000000001</v>
+      </c>
+      <c r="Z22" s="5"/>
+      <c r="AA22" s="35">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A23" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="53"/>
+      <c r="C23" s="54"/>
+      <c r="D23" s="55"/>
+      <c r="E23" s="56"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="58"/>
+      <c r="H23" s="56"/>
+      <c r="I23" s="57"/>
+      <c r="J23" s="58"/>
+      <c r="K23" s="56"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="53"/>
+      <c r="O23" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="P23" s="35">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Q23" s="39">
+        <v>0.113</v>
+      </c>
+      <c r="R23" s="31"/>
+      <c r="S23" s="44">
+        <v>2.3E-2</v>
+      </c>
+      <c r="T23" s="36"/>
+      <c r="U23" s="41">
+        <v>1.4E-2</v>
+      </c>
+      <c r="V23" s="32"/>
+      <c r="W23" s="36"/>
+      <c r="X23" s="34"/>
+      <c r="Y23" s="40">
+        <v>1E-3</v>
+      </c>
+      <c r="Z23" s="5"/>
+      <c r="AA23" s="29">
+        <v>0.22600000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" s="53"/>
+      <c r="C24" s="54"/>
+      <c r="D24" s="55"/>
+      <c r="E24" s="56"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="58"/>
+      <c r="H24" s="56"/>
+      <c r="I24" s="57"/>
+      <c r="J24" s="58"/>
+      <c r="K24" s="56"/>
+      <c r="L24" s="52"/>
+      <c r="M24" s="53"/>
+      <c r="O24" s="28" t="s">
+        <v>6</v>
+      </c>
+      <c r="P24" s="35">
+        <v>1</v>
+      </c>
+      <c r="Q24" s="39">
+        <v>0.63900000000000001</v>
+      </c>
+      <c r="R24" s="31"/>
+      <c r="S24" s="44">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="T24" s="36"/>
+      <c r="U24" s="37">
+        <v>0</v>
+      </c>
+      <c r="V24" s="32"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="34"/>
+      <c r="Y24" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="5"/>
+      <c r="AA24" s="29">
+        <v>0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A25" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="53"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="55"/>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="56"/>
+      <c r="I25" s="57"/>
+      <c r="J25" s="58"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="52"/>
+      <c r="M25" s="53"/>
+      <c r="O25" s="28" t="s">
+        <v>23</v>
+      </c>
+      <c r="P25" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q25" s="39">
+        <v>0.61899999999999999</v>
+      </c>
+      <c r="R25" s="31"/>
+      <c r="S25" s="32">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="T25" s="36"/>
+      <c r="U25" s="37">
+        <v>0</v>
+      </c>
+      <c r="V25" s="32"/>
+      <c r="W25" s="36"/>
+      <c r="X25" s="34"/>
+      <c r="Y25" s="40">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="5"/>
+      <c r="AA25" s="29">
+        <v>0.17199999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="53"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="55"/>
+      <c r="E26" s="56"/>
+      <c r="F26" s="57"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="56"/>
+      <c r="I26" s="57"/>
+      <c r="J26" s="58"/>
+      <c r="K26" s="56"/>
+      <c r="L26" s="52"/>
+      <c r="M26" s="53"/>
+      <c r="O26" s="28" t="s">
+        <v>12</v>
+      </c>
+      <c r="P26" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q26" s="39"/>
+      <c r="R26" s="31"/>
+      <c r="S26" s="32">
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="T26" s="36"/>
+      <c r="U26" s="37">
+        <v>0</v>
+      </c>
+      <c r="V26" s="32"/>
+      <c r="W26" s="33">
+        <v>0</v>
+      </c>
+      <c r="X26" s="34"/>
+      <c r="Y26" s="32"/>
+      <c r="Z26" s="5"/>
+      <c r="AA26" s="35">
+        <v>9.0999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A27" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="B27" s="53"/>
+      <c r="C27" s="54"/>
+      <c r="D27" s="55"/>
+      <c r="E27" s="56"/>
+      <c r="F27" s="57"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="56"/>
+      <c r="I27" s="57"/>
+      <c r="J27" s="58"/>
+      <c r="K27" s="56"/>
+      <c r="L27" s="52"/>
+      <c r="M27" s="53"/>
+      <c r="O27" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="P27" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q27" s="39"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="40">
+        <v>0</v>
+      </c>
+      <c r="T27" s="36"/>
+      <c r="U27" s="37">
+        <v>0</v>
+      </c>
+      <c r="V27" s="32"/>
+      <c r="W27" s="33">
+        <v>0</v>
+      </c>
+      <c r="X27" s="34"/>
+      <c r="Y27" s="32"/>
+      <c r="Z27" s="5"/>
+      <c r="AA27" s="29">
+        <v>0.20799999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A28" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="B28" s="53"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="55"/>
+      <c r="E28" s="56"/>
+      <c r="F28" s="57"/>
+      <c r="G28" s="58"/>
+      <c r="H28" s="56"/>
+      <c r="I28" s="57"/>
+      <c r="J28" s="58"/>
+      <c r="K28" s="56"/>
+      <c r="L28" s="52"/>
+      <c r="M28" s="53"/>
+      <c r="O28" s="28" t="s">
+        <v>19</v>
+      </c>
+      <c r="P28" s="38">
+        <v>1E-3</v>
+      </c>
+      <c r="Q28" s="39"/>
+      <c r="R28" s="31"/>
+      <c r="S28" s="40">
+        <v>0</v>
+      </c>
+      <c r="T28" s="36"/>
+      <c r="U28" s="37">
+        <v>0</v>
+      </c>
+      <c r="V28" s="32"/>
+      <c r="W28" s="33">
+        <v>0</v>
+      </c>
+      <c r="X28" s="34"/>
+      <c r="Y28" s="32"/>
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="35">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A29" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" s="53"/>
+      <c r="C29" s="54"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="56"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="56"/>
+      <c r="I29" s="57"/>
+      <c r="J29" s="58"/>
+      <c r="K29" s="56"/>
+      <c r="L29" s="52"/>
+      <c r="M29" s="53"/>
+      <c r="O29" s="28" t="s">
+        <v>17</v>
+      </c>
+      <c r="P29" s="35">
+        <v>0.69</v>
+      </c>
+      <c r="Q29" s="39">
+        <v>0.75</v>
+      </c>
+      <c r="R29" s="31"/>
+      <c r="S29" s="44">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="T29" s="36"/>
+      <c r="U29" s="34"/>
+      <c r="V29" s="40">
+        <v>0</v>
+      </c>
+      <c r="W29" s="33">
+        <v>0</v>
+      </c>
+      <c r="X29" s="34"/>
+      <c r="Y29" s="32"/>
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="29">
+        <v>0.32200000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A30" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="B30" s="53"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="55"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="57"/>
+      <c r="G30" s="58"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="57"/>
+      <c r="J30" s="58"/>
+      <c r="K30" s="56"/>
+      <c r="L30" s="52"/>
+      <c r="M30" s="53"/>
+      <c r="O30" s="28" t="s">
+        <v>27</v>
+      </c>
+      <c r="P30" s="35">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="Q30" s="39">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="R30" s="31"/>
+      <c r="S30" s="32">
+        <v>0.436</v>
+      </c>
+      <c r="T30" s="36"/>
+      <c r="U30" s="34"/>
+      <c r="V30" s="44">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="W30" s="36">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="X30" s="34"/>
+      <c r="Y30" s="32"/>
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="29">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="53"/>
+      <c r="C31" s="54"/>
+      <c r="D31" s="55"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="57"/>
+      <c r="G31" s="58"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="57"/>
+      <c r="J31" s="58"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="52"/>
+      <c r="M31" s="53"/>
+      <c r="O31" s="28" t="s">
+        <v>11</v>
+      </c>
+      <c r="P31" s="38">
+        <v>0</v>
+      </c>
+      <c r="Q31" s="39">
+        <v>0.38</v>
+      </c>
+      <c r="R31" s="31"/>
+      <c r="S31" s="44">
+        <v>1.4E-2</v>
+      </c>
+      <c r="T31" s="36"/>
+      <c r="U31" s="34"/>
+      <c r="V31" s="40">
+        <v>0</v>
+      </c>
+      <c r="W31" s="36"/>
+      <c r="X31" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y31" s="32"/>
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="29">
+        <v>0.106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A32" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="53"/>
+      <c r="C32" s="54"/>
+      <c r="D32" s="55"/>
+      <c r="E32" s="56"/>
+      <c r="F32" s="57"/>
+      <c r="G32" s="58"/>
+      <c r="H32" s="56"/>
+      <c r="I32" s="57"/>
+      <c r="J32" s="58"/>
+      <c r="K32" s="56"/>
+      <c r="L32" s="52"/>
+      <c r="M32" s="53"/>
+      <c r="O32" s="28" t="s">
+        <v>15</v>
+      </c>
+      <c r="P32" s="29">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Q32" s="39">
+        <v>0.214</v>
+      </c>
+      <c r="R32" s="31"/>
+      <c r="S32" s="44">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="T32" s="36"/>
+      <c r="U32" s="34"/>
+      <c r="V32" s="40">
+        <v>0</v>
+      </c>
+      <c r="W32" s="36"/>
+      <c r="X32" s="37">
+        <v>0</v>
+      </c>
+      <c r="Y32" s="32"/>
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="29">
+        <v>0.30199999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="A33" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" s="53"/>
+      <c r="C33" s="54"/>
+      <c r="D33" s="55"/>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="58"/>
+      <c r="H33" s="56"/>
+      <c r="I33" s="57"/>
+      <c r="J33" s="58"/>
+      <c r="K33" s="56"/>
+      <c r="L33" s="52"/>
+      <c r="M33" s="53"/>
+      <c r="O33" s="28" t="s">
+        <v>25</v>
+      </c>
+      <c r="P33" s="35">
+        <v>0.54600000000000004</v>
+      </c>
+      <c r="Q33" s="30">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="R33" s="31"/>
+      <c r="S33" s="32">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="T33" s="36"/>
+      <c r="U33" s="34"/>
+      <c r="V33" s="44">
+        <v>0.02</v>
+      </c>
+      <c r="W33" s="36"/>
+      <c r="X33" s="41">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="Y33" s="32"/>
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="29">
+        <v>0.20300000000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="10">
+    <mergeCell ref="B2:K2"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="F3:H3"/>
+    <mergeCell ref="I3:K3"/>
+    <mergeCell ref="P2:Y2"/>
+    <mergeCell ref="R3:S3"/>
+    <mergeCell ref="T3:V3"/>
+    <mergeCell ref="W3:Y3"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="Q3:Q4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Resolved multiple assessment years issue
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="868" uniqueCount="132">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="906" uniqueCount="133">
   <si>
     <t>Species</t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>2019 Local abundance</t>
+  </si>
+  <si>
+    <t>better than best model without Fproxy and Total biomass</t>
   </si>
 </sst>
 </file>
@@ -1569,6 +1572,30 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="36" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1597,30 +1624,6 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="36" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
@@ -1668,7 +1671,35 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="16">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -2031,7 +2062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M371"/>
   <sheetViews>
-    <sheetView topLeftCell="A313" workbookViewId="0">
+    <sheetView topLeftCell="A314" workbookViewId="0">
       <selection activeCell="F68" sqref="F68"/>
     </sheetView>
   </sheetViews>
@@ -13520,28 +13551,28 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D116 D118:D1048576">
-    <cfRule type="cellIs" dxfId="11" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B116 B118:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13552,20 +13583,20 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="L21" sqref="L21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -13600,7 +13631,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -13635,7 +13666,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -13670,7 +13701,7 @@
         <v>1019</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -13705,7 +13736,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -13740,7 +13771,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -13775,472 +13806,656 @@
         <v>423</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C8">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8">
+        <v>0</v>
+      </c>
+      <c r="H8">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="I8">
+        <v>0.19500000000000001</v>
+      </c>
+      <c r="J8">
+        <v>57.094000000000001</v>
+      </c>
+      <c r="K8">
+        <v>864</v>
+      </c>
+      <c r="L8" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>12</v>
+      </c>
+      <c r="B9">
+        <v>1E-3</v>
+      </c>
+      <c r="C9">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="D9">
+        <v>0.63200000000000001</v>
+      </c>
+      <c r="E9">
+        <v>6.3E-2</v>
+      </c>
+      <c r="F9">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="H9">
+        <v>0.08</v>
+      </c>
+      <c r="I9">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="J9">
+        <v>15.787000000000001</v>
+      </c>
+      <c r="K9">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
         <v>13</v>
       </c>
-      <c r="B8">
+      <c r="B10">
+        <v>0.628</v>
+      </c>
+      <c r="C10">
+        <v>0.82799999999999996</v>
+      </c>
+      <c r="D10">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="E10">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="F10">
+        <v>2E-3</v>
+      </c>
+      <c r="G10">
+        <v>0.05</v>
+      </c>
+      <c r="H10">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="I10">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="J10">
+        <v>13.131</v>
+      </c>
+      <c r="K10">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11">
+        <v>0.41699999999999998</v>
+      </c>
+      <c r="C11">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D11">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="E11">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="F11">
+        <v>0.443</v>
+      </c>
+      <c r="G11">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="H11">
+        <v>0.03</v>
+      </c>
+      <c r="I11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="J11">
+        <v>24.696000000000002</v>
+      </c>
+      <c r="K11">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>0.126</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="E12">
+        <v>3.1E-2</v>
+      </c>
+      <c r="F12">
+        <v>0.49399999999999999</v>
+      </c>
+      <c r="G12">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="H12">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="I12">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="J12">
+        <v>13.784000000000001</v>
+      </c>
+      <c r="K12">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
         <v>1</v>
       </c>
-      <c r="C8">
-        <v>0.16700000000000001</v>
-      </c>
-      <c r="D8">
-        <v>0.20799999999999999</v>
-      </c>
-      <c r="E8">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>4.2999999999999997E-2</v>
-      </c>
-      <c r="H8">
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="I13">
+        <v>0.154</v>
+      </c>
+      <c r="J13">
+        <v>57.262999999999998</v>
+      </c>
+      <c r="K13">
+        <v>1137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>17</v>
+      </c>
+      <c r="B14">
+        <v>0.999</v>
+      </c>
+      <c r="C14">
+        <v>0.41</v>
+      </c>
+      <c r="D14">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E14">
+        <v>0.21099999999999999</v>
+      </c>
+      <c r="F14">
+        <v>0</v>
+      </c>
+      <c r="G14">
+        <v>0.01</v>
+      </c>
+      <c r="H14">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="I14">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="J14">
+        <v>21.567</v>
+      </c>
+      <c r="K14">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>18</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="F15">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="G15">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="H15">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="I15">
+        <v>8.6999999999999994E-2</v>
+      </c>
+      <c r="J15">
+        <v>12.635</v>
+      </c>
+      <c r="K15">
+        <v>1098</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>19</v>
+      </c>
+      <c r="B16">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="C16">
+        <v>1.6E-2</v>
+      </c>
+      <c r="D16">
+        <v>0.68300000000000005</v>
+      </c>
+      <c r="E16">
+        <v>2E-3</v>
+      </c>
+      <c r="F16">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G16">
         <v>8.5999999999999993E-2</v>
       </c>
-      <c r="I8">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="J8">
-        <v>12.574999999999999</v>
-      </c>
-      <c r="K8">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9">
-        <v>0.65200000000000002</v>
-      </c>
-      <c r="C9">
-        <v>1.2999999999999999E-2</v>
-      </c>
-      <c r="D9">
-        <v>0.59599999999999997</v>
-      </c>
-      <c r="E9">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="F9">
-        <v>0.23</v>
-      </c>
-      <c r="G9">
-        <v>0.80900000000000005</v>
-      </c>
-      <c r="H9">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="I9">
-        <v>5.2999999999999999E-2</v>
-      </c>
-      <c r="J9">
-        <v>24.509</v>
-      </c>
-      <c r="K9">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="C10">
+      <c r="H16">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="I16">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="J16">
+        <v>47.557000000000002</v>
+      </c>
+      <c r="K16">
+        <v>443</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="C17">
+        <v>0.52400000000000002</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+      <c r="G17">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="H17">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="I17">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="J17">
+        <v>11.029</v>
+      </c>
+      <c r="K17">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>44</v>
+      </c>
+      <c r="B18">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C18">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0.89400000000000002</v>
+      </c>
+      <c r="F18">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0</v>
+      </c>
+      <c r="H18">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="I18">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="J18">
+        <v>21.541</v>
+      </c>
+      <c r="K18">
+        <v>439</v>
+      </c>
+      <c r="L18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19">
+        <v>0</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>0</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0</v>
+      </c>
+      <c r="G19">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="H19">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="I19">
+        <v>0.215</v>
+      </c>
+      <c r="J19">
+        <v>65.866</v>
+      </c>
+      <c r="K19">
+        <v>977</v>
+      </c>
+      <c r="L19" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20">
+        <v>0.65500000000000003</v>
+      </c>
+      <c r="C20">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="D20">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="E20">
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="F20">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="G20">
+        <v>0.627</v>
+      </c>
+      <c r="H20">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="I20">
+        <v>0.06</v>
+      </c>
+      <c r="J20">
+        <v>25.577999999999999</v>
+      </c>
+      <c r="K20">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21">
+        <v>0</v>
+      </c>
+      <c r="C21">
+        <v>1.7999999999999999E-2</v>
+      </c>
+      <c r="D21">
+        <v>0</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
         <v>1E-3</v>
       </c>
-      <c r="D10">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="E10">
-        <v>4.7E-2</v>
-      </c>
-      <c r="F10">
-        <v>0.78400000000000003</v>
-      </c>
-      <c r="G10">
-        <v>6.2E-2</v>
-      </c>
-      <c r="H10">
-        <v>7.0999999999999994E-2</v>
-      </c>
-      <c r="I10">
-        <v>8.5999999999999993E-2</v>
-      </c>
-      <c r="J10">
-        <v>13.86</v>
-      </c>
-      <c r="K10">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>16</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
-      </c>
-      <c r="C11">
+      <c r="G21">
+        <v>0</v>
+      </c>
+      <c r="H21">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I21">
+        <v>0.16600000000000001</v>
+      </c>
+      <c r="J21">
+        <v>122.947</v>
+      </c>
+      <c r="K21">
+        <v>1459</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22">
         <v>1</v>
       </c>
-      <c r="D11">
-        <v>0</v>
-      </c>
-      <c r="E11">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-      <c r="H11">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="I11">
-        <v>0.154</v>
-      </c>
-      <c r="J11">
-        <v>57.262999999999998</v>
-      </c>
-      <c r="K11">
-        <v>1137</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
-      </c>
-      <c r="C12">
-        <v>0.34699999999999998</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0.42899999999999999</v>
-      </c>
-      <c r="F12">
-        <v>0.64200000000000002</v>
-      </c>
-      <c r="G12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H12">
+      <c r="C22">
+        <v>1.4E-2</v>
+      </c>
+      <c r="D22">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="E22">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="F22">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G22">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="H22">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="I22">
         <v>7.6999999999999999E-2</v>
       </c>
-      <c r="I12">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="J12">
-        <v>12.635</v>
-      </c>
-      <c r="K12">
-        <v>1098</v>
-      </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13">
-        <v>0.29599999999999999</v>
-      </c>
-      <c r="C13">
-        <v>2.4E-2</v>
-      </c>
-      <c r="D13">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="E13">
-        <v>0</v>
-      </c>
-      <c r="F13">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="G13">
-        <v>0.16</v>
-      </c>
-      <c r="H13">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="I13">
-        <v>0.1</v>
-      </c>
-      <c r="J13">
-        <v>47.225000000000001</v>
-      </c>
-      <c r="K13">
-        <v>440</v>
-      </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14">
-        <v>4.0000000000000001E-3</v>
-      </c>
-      <c r="C14">
+      <c r="J22">
+        <v>14.313000000000001</v>
+      </c>
+      <c r="K22">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23">
+        <v>0.63400000000000001</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0.93</v>
+      </c>
+      <c r="E23">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="F23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="G23">
+        <v>0.437</v>
+      </c>
+      <c r="H23">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="I23">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J23">
+        <v>41.485999999999997</v>
+      </c>
+      <c r="K23">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24">
+        <v>0</v>
+      </c>
+      <c r="C24">
+        <v>0.70699999999999996</v>
+      </c>
+      <c r="D24">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="E24">
+        <v>0.373</v>
+      </c>
+      <c r="F24">
+        <v>0</v>
+      </c>
+      <c r="G24">
+        <v>0</v>
+      </c>
+      <c r="H24">
+        <v>0.09</v>
+      </c>
+      <c r="I24">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="J24">
+        <v>12.634</v>
+      </c>
+      <c r="K24">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25">
         <v>0.56899999999999995</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-      <c r="G14">
-        <v>1.7000000000000001E-2</v>
-      </c>
-      <c r="H14">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="I14">
-        <v>0.106</v>
-      </c>
-      <c r="J14">
-        <v>11.151</v>
-      </c>
-      <c r="K14">
-        <v>695</v>
-      </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>0.65500000000000003</v>
-      </c>
-      <c r="C15">
-        <v>6.9000000000000006E-2</v>
-      </c>
-      <c r="D15">
-        <v>4.1000000000000002E-2</v>
-      </c>
-      <c r="E15">
+      <c r="C25">
+        <v>0.38900000000000001</v>
+      </c>
+      <c r="D25">
         <v>3.2000000000000001E-2</v>
       </c>
-      <c r="F15">
-        <v>0.48499999999999999</v>
-      </c>
-      <c r="G15">
-        <v>0.627</v>
-      </c>
-      <c r="H15">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="I15">
-        <v>0.06</v>
-      </c>
-      <c r="J15">
-        <v>25.577999999999999</v>
-      </c>
-      <c r="K15">
-        <v>303</v>
-      </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>0</v>
-      </c>
-      <c r="C16">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-      <c r="F16">
-        <v>1E-3</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-      <c r="H16">
-        <v>0.14699999999999999</v>
-      </c>
-      <c r="I16">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="J16">
-        <v>122.947</v>
-      </c>
-      <c r="K16">
-        <v>1459</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>1</v>
-      </c>
-      <c r="C17">
-        <v>1.4E-2</v>
-      </c>
-      <c r="D17">
-        <v>0.36399999999999999</v>
-      </c>
-      <c r="E17">
-        <v>0.14399999999999999</v>
-      </c>
-      <c r="F17">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="G17">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="H17">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="I17">
-        <v>7.6999999999999999E-2</v>
-      </c>
-      <c r="J17">
-        <v>14.313000000000001</v>
-      </c>
-      <c r="K17">
-        <v>293</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18">
-        <v>0.63400000000000001</v>
-      </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18">
-        <v>0.93</v>
-      </c>
-      <c r="E18">
-        <v>0.66800000000000004</v>
-      </c>
-      <c r="F18">
-        <v>8.9999999999999993E-3</v>
-      </c>
-      <c r="G18">
-        <v>0.437</v>
-      </c>
-      <c r="H18">
-        <v>5.8000000000000003E-2</v>
-      </c>
-      <c r="I18">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="J18">
-        <v>41.485999999999997</v>
-      </c>
-      <c r="K18">
-        <v>173</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19">
-        <v>0</v>
-      </c>
-      <c r="C19">
-        <v>0.70699999999999996</v>
-      </c>
-      <c r="D19">
-        <v>0.85399999999999998</v>
-      </c>
-      <c r="E19">
-        <v>0.373</v>
-      </c>
-      <c r="F19">
-        <v>0</v>
-      </c>
-      <c r="G19">
-        <v>0</v>
-      </c>
-      <c r="H19">
-        <v>0.09</v>
-      </c>
-      <c r="I19">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="J19">
-        <v>12.634</v>
-      </c>
-      <c r="K19">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.35">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
-        <v>0.56899999999999995</v>
-      </c>
-      <c r="C20">
-        <v>0.38900000000000001</v>
-      </c>
-      <c r="D20">
-        <v>3.2000000000000001E-2</v>
-      </c>
-      <c r="E20">
+      <c r="E25">
         <v>0.63800000000000001</v>
       </c>
-      <c r="F20">
+      <c r="F25">
         <v>1.9E-2</v>
       </c>
-      <c r="G20">
+      <c r="G25">
         <v>0.34300000000000003</v>
       </c>
-      <c r="H20">
+      <c r="H25">
         <v>2.9000000000000001E-2</v>
       </c>
-      <c r="I20">
+      <c r="I25">
         <v>4.3999999999999997E-2</v>
       </c>
-      <c r="J20">
+      <c r="J25">
         <v>30.338999999999999</v>
       </c>
-      <c r="K20">
+      <c r="K25">
         <v>340</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="cellIs" dxfId="5" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14251,10 +14466,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AC33"/>
+  <dimension ref="A1:AK33"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView topLeftCell="P19" workbookViewId="0">
+      <selection activeCell="P20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -14269,105 +14484,105 @@
     <col min="23" max="23" width="9.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:37" x14ac:dyDescent="0.35">
       <c r="Q1">
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="54" t="s">
+      <c r="B2" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
-      <c r="K2" s="55"/>
-      <c r="L2" s="55"/>
-      <c r="M2" s="56"/>
+      <c r="C2" s="63"/>
+      <c r="D2" s="63"/>
+      <c r="E2" s="63"/>
+      <c r="F2" s="63"/>
+      <c r="G2" s="63"/>
+      <c r="H2" s="63"/>
+      <c r="I2" s="63"/>
+      <c r="J2" s="63"/>
+      <c r="K2" s="63"/>
+      <c r="L2" s="63"/>
+      <c r="M2" s="64"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="54" t="s">
+      <c r="R2" s="62" t="s">
         <v>114</v>
       </c>
-      <c r="S2" s="55"/>
-      <c r="T2" s="55"/>
-      <c r="U2" s="55"/>
-      <c r="V2" s="55"/>
-      <c r="W2" s="55"/>
-      <c r="X2" s="55"/>
-      <c r="Y2" s="55"/>
-      <c r="Z2" s="55"/>
-      <c r="AA2" s="56"/>
+      <c r="S2" s="63"/>
+      <c r="T2" s="63"/>
+      <c r="U2" s="63"/>
+      <c r="V2" s="63"/>
+      <c r="W2" s="63"/>
+      <c r="X2" s="63"/>
+      <c r="Y2" s="63"/>
+      <c r="Z2" s="63"/>
+      <c r="AA2" s="64"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="68" t="s">
         <v>118</v>
       </c>
-      <c r="D3" s="62" t="s">
+      <c r="D3" s="70" t="s">
         <v>47</v>
       </c>
-      <c r="E3" s="60" t="s">
+      <c r="E3" s="68" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="57" t="s">
+      <c r="F3" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="G3" s="58"/>
-      <c r="H3" s="57" t="s">
+      <c r="G3" s="66"/>
+      <c r="H3" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="I3" s="59"/>
-      <c r="J3" s="58"/>
-      <c r="K3" s="57" t="s">
+      <c r="I3" s="67"/>
+      <c r="J3" s="66"/>
+      <c r="K3" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="L3" s="59"/>
-      <c r="M3" s="58"/>
+      <c r="L3" s="67"/>
+      <c r="M3" s="66"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="60" t="s">
+      <c r="S3" s="68" t="s">
         <v>118</v>
       </c>
-      <c r="T3" s="57" t="s">
+      <c r="T3" s="65" t="s">
         <v>115</v>
       </c>
-      <c r="U3" s="58"/>
-      <c r="V3" s="57" t="s">
+      <c r="U3" s="66"/>
+      <c r="V3" s="65" t="s">
         <v>116</v>
       </c>
-      <c r="W3" s="59"/>
-      <c r="X3" s="58"/>
-      <c r="Y3" s="57" t="s">
+      <c r="W3" s="67"/>
+      <c r="X3" s="66"/>
+      <c r="Y3" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="Z3" s="59"/>
-      <c r="AA3" s="58"/>
+      <c r="Z3" s="67"/>
+      <c r="AA3" s="66"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
     </row>
-    <row r="4" spans="1:29" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:37" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C4" s="61"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="61"/>
+      <c r="C4" s="69"/>
+      <c r="D4" s="71"/>
+      <c r="E4" s="69"/>
       <c r="F4" s="10" t="s">
         <v>119</v>
       </c>
@@ -14402,7 +14617,7 @@
       <c r="R4" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="61"/>
+      <c r="S4" s="69"/>
       <c r="T4" s="10" t="s">
         <v>119</v>
       </c>
@@ -14431,25 +14646,46 @@
       <c r="AC4" s="8" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>122</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>2</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
       <c r="B5" s="40">
         <v>0.107</v>
       </c>
-      <c r="C5" s="64"/>
-      <c r="D5" s="64">
+      <c r="C5" s="54"/>
+      <c r="D5" s="54">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E5" s="65">
+      <c r="E5" s="55">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F5" s="70">
+      <c r="F5" s="60">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="G5" s="68"/>
+      <c r="G5" s="58"/>
       <c r="H5" s="43"/>
       <c r="I5" s="41">
         <v>0.01</v>
@@ -14491,25 +14727,46 @@
       <c r="AC5" s="21">
         <v>0.10100000000000001</v>
       </c>
-    </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AF5">
+        <v>0.12</v>
+      </c>
+      <c r="AG5">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AH5">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="AI5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>8.1000000000000003E-2</v>
+      </c>
+      <c r="AK5">
+        <v>0.10100000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>7</v>
       </c>
       <c r="B6" s="46">
         <v>2.4E-2</v>
       </c>
-      <c r="C6" s="66"/>
-      <c r="D6" s="66">
+      <c r="C6" s="56"/>
+      <c r="D6" s="56">
         <v>1E-3</v>
       </c>
-      <c r="E6" s="67">
+      <c r="E6" s="57">
         <v>1E-3</v>
       </c>
-      <c r="F6" s="71">
+      <c r="F6" s="61">
         <v>1</v>
       </c>
-      <c r="G6" s="69"/>
+      <c r="G6" s="59"/>
       <c r="H6" s="50"/>
       <c r="I6" s="48">
         <v>0.47599999999999998</v>
@@ -14551,25 +14808,46 @@
       <c r="AC6" s="29">
         <v>7.1999999999999995E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE6" t="s">
+        <v>7</v>
+      </c>
+      <c r="AF6">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AG6">
+        <v>0</v>
+      </c>
+      <c r="AH6">
+        <v>0.02</v>
+      </c>
+      <c r="AI6">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="AJ6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AK6">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
       <c r="B7" s="46">
         <v>0</v>
       </c>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66">
+      <c r="C7" s="56"/>
+      <c r="D7" s="56">
         <v>3.0000000000000001E-3</v>
       </c>
-      <c r="E7" s="67">
+      <c r="E7" s="57">
         <v>4.0000000000000001E-3</v>
       </c>
-      <c r="F7" s="71">
+      <c r="F7" s="61">
         <v>0.246</v>
       </c>
-      <c r="G7" s="69"/>
+      <c r="G7" s="59"/>
       <c r="H7" s="50"/>
       <c r="I7" s="48">
         <v>2.7E-2</v>
@@ -14611,25 +14889,46 @@
       <c r="AC7" s="23">
         <v>0.122</v>
       </c>
-    </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE7" t="s">
+        <v>8</v>
+      </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
+      <c r="AG7">
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="AH7">
+        <v>0.154</v>
+      </c>
+      <c r="AI7">
+        <v>0.122</v>
+      </c>
+      <c r="AJ7">
+        <v>2.4E-2</v>
+      </c>
+      <c r="AK7">
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="46">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="C8" s="66"/>
-      <c r="D8" s="66">
+      <c r="C8" s="56"/>
+      <c r="D8" s="56">
         <v>0.74199999999999999</v>
       </c>
-      <c r="E8" s="67">
-        <v>0</v>
-      </c>
-      <c r="F8" s="71">
+      <c r="E8" s="57">
+        <v>0</v>
+      </c>
+      <c r="F8" s="61">
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="G8" s="69"/>
+      <c r="G8" s="59"/>
       <c r="H8" s="50"/>
       <c r="I8" s="48">
         <v>3.0000000000000001E-3</v>
@@ -14671,25 +14970,46 @@
       <c r="AC8" s="23">
         <v>0.17</v>
       </c>
-    </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE8" t="s">
+        <v>9</v>
+      </c>
+      <c r="AF8">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AG8">
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="AH8">
+        <v>0</v>
+      </c>
+      <c r="AI8">
+        <v>0.191</v>
+      </c>
+      <c r="AJ8">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="AK8">
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
       <c r="B9" s="46">
         <v>1E-3</v>
       </c>
-      <c r="C9" s="66"/>
-      <c r="D9" s="66">
-        <v>0</v>
-      </c>
-      <c r="E9" s="67">
+      <c r="C9" s="56"/>
+      <c r="D9" s="56">
+        <v>0</v>
+      </c>
+      <c r="E9" s="57">
         <v>0.36599999999999999</v>
       </c>
-      <c r="F9" s="71">
-        <v>0</v>
-      </c>
-      <c r="G9" s="69"/>
+      <c r="F9" s="61">
+        <v>0</v>
+      </c>
+      <c r="G9" s="59"/>
       <c r="H9" s="50"/>
       <c r="I9" s="48">
         <v>1.7999999999999999E-2</v>
@@ -14731,14 +15051,35 @@
       <c r="AC9" s="23">
         <v>0.107</v>
       </c>
-    </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE9" t="s">
+        <v>10</v>
+      </c>
+      <c r="AF9">
+        <v>2E-3</v>
+      </c>
+      <c r="AG9">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="AH9">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="AI9">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="AJ9">
+        <v>2.3E-2</v>
+      </c>
+      <c r="AK9">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>41</v>
       </c>
       <c r="B10" s="46"/>
-      <c r="C10" s="66"/>
-      <c r="D10" s="67"/>
+      <c r="C10" s="56"/>
+      <c r="D10" s="57"/>
       <c r="E10" s="47"/>
       <c r="F10" s="48"/>
       <c r="G10" s="49"/>
@@ -14777,14 +15118,35 @@
       <c r="AC10" s="23">
         <v>0.23799999999999999</v>
       </c>
-    </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE10" t="s">
+        <v>11</v>
+      </c>
+      <c r="AF10">
+        <v>2E-3</v>
+      </c>
+      <c r="AG10">
+        <v>0.3</v>
+      </c>
+      <c r="AH10">
+        <v>0</v>
+      </c>
+      <c r="AI10">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AJ10">
+        <v>0.06</v>
+      </c>
+      <c r="AK10">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="46"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="67"/>
+      <c r="C11" s="56"/>
+      <c r="D11" s="57"/>
       <c r="E11" s="47"/>
       <c r="F11" s="48"/>
       <c r="G11" s="49"/>
@@ -14823,14 +15185,35 @@
       <c r="AC11" s="23">
         <v>0.191</v>
       </c>
-    </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE11" t="s">
+        <v>12</v>
+      </c>
+      <c r="AF11">
+        <v>0</v>
+      </c>
+      <c r="AG11">
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="AH11">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AI11">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ11">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AK11">
+        <v>8.4000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="46"/>
-      <c r="C12" s="66"/>
-      <c r="D12" s="67"/>
+      <c r="C12" s="56"/>
+      <c r="D12" s="57"/>
       <c r="E12" s="47"/>
       <c r="F12" s="48"/>
       <c r="G12" s="49"/>
@@ -14869,19 +15252,40 @@
       <c r="AC12" s="23">
         <v>0.113</v>
       </c>
-    </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE12" t="s">
+        <v>13</v>
+      </c>
+      <c r="AF12">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="AG12">
+        <v>0.67700000000000005</v>
+      </c>
+      <c r="AH12">
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AJ12">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AK12">
+        <v>9.9000000000000005E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="46">
         <v>1</v>
       </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="66">
+      <c r="C13" s="56"/>
+      <c r="D13" s="56">
         <v>0.16700000000000001</v>
       </c>
-      <c r="E13" s="67">
+      <c r="E13" s="57">
         <v>0.20799999999999999</v>
       </c>
       <c r="F13" s="47">
@@ -14929,19 +15333,40 @@
       <c r="AC13" s="29">
         <v>9.6000000000000002E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE13" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF13">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="AG13">
+        <v>0.42599999999999999</v>
+      </c>
+      <c r="AH13">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="AI13">
+        <v>0.215</v>
+      </c>
+      <c r="AJ13">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="AK13">
+        <v>1.7000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="46">
         <v>0.65200000000000002</v>
       </c>
-      <c r="C14" s="66"/>
-      <c r="D14" s="66">
+      <c r="C14" s="56"/>
+      <c r="D14" s="56">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="E14" s="67">
+      <c r="E14" s="57">
         <v>0.59599999999999997</v>
       </c>
       <c r="F14" s="47">
@@ -14989,19 +15414,40 @@
       <c r="AC14" s="23">
         <v>0.154</v>
       </c>
-    </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE14" t="s">
+        <v>15</v>
+      </c>
+      <c r="AF14">
+        <v>0</v>
+      </c>
+      <c r="AG14">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="AH14">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AI14">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="AJ14">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="AK14">
+        <v>6.5000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B15" s="46">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="66">
+      <c r="C15" s="56"/>
+      <c r="D15" s="56">
         <v>1E-3</v>
       </c>
-      <c r="E15" s="67">
+      <c r="E15" s="57">
         <v>4.0000000000000001E-3</v>
       </c>
       <c r="F15" s="47">
@@ -15049,19 +15495,40 @@
       <c r="AC15" s="23">
         <v>0.42099999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE15" t="s">
+        <v>16</v>
+      </c>
+      <c r="AF15">
+        <v>0</v>
+      </c>
+      <c r="AG15">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="AH15">
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <v>0</v>
+      </c>
+      <c r="AJ15">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="AK15">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="46">
         <v>0</v>
       </c>
-      <c r="C16" s="66"/>
-      <c r="D16" s="66">
+      <c r="C16" s="56"/>
+      <c r="D16" s="56">
         <v>1</v>
       </c>
-      <c r="E16" s="67">
+      <c r="E16" s="57">
         <v>0</v>
       </c>
       <c r="F16" s="47">
@@ -15109,14 +15576,35 @@
       <c r="AC16" s="23">
         <v>0.252</v>
       </c>
-    </row>
-    <row r="17" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE16" t="s">
+        <v>17</v>
+      </c>
+      <c r="AF16">
+        <v>1</v>
+      </c>
+      <c r="AG16">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AH16">
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <v>0</v>
+      </c>
+      <c r="AJ16">
+        <v>0.154</v>
+      </c>
+      <c r="AK16">
+        <v>0.17100000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>42</v>
       </c>
       <c r="B17" s="46"/>
-      <c r="C17" s="66"/>
-      <c r="D17" s="67"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="57"/>
       <c r="E17" s="47"/>
       <c r="F17" s="48"/>
       <c r="G17" s="49"/>
@@ -15153,14 +15641,35 @@
       <c r="AC17" s="23">
         <v>0.125</v>
       </c>
-    </row>
-    <row r="18" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE17" t="s">
+        <v>18</v>
+      </c>
+      <c r="AF17">
+        <v>0</v>
+      </c>
+      <c r="AG17">
+        <v>0.53</v>
+      </c>
+      <c r="AH17">
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <v>1E-3</v>
+      </c>
+      <c r="AJ17">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AK17">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="46"/>
-      <c r="C18" s="66"/>
-      <c r="D18" s="67"/>
+      <c r="C18" s="56"/>
+      <c r="D18" s="57"/>
       <c r="E18" s="47"/>
       <c r="F18" s="48"/>
       <c r="G18" s="49"/>
@@ -15199,14 +15708,35 @@
       <c r="AC18" s="23">
         <v>0.19600000000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE18" t="s">
+        <v>19</v>
+      </c>
+      <c r="AF18">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="AG18">
+        <v>0.27700000000000002</v>
+      </c>
+      <c r="AH18">
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <v>0</v>
+      </c>
+      <c r="AJ18">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="AK18">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="46"/>
-      <c r="C19" s="66"/>
-      <c r="D19" s="67"/>
+      <c r="C19" s="56"/>
+      <c r="D19" s="57"/>
       <c r="E19" s="47"/>
       <c r="F19" s="48"/>
       <c r="G19" s="49"/>
@@ -15245,14 +15775,35 @@
       <c r="AC19" s="23">
         <v>0.21199999999999999</v>
       </c>
-    </row>
-    <row r="20" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE19" t="s">
+        <v>20</v>
+      </c>
+      <c r="AF19">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="AG19">
+        <v>0.113</v>
+      </c>
+      <c r="AH19">
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AJ19">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="AK19">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>43</v>
       </c>
       <c r="B20" s="46"/>
-      <c r="C20" s="66"/>
-      <c r="D20" s="67"/>
+      <c r="C20" s="56"/>
+      <c r="D20" s="57"/>
       <c r="E20" s="47"/>
       <c r="F20" s="48"/>
       <c r="G20" s="49"/>
@@ -15291,14 +15842,35 @@
       <c r="AC20" s="23">
         <v>0.38500000000000001</v>
       </c>
-    </row>
-    <row r="21" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE20" t="s">
+        <v>44</v>
+      </c>
+      <c r="AF20">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG20">
+        <v>0.65700000000000003</v>
+      </c>
+      <c r="AH20">
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <v>0.34599999999999997</v>
+      </c>
+      <c r="AJ20">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AK20">
+        <v>0.10199999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="46"/>
-      <c r="C21" s="66"/>
-      <c r="D21" s="67"/>
+      <c r="C21" s="56"/>
+      <c r="D21" s="57"/>
       <c r="E21" s="47"/>
       <c r="F21" s="48"/>
       <c r="G21" s="49"/>
@@ -15335,14 +15907,35 @@
       <c r="AC21" s="29">
         <v>9.2999999999999999E-2</v>
       </c>
-    </row>
-    <row r="22" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE21" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF21">
+        <v>0</v>
+      </c>
+      <c r="AG21">
+        <v>0.19</v>
+      </c>
+      <c r="AH21">
+        <v>0.41299999999999998</v>
+      </c>
+      <c r="AI21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>0.189</v>
+      </c>
+      <c r="AK21">
+        <v>0.20100000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>20</v>
       </c>
       <c r="B22" s="46"/>
-      <c r="C22" s="66"/>
-      <c r="D22" s="67"/>
+      <c r="C22" s="56"/>
+      <c r="D22" s="57"/>
       <c r="E22" s="47"/>
       <c r="F22" s="48"/>
       <c r="G22" s="49"/>
@@ -15381,14 +15974,35 @@
       <c r="AC22" s="29">
         <v>0.05</v>
       </c>
-    </row>
-    <row r="23" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE22" t="s">
+        <v>22</v>
+      </c>
+      <c r="AF22">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="AG22">
+        <v>1</v>
+      </c>
+      <c r="AH22">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="AI22">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="AJ22">
+        <v>0.04</v>
+      </c>
+      <c r="AK22">
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>44</v>
       </c>
       <c r="B23" s="46"/>
-      <c r="C23" s="66"/>
-      <c r="D23" s="67"/>
+      <c r="C23" s="56"/>
+      <c r="D23" s="57"/>
       <c r="E23" s="47"/>
       <c r="F23" s="48"/>
       <c r="G23" s="49"/>
@@ -15427,14 +16041,35 @@
       <c r="AC23" s="23">
         <v>0.22600000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE23" t="s">
+        <v>23</v>
+      </c>
+      <c r="AF23">
+        <v>0</v>
+      </c>
+      <c r="AG23">
+        <v>4.7E-2</v>
+      </c>
+      <c r="AH23">
+        <v>0</v>
+      </c>
+      <c r="AI23">
+        <v>0</v>
+      </c>
+      <c r="AJ23">
+        <v>9.4E-2</v>
+      </c>
+      <c r="AK23">
+        <v>0.10299999999999999</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>21</v>
       </c>
       <c r="B24" s="46"/>
-      <c r="C24" s="66"/>
-      <c r="D24" s="67"/>
+      <c r="C24" s="56"/>
+      <c r="D24" s="57"/>
       <c r="E24" s="47"/>
       <c r="F24" s="48"/>
       <c r="G24" s="49"/>
@@ -15473,14 +16108,35 @@
       <c r="AC24" s="23">
         <v>0.14000000000000001</v>
       </c>
-    </row>
-    <row r="25" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE24" t="s">
+        <v>24</v>
+      </c>
+      <c r="AF24">
+        <v>0</v>
+      </c>
+      <c r="AG24">
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="AH24">
+        <v>0</v>
+      </c>
+      <c r="AI24">
+        <v>0.108</v>
+      </c>
+      <c r="AJ24">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="AK24">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
         <v>22</v>
       </c>
       <c r="B25" s="46"/>
-      <c r="C25" s="66"/>
-      <c r="D25" s="67"/>
+      <c r="C25" s="56"/>
+      <c r="D25" s="57"/>
       <c r="E25" s="47"/>
       <c r="F25" s="48"/>
       <c r="G25" s="49"/>
@@ -15519,14 +16175,35 @@
       <c r="AC25" s="23">
         <v>0.17199999999999999</v>
       </c>
-    </row>
-    <row r="26" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE25" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF25">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="AG25">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AH25">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AI25">
+        <v>0</v>
+      </c>
+      <c r="AJ25">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AK25">
+        <v>7.1999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
         <v>23</v>
       </c>
       <c r="B26" s="46"/>
-      <c r="C26" s="66"/>
-      <c r="D26" s="67"/>
+      <c r="C26" s="56"/>
+      <c r="D26" s="57"/>
       <c r="E26" s="47"/>
       <c r="F26" s="48"/>
       <c r="G26" s="49"/>
@@ -15563,14 +16240,35 @@
       <c r="AC26" s="29">
         <v>9.0999999999999998E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE26" t="s">
+        <v>26</v>
+      </c>
+      <c r="AF26">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="AG26">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="AH26">
+        <v>0</v>
+      </c>
+      <c r="AI26">
+        <v>0.02</v>
+      </c>
+      <c r="AJ26">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AK26">
+        <v>7.2999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>24</v>
       </c>
       <c r="B27" s="46"/>
-      <c r="C27" s="66"/>
-      <c r="D27" s="67"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="57"/>
       <c r="E27" s="47"/>
       <c r="F27" s="48"/>
       <c r="G27" s="49"/>
@@ -15607,14 +16305,35 @@
       <c r="AC27" s="23">
         <v>0.20799999999999999</v>
       </c>
-    </row>
-    <row r="28" spans="1:29" x14ac:dyDescent="0.35">
+      <c r="AE27" t="s">
+        <v>27</v>
+      </c>
+      <c r="AF27">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AG27">
+        <v>0.68100000000000005</v>
+      </c>
+      <c r="AH27">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="AI27">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="AJ27">
+        <v>0.02</v>
+      </c>
+      <c r="AK27">
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
         <v>25</v>
       </c>
       <c r="B28" s="46"/>
-      <c r="C28" s="66"/>
-      <c r="D28" s="67"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="57"/>
       <c r="E28" s="47"/>
       <c r="F28" s="48"/>
       <c r="G28" s="49"/>
@@ -15652,13 +16371,13 @@
         <v>9.9000000000000005E-2</v>
       </c>
     </row>
-    <row r="29" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
         <v>45</v>
       </c>
       <c r="B29" s="46"/>
-      <c r="C29" s="66"/>
-      <c r="D29" s="67"/>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
       <c r="E29" s="47"/>
       <c r="F29" s="48"/>
       <c r="G29" s="49"/>
@@ -15698,13 +16417,13 @@
         <v>0.32200000000000001</v>
       </c>
     </row>
-    <row r="30" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>26</v>
       </c>
       <c r="B30" s="46"/>
-      <c r="C30" s="66"/>
-      <c r="D30" s="67"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="57"/>
       <c r="E30" s="47"/>
       <c r="F30" s="48"/>
       <c r="G30" s="49"/>
@@ -15744,13 +16463,13 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="31" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
         <v>46</v>
       </c>
       <c r="B31" s="46"/>
-      <c r="C31" s="66"/>
-      <c r="D31" s="67"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="57"/>
       <c r="E31" s="47"/>
       <c r="F31" s="48"/>
       <c r="G31" s="49"/>
@@ -15790,13 +16509,13 @@
         <v>0.106</v>
       </c>
     </row>
-    <row r="32" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:37" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
         <v>27</v>
       </c>
       <c r="B32" s="46"/>
-      <c r="C32" s="66"/>
-      <c r="D32" s="67"/>
+      <c r="C32" s="56"/>
+      <c r="D32" s="57"/>
       <c r="E32" s="47"/>
       <c r="F32" s="48"/>
       <c r="G32" s="49"/>
@@ -15841,8 +16560,8 @@
         <v>28</v>
       </c>
       <c r="B33" s="46"/>
-      <c r="C33" s="66"/>
-      <c r="D33" s="67"/>
+      <c r="C33" s="56"/>
+      <c r="D33" s="57"/>
       <c r="E33" s="47"/>
       <c r="F33" s="48"/>
       <c r="G33" s="49"/>
@@ -15898,14 +16617,19 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AK1:AK1048576">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>

</xml_diff>

<commit_message>
Attempting to output AIC scores into output. No luck yet.
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -17,7 +17,6 @@
     <sheet name="MechanismSummaryTable" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1881,6 +1880,49 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>304229</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>151829</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8191500" y="184150"/>
+          <a:ext cx="4571429" cy="4571429"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -2146,8 +2188,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M426"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2168,7 +2210,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -14839,6 +14881,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Ran GAMs of individual indices for 2021 SOE and added output for looking into GOM haddock commecial catch live weight conversions in relation to condition
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="1" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
@@ -1742,14 +1742,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="110">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="109">
     <dxf>
       <fill>
         <patternFill>
@@ -15533,44 +15526,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="109" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="108" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="106" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="105" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="103" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="101" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18156,145 +18149,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="99" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="98" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="98" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="96" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="95" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="95" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="93" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="92" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="92" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="90" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="89" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="89" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="87" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="86" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="86" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="84" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="83" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="83" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="81" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="80" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="80" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="78" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="77" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="75" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="74" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="72" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="71" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="69" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="68" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18307,7 +18300,7 @@
   <dimension ref="A1:Y46"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="93" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -20117,168 +20110,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="66" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30:B119 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17">
-    <cfRule type="cellIs" dxfId="65" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="63" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="61" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="59" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="57" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="56" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="54" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="54" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="53" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26">
-    <cfRule type="cellIs" dxfId="51" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P16 P30:P31 P18:P26">
-    <cfRule type="cellIs" dxfId="50" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="48" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="47" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="47" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13">
-    <cfRule type="cellIs" dxfId="45" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="44" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R4 R16:R31 R6:R13">
-    <cfRule type="cellIs" dxfId="44" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="42" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="41" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="39" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="38" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="36" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="35" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119">
-    <cfRule type="cellIs" dxfId="33" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="32" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="32" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="31" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="30" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20291,8 +20284,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z192"/>
   <sheetViews>
-    <sheetView topLeftCell="A116" workbookViewId="0">
-      <selection activeCell="X163" sqref="X163"/>
+    <sheetView topLeftCell="A157" workbookViewId="0">
+      <selection activeCell="T165" sqref="T165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26534,15 +26527,15 @@
         <v>917</v>
       </c>
       <c r="N164">
-        <f>J164-J136</f>
+        <f t="shared" ref="N164:N187" si="9">J164-J136</f>
         <v>6.0000000000000053E-3</v>
       </c>
       <c r="O164">
-        <f>L164-L136</f>
+        <f t="shared" ref="O164:O187" si="10">L164-L136</f>
         <v>394</v>
       </c>
       <c r="P164">
-        <f>K164-K136</f>
+        <f t="shared" ref="P164:P187" si="11">K164-K136</f>
         <v>2.5869999999999997</v>
       </c>
       <c r="R164" t="s">
@@ -26613,15 +26606,15 @@
         <v>1591</v>
       </c>
       <c r="N165">
-        <f>J165-J137</f>
+        <f t="shared" si="9"/>
         <v>-2.0999999999999998E-2</v>
       </c>
       <c r="O165">
-        <f>L165-L137</f>
+        <f t="shared" si="10"/>
         <v>671</v>
       </c>
       <c r="P165">
-        <f>K165-K137</f>
+        <f t="shared" si="11"/>
         <v>-0.68699999999999761</v>
       </c>
       <c r="R165" t="s">
@@ -26631,7 +26624,7 @@
         <v>0.35099999999999998</v>
       </c>
       <c r="T165">
-        <f t="shared" ref="T165:T192" si="9">S165-X165</f>
+        <f t="shared" ref="T165:T192" si="12">S165-X165</f>
         <v>2.899999999999997E-2</v>
       </c>
       <c r="U165" t="s">
@@ -26647,7 +26640,7 @@
         <v>0.32200000000000001</v>
       </c>
       <c r="Y165">
-        <f t="shared" ref="Y165:Y192" si="10">V165-X165</f>
+        <f t="shared" ref="Y165:Y192" si="13">V165-X165</f>
         <v>-0.10100000000000001</v>
       </c>
       <c r="Z165" t="s">
@@ -26692,15 +26685,15 @@
         <v>881</v>
       </c>
       <c r="N166">
-        <f>J166-J138</f>
+        <f t="shared" si="9"/>
         <v>-5.099999999999999E-2</v>
       </c>
       <c r="O166">
-        <f>L166-L138</f>
+        <f t="shared" si="10"/>
         <v>372</v>
       </c>
       <c r="P166">
-        <f>K166-K138</f>
+        <f t="shared" si="11"/>
         <v>2.593</v>
       </c>
       <c r="R166" t="s">
@@ -26710,7 +26703,7 @@
         <v>0.129</v>
       </c>
       <c r="T166">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>3.8000000000000006E-2</v>
       </c>
       <c r="U166" t="s">
@@ -26726,7 +26719,7 @@
         <v>9.0999999999999998E-2</v>
       </c>
       <c r="Y166">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-2.0999999999999991E-2</v>
       </c>
       <c r="Z166" t="s">
@@ -26771,15 +26764,15 @@
         <v>1652</v>
       </c>
       <c r="N167">
-        <f>J167-J139</f>
+        <f t="shared" si="9"/>
         <v>-8.9999999999999941E-3</v>
       </c>
       <c r="O167">
-        <f>L167-L139</f>
+        <f t="shared" si="10"/>
         <v>526</v>
       </c>
       <c r="P167">
-        <f>K167-K139</f>
+        <f t="shared" si="11"/>
         <v>4.0990000000000038</v>
       </c>
       <c r="R167" t="s">
@@ -26789,7 +26782,7 @@
         <v>0.32300000000000001</v>
       </c>
       <c r="T167">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.23</v>
       </c>
       <c r="U167" t="s">
@@ -26805,7 +26798,7 @@
         <v>9.2999999999999999E-2</v>
       </c>
       <c r="Y167">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>0.11299999999999999</v>
       </c>
       <c r="Z167" t="s">
@@ -26850,15 +26843,15 @@
         <v>548</v>
       </c>
       <c r="N168">
-        <f>J168-J140</f>
+        <f t="shared" si="9"/>
         <v>-1.4000000000000012E-2</v>
       </c>
       <c r="O168">
-        <f>L168-L140</f>
+        <f t="shared" si="10"/>
         <v>176</v>
       </c>
       <c r="P168">
-        <f>K168-K140</f>
+        <f t="shared" si="11"/>
         <v>2.2000000000000028</v>
       </c>
       <c r="R168" t="s">
@@ -26868,7 +26861,7 @@
         <v>0.11700000000000001</v>
       </c>
       <c r="T168">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-7.9999999999999932E-3</v>
       </c>
       <c r="U168" t="s">
@@ -26884,7 +26877,7 @@
         <v>0.125</v>
       </c>
       <c r="Y168">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-4.3999999999999997E-2</v>
       </c>
       <c r="Z168" t="s">
@@ -26929,15 +26922,15 @@
         <v>1177</v>
       </c>
       <c r="N169">
-        <f>J169-J141</f>
+        <f t="shared" si="9"/>
         <v>-0.11700000000000002</v>
       </c>
       <c r="O169">
-        <f>L169-L141</f>
+        <f t="shared" si="10"/>
         <v>581</v>
       </c>
       <c r="P169">
-        <f>K169-K141</f>
+        <f t="shared" si="11"/>
         <v>-4.5379999999999967</v>
       </c>
       <c r="R169" t="s">
@@ -26947,7 +26940,7 @@
         <v>0.127</v>
       </c>
       <c r="T169">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-7.6000000000000012E-2</v>
       </c>
       <c r="U169" t="s">
@@ -26963,7 +26956,7 @@
         <v>0.20300000000000001</v>
       </c>
       <c r="Y169">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.15800000000000003</v>
       </c>
       <c r="Z169" t="s">
@@ -27008,15 +27001,15 @@
         <v>2329</v>
       </c>
       <c r="N170">
-        <f>J170-J142</f>
+        <f t="shared" si="9"/>
         <v>-0.14199999999999999</v>
       </c>
       <c r="O170">
-        <f>L170-L142</f>
+        <f t="shared" si="10"/>
         <v>1519</v>
       </c>
       <c r="P170">
-        <f>K170-K142</f>
+        <f t="shared" si="11"/>
         <v>-3.3320000000000007</v>
       </c>
       <c r="R170" t="s">
@@ -27026,7 +27019,7 @@
         <v>0.10299999999999999</v>
       </c>
       <c r="T170">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.13500000000000001</v>
       </c>
       <c r="U170" t="s">
@@ -27042,7 +27035,7 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="Y170">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.10699999999999998</v>
       </c>
       <c r="Z170" t="s">
@@ -27087,15 +27080,15 @@
         <v>954</v>
       </c>
       <c r="N171">
-        <f>J171-J143</f>
+        <f t="shared" si="9"/>
         <v>-5.8999999999999997E-2</v>
       </c>
       <c r="O171">
-        <f>L171-L143</f>
+        <f t="shared" si="10"/>
         <v>678</v>
       </c>
       <c r="P171">
-        <f>K171-K143</f>
+        <f t="shared" si="11"/>
         <v>-0.64799999999999969</v>
       </c>
       <c r="R171" t="s">
@@ -27105,7 +27098,7 @@
         <v>0.16400000000000001</v>
       </c>
       <c r="T171">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-7.9999999999999793E-3</v>
       </c>
       <c r="U171" t="s">
@@ -27121,7 +27114,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="Y171">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-3.2999999999999974E-2</v>
       </c>
       <c r="Z171" t="s">
@@ -27166,19 +27159,19 @@
         <v>1180</v>
       </c>
       <c r="N172">
-        <f>J172-J144</f>
+        <f t="shared" si="9"/>
         <v>-9.7000000000000017E-2</v>
       </c>
       <c r="O172">
-        <f>L172-L144</f>
+        <f t="shared" si="10"/>
         <v>899</v>
       </c>
       <c r="P172">
-        <f>K172-K144</f>
+        <f t="shared" si="11"/>
         <v>0.5</v>
       </c>
       <c r="T172">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.17</v>
       </c>
       <c r="W172" t="s">
@@ -27188,7 +27181,7 @@
         <v>0.17</v>
       </c>
       <c r="Y172">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.17</v>
       </c>
       <c r="Z172" t="s">
@@ -27233,19 +27226,19 @@
         <v>597</v>
       </c>
       <c r="N173">
-        <f>J173-J145</f>
+        <f t="shared" si="9"/>
         <v>-4.0000000000000036E-3</v>
       </c>
       <c r="O173">
-        <f>L173-L145</f>
+        <f t="shared" si="10"/>
         <v>276</v>
       </c>
       <c r="P173">
-        <f>K173-K145</f>
+        <f t="shared" si="11"/>
         <v>-0.13899999999999935</v>
       </c>
       <c r="T173">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-7.1999999999999995E-2</v>
       </c>
       <c r="W173" t="s">
@@ -27255,7 +27248,7 @@
         <v>7.1999999999999995E-2</v>
       </c>
       <c r="Y173">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-7.1999999999999995E-2</v>
       </c>
       <c r="Z173" t="s">
@@ -27300,15 +27293,15 @@
         <v>1041</v>
       </c>
       <c r="N174">
-        <f>J174-J146</f>
+        <f t="shared" si="9"/>
         <v>-4.9000000000000016E-2</v>
       </c>
       <c r="O174">
-        <f>L174-L146</f>
+        <f t="shared" si="10"/>
         <v>639</v>
       </c>
       <c r="P174">
-        <f>K174-K146</f>
+        <f t="shared" si="11"/>
         <v>3.1489999999999991</v>
       </c>
       <c r="R174" t="s">
@@ -27318,7 +27311,7 @@
         <v>0.19900000000000001</v>
       </c>
       <c r="T174">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-5.2999999999999992E-2</v>
       </c>
       <c r="U174" t="s">
@@ -27334,7 +27327,7 @@
         <v>0.252</v>
       </c>
       <c r="Y174">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.15000000000000002</v>
       </c>
       <c r="Z174" t="s">
@@ -27379,15 +27372,15 @@
         <v>1793</v>
       </c>
       <c r="N175">
-        <f>J175-J147</f>
+        <f t="shared" si="9"/>
         <v>-4.9000000000000002E-2</v>
       </c>
       <c r="O175">
-        <f>L175-L147</f>
+        <f t="shared" si="10"/>
         <v>773</v>
       </c>
       <c r="P175">
-        <f>K175-K147</f>
+        <f t="shared" si="11"/>
         <v>-3.0130000000000052</v>
       </c>
       <c r="R175" t="s">
@@ -27397,7 +27390,7 @@
         <v>7.6999999999999999E-2</v>
       </c>
       <c r="T175">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>2.6999999999999996E-2</v>
       </c>
       <c r="U175" t="s">
@@ -27413,7 +27406,7 @@
         <v>0.05</v>
       </c>
       <c r="Y175">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1.8000000000000002E-2</v>
       </c>
       <c r="Z175" t="s">
@@ -27458,15 +27451,15 @@
         <v>958</v>
       </c>
       <c r="N176">
-        <f>J176-J148</f>
+        <f t="shared" si="9"/>
         <v>-0.12999999999999998</v>
       </c>
       <c r="O176">
-        <f>L176-L148</f>
+        <f t="shared" si="10"/>
         <v>488</v>
       </c>
       <c r="P176">
-        <f>K176-K148</f>
+        <f t="shared" si="11"/>
         <v>0.26000000000000156</v>
       </c>
       <c r="R176" t="s">
@@ -27476,7 +27469,7 @@
         <v>0.112</v>
       </c>
       <c r="T176">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-7.9999999999999932E-3</v>
       </c>
       <c r="U176" t="s">
@@ -27492,7 +27485,7 @@
         <v>0.12</v>
       </c>
       <c r="Y176">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-3.3000000000000002E-2</v>
       </c>
       <c r="Z176" t="s">
@@ -27537,15 +27530,15 @@
         <v>1465</v>
       </c>
       <c r="N177">
-        <f>J177-J149</f>
+        <f t="shared" si="9"/>
         <v>-1.2999999999999998E-2</v>
       </c>
       <c r="O177">
-        <f>L177-L149</f>
+        <f t="shared" si="10"/>
         <v>408</v>
       </c>
       <c r="P177">
-        <f>K177-K149</f>
+        <f t="shared" si="11"/>
         <v>0.69700000000000095</v>
       </c>
       <c r="R177" t="s">
@@ -27555,7 +27548,7 @@
         <v>6.8000000000000005E-2</v>
       </c>
       <c r="T177">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-3.8999999999999993E-2</v>
       </c>
       <c r="U177" t="s">
@@ -27571,7 +27564,7 @@
         <v>0.107</v>
       </c>
       <c r="Y177">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-4.2999999999999997E-2</v>
       </c>
       <c r="Z177" t="s">
@@ -27616,15 +27609,15 @@
         <v>945</v>
       </c>
       <c r="N178">
-        <f>J178-J150</f>
+        <f t="shared" si="9"/>
         <v>1.100000000000001E-2</v>
       </c>
       <c r="O178">
-        <f>L178-L150</f>
+        <f t="shared" si="10"/>
         <v>558</v>
       </c>
       <c r="P178">
-        <f>K178-K150</f>
+        <f t="shared" si="11"/>
         <v>7.5549999999999997</v>
       </c>
       <c r="R178" t="s">
@@ -27634,7 +27627,7 @@
         <v>0.16200000000000001</v>
       </c>
       <c r="T178">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-4.9999999999999989E-2</v>
       </c>
       <c r="U178" t="s">
@@ -27650,7 +27643,7 @@
         <v>0.21199999999999999</v>
       </c>
       <c r="Y178">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-9.8999999999999991E-2</v>
       </c>
       <c r="Z178" t="s">
@@ -27695,19 +27688,19 @@
         <v>1194</v>
       </c>
       <c r="N179">
-        <f>J179-J151</f>
+        <f t="shared" si="9"/>
         <v>8.0000000000000071E-3</v>
       </c>
       <c r="O179">
-        <f>L179-L151</f>
+        <f t="shared" si="10"/>
         <v>548</v>
       </c>
       <c r="P179">
-        <f>K179-K151</f>
+        <f t="shared" si="11"/>
         <v>0.57699999999999996</v>
       </c>
       <c r="T179">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.22600000000000001</v>
       </c>
       <c r="W179" t="s">
@@ -27717,7 +27710,7 @@
         <v>0.22600000000000001</v>
       </c>
       <c r="Y179">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.22600000000000001</v>
       </c>
       <c r="Z179" t="s">
@@ -27762,15 +27755,15 @@
         <v>853</v>
       </c>
       <c r="N180">
-        <f>J180-J152</f>
+        <f t="shared" si="9"/>
         <v>-4.8999999999999988E-2</v>
       </c>
       <c r="O180">
-        <f>L180-L152</f>
+        <f t="shared" si="10"/>
         <v>483</v>
       </c>
       <c r="P180">
-        <f>K180-K152</f>
+        <f t="shared" si="11"/>
         <v>5.0749999999999993</v>
       </c>
       <c r="R180" t="s">
@@ -27780,7 +27773,7 @@
         <v>0.23799999999999999</v>
       </c>
       <c r="T180">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>0.13200000000000001</v>
       </c>
       <c r="U180" t="s">
@@ -27796,7 +27789,7 @@
         <v>0.106</v>
       </c>
       <c r="Y180">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-9.999999999999995E-3</v>
       </c>
       <c r="Z180" t="s">
@@ -27841,15 +27834,15 @@
         <v>1412</v>
       </c>
       <c r="N181">
-        <f>J181-J153</f>
+        <f t="shared" si="9"/>
         <v>1.3000000000000012E-2</v>
       </c>
       <c r="O181">
-        <f>L181-L153</f>
+        <f t="shared" si="10"/>
         <v>508</v>
       </c>
       <c r="P181">
-        <f>K181-K153</f>
+        <f t="shared" si="11"/>
         <v>4.9430000000000121</v>
       </c>
       <c r="R181" t="s">
@@ -27859,7 +27852,7 @@
         <v>7.9000000000000001E-2</v>
       </c>
       <c r="T181">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-6.1000000000000013E-2</v>
       </c>
       <c r="U181" t="s">
@@ -27875,7 +27868,7 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="Y181">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-5.5000000000000007E-2</v>
       </c>
       <c r="Z181" t="s">
@@ -27920,15 +27913,15 @@
         <v>489</v>
       </c>
       <c r="N182">
-        <f>J182-J154</f>
+        <f t="shared" si="9"/>
         <v>-3.6000000000000004E-2</v>
       </c>
       <c r="O182">
-        <f>L182-L154</f>
+        <f t="shared" si="10"/>
         <v>225</v>
       </c>
       <c r="P182">
-        <f>K182-K154</f>
+        <f t="shared" si="11"/>
         <v>-1.4109999999999978</v>
       </c>
       <c r="R182" t="s">
@@ -27938,7 +27931,7 @@
         <v>7.5999999999999998E-2</v>
       </c>
       <c r="T182">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-2.0000000000000004E-2</v>
       </c>
       <c r="U182" t="s">
@@ -27954,7 +27947,7 @@
         <v>9.6000000000000002E-2</v>
       </c>
       <c r="Y182">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-4.1000000000000002E-2</v>
       </c>
       <c r="Z182" t="s">
@@ -27999,19 +27992,19 @@
         <v>2491</v>
       </c>
       <c r="N183">
-        <f>J183-J155</f>
+        <f t="shared" si="9"/>
         <v>-2.4999999999999994E-2</v>
       </c>
       <c r="O183">
-        <f>L183-L155</f>
+        <f t="shared" si="10"/>
         <v>1127</v>
       </c>
       <c r="P183">
-        <f>K183-K155</f>
+        <f t="shared" si="11"/>
         <v>14.920000000000016</v>
       </c>
       <c r="T183">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.10100000000000001</v>
       </c>
       <c r="W183" t="s">
@@ -28021,7 +28014,7 @@
         <v>0.10100000000000001</v>
       </c>
       <c r="Y183">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.10100000000000001</v>
       </c>
       <c r="Z183" t="s">
@@ -28066,15 +28059,15 @@
         <v>856</v>
       </c>
       <c r="N184">
-        <f>J184-J156</f>
+        <f t="shared" si="9"/>
         <v>2.8000000000000011E-2</v>
       </c>
       <c r="O184">
-        <f>L184-L156</f>
+        <f t="shared" si="10"/>
         <v>579</v>
       </c>
       <c r="P184">
-        <f>K184-K156</f>
+        <f t="shared" si="11"/>
         <v>2.7280000000000015</v>
       </c>
       <c r="R184" t="s">
@@ -28084,7 +28077,7 @@
         <v>8.6999999999999994E-2</v>
       </c>
       <c r="T184">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-3.5000000000000003E-2</v>
       </c>
       <c r="U184" t="s">
@@ -28100,7 +28093,7 @@
         <v>0.122</v>
       </c>
       <c r="Y184">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-4.8000000000000001E-2</v>
       </c>
       <c r="Z184" t="s">
@@ -28145,15 +28138,15 @@
         <v>704</v>
       </c>
       <c r="N185">
-        <f>J185-J157</f>
+        <f t="shared" si="9"/>
         <v>-8.2000000000000003E-2</v>
       </c>
       <c r="O185">
-        <f>L185-L157</f>
+        <f t="shared" si="10"/>
         <v>545</v>
       </c>
       <c r="P185">
-        <f>K185-K157</f>
+        <f t="shared" si="11"/>
         <v>10.032999999999994</v>
       </c>
       <c r="R185" t="s">
@@ -28163,7 +28156,7 @@
         <v>0.253</v>
       </c>
       <c r="T185">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>5.6999999999999995E-2</v>
       </c>
       <c r="U185" t="s">
@@ -28179,7 +28172,7 @@
         <v>0.19600000000000001</v>
       </c>
       <c r="Y185">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.2999999999999983E-2</v>
       </c>
       <c r="Z185" t="s">
@@ -28224,19 +28217,19 @@
         <v>803</v>
       </c>
       <c r="N186">
-        <f>J186-J158</f>
+        <f t="shared" si="9"/>
         <v>-1.4999999999999999E-2</v>
       </c>
       <c r="O186">
-        <f>L186-L158</f>
+        <f t="shared" si="10"/>
         <v>501</v>
       </c>
       <c r="P186">
-        <f>K186-K158</f>
+        <f t="shared" si="11"/>
         <v>0.93599999999999994</v>
       </c>
       <c r="T186">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.42099999999999999</v>
       </c>
       <c r="W186" t="s">
@@ -28246,7 +28239,7 @@
         <v>0.42099999999999999</v>
       </c>
       <c r="Y186">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.42099999999999999</v>
       </c>
       <c r="Z186" t="s">
@@ -28291,15 +28284,15 @@
         <v>631</v>
       </c>
       <c r="N187">
-        <f>J187-J159</f>
+        <f t="shared" si="9"/>
         <v>-2.5000000000000008E-2</v>
       </c>
       <c r="O187">
-        <f>L187-L159</f>
+        <f t="shared" si="10"/>
         <v>321</v>
       </c>
       <c r="P187">
-        <f>K187-K159</f>
+        <f t="shared" si="11"/>
         <v>2.2580000000000027</v>
       </c>
       <c r="R187" t="s">
@@ -28309,7 +28302,7 @@
         <v>0.13800000000000001</v>
       </c>
       <c r="T187">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-0.16399999999999998</v>
       </c>
       <c r="U187" t="s">
@@ -28325,7 +28318,7 @@
         <v>0.30199999999999999</v>
       </c>
       <c r="Y187">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-0.21299999999999999</v>
       </c>
       <c r="Z187" t="s">
@@ -28340,7 +28333,7 @@
         <v>0.24</v>
       </c>
       <c r="T188">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>3.2000000000000001E-2</v>
       </c>
       <c r="U188" t="s">
@@ -28356,7 +28349,7 @@
         <v>0.20799999999999999</v>
       </c>
       <c r="Y188">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>4.5000000000000012E-2</v>
       </c>
       <c r="Z188" t="s">
@@ -28371,7 +28364,7 @@
         <v>0.154</v>
       </c>
       <c r="T189">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-3.7000000000000005E-2</v>
       </c>
       <c r="U189" t="s">
@@ -28387,7 +28380,7 @@
         <v>0.191</v>
       </c>
       <c r="Y189">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-2.8999999999999998E-2</v>
       </c>
       <c r="Z189" t="s">
@@ -28402,7 +28395,7 @@
         <v>0.12</v>
       </c>
       <c r="T190">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>-3.4000000000000002E-2</v>
       </c>
       <c r="U190" t="s">
@@ -28418,7 +28411,7 @@
         <v>0.154</v>
       </c>
       <c r="Y190">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>-8.4999999999999992E-2</v>
       </c>
       <c r="Z190" t="s">
@@ -28433,7 +28426,7 @@
         <v>0.186</v>
       </c>
       <c r="T191">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>7.2999999999999995E-2</v>
       </c>
       <c r="U191" t="s">
@@ -28449,7 +28442,7 @@
         <v>0.113</v>
       </c>
       <c r="Y191">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2.4000000000000007E-2</v>
       </c>
       <c r="Z191" t="s">
@@ -28464,7 +28457,7 @@
         <v>0.17199999999999999</v>
       </c>
       <c r="T192">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>7.2999999999999982E-2</v>
       </c>
       <c r="U192" t="s">
@@ -28480,7 +28473,7 @@
         <v>9.9000000000000005E-2</v>
       </c>
       <c r="Y192">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>8.3999999999999991E-2</v>
       </c>
       <c r="Z192" t="s">
@@ -28492,87 +28485,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="28" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="27" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="24" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="23" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="21" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="20" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="18" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="17" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="17" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="16" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="13" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="10" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31544,41 +31537,41 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="9" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="7" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="6" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Condition data only from N<=3 and years>20
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="1" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1465" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1506" uniqueCount="162">
   <si>
     <t>Species</t>
   </si>
@@ -491,6 +491,24 @@
   </si>
   <si>
     <t>Same as above without null space penalty or adding na.gam.replace</t>
+  </si>
+  <si>
+    <t>Scup</t>
+  </si>
+  <si>
+    <t>Clearnose skate</t>
+  </si>
+  <si>
+    <t>Smooth skate</t>
+  </si>
+  <si>
+    <t>Barndoor skate</t>
+  </si>
+  <si>
+    <t>Rosette skate</t>
+  </si>
+  <si>
+    <t>With revised calibrations in survdat</t>
   </si>
 </sst>
 </file>
@@ -1742,7 +1760,161 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="109">
+  <dxfs count="131">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="7" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -15526,44 +15698,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="108" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="130" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="107" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="105" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="104" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="102" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="100" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="99" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15577,7 +15749,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC46"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
@@ -18149,145 +18321,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="98" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="120" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="97" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="96" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="95" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="117" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="94" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="92" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="114" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="91" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="90" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="89" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="111" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="88" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="86" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="85" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="83" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="105" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="82" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="80" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="102" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="79" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="77" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="99" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="76" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="74" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="96" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="73" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="72" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="93" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="70" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="68" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="90" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="67" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="66" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20110,168 +20282,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="65" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17 B38:B119">
-    <cfRule type="cellIs" dxfId="64" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="62" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="60" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 J5 J10 J14 J17:J18 J21:J22 J24:J25 J27:J29">
-    <cfRule type="cellIs" dxfId="58" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31 L5 L10 L14 L17:L18 L21:L22 L27:L29 L24:L25">
-    <cfRule type="cellIs" dxfId="56" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L4 L6:L9 L11:L13 L15:L16 L19:L20 L23 L30:L31 L26">
-    <cfRule type="cellIs" dxfId="55" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="53" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="52" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26 P4:P9 P11 P13:P15 P19:P21 P24 P30">
-    <cfRule type="cellIs" dxfId="50" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="72" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P31 P18 P10 P12 P16 P22:P23 P25:P26">
-    <cfRule type="cellIs" dxfId="49" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="47" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="69" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="46" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13 R10 R12 R16:R18 R22:R23 R25:R29 R31 R3">
-    <cfRule type="cellIs" dxfId="44" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2 R19:R21 R6:R9 R11 R13 R24 R30 R4">
-    <cfRule type="cellIs" dxfId="43" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="41" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="40" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="38" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="60" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119 B31:B37">
-    <cfRule type="cellIs" dxfId="32" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="30" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="29" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 J3:J4 J6:J9 J11:J13 J15:J16 J19:J20 J23 J26 J30:J31">
-    <cfRule type="cellIs" dxfId="28" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20284,7 +20456,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z192"/>
   <sheetViews>
-    <sheetView topLeftCell="A140" workbookViewId="0">
+    <sheetView topLeftCell="A142" workbookViewId="0">
       <selection activeCell="P153" sqref="P153"/>
     </sheetView>
   </sheetViews>
@@ -28490,87 +28662,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="27" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="26" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="24" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="23" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="22" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="20" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="19" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="17" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="16" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="15" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28581,10 +28753,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AX33"/>
+  <dimension ref="A1:BL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M22" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView topLeftCell="AX4" workbookViewId="0">
+      <selection activeCell="BJ8" sqref="BJ8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -28597,14 +28769,15 @@
     <col min="21" max="21" width="9.90625" customWidth="1"/>
     <col min="22" max="22" width="11.08984375" customWidth="1"/>
     <col min="23" max="23" width="9.6328125" customWidth="1"/>
+    <col min="53" max="53" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:64" x14ac:dyDescent="0.35">
       <c r="Q1">
         <v>2019</v>
       </c>
     </row>
-    <row r="2" spans="1:50" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="62" t="s">
         <v>107</v>
@@ -28637,8 +28810,14 @@
       <c r="AA2" s="64"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
-    </row>
-    <row r="3" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA2">
+        <v>2021</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
       <c r="C3" s="68" t="s">
@@ -28691,7 +28870,7 @@
         <v>2020</v>
       </c>
     </row>
-    <row r="4" spans="1:50" ht="39.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:64" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -28821,8 +29000,44 @@
       <c r="AX4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA4" t="s">
+        <v>0</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>46</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>143</v>
+      </c>
+      <c r="BD4" t="s">
+        <v>144</v>
+      </c>
+      <c r="BE4" t="s">
+        <v>145</v>
+      </c>
+      <c r="BF4" t="s">
+        <v>40</v>
+      </c>
+      <c r="BG4" t="s">
+        <v>1</v>
+      </c>
+      <c r="BH4" t="s">
+        <v>115</v>
+      </c>
+      <c r="BI4" t="s">
+        <v>2</v>
+      </c>
+      <c r="BJ4" t="s">
+        <v>3</v>
+      </c>
+      <c r="BK4" t="s">
+        <v>4</v>
+      </c>
+      <c r="BL4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A5" s="13" t="s">
         <v>6</v>
       </c>
@@ -28935,8 +29150,44 @@
       <c r="AX5">
         <v>9.5000000000000001E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA5" t="s">
+        <v>9</v>
+      </c>
+      <c r="BB5">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="BC5">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="BD5">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="BE5">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="BF5">
+        <v>2E-3</v>
+      </c>
+      <c r="BG5">
+        <v>0</v>
+      </c>
+      <c r="BH5">
+        <v>0.161</v>
+      </c>
+      <c r="BI5">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="BJ5">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="BK5">
+        <v>128.63</v>
+      </c>
+      <c r="BL5">
+        <v>2252</v>
+      </c>
+    </row>
+    <row r="6" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>7</v>
       </c>
@@ -29049,8 +29300,44 @@
       <c r="AX6">
         <v>4.2999999999999997E-2</v>
       </c>
-    </row>
-    <row r="7" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA6" t="s">
+        <v>11</v>
+      </c>
+      <c r="BB6">
+        <v>0.222</v>
+      </c>
+      <c r="BC6">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="BD6">
+        <v>0</v>
+      </c>
+      <c r="BE6">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="BF6">
+        <v>0</v>
+      </c>
+      <c r="BG6">
+        <v>0</v>
+      </c>
+      <c r="BH6">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="BI6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="BJ6">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="BK6">
+        <v>585.56899999999996</v>
+      </c>
+      <c r="BL6">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="7" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
@@ -29163,8 +29450,44 @@
       <c r="AX7">
         <v>7.2999999999999995E-2</v>
       </c>
-    </row>
-    <row r="8" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA7" t="s">
+        <v>20</v>
+      </c>
+      <c r="BB7">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="BC7">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BD7">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BE7">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="BF7">
+        <v>6.4000000000000001E-2</v>
+      </c>
+      <c r="BG7">
+        <v>6.3E-2</v>
+      </c>
+      <c r="BH7">
+        <v>0</v>
+      </c>
+      <c r="BI7">
+        <v>7.8E-2</v>
+      </c>
+      <c r="BJ7">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="BK7">
+        <v>55.920999999999999</v>
+      </c>
+      <c r="BL7">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="8" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>9</v>
       </c>
@@ -29277,8 +29600,44 @@
       <c r="AX8">
         <v>6.5000000000000002E-2</v>
       </c>
-    </row>
-    <row r="9" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA8" t="s">
+        <v>23</v>
+      </c>
+      <c r="BB8">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="BC8">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="BD8">
+        <v>0.38300000000000001</v>
+      </c>
+      <c r="BE8">
+        <v>0.248</v>
+      </c>
+      <c r="BF8">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="BG8">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="BH8">
+        <v>0</v>
+      </c>
+      <c r="BI8">
+        <v>1.2999999999999999E-2</v>
+      </c>
+      <c r="BJ8">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="BK8">
+        <v>8812.6020000000008</v>
+      </c>
+      <c r="BL8">
+        <v>4636</v>
+      </c>
+    </row>
+    <row r="9" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>10</v>
       </c>
@@ -29391,8 +29750,44 @@
       <c r="AX9">
         <v>0.13900000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA9" t="s">
+        <v>7</v>
+      </c>
+      <c r="BB9">
+        <v>0</v>
+      </c>
+      <c r="BC9">
+        <v>0.96899999999999997</v>
+      </c>
+      <c r="BD9">
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="BE9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BF9">
+        <v>0</v>
+      </c>
+      <c r="BG9">
+        <v>0</v>
+      </c>
+      <c r="BH9">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="BI9">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="BJ9">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="BK9">
+        <v>71.051000000000002</v>
+      </c>
+      <c r="BL9">
+        <v>1987</v>
+      </c>
+    </row>
+    <row r="10" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>34</v>
       </c>
@@ -29491,8 +29886,44 @@
       <c r="AX10">
         <v>0.189</v>
       </c>
-    </row>
-    <row r="11" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA10" t="s">
+        <v>24</v>
+      </c>
+      <c r="BB10">
+        <v>0</v>
+      </c>
+      <c r="BC10">
+        <v>9.1999999999999998E-2</v>
+      </c>
+      <c r="BD10">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="BE10">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="BF10">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="BG10">
+        <v>0.12</v>
+      </c>
+      <c r="BH10">
+        <v>1E-3</v>
+      </c>
+      <c r="BI10">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="BJ10">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="BK10">
+        <v>137.50200000000001</v>
+      </c>
+      <c r="BL10">
+        <v>1864</v>
+      </c>
+    </row>
+    <row r="11" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>11</v>
       </c>
@@ -29595,8 +30026,44 @@
       <c r="AX11">
         <v>0.14699999999999999</v>
       </c>
-    </row>
-    <row r="12" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA11" t="s">
+        <v>21</v>
+      </c>
+      <c r="BB11">
+        <v>0</v>
+      </c>
+      <c r="BC11">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="BD11">
+        <v>0</v>
+      </c>
+      <c r="BE11">
+        <v>0</v>
+      </c>
+      <c r="BF11">
+        <v>0.27300000000000002</v>
+      </c>
+      <c r="BG11">
+        <v>0</v>
+      </c>
+      <c r="BH11">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="BI11">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="BJ11">
+        <v>0.156</v>
+      </c>
+      <c r="BK11">
+        <v>155.541</v>
+      </c>
+      <c r="BL11">
+        <v>2108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>12</v>
       </c>
@@ -29695,8 +30162,44 @@
       <c r="AX12">
         <v>0.11700000000000001</v>
       </c>
-    </row>
-    <row r="13" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA12" t="s">
+        <v>156</v>
+      </c>
+      <c r="BB12">
+        <v>0</v>
+      </c>
+      <c r="BC12">
+        <v>0.26</v>
+      </c>
+      <c r="BD12">
+        <v>1.4E-2</v>
+      </c>
+      <c r="BE12">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="BF12">
+        <v>0</v>
+      </c>
+      <c r="BG12">
+        <v>0</v>
+      </c>
+      <c r="BH12">
+        <v>0.33900000000000002</v>
+      </c>
+      <c r="BI12">
+        <v>0.159</v>
+      </c>
+      <c r="BJ12">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="BK12">
+        <v>126.777</v>
+      </c>
+      <c r="BL12">
+        <v>2423</v>
+      </c>
+    </row>
+    <row r="13" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>13</v>
       </c>
@@ -29809,8 +30312,44 @@
       <c r="AX13">
         <v>3.7999999999999999E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA13" t="s">
+        <v>13</v>
+      </c>
+      <c r="BB13">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="BC13">
+        <v>0.01</v>
+      </c>
+      <c r="BD13">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="BE13">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="BF13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BG13">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="BH13">
+        <v>0</v>
+      </c>
+      <c r="BI13">
+        <v>6.2E-2</v>
+      </c>
+      <c r="BJ13">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="BK13">
+        <v>71.972999999999999</v>
+      </c>
+      <c r="BL13">
+        <v>1752</v>
+      </c>
+    </row>
+    <row r="14" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A14" s="22" t="s">
         <v>14</v>
       </c>
@@ -29923,8 +30462,44 @@
       <c r="AX14">
         <v>9.8000000000000004E-2</v>
       </c>
-    </row>
-    <row r="15" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA14" t="s">
+        <v>16</v>
+      </c>
+      <c r="BB14">
+        <v>0</v>
+      </c>
+      <c r="BC14">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="BD14">
+        <v>3.4000000000000002E-2</v>
+      </c>
+      <c r="BE14">
+        <v>0.86499999999999999</v>
+      </c>
+      <c r="BF14">
+        <v>5.5E-2</v>
+      </c>
+      <c r="BG14">
+        <v>0</v>
+      </c>
+      <c r="BH14">
+        <v>0</v>
+      </c>
+      <c r="BI14">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="BJ14">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="BK14">
+        <v>935.92200000000003</v>
+      </c>
+      <c r="BL14">
+        <v>2723</v>
+      </c>
+    </row>
+    <row r="15" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A15" s="22" t="s">
         <v>15</v>
       </c>
@@ -30037,8 +30612,44 @@
       <c r="AX15">
         <v>0.14299999999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA15" t="s">
+        <v>27</v>
+      </c>
+      <c r="BB15">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BC15">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="BD15">
+        <v>0</v>
+      </c>
+      <c r="BE15">
+        <v>0.109</v>
+      </c>
+      <c r="BF15">
+        <v>0</v>
+      </c>
+      <c r="BG15">
+        <v>0.622</v>
+      </c>
+      <c r="BH15">
+        <v>0.109</v>
+      </c>
+      <c r="BI15">
+        <v>0.155</v>
+      </c>
+      <c r="BJ15">
+        <v>0.18</v>
+      </c>
+      <c r="BK15">
+        <v>179.779</v>
+      </c>
+      <c r="BL15">
+        <v>929</v>
+      </c>
+    </row>
+    <row r="16" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A16" s="22" t="s">
         <v>16</v>
       </c>
@@ -30151,8 +30762,44 @@
       <c r="AX16">
         <v>0.22900000000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA16" t="s">
+        <v>15</v>
+      </c>
+      <c r="BB16">
+        <v>0</v>
+      </c>
+      <c r="BC16">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="BD16">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="BE16">
+        <v>2.3E-2</v>
+      </c>
+      <c r="BF16">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BG16">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="BH16">
+        <v>0</v>
+      </c>
+      <c r="BI16">
+        <v>0.109</v>
+      </c>
+      <c r="BJ16">
+        <v>0.126</v>
+      </c>
+      <c r="BK16">
+        <v>123.896</v>
+      </c>
+      <c r="BL16">
+        <v>1485</v>
+      </c>
+    </row>
+    <row r="17" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A17" s="22" t="s">
         <v>35</v>
       </c>
@@ -30249,8 +30896,44 @@
       <c r="AX17">
         <v>8.7999999999999995E-2</v>
       </c>
-    </row>
-    <row r="18" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA17" t="s">
+        <v>8</v>
+      </c>
+      <c r="BB17">
+        <v>1E-3</v>
+      </c>
+      <c r="BC17">
+        <v>8.7999999999999995E-2</v>
+      </c>
+      <c r="BD17">
+        <v>0.161</v>
+      </c>
+      <c r="BE17">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="BF17">
+        <v>0</v>
+      </c>
+      <c r="BG17">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="BH17">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="BI17">
+        <v>6.3E-2</v>
+      </c>
+      <c r="BJ17">
+        <v>7.8E-2</v>
+      </c>
+      <c r="BK17">
+        <v>136.00299999999999</v>
+      </c>
+      <c r="BL17">
+        <v>1270</v>
+      </c>
+    </row>
+    <row r="18" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A18" s="22" t="s">
         <v>17</v>
       </c>
@@ -30353,8 +31036,44 @@
       <c r="AX18">
         <v>0.109</v>
       </c>
-    </row>
-    <row r="19" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA18" t="s">
+        <v>18</v>
+      </c>
+      <c r="BB18">
+        <v>0</v>
+      </c>
+      <c r="BC18">
+        <v>0.26800000000000002</v>
+      </c>
+      <c r="BD18">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="BE18">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="BF18">
+        <v>0</v>
+      </c>
+      <c r="BG18">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="BH18">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="BI18">
+        <v>0.12</v>
+      </c>
+      <c r="BJ18">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="BK18">
+        <v>56.012999999999998</v>
+      </c>
+      <c r="BL18">
+        <v>2126</v>
+      </c>
+    </row>
+    <row r="19" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A19" s="22" t="s">
         <v>18</v>
       </c>
@@ -30453,8 +31172,44 @@
       <c r="AX19">
         <v>0.123</v>
       </c>
-    </row>
-    <row r="20" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA19" t="s">
+        <v>19</v>
+      </c>
+      <c r="BB19">
+        <v>1E-3</v>
+      </c>
+      <c r="BC19">
+        <v>0</v>
+      </c>
+      <c r="BD19">
+        <v>0.432</v>
+      </c>
+      <c r="BE19">
+        <v>0.36899999999999999</v>
+      </c>
+      <c r="BF19">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="BG19">
+        <v>0.109</v>
+      </c>
+      <c r="BH19">
+        <v>0</v>
+      </c>
+      <c r="BI19">
+        <v>0.1</v>
+      </c>
+      <c r="BJ19">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="BK19">
+        <v>499.33</v>
+      </c>
+      <c r="BL19">
+        <v>1216</v>
+      </c>
+    </row>
+    <row r="20" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A20" s="22" t="s">
         <v>36</v>
       </c>
@@ -30553,8 +31308,44 @@
       <c r="AX20">
         <v>0.15</v>
       </c>
-    </row>
-    <row r="21" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA20" t="s">
+        <v>12</v>
+      </c>
+      <c r="BB20">
+        <v>0</v>
+      </c>
+      <c r="BC20">
+        <v>0.94799999999999995</v>
+      </c>
+      <c r="BD20">
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="BE20">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="BF20">
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="BG20">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="BH20">
+        <v>0</v>
+      </c>
+      <c r="BI20">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="BJ20">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="BK20">
+        <v>105.014</v>
+      </c>
+      <c r="BL20">
+        <v>1260</v>
+      </c>
+    </row>
+    <row r="21" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A21" s="22" t="s">
         <v>19</v>
       </c>
@@ -30655,8 +31446,44 @@
       <c r="AX21">
         <v>0.20399999999999999</v>
       </c>
-    </row>
-    <row r="22" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA21" t="s">
+        <v>22</v>
+      </c>
+      <c r="BB21">
+        <v>0</v>
+      </c>
+      <c r="BC21">
+        <v>1.4999999999999999E-2</v>
+      </c>
+      <c r="BD21">
+        <v>3.9E-2</v>
+      </c>
+      <c r="BE21">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="BF21">
+        <v>0.05</v>
+      </c>
+      <c r="BG21">
+        <v>0.24</v>
+      </c>
+      <c r="BH21">
+        <v>2E-3</v>
+      </c>
+      <c r="BI21">
+        <v>0.106</v>
+      </c>
+      <c r="BJ21">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="BK21">
+        <v>96.477000000000004</v>
+      </c>
+      <c r="BL21">
+        <v>926</v>
+      </c>
+    </row>
+    <row r="22" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A22" s="22" t="s">
         <v>20</v>
       </c>
@@ -30755,8 +31582,44 @@
       <c r="AX22">
         <v>6.9000000000000006E-2</v>
       </c>
-    </row>
-    <row r="23" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA22" t="s">
+        <v>37</v>
+      </c>
+      <c r="BB22">
+        <v>0.36699999999999999</v>
+      </c>
+      <c r="BC22">
+        <v>0.01</v>
+      </c>
+      <c r="BD22">
+        <v>0</v>
+      </c>
+      <c r="BE22">
+        <v>0</v>
+      </c>
+      <c r="BF22">
+        <v>0.65100000000000002</v>
+      </c>
+      <c r="BG22">
+        <v>0.111</v>
+      </c>
+      <c r="BH22">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="BI22">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="BJ22">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="BK22">
+        <v>282.221</v>
+      </c>
+      <c r="BL22">
+        <v>1146</v>
+      </c>
+    </row>
+    <row r="23" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>37</v>
       </c>
@@ -30855,8 +31718,44 @@
       <c r="AX23">
         <v>0.161</v>
       </c>
-    </row>
-    <row r="24" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA23" t="s">
+        <v>10</v>
+      </c>
+      <c r="BB23">
+        <v>1E-3</v>
+      </c>
+      <c r="BC23">
+        <v>9.8000000000000004E-2</v>
+      </c>
+      <c r="BD23">
+        <v>8.9999999999999993E-3</v>
+      </c>
+      <c r="BE23">
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="BF23">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="BG23">
+        <v>0</v>
+      </c>
+      <c r="BH23">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="BI23">
+        <v>0.107</v>
+      </c>
+      <c r="BJ23">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="BK23">
+        <v>143.803</v>
+      </c>
+      <c r="BL23">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="24" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A24" s="22" t="s">
         <v>21</v>
       </c>
@@ -30955,8 +31854,44 @@
       <c r="AX24">
         <v>3.3000000000000002E-2</v>
       </c>
-    </row>
-    <row r="25" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA24" t="s">
+        <v>17</v>
+      </c>
+      <c r="BB24">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BC24">
+        <v>0.7</v>
+      </c>
+      <c r="BD24">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="BE24">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="BF24">
+        <v>0.52</v>
+      </c>
+      <c r="BG24">
+        <v>0.192</v>
+      </c>
+      <c r="BH24">
+        <v>0</v>
+      </c>
+      <c r="BI24">
+        <v>9.2999999999999999E-2</v>
+      </c>
+      <c r="BJ24">
+        <v>0.115</v>
+      </c>
+      <c r="BK24">
+        <v>187.71899999999999</v>
+      </c>
+      <c r="BL24">
+        <v>1343</v>
+      </c>
+    </row>
+    <row r="25" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
         <v>22</v>
       </c>
@@ -31055,8 +31990,44 @@
       <c r="AX25">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA25" t="s">
+        <v>26</v>
+      </c>
+      <c r="BB25">
+        <v>0</v>
+      </c>
+      <c r="BC25">
+        <v>0.02</v>
+      </c>
+      <c r="BD25">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="BE25">
+        <v>0.6</v>
+      </c>
+      <c r="BF25">
+        <v>2E-3</v>
+      </c>
+      <c r="BG25">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BH25">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="BI25">
+        <v>8.3000000000000004E-2</v>
+      </c>
+      <c r="BJ25">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="BK25">
+        <v>149.749</v>
+      </c>
+      <c r="BL25">
+        <v>1224</v>
+      </c>
+    </row>
+    <row r="26" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A26" s="22" t="s">
         <v>23</v>
       </c>
@@ -31153,8 +32124,44 @@
       <c r="AX26">
         <v>0.13</v>
       </c>
-    </row>
-    <row r="27" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA26" t="s">
+        <v>14</v>
+      </c>
+      <c r="BB26">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="BC26">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="BD26">
+        <v>0.433</v>
+      </c>
+      <c r="BE26">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="BF26">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="BG26">
+        <v>0</v>
+      </c>
+      <c r="BH26">
+        <v>1.6E-2</v>
+      </c>
+      <c r="BI26">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="BJ26">
+        <v>0.153</v>
+      </c>
+      <c r="BK26">
+        <v>63.503</v>
+      </c>
+      <c r="BL26">
+        <v>735</v>
+      </c>
+    </row>
+    <row r="27" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A27" s="22" t="s">
         <v>24</v>
       </c>
@@ -31251,8 +32258,44 @@
       <c r="AX27">
         <v>8.6999999999999994E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA27" t="s">
+        <v>34</v>
+      </c>
+      <c r="BB27">
+        <v>0.877</v>
+      </c>
+      <c r="BC27">
+        <v>0</v>
+      </c>
+      <c r="BD27">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="BE27">
+        <v>0.92300000000000004</v>
+      </c>
+      <c r="BF27">
+        <v>1E-3</v>
+      </c>
+      <c r="BG27">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="BH27">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="BI27">
+        <v>0.95799999999999996</v>
+      </c>
+      <c r="BJ27">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="BK27">
+        <v>213891.552</v>
+      </c>
+      <c r="BL27">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="28" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A28" s="22" t="s">
         <v>25</v>
       </c>
@@ -31295,8 +32338,44 @@
       <c r="AC28" s="29">
         <v>9.9000000000000005E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA28" t="s">
+        <v>25</v>
+      </c>
+      <c r="BB28">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="BC28">
+        <v>0.47899999999999998</v>
+      </c>
+      <c r="BD28">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="BE28">
+        <v>0.45700000000000002</v>
+      </c>
+      <c r="BF28">
+        <v>0</v>
+      </c>
+      <c r="BG28">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="BH28">
+        <v>0.25</v>
+      </c>
+      <c r="BI28">
+        <v>7.8E-2</v>
+      </c>
+      <c r="BJ28">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="BK28">
+        <v>636.47299999999996</v>
+      </c>
+      <c r="BL28">
+        <v>1402</v>
+      </c>
+    </row>
+    <row r="29" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A29" s="22" t="s">
         <v>38</v>
       </c>
@@ -31341,8 +32420,44 @@
       <c r="AC29" s="23">
         <v>0.32200000000000001</v>
       </c>
-    </row>
-    <row r="30" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA29" t="s">
+        <v>157</v>
+      </c>
+      <c r="BB29">
+        <v>0.71199999999999997</v>
+      </c>
+      <c r="BC29">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="BD29">
+        <v>2E-3</v>
+      </c>
+      <c r="BE29">
+        <v>1E-3</v>
+      </c>
+      <c r="BF29">
+        <v>0.48599999999999999</v>
+      </c>
+      <c r="BG29">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="BH29">
+        <v>1.6E-2</v>
+      </c>
+      <c r="BI29">
+        <v>3.1E-2</v>
+      </c>
+      <c r="BJ29">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="BK29">
+        <v>312.63099999999997</v>
+      </c>
+      <c r="BL29">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="30" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A30" s="22" t="s">
         <v>26</v>
       </c>
@@ -31387,8 +32502,44 @@
       <c r="AC30" s="23">
         <v>0.12</v>
       </c>
-    </row>
-    <row r="31" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA30" t="s">
+        <v>158</v>
+      </c>
+      <c r="BB30">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="BC30">
+        <v>0.432</v>
+      </c>
+      <c r="BD30">
+        <v>1.4E-2</v>
+      </c>
+      <c r="BE30">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="BF30">
+        <v>0</v>
+      </c>
+      <c r="BG30">
+        <v>1E-3</v>
+      </c>
+      <c r="BH30">
+        <v>0</v>
+      </c>
+      <c r="BI30">
+        <v>0.20799999999999999</v>
+      </c>
+      <c r="BJ30">
+        <v>0.25</v>
+      </c>
+      <c r="BK30">
+        <v>104.312</v>
+      </c>
+      <c r="BL30">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="31" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A31" s="22" t="s">
         <v>39</v>
       </c>
@@ -31433,8 +32584,44 @@
       <c r="AC31" s="23">
         <v>0.106</v>
       </c>
-    </row>
-    <row r="32" spans="1:50" x14ac:dyDescent="0.35">
+      <c r="BA31" t="s">
+        <v>159</v>
+      </c>
+      <c r="BB31">
+        <v>1E-3</v>
+      </c>
+      <c r="BC31">
+        <v>1.9E-2</v>
+      </c>
+      <c r="BD31">
+        <v>0</v>
+      </c>
+      <c r="BE31">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="BF31">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="BG31">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="BH31">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="BI31">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="BJ31">
+        <v>0.151</v>
+      </c>
+      <c r="BK31">
+        <v>94.238</v>
+      </c>
+      <c r="BL31">
+        <v>731</v>
+      </c>
+    </row>
+    <row r="32" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A32" s="22" t="s">
         <v>27</v>
       </c>
@@ -31479,6 +32666,42 @@
       <c r="AC32" s="23">
         <v>0.30199999999999999</v>
       </c>
+      <c r="BA32" t="s">
+        <v>160</v>
+      </c>
+      <c r="BB32">
+        <v>0.376</v>
+      </c>
+      <c r="BC32">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="BD32">
+        <v>0.93700000000000006</v>
+      </c>
+      <c r="BE32">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="BF32">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="BG32">
+        <v>1E-3</v>
+      </c>
+      <c r="BH32">
+        <v>0.70299999999999996</v>
+      </c>
+      <c r="BI32">
+        <v>4.7E-2</v>
+      </c>
+      <c r="BJ32">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="BK32">
+        <v>29106.073</v>
+      </c>
+      <c r="BL32">
+        <v>467</v>
+      </c>
     </row>
     <row r="33" spans="1:29" x14ac:dyDescent="0.35">
       <c r="A33" s="22" t="s">
@@ -31542,42 +32765,68 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="5" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="4" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
       <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BJ4:BJ27">
+    <cfRule type="cellIs" dxfId="12" priority="6" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB4:BH27">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="lessThan">
+      <formula>0.05</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BJ28:BJ32">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="greaterThan">
+      <formula>0.1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BB28:BH32">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>0.01</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="lessThan">
+      <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Limited relative condition to <300 to remove remaining outliers
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="4" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1885" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="211">
   <si>
     <t>Species</t>
   </si>
@@ -650,6 +650,15 @@
   <si>
     <t>Deviance Explained worse</t>
   </si>
+  <si>
+    <t>GAM check</t>
+  </si>
+  <si>
+    <t>Might need more K (degrees freedom)</t>
+  </si>
+  <si>
+    <t>Average Lat/Lon by Strata</t>
+  </si>
 </sst>
 </file>
 
@@ -1033,7 +1042,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="47">
+  <borders count="49">
     <border>
       <left/>
       <right/>
@@ -1635,6 +1644,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1680,7 +1707,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1871,6 +1898,9 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1902,6 +1932,12 @@
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -28973,7 +29009,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+    <sheetView topLeftCell="P1" workbookViewId="0">
       <selection activeCell="AD29" sqref="AD29"/>
     </sheetView>
   </sheetViews>
@@ -28997,35 +29033,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="69"/>
-      <c r="I2" s="69"/>
-      <c r="J2" s="69"/>
-      <c r="K2" s="69"/>
-      <c r="L2" s="69"/>
-      <c r="M2" s="70"/>
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="70"/>
+      <c r="G2" s="70"/>
+      <c r="H2" s="70"/>
+      <c r="I2" s="70"/>
+      <c r="J2" s="70"/>
+      <c r="K2" s="70"/>
+      <c r="L2" s="70"/>
+      <c r="M2" s="71"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="68" t="s">
+      <c r="R2" s="69" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="69"/>
-      <c r="T2" s="69"/>
-      <c r="U2" s="69"/>
-      <c r="V2" s="69"/>
-      <c r="W2" s="69"/>
-      <c r="X2" s="69"/>
-      <c r="Y2" s="69"/>
-      <c r="Z2" s="69"/>
-      <c r="AA2" s="70"/>
+      <c r="S2" s="70"/>
+      <c r="T2" s="70"/>
+      <c r="U2" s="70"/>
+      <c r="V2" s="70"/>
+      <c r="W2" s="70"/>
+      <c r="X2" s="70"/>
+      <c r="Y2" s="70"/>
+      <c r="Z2" s="70"/>
+      <c r="AA2" s="71"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -29038,50 +29074,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="74" t="s">
+      <c r="C3" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="76" t="s">
+      <c r="D3" s="77" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="74" t="s">
+      <c r="E3" s="75" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="71" t="s">
+      <c r="F3" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="72"/>
-      <c r="H3" s="71" t="s">
+      <c r="G3" s="73"/>
+      <c r="H3" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="73"/>
-      <c r="J3" s="72"/>
-      <c r="K3" s="71" t="s">
+      <c r="I3" s="74"/>
+      <c r="J3" s="73"/>
+      <c r="K3" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="73"/>
-      <c r="M3" s="72"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="73"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="74" t="s">
+      <c r="S3" s="75" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="71" t="s">
+      <c r="T3" s="72" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="72"/>
-      <c r="V3" s="71" t="s">
+      <c r="U3" s="73"/>
+      <c r="V3" s="72" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="73"/>
-      <c r="X3" s="72"/>
-      <c r="Y3" s="71" t="s">
+      <c r="W3" s="74"/>
+      <c r="X3" s="73"/>
+      <c r="Y3" s="72" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="73"/>
-      <c r="AA3" s="72"/>
+      <c r="Z3" s="74"/>
+      <c r="AA3" s="73"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -29095,9 +29131,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="75"/>
-      <c r="D4" s="77"/>
-      <c r="E4" s="75"/>
+      <c r="C4" s="76"/>
+      <c r="D4" s="78"/>
+      <c r="E4" s="76"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -29132,7 +29168,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="75"/>
+      <c r="S4" s="76"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -33054,10 +33090,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R232"/>
+  <dimension ref="A1:T232"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:XFD14"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33066,7 +33102,7 @@
     <col min="9" max="9" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>186</v>
       </c>
@@ -33085,7 +33121,7 @@
       <c r="J1" s="67"/>
       <c r="K1" s="67"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -33134,8 +33170,11 @@
       <c r="R2" t="s">
         <v>205</v>
       </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="T2" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -33161,35 +33200,35 @@
         <v>0</v>
       </c>
       <c r="K3">
-        <v>4.8000000000000001E-2</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="L3">
-        <v>5.5E-2</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="M3">
-        <v>14.795999999999999</v>
+        <v>14.656000000000001</v>
       </c>
       <c r="N3">
-        <v>1056</v>
+        <v>1055</v>
       </c>
       <c r="O3">
         <f>F3-N3</f>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="P3">
         <f>O3/N3</f>
-        <v>1.7045454545454544E-2</v>
+        <v>1.8009478672985781E-2</v>
       </c>
       <c r="Q3">
         <f>D3-L3</f>
-        <v>-3.0000000000000027E-3</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="R3">
         <f>E3-M3</f>
-        <v>2.2810000000000024</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.35">
+        <v>2.4210000000000012</v>
+      </c>
+    </row>
+    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>17</v>
       </c>
@@ -33227,7 +33266,7 @@
         <v>1253</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O43" si="0">F4-N4</f>
+        <f t="shared" ref="O4:O29" si="0">F4-N4</f>
         <v>15</v>
       </c>
       <c r="P4">
@@ -33235,15 +33274,15 @@
         <v>1.1971268954509178E-2</v>
       </c>
       <c r="Q4">
-        <f t="shared" ref="Q4:Q42" si="2">D4-L4</f>
+        <f t="shared" ref="Q4:Q28" si="2">D4-L4</f>
         <v>-3.0000000000000027E-3</v>
       </c>
       <c r="R4">
-        <f t="shared" ref="R4:R42" si="3">E4-M4</f>
+        <f t="shared" ref="R4:R29" si="3">E4-M4</f>
         <v>2.5839999999999996</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A5" s="66" t="s">
         <v>12</v>
       </c>
@@ -33297,7 +33336,7 @@
         <v>1.4760000000000009</v>
       </c>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>191</v>
       </c>
@@ -33351,7 +33390,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>34</v>
       </c>
@@ -33377,35 +33416,38 @@
         <v>0</v>
       </c>
       <c r="K7">
-        <v>5.6000000000000001E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="L7">
-        <v>6.2E-2</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M7">
-        <v>96.352000000000004</v>
+        <v>18.178999999999998</v>
       </c>
       <c r="N7">
-        <v>1496</v>
+        <v>1378</v>
       </c>
       <c r="O7">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>119</v>
       </c>
       <c r="P7">
         <f t="shared" si="1"/>
-        <v>6.6844919786096253E-4</v>
+        <v>8.6357039187227869E-2</v>
       </c>
       <c r="Q7">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R7">
         <f t="shared" si="3"/>
-        <v>0.17099999999999227</v>
-      </c>
-    </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
+        <v>78.343999999999994</v>
+      </c>
+      <c r="T7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -33459,7 +33501,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>159</v>
       </c>
@@ -33513,7 +33555,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>25</v>
       </c>
@@ -33539,35 +33581,35 @@
         <v>0</v>
       </c>
       <c r="K10">
-        <v>3.5000000000000003E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L10">
-        <v>0.04</v>
+        <v>0.03</v>
       </c>
       <c r="M10">
-        <v>46.838000000000001</v>
+        <v>29.227</v>
       </c>
       <c r="N10">
-        <v>1185</v>
+        <v>1091</v>
       </c>
       <c r="O10">
         <f t="shared" si="0"/>
-        <v>95</v>
+        <v>189</v>
       </c>
       <c r="P10">
         <f t="shared" si="1"/>
-        <v>8.0168776371308023E-2</v>
+        <v>0.17323556370302476</v>
       </c>
       <c r="Q10">
         <f t="shared" si="2"/>
-        <v>3.9999999999999966E-3</v>
+        <v>1.3999999999999999E-2</v>
       </c>
       <c r="R10">
         <f t="shared" si="3"/>
-        <v>15.536999999999999</v>
-      </c>
-    </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
+        <v>33.147999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -33593,35 +33635,35 @@
         <v>0</v>
       </c>
       <c r="K11">
-        <v>2.7E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="L11">
-        <v>2.9000000000000001E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="M11">
-        <v>25.256</v>
+        <v>23.626999999999999</v>
       </c>
       <c r="N11">
-        <v>1622</v>
+        <v>1599</v>
       </c>
       <c r="O11">
         <f t="shared" si="0"/>
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="P11">
         <f t="shared" si="1"/>
-        <v>2.2194821208384709E-2</v>
+        <v>3.6898061288305188E-2</v>
       </c>
       <c r="Q11">
         <f t="shared" si="2"/>
-        <v>1.2E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="R11">
         <f t="shared" si="3"/>
-        <v>2.9649999999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
+        <v>4.5940000000000012</v>
+      </c>
+    </row>
+    <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>188</v>
       </c>
@@ -33644,38 +33686,38 @@
         <v>188</v>
       </c>
       <c r="J12">
-        <v>3.0000000000000001E-3</v>
+        <v>0</v>
       </c>
       <c r="K12">
-        <v>5.0999999999999997E-2</v>
+        <v>7.5999999999999998E-2</v>
       </c>
       <c r="L12">
-        <v>6.9000000000000006E-2</v>
+        <v>8.4000000000000005E-2</v>
       </c>
       <c r="M12">
-        <v>119.63800000000001</v>
+        <v>20.562999999999999</v>
       </c>
       <c r="N12">
-        <v>380</v>
+        <v>321</v>
       </c>
       <c r="O12">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>59</v>
       </c>
       <c r="P12">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.18380062305295949</v>
       </c>
       <c r="Q12">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>-1.4999999999999999E-2</v>
       </c>
       <c r="R12">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
+        <v>99.075000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="66" t="s">
         <v>189</v>
       </c>
@@ -33698,38 +33740,38 @@
         <v>189</v>
       </c>
       <c r="J13">
-        <v>0.17699999999999999</v>
+        <v>0.36299999999999999</v>
       </c>
       <c r="K13">
-        <v>8.0000000000000002E-3</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="L13">
-        <v>1.2999999999999999E-2</v>
+        <v>7.0000000000000001E-3</v>
       </c>
       <c r="M13">
-        <v>13.912000000000001</v>
+        <v>11.901999999999999</v>
       </c>
       <c r="N13">
-        <v>426</v>
+        <v>417</v>
       </c>
       <c r="O13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="P13">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>2.1582733812949641E-2</v>
       </c>
       <c r="Q13">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>5.9999999999999993E-3</v>
       </c>
       <c r="R13">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
+        <v>2.0100000000000016</v>
+      </c>
+    </row>
+    <row r="14" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>23</v>
       </c>
@@ -33755,35 +33797,35 @@
         <v>0</v>
       </c>
       <c r="K14">
-        <v>4.2999999999999997E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="L14">
-        <v>4.4999999999999998E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M14">
-        <v>221.203</v>
+        <v>56.021000000000001</v>
       </c>
       <c r="N14">
-        <v>4458</v>
+        <v>3973</v>
       </c>
       <c r="O14">
         <f t="shared" si="0"/>
-        <v>130</v>
+        <v>615</v>
       </c>
       <c r="P14">
         <f t="shared" si="1"/>
-        <v>2.9161058770749215E-2</v>
+        <v>0.15479486534105211</v>
       </c>
       <c r="Q14">
         <f t="shared" si="2"/>
-        <v>-6.9999999999999993E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="R14">
         <f t="shared" si="3"/>
-        <v>43.876999999999981</v>
-      </c>
-    </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.35">
+        <v>209.05899999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>157</v>
       </c>
@@ -33806,38 +33848,38 @@
         <v>157</v>
       </c>
       <c r="J15">
-        <v>0</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="K15">
-        <v>4.1000000000000002E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="L15">
-        <v>0.05</v>
+        <v>3.1E-2</v>
       </c>
       <c r="M15">
-        <v>94.92</v>
+        <v>43.811999999999998</v>
       </c>
       <c r="N15">
-        <v>674</v>
+        <v>618</v>
       </c>
       <c r="O15">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>56</v>
       </c>
       <c r="P15">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>9.0614886731391592E-2</v>
       </c>
       <c r="Q15">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.9000000000000003E-2</v>
       </c>
       <c r="R15">
         <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.35">
+        <v>51.108000000000004</v>
+      </c>
+    </row>
+    <row r="16" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>36</v>
       </c>
@@ -33914,35 +33956,35 @@
         <v>28</v>
       </c>
       <c r="J17">
-        <v>1E-3</v>
+        <v>0</v>
       </c>
       <c r="K17">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="L17">
-        <v>8.0000000000000002E-3</v>
+        <v>8.9999999999999993E-3</v>
       </c>
       <c r="M17">
-        <v>56.027000000000001</v>
+        <v>52.084000000000003</v>
       </c>
       <c r="N17">
-        <v>1871</v>
+        <v>1847</v>
       </c>
       <c r="O17">
         <f t="shared" si="0"/>
-        <v>5</v>
+        <v>29</v>
       </c>
       <c r="P17">
         <f t="shared" si="1"/>
-        <v>2.6723677177979692E-3</v>
+        <v>1.5701136978884679E-2</v>
       </c>
       <c r="Q17">
         <f t="shared" si="2"/>
-        <v>9.9999999999999915E-4</v>
+        <v>0</v>
       </c>
       <c r="R17">
         <f t="shared" si="3"/>
-        <v>0.22099999999999653</v>
+        <v>4.1639999999999944</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.35">
@@ -33971,32 +34013,32 @@
         <v>0</v>
       </c>
       <c r="K18">
-        <v>3.7999999999999999E-2</v>
+        <v>3.5999999999999997E-2</v>
       </c>
       <c r="L18">
-        <v>4.2000000000000003E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M18">
-        <v>14.353</v>
+        <v>14.28</v>
       </c>
       <c r="N18">
-        <v>1581</v>
+        <v>1580</v>
       </c>
       <c r="O18">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P18">
         <f t="shared" si="1"/>
-        <v>1.8975332068311196E-3</v>
+        <v>2.5316455696202532E-3</v>
       </c>
       <c r="Q18">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="R18">
         <f t="shared" si="3"/>
-        <v>5.1000000000000156E-2</v>
+        <v>0.12400000000000055</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.35">
@@ -34022,35 +34064,35 @@
         <v>9</v>
       </c>
       <c r="J19">
-        <v>0</v>
+        <v>0.01</v>
       </c>
       <c r="K19">
-        <v>2.3E-2</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="L19">
-        <v>2.5999999999999999E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="M19">
-        <v>62.2</v>
+        <v>26.684999999999999</v>
       </c>
       <c r="N19">
-        <v>2213</v>
+        <v>2040</v>
       </c>
       <c r="O19">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>176</v>
       </c>
       <c r="P19">
         <f t="shared" si="1"/>
-        <v>1.3556258472661546E-3</v>
+        <v>8.6274509803921567E-2</v>
       </c>
       <c r="Q19">
         <f t="shared" si="2"/>
-        <v>0</v>
+        <v>1.4999999999999999E-2</v>
       </c>
       <c r="R19">
         <f t="shared" si="3"/>
-        <v>0.45199999999999818</v>
+        <v>35.966999999999999</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
@@ -34076,35 +34118,35 @@
         <v>192</v>
       </c>
       <c r="J20">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="K20">
-        <v>3.2000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="L20">
-        <v>0.04</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="M20">
-        <v>24.454999999999998</v>
+        <v>21.431000000000001</v>
       </c>
       <c r="N20">
-        <v>842</v>
+        <v>827</v>
       </c>
       <c r="O20">
         <f t="shared" si="0"/>
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="P20">
         <f t="shared" si="1"/>
-        <v>2.8503562945368172E-2</v>
+        <v>4.7158403869407499E-2</v>
       </c>
       <c r="Q20">
         <f t="shared" si="2"/>
-        <v>-2.0000000000000018E-3</v>
+        <v>3.9999999999999966E-3</v>
       </c>
       <c r="R20">
         <f t="shared" si="3"/>
-        <v>4.5840000000000032</v>
+        <v>7.6080000000000005</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.35">
@@ -34238,35 +34280,35 @@
         <v>14</v>
       </c>
       <c r="J23">
-        <v>0</v>
+        <v>1E-3</v>
       </c>
       <c r="K23">
-        <v>5.0999999999999997E-2</v>
+        <v>3.3000000000000002E-2</v>
       </c>
       <c r="L23">
-        <v>5.8999999999999997E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="M23">
-        <v>23.785</v>
+        <v>17.109000000000002</v>
       </c>
       <c r="N23">
-        <v>673</v>
+        <v>637</v>
       </c>
       <c r="O23">
         <f t="shared" si="0"/>
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="P23">
         <f t="shared" si="1"/>
-        <v>1.4858841010401188E-3</v>
+        <v>5.8084772370486655E-2</v>
       </c>
       <c r="Q23">
         <f t="shared" si="2"/>
-        <v>-1.9999999999999948E-3</v>
+        <v>1.6E-2</v>
       </c>
       <c r="R23">
         <f t="shared" si="3"/>
-        <v>4.5999999999999375E-2</v>
+        <v>6.7219999999999978</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.35">
@@ -34295,32 +34337,32 @@
         <v>0</v>
       </c>
       <c r="K24">
-        <v>2.1999999999999999E-2</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="L24">
-        <v>2.4E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="M24">
-        <v>24.63</v>
+        <v>21.477</v>
       </c>
       <c r="N24">
-        <v>2168</v>
+        <v>2133</v>
       </c>
       <c r="O24">
         <f t="shared" si="0"/>
-        <v>318</v>
+        <v>353</v>
       </c>
       <c r="P24">
         <f t="shared" si="1"/>
-        <v>0.14667896678966791</v>
+        <v>0.16549460853258322</v>
       </c>
       <c r="Q24">
         <f t="shared" si="2"/>
-        <v>1.8999999999999996E-2</v>
+        <v>1.9999999999999997E-2</v>
       </c>
       <c r="R24">
         <f t="shared" si="3"/>
-        <v>31.498999999999999</v>
+        <v>34.652000000000001</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.35">
@@ -34346,35 +34388,35 @@
         <v>160</v>
       </c>
       <c r="J25">
-        <v>8.9999999999999993E-3</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="K25">
-        <v>3.1E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="L25">
-        <v>4.1000000000000002E-2</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="M25">
-        <v>97.986000000000004</v>
+        <v>29.831</v>
       </c>
       <c r="N25">
-        <v>462</v>
+        <v>410</v>
       </c>
       <c r="O25">
         <f t="shared" si="0"/>
-        <v>4</v>
+        <v>56</v>
       </c>
       <c r="P25">
         <f t="shared" si="1"/>
-        <v>8.658008658008658E-3</v>
+        <v>0.13658536585365855</v>
       </c>
       <c r="Q25">
         <f t="shared" si="2"/>
-        <v>-1.2E-2</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="R25">
         <f t="shared" si="3"/>
-        <v>5.9779999999999944</v>
+        <v>74.132999999999996</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
@@ -34457,32 +34499,32 @@
         <v>0</v>
       </c>
       <c r="K27">
-        <v>6.6000000000000003E-2</v>
+        <v>6.8000000000000005E-2</v>
       </c>
       <c r="L27">
-        <v>6.9000000000000006E-2</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="M27">
-        <v>35.896000000000001</v>
+        <v>35.003999999999998</v>
       </c>
       <c r="N27">
-        <v>2154</v>
+        <v>2144</v>
       </c>
       <c r="O27">
         <f t="shared" si="0"/>
-        <v>114</v>
+        <v>124</v>
       </c>
       <c r="P27">
         <f t="shared" si="1"/>
-        <v>5.2924791086350974E-2</v>
+        <v>5.7835820895522388E-2</v>
       </c>
       <c r="Q27">
         <f t="shared" si="2"/>
-        <v>2.6999999999999996E-2</v>
+        <v>2.5000000000000008E-2</v>
       </c>
       <c r="R27">
         <f t="shared" si="3"/>
-        <v>10.591000000000001</v>
+        <v>11.483000000000004</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.35">
@@ -34562,27 +34604,27 @@
         <v>11</v>
       </c>
       <c r="J29">
-        <v>3.0000000000000001E-3</v>
+        <v>1.2E-2</v>
       </c>
       <c r="K29">
-        <v>5.0000000000000001E-3</v>
+        <v>4.0000000000000001E-3</v>
       </c>
       <c r="L29">
         <v>6.0000000000000001E-3</v>
       </c>
       <c r="M29">
-        <v>27.884</v>
+        <v>22.841000000000001</v>
       </c>
       <c r="N29">
-        <v>3115</v>
+        <v>3060</v>
       </c>
       <c r="O29">
         <f t="shared" si="0"/>
-        <v>447</v>
+        <v>502</v>
       </c>
       <c r="P29">
         <f t="shared" si="1"/>
-        <v>0.14349919743178169</v>
+        <v>0.16405228758169935</v>
       </c>
       <c r="Q29">
         <f>D29-L29</f>
@@ -34590,7 +34632,7 @@
       </c>
       <c r="R29">
         <f t="shared" si="3"/>
-        <v>32.805</v>
+        <v>37.847999999999999</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.35">
@@ -34670,35 +34712,35 @@
         <v>193</v>
       </c>
       <c r="J31">
-        <v>0</v>
+        <v>1.9E-2</v>
       </c>
       <c r="K31">
-        <v>0.09</v>
+        <v>0.05</v>
       </c>
       <c r="L31">
-        <v>0.11</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="M31">
-        <v>19.895</v>
+        <v>13.486000000000001</v>
       </c>
       <c r="N31">
-        <v>246</v>
+        <v>206</v>
       </c>
       <c r="O31">
         <f t="shared" ref="O31:O42" si="4">F32-N31</f>
-        <v>0</v>
+        <v>40</v>
       </c>
       <c r="P31">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>0.1941747572815534</v>
       </c>
       <c r="Q31">
-        <f t="shared" ref="Q31:Q44" si="5">D32-L31</f>
-        <v>0</v>
+        <f t="shared" ref="Q31:Q42" si="5">D32-L31</f>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="R31">
         <f t="shared" ref="R31:R42" si="6">E32-M31</f>
-        <v>0</v>
+        <v>6.4089999999999989</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
@@ -34838,29 +34880,29 @@
         <v>2.1000000000000001E-2</v>
       </c>
       <c r="L34">
-        <v>2.4E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="M34">
-        <v>13.988</v>
+        <v>13.37</v>
       </c>
       <c r="N34">
-        <v>1927</v>
+        <v>1914</v>
       </c>
       <c r="O34">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>13</v>
       </c>
       <c r="P34">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>6.7920585161964468E-3</v>
       </c>
       <c r="Q34">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.0000000000000009E-3</v>
       </c>
       <c r="R34">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>0.61800000000000033</v>
       </c>
     </row>
     <row r="35" spans="1:18" x14ac:dyDescent="0.35">
@@ -34886,35 +34928,35 @@
         <v>10</v>
       </c>
       <c r="J35">
-        <v>6.0999999999999999E-2</v>
+        <v>5.0000000000000001E-3</v>
       </c>
       <c r="K35">
-        <v>0.01</v>
+        <v>2.8000000000000001E-2</v>
       </c>
       <c r="L35">
-        <v>1.4E-2</v>
+        <v>0.04</v>
       </c>
       <c r="M35">
-        <v>45.295999999999999</v>
+        <v>36.688000000000002</v>
       </c>
       <c r="N35">
-        <v>664</v>
+        <v>641</v>
       </c>
       <c r="O35">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>23</v>
       </c>
       <c r="P35">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>3.5881435257410298E-2</v>
       </c>
       <c r="Q35">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-2.6000000000000002E-2</v>
       </c>
       <c r="R35">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8.607999999999997</v>
       </c>
     </row>
     <row r="36" spans="1:18" x14ac:dyDescent="0.35">
@@ -34943,32 +34985,32 @@
         <v>0</v>
       </c>
       <c r="K36">
-        <v>3.7999999999999999E-2</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="L36">
-        <v>4.2000000000000003E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="M36">
-        <v>17.315000000000001</v>
+        <v>16.640999999999998</v>
       </c>
       <c r="N36">
-        <v>1409</v>
+        <v>1406</v>
       </c>
       <c r="O36">
         <f t="shared" si="4"/>
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="P36">
         <f t="shared" si="1"/>
-        <v>7.1682044002838896E-2</v>
+        <v>7.3968705547652919E-2</v>
       </c>
       <c r="Q36">
         <f t="shared" si="5"/>
-        <v>4.7999999999999994E-2</v>
+        <v>4.4999999999999998E-2</v>
       </c>
       <c r="R36">
         <f t="shared" si="6"/>
-        <v>36.551999999999992</v>
+        <v>37.225999999999999</v>
       </c>
     </row>
     <row r="37" spans="1:18" x14ac:dyDescent="0.35">
@@ -34994,35 +35036,35 @@
         <v>15</v>
       </c>
       <c r="J37">
-        <v>0</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="K37">
-        <v>1.9E-2</v>
+        <v>1.6E-2</v>
       </c>
       <c r="L37">
-        <v>2.5000000000000001E-2</v>
+        <v>2.1999999999999999E-2</v>
       </c>
       <c r="M37">
-        <v>20.257000000000001</v>
+        <v>17.803000000000001</v>
       </c>
       <c r="N37">
-        <v>1348</v>
+        <v>1331</v>
       </c>
       <c r="O37">
         <f t="shared" si="4"/>
-        <v>20</v>
+        <v>37</v>
       </c>
       <c r="P37">
         <f t="shared" si="1"/>
-        <v>1.483679525222552E-2</v>
+        <v>2.7798647633358379E-2</v>
       </c>
       <c r="Q37">
         <f t="shared" si="5"/>
-        <v>4.0000000000000001E-3</v>
+        <v>7.0000000000000027E-3</v>
       </c>
       <c r="R37">
         <f t="shared" si="6"/>
-        <v>1.6289999999999978</v>
+        <v>4.0829999999999984</v>
       </c>
     </row>
     <row r="38" spans="1:18" x14ac:dyDescent="0.35">
@@ -35105,32 +35147,32 @@
         <v>0</v>
       </c>
       <c r="K39">
-        <v>0.04</v>
+        <v>3.7999999999999999E-2</v>
       </c>
       <c r="L39">
-        <v>4.3999999999999997E-2</v>
+        <v>4.2999999999999997E-2</v>
       </c>
       <c r="M39">
-        <v>11.335000000000001</v>
+        <v>11.081</v>
       </c>
       <c r="N39">
-        <v>1572</v>
+        <v>1569</v>
       </c>
       <c r="O39">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="P39">
         <f t="shared" si="1"/>
-        <v>1.9083969465648854E-3</v>
+        <v>3.8240917782026767E-3</v>
       </c>
       <c r="Q39">
         <f t="shared" si="5"/>
-        <v>1.0000000000000009E-3</v>
+        <v>2.0000000000000018E-3</v>
       </c>
       <c r="R39">
         <f t="shared" si="6"/>
-        <v>0.13599999999999923</v>
+        <v>0.39000000000000057</v>
       </c>
     </row>
     <row r="40" spans="1:18" x14ac:dyDescent="0.35">
@@ -35156,35 +35198,35 @@
         <v>8</v>
       </c>
       <c r="J40">
-        <v>1E-3</v>
+        <v>4.8000000000000001E-2</v>
       </c>
       <c r="K40">
-        <v>2.1000000000000001E-2</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="L40">
-        <v>2.8000000000000001E-2</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="M40">
-        <v>34.43</v>
+        <v>26.292999999999999</v>
       </c>
       <c r="N40">
-        <v>1170</v>
+        <v>1117</v>
       </c>
       <c r="O40">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>53</v>
       </c>
       <c r="P40">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>4.7448522829006266E-2</v>
       </c>
       <c r="Q40">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1.0999999999999999E-2</v>
       </c>
       <c r="R40">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>8.1370000000000005</v>
       </c>
     </row>
     <row r="41" spans="1:18" x14ac:dyDescent="0.35">
@@ -35267,32 +35309,32 @@
         <v>0</v>
       </c>
       <c r="K42">
-        <v>5.3999999999999999E-2</v>
+        <v>5.1999999999999998E-2</v>
       </c>
       <c r="L42">
-        <v>5.8000000000000003E-2</v>
+        <v>5.7000000000000002E-2</v>
       </c>
       <c r="M42">
-        <v>15.227</v>
+        <v>13.622</v>
       </c>
       <c r="N42">
-        <v>1080</v>
+        <v>1068</v>
       </c>
       <c r="O42">
         <f t="shared" si="4"/>
-        <v>98</v>
+        <v>110</v>
       </c>
       <c r="P42">
         <f t="shared" si="1"/>
-        <v>9.0740740740740747E-2</v>
+        <v>0.10299625468164794</v>
       </c>
       <c r="Q42">
         <f t="shared" si="5"/>
-        <v>2.4E-2</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="R42">
         <f t="shared" si="6"/>
-        <v>24.602</v>
+        <v>26.207000000000001</v>
       </c>
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.35">
@@ -35316,19 +35358,19 @@
       </c>
       <c r="L43">
         <f>SUM(L3:L42)+D30</f>
-        <v>1.5250000000000004</v>
+        <v>1.3749999999999998</v>
       </c>
       <c r="O43">
         <f>SUM(O3:O42)</f>
-        <v>2031</v>
+        <v>3441</v>
       </c>
       <c r="Q43">
         <f>SUM(Q3:Q42)</f>
-        <v>0.159</v>
+        <v>0.30900000000000005</v>
       </c>
       <c r="R43">
         <f>SUM(R3:R42)</f>
-        <v>325.84999999999991</v>
+        <v>896.01100000000008</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.35">
@@ -38952,8 +38994,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A3:F43">
-    <sortCondition ref="A2"/>
+  <sortState ref="I3:N42">
+    <sortCondition ref="I2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
     <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
@@ -38987,18 +39029,19 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AO20"/>
+  <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="AL2" sqref="AL2"/>
+    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="W7" sqref="W7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="25" max="25" width="12.54296875" customWidth="1"/>
+    <col min="26" max="26" width="12.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:40" x14ac:dyDescent="0.35">
       <c r="B1" t="s">
         <v>144</v>
       </c>
@@ -39060,7 +39103,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -39121,45 +39164,44 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="78" t="s">
+      <c r="W2" s="79" t="s">
         <v>108</v>
       </c>
-      <c r="X2" s="78"/>
+      <c r="X2" s="79"/>
       <c r="Y2" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="Z2" s="78" t="s">
+      <c r="Z2" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA2" s="80" t="s">
         <v>179</v>
       </c>
-      <c r="AA2" s="78"/>
-      <c r="AB2" s="78" t="s">
+      <c r="AB2" s="81"/>
+      <c r="AC2" s="79" t="s">
         <v>180</v>
       </c>
-      <c r="AC2" s="78"/>
-      <c r="AD2" s="78"/>
-      <c r="AE2" s="78"/>
-      <c r="AF2" s="63" t="s">
+      <c r="AD2" s="79"/>
+      <c r="AE2" s="79"/>
+      <c r="AF2" s="79"/>
+      <c r="AG2" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="AG2" s="78" t="s">
+      <c r="AH2" s="79" t="s">
         <v>182</v>
       </c>
-      <c r="AH2" s="78"/>
-      <c r="AI2" s="78"/>
-      <c r="AJ2" s="78"/>
-      <c r="AK2" s="78"/>
-      <c r="AL2" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="AM2" s="78" t="s">
+      <c r="AI2" s="79"/>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="79"/>
+      <c r="AL2" s="79"/>
+      <c r="AM2" s="68" t="s">
         <v>194</v>
       </c>
-      <c r="AN2" s="78"/>
-      <c r="AO2" s="63" t="s">
+      <c r="AN2" s="63" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="3" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -39230,55 +39272,52 @@
         <v>171</v>
       </c>
       <c r="Z3" s="64" t="s">
+        <v>1</v>
+      </c>
+      <c r="AA3" s="64" t="s">
         <v>162</v>
       </c>
-      <c r="AA3" s="64" t="s">
+      <c r="AB3" s="64" t="s">
         <v>174</v>
       </c>
-      <c r="AB3" s="64" t="s">
+      <c r="AC3" s="64" t="s">
         <v>163</v>
       </c>
-      <c r="AC3" s="64" t="s">
+      <c r="AD3" s="64" t="s">
         <v>164</v>
       </c>
-      <c r="AD3" s="64" t="s">
+      <c r="AE3" s="64" t="s">
         <v>165</v>
       </c>
-      <c r="AE3" s="64" t="s">
+      <c r="AF3" s="64" t="s">
         <v>166</v>
       </c>
-      <c r="AF3" s="64" t="s">
+      <c r="AG3" s="64" t="s">
         <v>167</v>
       </c>
-      <c r="AG3" s="64" t="s">
+      <c r="AH3" s="64" t="s">
         <v>168</v>
       </c>
-      <c r="AH3" s="64" t="s">
+      <c r="AI3" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="AI3" s="64" t="s">
+      <c r="AJ3" s="64" t="s">
         <v>170</v>
       </c>
-      <c r="AJ3" s="64" t="s">
+      <c r="AK3" s="64" t="s">
         <v>172</v>
       </c>
-      <c r="AK3" s="64" t="s">
+      <c r="AL3" s="64" t="s">
         <v>173</v>
       </c>
-      <c r="AL3" s="64" t="s">
-        <v>1</v>
-      </c>
       <c r="AM3" s="64" t="s">
-        <v>175</v>
+        <v>210</v>
       </c>
       <c r="AN3" s="64" t="s">
-        <v>176</v>
-      </c>
-      <c r="AO3" s="64" t="s">
         <v>177</v>
       </c>
     </row>
-    <row r="4" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>162</v>
       </c>
@@ -39340,7 +39379,7 @@
         <v>5.5942452752326297E-6</v>
       </c>
     </row>
-    <row r="5" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>163</v>
       </c>
@@ -39402,7 +39441,7 @@
         <v>-7.3686962765428604E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>164</v>
       </c>
@@ -39464,7 +39503,7 @@
         <v>2.9393003925370101E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>165</v>
       </c>
@@ -39526,7 +39565,7 @@
         <v>0.13362405085409901</v>
       </c>
     </row>
-    <row r="8" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>166</v>
       </c>
@@ -39588,7 +39627,7 @@
         <v>0.473067198112951</v>
       </c>
     </row>
-    <row r="9" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>167</v>
       </c>
@@ -39650,7 +39689,7 @@
         <v>0.107278697146521</v>
       </c>
     </row>
-    <row r="10" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>168</v>
       </c>
@@ -39712,7 +39751,7 @@
         <v>-0.23302181614993001</v>
       </c>
     </row>
-    <row r="11" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>169</v>
       </c>
@@ -39774,7 +39813,7 @@
         <v>-0.111524530431619</v>
       </c>
     </row>
-    <row r="12" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>170</v>
       </c>
@@ -39836,7 +39875,7 @@
         <v>7.5981980401873303E-2</v>
       </c>
     </row>
-    <row r="13" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>1</v>
       </c>
@@ -39898,7 +39937,7 @@
         <v>-0.233223687346237</v>
       </c>
     </row>
-    <row r="14" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>171</v>
       </c>
@@ -39960,7 +39999,7 @@
         <v>5.1378752191800402E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>172</v>
       </c>
@@ -40022,7 +40061,7 @@
         <v>0.207532880594967</v>
       </c>
     </row>
-    <row r="16" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:40" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>173</v>
       </c>
@@ -40333,12 +40372,11 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="4">
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="AB2:AE2"/>
-    <mergeCell ref="AG2:AK2"/>
-    <mergeCell ref="AM2:AN2"/>
+    <mergeCell ref="AA2:AB2"/>
+    <mergeCell ref="AC2:AF2"/>
+    <mergeCell ref="AH2:AL2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Changed renaming of variables so it is outside of species loop
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="4" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
@@ -561,9 +561,6 @@
     <t>Year</t>
   </si>
   <si>
-    <t>Kn ~ local environment + broad env + resource quality + resource availability + fish pressure + local density + population density</t>
-  </si>
-  <si>
     <t>Local Environment</t>
   </si>
   <si>
@@ -658,6 +655,9 @@
   </si>
   <si>
     <t>Average Lat/Lon by Strata</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Kn ~ local environment + broad env + resource quality + resource availability + local density + population density + fish pressure </t>
   </si>
 </sst>
 </file>
@@ -20710,7 +20710,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z192"/>
   <sheetViews>
-    <sheetView topLeftCell="O161" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I161" workbookViewId="0">
       <selection activeCell="P153" sqref="P153"/>
     </sheetView>
   </sheetViews>
@@ -29009,8 +29009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BL33"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AD29" sqref="AD29"/>
+    <sheetView topLeftCell="AV1" workbookViewId="0">
+      <selection activeCell="BH4" sqref="BH4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -33104,10 +33104,10 @@
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B1" s="66" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C1" s="66"/>
       <c r="D1" s="66"/>
@@ -33116,7 +33116,7 @@
       <c r="G1" s="66"/>
       <c r="H1" s="66"/>
       <c r="I1" s="67" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="J1" s="67"/>
       <c r="K1" s="67"/>
@@ -33126,7 +33126,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
@@ -33144,7 +33144,7 @@
         <v>0</v>
       </c>
       <c r="J2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="K2" t="s">
         <v>2</v>
@@ -33159,19 +33159,19 @@
         <v>5</v>
       </c>
       <c r="O2" t="s">
+        <v>201</v>
+      </c>
+      <c r="P2" t="s">
         <v>202</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>203</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>204</v>
       </c>
-      <c r="R2" t="s">
-        <v>205</v>
-      </c>
       <c r="T2" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.35">
@@ -33338,7 +33338,7 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B6">
         <v>1E-3</v>
@@ -33356,7 +33356,7 @@
         <v>902</v>
       </c>
       <c r="I6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="J6">
         <v>1E-3</v>
@@ -33444,7 +33444,7 @@
         <v>78.343999999999994</v>
       </c>
       <c r="T7" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.35">
@@ -33665,7 +33665,7 @@
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B12">
         <v>3.0000000000000001E-3</v>
@@ -33683,7 +33683,7 @@
         <v>380</v>
       </c>
       <c r="I12" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="J12">
         <v>0</v>
@@ -33719,7 +33719,7 @@
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.35">
       <c r="A13" s="66" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B13">
         <v>0.17699999999999999</v>
@@ -33737,7 +33737,7 @@
         <v>426</v>
       </c>
       <c r="I13" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J13">
         <v>0.36299999999999999</v>
@@ -34097,7 +34097,7 @@
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B20">
         <v>0</v>
@@ -34115,7 +34115,7 @@
         <v>866</v>
       </c>
       <c r="I20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="J20">
         <v>1E-3</v>
@@ -34205,7 +34205,7 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B22">
         <v>2E-3</v>
@@ -34223,7 +34223,7 @@
         <v>299</v>
       </c>
       <c r="I22" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="J22">
         <v>4.0000000000000001E-3</v>
@@ -34421,7 +34421,7 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A26" s="67" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B26">
         <v>8.3000000000000004E-2</v>
@@ -34439,7 +34439,7 @@
         <v>201</v>
       </c>
       <c r="I26" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="J26">
         <v>8.3000000000000004E-2</v>
@@ -34709,7 +34709,7 @@
         <v>523</v>
       </c>
       <c r="I31" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="J31">
         <v>1.9E-2</v>
@@ -34745,7 +34745,7 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B32">
         <v>0</v>
@@ -35379,18 +35379,18 @@
         <v>1.6840000000000002</v>
       </c>
       <c r="Q44" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="R44" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B45" s="66" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="46" spans="1:18" x14ac:dyDescent="0.35">
@@ -35398,7 +35398,7 @@
         <v>0</v>
       </c>
       <c r="B46" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C46" t="s">
         <v>2</v>
@@ -35415,7 +35415,7 @@
     </row>
     <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B47">
         <v>3.0000000000000001E-3</v>
@@ -35475,7 +35475,7 @@
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B50">
         <v>0</v>
@@ -35495,7 +35495,7 @@
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B51">
         <v>7.0000000000000001E-3</v>
@@ -35675,7 +35675,7 @@
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A60" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B60">
         <v>0.04</v>
@@ -36035,7 +36035,7 @@
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A78" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -36135,7 +36135,7 @@
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -36215,7 +36215,7 @@
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="66" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B87">
         <v>0.46600000000000003</v>
@@ -36260,7 +36260,7 @@
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B91">
         <v>4.1000000000000002E-2</v>
@@ -36320,7 +36320,7 @@
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A94" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B94">
         <v>0</v>
@@ -36340,7 +36340,7 @@
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A95" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B95">
         <v>0.115</v>
@@ -36520,7 +36520,7 @@
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A104" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B104">
         <v>2E-3</v>
@@ -36880,7 +36880,7 @@
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A122" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -36980,7 +36980,7 @@
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A127" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B127">
         <v>0.36</v>
@@ -37060,7 +37060,7 @@
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A131" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B131">
         <v>0.184</v>
@@ -37105,7 +37105,7 @@
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A135" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -37165,7 +37165,7 @@
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A138" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B138">
         <v>8.9999999999999993E-3</v>
@@ -37185,7 +37185,7 @@
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A139" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B139">
         <v>0.41399999999999998</v>
@@ -37365,7 +37365,7 @@
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A148" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B148">
         <v>1E-3</v>
@@ -37725,7 +37725,7 @@
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A166" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B166">
         <v>0.61299999999999999</v>
@@ -37825,7 +37825,7 @@
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A171" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B171">
         <v>3.0000000000000001E-3</v>
@@ -37905,7 +37905,7 @@
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A175" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B175">
         <v>0.19800000000000001</v>
@@ -37950,7 +37950,7 @@
     </row>
     <row r="179" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A179" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B179">
         <v>2.4E-2</v>
@@ -38010,7 +38010,7 @@
     </row>
     <row r="182" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A182" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B182">
         <v>0.104</v>
@@ -38030,7 +38030,7 @@
     </row>
     <row r="183" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A183" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B183">
         <v>0.59099999999999997</v>
@@ -38210,7 +38210,7 @@
     </row>
     <row r="192" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A192" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B192">
         <v>5.8999999999999997E-2</v>
@@ -38570,7 +38570,7 @@
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A210" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B210">
         <v>2E-3</v>
@@ -38670,7 +38670,7 @@
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A215" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B215">
         <v>4.2000000000000003E-2</v>
@@ -38750,7 +38750,7 @@
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A219" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B219">
         <v>0.33800000000000002</v>
@@ -38770,7 +38770,7 @@
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A221" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.35">
@@ -38778,7 +38778,7 @@
         <v>0</v>
       </c>
       <c r="B222" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C222" t="s">
         <v>2</v>
@@ -38795,7 +38795,7 @@
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A223" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B223">
         <v>0.13400000000000001</v>
@@ -38855,7 +38855,7 @@
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A226" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -38875,7 +38875,7 @@
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A227" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B227">
         <v>0.42199999999999999</v>
@@ -39031,14 +39031,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" zoomScale="117" workbookViewId="0">
-      <selection activeCell="W7" sqref="W7"/>
+    <sheetView topLeftCell="V1" zoomScale="146" workbookViewId="0">
+      <selection activeCell="AC3" sqref="AC3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="25" max="25" width="12.54296875" customWidth="1"/>
-    <col min="26" max="26" width="12.81640625" customWidth="1"/>
+    <col min="23" max="23" width="17" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="20.08984375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.7265625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="8.81640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="18.7265625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="18.81640625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.1796875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.08984375" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="11.81640625" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.54296875" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="22.36328125" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.35">
@@ -39100,7 +39116,7 @@
         <v>177</v>
       </c>
       <c r="W1" s="62" t="s">
-        <v>178</v>
+        <v>210</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.35">
@@ -39164,41 +39180,41 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="79" t="s">
-        <v>108</v>
-      </c>
-      <c r="X2" s="79"/>
-      <c r="Y2" s="63" t="s">
-        <v>184</v>
-      </c>
-      <c r="Z2" s="63" t="s">
-        <v>183</v>
-      </c>
-      <c r="AA2" s="80" t="s">
+      <c r="W2" s="80" t="s">
+        <v>178</v>
+      </c>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="79" t="s">
         <v>179</v>
       </c>
-      <c r="AB2" s="81"/>
-      <c r="AC2" s="79" t="s">
+      <c r="Z2" s="79"/>
+      <c r="AA2" s="79"/>
+      <c r="AB2" s="79"/>
+      <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="79"/>
+      <c r="AD2" s="79" t="s">
+        <v>181</v>
+      </c>
       <c r="AE2" s="79"/>
       <c r="AF2" s="79"/>
-      <c r="AG2" s="63" t="s">
-        <v>181</v>
-      </c>
-      <c r="AH2" s="79" t="s">
+      <c r="AG2" s="79"/>
+      <c r="AH2" s="79"/>
+      <c r="AI2" s="79" t="s">
+        <v>108</v>
+      </c>
+      <c r="AJ2" s="79"/>
+      <c r="AK2" s="63" t="s">
+        <v>183</v>
+      </c>
+      <c r="AL2" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="AI2" s="79"/>
-      <c r="AJ2" s="79"/>
-      <c r="AK2" s="79"/>
-      <c r="AL2" s="79"/>
       <c r="AM2" s="68" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="AN2" s="63" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.35">
@@ -39263,55 +39279,55 @@
         <v>6.04172529893826E-3</v>
       </c>
       <c r="W3" s="64" t="s">
+        <v>162</v>
+      </c>
+      <c r="X3" s="64" t="s">
+        <v>174</v>
+      </c>
+      <c r="Y3" s="64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z3" s="64" t="s">
+        <v>164</v>
+      </c>
+      <c r="AA3" s="64" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB3" s="64" t="s">
+        <v>166</v>
+      </c>
+      <c r="AC3" s="64" t="s">
+        <v>167</v>
+      </c>
+      <c r="AD3" s="64" t="s">
+        <v>168</v>
+      </c>
+      <c r="AE3" s="64" t="s">
+        <v>169</v>
+      </c>
+      <c r="AF3" s="64" t="s">
+        <v>170</v>
+      </c>
+      <c r="AG3" s="64" t="s">
+        <v>172</v>
+      </c>
+      <c r="AH3" s="64" t="s">
+        <v>173</v>
+      </c>
+      <c r="AI3" s="64" t="s">
         <v>144</v>
       </c>
-      <c r="X3" s="64" t="s">
+      <c r="AJ3" s="64" t="s">
         <v>145</v>
       </c>
-      <c r="Y3" s="64" t="s">
+      <c r="AK3" s="64" t="s">
         <v>171</v>
       </c>
-      <c r="Z3" s="64" t="s">
+      <c r="AL3" s="64" t="s">
         <v>1</v>
       </c>
-      <c r="AA3" s="64" t="s">
-        <v>162</v>
-      </c>
-      <c r="AB3" s="64" t="s">
-        <v>174</v>
-      </c>
-      <c r="AC3" s="64" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD3" s="64" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE3" s="64" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF3" s="64" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG3" s="64" t="s">
-        <v>167</v>
-      </c>
-      <c r="AH3" s="64" t="s">
-        <v>168</v>
-      </c>
-      <c r="AI3" s="64" t="s">
-        <v>169</v>
-      </c>
-      <c r="AJ3" s="64" t="s">
-        <v>170</v>
-      </c>
-      <c r="AK3" s="64" t="s">
-        <v>172</v>
-      </c>
-      <c r="AL3" s="64" t="s">
-        <v>173</v>
-      </c>
       <c r="AM3" s="64" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="AN3" s="64" t="s">
         <v>177</v>
@@ -40373,10 +40389,10 @@
     </row>
   </sheetData>
   <mergeCells count="4">
+    <mergeCell ref="AI2:AJ2"/>
     <mergeCell ref="W2:X2"/>
-    <mergeCell ref="AA2:AB2"/>
-    <mergeCell ref="AC2:AF2"/>
-    <mergeCell ref="AH2:AL2"/>
+    <mergeCell ref="Y2:AB2"/>
+    <mergeCell ref="AD2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
     <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">

</xml_diff>

<commit_message>
Bringing in copepod small/large and total by NEFSC survey strata instead of EPU
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="5" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
@@ -19,13 +19,14 @@
     <sheet name="MechanismSummaryTable" sheetId="2" r:id="rId5"/>
     <sheet name="2021 SingleGAMs" sheetId="7" r:id="rId6"/>
     <sheet name="Correlations 2021GAM selection" sheetId="6" r:id="rId7"/>
+    <sheet name="AutoGAMsEPUfullmissingdata" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1886" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="212">
   <si>
     <t>Species</t>
   </si>
@@ -658,6 +659,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kn ~ local environment + broad env + resource quality + resource availability + local density + population density + fish pressure </t>
+  </si>
+  <si>
+    <t>x</t>
   </si>
 </sst>
 </file>
@@ -1707,7 +1711,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="88">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1939,6 +1943,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -20710,7 +20732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z192"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I161" workbookViewId="0">
+    <sheetView topLeftCell="I161" workbookViewId="0">
       <selection activeCell="P153" sqref="P153"/>
     </sheetView>
   </sheetViews>
@@ -39031,8 +39053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView topLeftCell="V1" zoomScale="146" workbookViewId="0">
-      <selection activeCell="AC3" sqref="AC3"/>
+    <sheetView topLeftCell="U1" zoomScale="146" workbookViewId="0">
+      <selection activeCell="AM3" sqref="W1:AM3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40414,4 +40436,757 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <pane xSplit="8" ySplit="1" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
+      <selection activeCell="A3" sqref="A3"/>
+      <selection pane="topRight" activeCell="I3" sqref="I3"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="15.54296875" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" customWidth="1"/>
+    <col min="3" max="3" width="12" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" customWidth="1"/>
+    <col min="16" max="16" width="9.81640625" customWidth="1"/>
+    <col min="18" max="18" width="11.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="B1" s="62" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="82" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B2" s="83" t="s">
+        <v>178</v>
+      </c>
+      <c r="C2" s="84"/>
+      <c r="D2" s="85" t="s">
+        <v>179</v>
+      </c>
+      <c r="E2" s="85"/>
+      <c r="F2" s="85"/>
+      <c r="G2" s="85"/>
+      <c r="H2" s="86" t="s">
+        <v>180</v>
+      </c>
+      <c r="I2" s="85" t="s">
+        <v>181</v>
+      </c>
+      <c r="J2" s="85"/>
+      <c r="K2" s="85"/>
+      <c r="L2" s="85"/>
+      <c r="M2" s="85"/>
+      <c r="N2" s="85" t="s">
+        <v>108</v>
+      </c>
+      <c r="O2" s="85"/>
+      <c r="P2" s="86" t="s">
+        <v>183</v>
+      </c>
+      <c r="Q2" s="86" t="s">
+        <v>182</v>
+      </c>
+      <c r="R2" s="86" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="82" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B3" s="87" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="D3" s="87" t="s">
+        <v>163</v>
+      </c>
+      <c r="E3" s="87" t="s">
+        <v>164</v>
+      </c>
+      <c r="F3" s="87" t="s">
+        <v>165</v>
+      </c>
+      <c r="G3" s="87" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="87" t="s">
+        <v>167</v>
+      </c>
+      <c r="I3" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="J3" s="87" t="s">
+        <v>169</v>
+      </c>
+      <c r="K3" s="87" t="s">
+        <v>170</v>
+      </c>
+      <c r="L3" s="87" t="s">
+        <v>172</v>
+      </c>
+      <c r="M3" s="87" t="s">
+        <v>173</v>
+      </c>
+      <c r="N3" s="87" t="s">
+        <v>144</v>
+      </c>
+      <c r="O3" s="87" t="s">
+        <v>145</v>
+      </c>
+      <c r="P3" s="87" t="s">
+        <v>171</v>
+      </c>
+      <c r="Q3" s="87" t="s">
+        <v>1</v>
+      </c>
+      <c r="R3" s="87" t="s">
+        <v>209</v>
+      </c>
+      <c r="S3" s="82" t="s">
+        <v>4</v>
+      </c>
+      <c r="T3" s="82" t="s">
+        <v>3</v>
+      </c>
+      <c r="U3" s="82" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4" t="s">
+        <v>211</v>
+      </c>
+      <c r="H4" t="s">
+        <v>211</v>
+      </c>
+      <c r="L4" t="s">
+        <v>211</v>
+      </c>
+      <c r="N4" t="s">
+        <v>211</v>
+      </c>
+      <c r="P4" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>211</v>
+      </c>
+      <c r="R4" t="s">
+        <v>211</v>
+      </c>
+      <c r="S4">
+        <v>23.66</v>
+      </c>
+      <c r="T4">
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="U4">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5" t="s">
+        <v>211</v>
+      </c>
+      <c r="L5" t="s">
+        <v>211</v>
+      </c>
+      <c r="N5" t="s">
+        <v>211</v>
+      </c>
+      <c r="R5" t="s">
+        <v>211</v>
+      </c>
+      <c r="S5">
+        <v>19.489999999999998</v>
+      </c>
+      <c r="T5">
+        <v>0.1578</v>
+      </c>
+      <c r="U5">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6" t="s">
+        <v>211</v>
+      </c>
+      <c r="M6" t="s">
+        <v>211</v>
+      </c>
+      <c r="O6" t="s">
+        <v>211</v>
+      </c>
+      <c r="R6" t="s">
+        <v>211</v>
+      </c>
+      <c r="S6">
+        <v>24.05</v>
+      </c>
+      <c r="T6">
+        <v>0.17219999999999999</v>
+      </c>
+      <c r="U6">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B7" t="s">
+        <v>211</v>
+      </c>
+      <c r="E7" t="s">
+        <v>211</v>
+      </c>
+      <c r="H7" t="s">
+        <v>211</v>
+      </c>
+      <c r="J7" t="s">
+        <v>211</v>
+      </c>
+      <c r="O7" t="s">
+        <v>211</v>
+      </c>
+      <c r="P7" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>211</v>
+      </c>
+      <c r="R7" t="s">
+        <v>211</v>
+      </c>
+      <c r="S7">
+        <v>8.4600000000000009</v>
+      </c>
+      <c r="T7">
+        <v>0.2122</v>
+      </c>
+      <c r="U7">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" t="s">
+        <v>211</v>
+      </c>
+      <c r="D8" t="s">
+        <v>211</v>
+      </c>
+      <c r="L8" t="s">
+        <v>211</v>
+      </c>
+      <c r="O8" t="s">
+        <v>211</v>
+      </c>
+      <c r="R8" t="s">
+        <v>211</v>
+      </c>
+      <c r="S8">
+        <v>46.67</v>
+      </c>
+      <c r="T8">
+        <v>0.14990000000000001</v>
+      </c>
+      <c r="U8">
+        <v>1082</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B9" t="s">
+        <v>211</v>
+      </c>
+      <c r="D9" t="s">
+        <v>211</v>
+      </c>
+      <c r="M9" t="s">
+        <v>211</v>
+      </c>
+      <c r="N9" t="s">
+        <v>211</v>
+      </c>
+      <c r="R9" t="s">
+        <v>211</v>
+      </c>
+      <c r="S9">
+        <v>18.89</v>
+      </c>
+      <c r="T9">
+        <v>0.1711</v>
+      </c>
+      <c r="U9">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10" t="s">
+        <v>211</v>
+      </c>
+      <c r="M10" t="s">
+        <v>211</v>
+      </c>
+      <c r="N10" t="s">
+        <v>211</v>
+      </c>
+      <c r="R10" t="s">
+        <v>211</v>
+      </c>
+      <c r="S10">
+        <v>16.059999999999999</v>
+      </c>
+      <c r="T10">
+        <v>0.1303</v>
+      </c>
+      <c r="U10">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B11" t="s">
+        <v>211</v>
+      </c>
+      <c r="D11" t="s">
+        <v>211</v>
+      </c>
+      <c r="H11" t="s">
+        <v>211</v>
+      </c>
+      <c r="M11" t="s">
+        <v>211</v>
+      </c>
+      <c r="O11" t="s">
+        <v>211</v>
+      </c>
+      <c r="P11" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>211</v>
+      </c>
+      <c r="R11" t="s">
+        <v>211</v>
+      </c>
+      <c r="S11">
+        <v>20.85</v>
+      </c>
+      <c r="T11">
+        <v>0.32519999999999999</v>
+      </c>
+      <c r="U11">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" t="s">
+        <v>211</v>
+      </c>
+      <c r="H12" t="s">
+        <v>211</v>
+      </c>
+      <c r="I12" t="s">
+        <v>211</v>
+      </c>
+      <c r="N12" t="s">
+        <v>211</v>
+      </c>
+      <c r="P12" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>211</v>
+      </c>
+      <c r="R12" t="s">
+        <v>211</v>
+      </c>
+      <c r="S12">
+        <v>33.68</v>
+      </c>
+      <c r="T12">
+        <v>0.11020000000000001</v>
+      </c>
+      <c r="U12">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>211</v>
+      </c>
+      <c r="D13" t="s">
+        <v>211</v>
+      </c>
+      <c r="I13" t="s">
+        <v>211</v>
+      </c>
+      <c r="O13" t="s">
+        <v>211</v>
+      </c>
+      <c r="R13" t="s">
+        <v>211</v>
+      </c>
+      <c r="S13">
+        <v>13.17</v>
+      </c>
+      <c r="T13">
+        <v>0.2238</v>
+      </c>
+      <c r="U13">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>16</v>
+      </c>
+      <c r="B14" t="s">
+        <v>211</v>
+      </c>
+      <c r="F14" t="s">
+        <v>211</v>
+      </c>
+      <c r="H14" t="s">
+        <v>211</v>
+      </c>
+      <c r="J14" t="s">
+        <v>211</v>
+      </c>
+      <c r="N14" t="s">
+        <v>211</v>
+      </c>
+      <c r="P14" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>211</v>
+      </c>
+      <c r="R14" t="s">
+        <v>211</v>
+      </c>
+      <c r="S14">
+        <v>19.57</v>
+      </c>
+      <c r="T14">
+        <v>0.23630000000000001</v>
+      </c>
+      <c r="U14">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>211</v>
+      </c>
+      <c r="E15" t="s">
+        <v>211</v>
+      </c>
+      <c r="M15" t="s">
+        <v>211</v>
+      </c>
+      <c r="O15" t="s">
+        <v>211</v>
+      </c>
+      <c r="R15" t="s">
+        <v>211</v>
+      </c>
+      <c r="S15">
+        <v>52.53</v>
+      </c>
+      <c r="T15">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="U15">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>27</v>
+      </c>
+      <c r="B16" t="s">
+        <v>211</v>
+      </c>
+      <c r="D16" t="s">
+        <v>211</v>
+      </c>
+      <c r="H16" t="s">
+        <v>211</v>
+      </c>
+      <c r="M16" t="s">
+        <v>211</v>
+      </c>
+      <c r="O16" t="s">
+        <v>211</v>
+      </c>
+      <c r="P16" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q16" t="s">
+        <v>211</v>
+      </c>
+      <c r="R16" t="s">
+        <v>211</v>
+      </c>
+      <c r="S16">
+        <v>31.77</v>
+      </c>
+      <c r="T16">
+        <v>0.18279999999999999</v>
+      </c>
+      <c r="U16">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+      <c r="B17" t="s">
+        <v>211</v>
+      </c>
+      <c r="F17" t="s">
+        <v>211</v>
+      </c>
+      <c r="H17" t="s">
+        <v>211</v>
+      </c>
+      <c r="M17" t="s">
+        <v>211</v>
+      </c>
+      <c r="O17" t="s">
+        <v>211</v>
+      </c>
+      <c r="P17" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>211</v>
+      </c>
+      <c r="R17" t="s">
+        <v>211</v>
+      </c>
+      <c r="S17">
+        <v>13.96</v>
+      </c>
+      <c r="T17">
+        <v>0.1061</v>
+      </c>
+      <c r="U17">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>211</v>
+      </c>
+      <c r="G18" t="s">
+        <v>211</v>
+      </c>
+      <c r="H18" t="s">
+        <v>211</v>
+      </c>
+      <c r="L18" t="s">
+        <v>211</v>
+      </c>
+      <c r="O18" t="s">
+        <v>211</v>
+      </c>
+      <c r="P18" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>211</v>
+      </c>
+      <c r="R18" t="s">
+        <v>211</v>
+      </c>
+      <c r="S18">
+        <v>22.79</v>
+      </c>
+      <c r="T18">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="U18">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" t="s">
+        <v>211</v>
+      </c>
+      <c r="E19" t="s">
+        <v>211</v>
+      </c>
+      <c r="J19" t="s">
+        <v>211</v>
+      </c>
+      <c r="N19" t="s">
+        <v>211</v>
+      </c>
+      <c r="R19" t="s">
+        <v>211</v>
+      </c>
+      <c r="S19">
+        <v>63.69</v>
+      </c>
+      <c r="T19">
+        <v>0.1002</v>
+      </c>
+      <c r="U19">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" t="s">
+        <v>211</v>
+      </c>
+      <c r="E20" t="s">
+        <v>211</v>
+      </c>
+      <c r="H20" t="s">
+        <v>211</v>
+      </c>
+      <c r="M20" t="s">
+        <v>211</v>
+      </c>
+      <c r="O20" t="s">
+        <v>211</v>
+      </c>
+      <c r="P20" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q20" t="s">
+        <v>211</v>
+      </c>
+      <c r="R20" t="s">
+        <v>211</v>
+      </c>
+      <c r="S20">
+        <v>11.31</v>
+      </c>
+      <c r="T20">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="U20">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" t="s">
+        <v>211</v>
+      </c>
+      <c r="G21" t="s">
+        <v>211</v>
+      </c>
+      <c r="H21" t="s">
+        <v>211</v>
+      </c>
+      <c r="J21" t="s">
+        <v>211</v>
+      </c>
+      <c r="O21" t="s">
+        <v>211</v>
+      </c>
+      <c r="P21" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q21" t="s">
+        <v>211</v>
+      </c>
+      <c r="R21" t="s">
+        <v>211</v>
+      </c>
+      <c r="S21">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="T21">
+        <v>0.37130000000000002</v>
+      </c>
+      <c r="U21">
+        <v>236</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B2:C2"/>
+    <mergeCell ref="D2:G2"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="N2:O2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Created StockUnit to include "Unit" when outside of PopDy survey strata definition. This allows unit stocks to merge assessment data with all data points for years assessed.
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2053" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="217">
   <si>
     <t>Species</t>
   </si>
@@ -663,6 +663,21 @@
   <si>
     <t>x</t>
   </si>
+  <si>
+    <t>Excludes assessment data for unit stocks when strata not assigned to that stock</t>
+  </si>
+  <si>
+    <t>All strata for unit stocks</t>
+  </si>
+  <si>
+    <t>Removed after increased unit stock strata</t>
+  </si>
+  <si>
+    <t>Assessment data has few NAs but not included</t>
+  </si>
+  <si>
+    <t>Added after increased unit stock strata</t>
+  </si>
 </sst>
 </file>
 
@@ -823,7 +838,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="40">
+  <fills count="41">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1042,6 +1057,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1711,7 +1732,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1905,6 +1926,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1944,9 +1980,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="48" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="47" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -1956,11 +1989,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="46" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -29055,35 +29096,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71"/>
+      <c r="C2" s="75"/>
+      <c r="D2" s="75"/>
+      <c r="E2" s="75"/>
+      <c r="F2" s="75"/>
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="76"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="69" t="s">
+      <c r="R2" s="74" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Y2" s="70"/>
-      <c r="Z2" s="70"/>
-      <c r="AA2" s="71"/>
+      <c r="S2" s="75"/>
+      <c r="T2" s="75"/>
+      <c r="U2" s="75"/>
+      <c r="V2" s="75"/>
+      <c r="W2" s="75"/>
+      <c r="X2" s="75"/>
+      <c r="Y2" s="75"/>
+      <c r="Z2" s="75"/>
+      <c r="AA2" s="76"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -29096,50 +29137,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="75" t="s">
+      <c r="C3" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="77" t="s">
+      <c r="D3" s="82" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="75" t="s">
+      <c r="E3" s="80" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="72" t="s">
+      <c r="F3" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="72" t="s">
+      <c r="G3" s="78"/>
+      <c r="H3" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="74"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="72" t="s">
+      <c r="I3" s="79"/>
+      <c r="J3" s="78"/>
+      <c r="K3" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="74"/>
-      <c r="M3" s="73"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="78"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="75" t="s">
+      <c r="S3" s="80" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="72" t="s">
+      <c r="T3" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="73"/>
-      <c r="V3" s="72" t="s">
+      <c r="U3" s="78"/>
+      <c r="V3" s="77" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="74"/>
-      <c r="X3" s="73"/>
-      <c r="Y3" s="72" t="s">
+      <c r="W3" s="79"/>
+      <c r="X3" s="78"/>
+      <c r="Y3" s="77" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="74"/>
-      <c r="AA3" s="73"/>
+      <c r="Z3" s="79"/>
+      <c r="AA3" s="78"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -29153,9 +29194,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="76"/>
-      <c r="D4" s="78"/>
-      <c r="E4" s="76"/>
+      <c r="C4" s="81"/>
+      <c r="D4" s="83"/>
+      <c r="E4" s="81"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -29190,7 +29231,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="76"/>
+      <c r="S4" s="81"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -39202,30 +39243,30 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="80" t="s">
+      <c r="W2" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="79" t="s">
+      <c r="X2" s="86"/>
+      <c r="Y2" s="84" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="79"/>
-      <c r="AA2" s="79"/>
-      <c r="AB2" s="79"/>
+      <c r="Z2" s="84"/>
+      <c r="AA2" s="84"/>
+      <c r="AB2" s="84"/>
       <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="79" t="s">
+      <c r="AD2" s="84" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" s="79"/>
-      <c r="AF2" s="79"/>
-      <c r="AG2" s="79"/>
-      <c r="AH2" s="79"/>
-      <c r="AI2" s="79" t="s">
+      <c r="AE2" s="84"/>
+      <c r="AF2" s="84"/>
+      <c r="AG2" s="84"/>
+      <c r="AH2" s="84"/>
+      <c r="AI2" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="79"/>
+      <c r="AJ2" s="84"/>
       <c r="AK2" s="63" t="s">
         <v>183</v>
       </c>
@@ -40440,14 +40481,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U21"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <pane xSplit="8" ySplit="1" topLeftCell="I21" activePane="bottomRight" state="frozen"/>
-      <selection activeCell="A3" sqref="A3"/>
-      <selection pane="topRight" activeCell="I3" sqref="I3"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1:Q1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40463,151 +40500,153 @@
     <col min="15" max="15" width="10.26953125" customWidth="1"/>
     <col min="16" max="16" width="9.81640625" customWidth="1"/>
     <col min="18" max="18" width="11.26953125" customWidth="1"/>
+    <col min="23" max="25" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="B1" s="62" t="s">
+    <row r="1" spans="1:25" s="69" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="B1" s="94" t="s">
+        <v>216</v>
+      </c>
+      <c r="C1" s="72"/>
+      <c r="D1" s="73"/>
+      <c r="E1" s="73"/>
+      <c r="F1" s="95" t="s">
+        <v>214</v>
+      </c>
+      <c r="G1" s="73"/>
+      <c r="H1" s="73"/>
+      <c r="I1" s="73"/>
+      <c r="J1" s="73"/>
+      <c r="K1" s="73"/>
+      <c r="L1" s="73"/>
+      <c r="M1" s="73"/>
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="92" t="s">
+        <v>215</v>
+      </c>
+      <c r="R1" s="73"/>
+      <c r="S1" s="90" t="s">
+        <v>212</v>
+      </c>
+      <c r="W1" s="91" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="2" spans="1:21" s="82" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B2" s="83" t="s">
+    <row r="3" spans="1:25" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="87" t="s">
         <v>178</v>
       </c>
-      <c r="C2" s="84"/>
-      <c r="D2" s="85" t="s">
+      <c r="C3" s="88"/>
+      <c r="D3" s="89" t="s">
         <v>179</v>
       </c>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="86" t="s">
+      <c r="E3" s="89"/>
+      <c r="F3" s="89"/>
+      <c r="G3" s="89"/>
+      <c r="H3" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="I2" s="85" t="s">
+      <c r="I3" s="89" t="s">
         <v>181</v>
       </c>
-      <c r="J2" s="85"/>
-      <c r="K2" s="85"/>
-      <c r="L2" s="85"/>
-      <c r="M2" s="85"/>
-      <c r="N2" s="85" t="s">
+      <c r="J3" s="89"/>
+      <c r="K3" s="89"/>
+      <c r="L3" s="89"/>
+      <c r="M3" s="89"/>
+      <c r="N3" s="89" t="s">
         <v>108</v>
       </c>
-      <c r="O2" s="85"/>
-      <c r="P2" s="86" t="s">
+      <c r="O3" s="89"/>
+      <c r="P3" s="70" t="s">
         <v>183</v>
       </c>
-      <c r="Q2" s="86" t="s">
+      <c r="Q3" s="70" t="s">
         <v>182</v>
       </c>
-      <c r="R2" s="86" t="s">
+      <c r="R3" s="70" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="3" spans="1:21" s="82" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="B3" s="87" t="s">
+    <row r="4" spans="1:25" s="69" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
-      <c r="C3" s="87" t="s">
+      <c r="C4" s="71" t="s">
         <v>174</v>
       </c>
-      <c r="D3" s="87" t="s">
+      <c r="D4" s="71" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E4" s="71" t="s">
         <v>164</v>
       </c>
-      <c r="F3" s="87" t="s">
+      <c r="F4" s="71" t="s">
         <v>165</v>
       </c>
-      <c r="G3" s="87" t="s">
+      <c r="G4" s="71" t="s">
         <v>166</v>
       </c>
-      <c r="H3" s="87" t="s">
+      <c r="H4" s="71" t="s">
         <v>167</v>
       </c>
-      <c r="I3" s="87" t="s">
+      <c r="I4" s="71" t="s">
         <v>168</v>
       </c>
-      <c r="J3" s="87" t="s">
+      <c r="J4" s="71" t="s">
         <v>169</v>
       </c>
-      <c r="K3" s="87" t="s">
+      <c r="K4" s="71" t="s">
         <v>170</v>
       </c>
-      <c r="L3" s="87" t="s">
+      <c r="L4" s="71" t="s">
         <v>172</v>
       </c>
-      <c r="M3" s="87" t="s">
+      <c r="M4" s="71" t="s">
         <v>173</v>
       </c>
-      <c r="N3" s="87" t="s">
+      <c r="N4" s="71" t="s">
         <v>144</v>
       </c>
-      <c r="O3" s="87" t="s">
+      <c r="O4" s="71" t="s">
         <v>145</v>
       </c>
-      <c r="P3" s="87" t="s">
+      <c r="P4" s="71" t="s">
         <v>171</v>
       </c>
-      <c r="Q3" s="87" t="s">
+      <c r="Q4" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="R3" s="87" t="s">
+      <c r="R4" s="71" t="s">
         <v>209</v>
       </c>
-      <c r="S3" s="82" t="s">
+      <c r="S4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="T3" s="82" t="s">
+      <c r="T4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="U3" s="82" t="s">
+      <c r="U4" s="69" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
+      <c r="W4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="X4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="Y4" s="69" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
         <v>9</v>
-      </c>
-      <c r="B4" t="s">
-        <v>211</v>
-      </c>
-      <c r="G4" t="s">
-        <v>211</v>
-      </c>
-      <c r="H4" t="s">
-        <v>211</v>
-      </c>
-      <c r="L4" t="s">
-        <v>211</v>
-      </c>
-      <c r="N4" t="s">
-        <v>211</v>
-      </c>
-      <c r="P4" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>211</v>
-      </c>
-      <c r="R4" t="s">
-        <v>211</v>
-      </c>
-      <c r="S4">
-        <v>23.66</v>
-      </c>
-      <c r="T4">
-        <v>6.7900000000000002E-2</v>
-      </c>
-      <c r="U4">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>211</v>
@@ -40615,28 +40654,37 @@
       <c r="G5" t="s">
         <v>211</v>
       </c>
+      <c r="H5" t="s">
+        <v>211</v>
+      </c>
       <c r="L5" t="s">
         <v>211</v>
       </c>
       <c r="N5" t="s">
         <v>211</v>
       </c>
+      <c r="P5" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>211</v>
+      </c>
       <c r="R5" t="s">
         <v>211</v>
       </c>
       <c r="S5">
-        <v>19.489999999999998</v>
+        <v>23.66</v>
       </c>
       <c r="T5">
-        <v>0.1578</v>
+        <v>6.7900000000000002E-2</v>
       </c>
       <c r="U5">
-        <v>918</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.35">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
         <v>211</v>
@@ -40644,95 +40692,96 @@
       <c r="G6" t="s">
         <v>211</v>
       </c>
-      <c r="M6" t="s">
+      <c r="L6" t="s">
         <v>211</v>
       </c>
-      <c r="O6" t="s">
+      <c r="N6" t="s">
         <v>211</v>
       </c>
+      <c r="Q6" s="66"/>
       <c r="R6" t="s">
         <v>211</v>
       </c>
       <c r="S6">
-        <v>24.05</v>
+        <v>19.489999999999998</v>
       </c>
       <c r="T6">
-        <v>0.17219999999999999</v>
+        <v>0.1578</v>
       </c>
       <c r="U6">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.35">
+        <v>918</v>
+      </c>
+    </row>
+    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
         <v>211</v>
       </c>
-      <c r="E7" t="s">
+      <c r="G7" t="s">
         <v>211</v>
       </c>
-      <c r="H7" t="s">
-        <v>211</v>
-      </c>
-      <c r="J7" t="s">
+      <c r="M7" t="s">
         <v>211</v>
       </c>
       <c r="O7" t="s">
         <v>211</v>
       </c>
-      <c r="P7" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>211</v>
-      </c>
       <c r="R7" t="s">
         <v>211</v>
       </c>
       <c r="S7">
-        <v>8.4600000000000009</v>
+        <v>24.05</v>
       </c>
       <c r="T7">
-        <v>0.2122</v>
+        <v>0.17219999999999999</v>
       </c>
       <c r="U7">
-        <v>434</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
         <v>211</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E8" t="s">
         <v>211</v>
       </c>
-      <c r="L8" t="s">
+      <c r="H8" t="s">
+        <v>211</v>
+      </c>
+      <c r="J8" t="s">
         <v>211</v>
       </c>
       <c r="O8" t="s">
         <v>211</v>
       </c>
+      <c r="P8" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>211</v>
+      </c>
       <c r="R8" t="s">
         <v>211</v>
       </c>
       <c r="S8">
-        <v>46.67</v>
+        <v>8.4600000000000009</v>
       </c>
       <c r="T8">
-        <v>0.14990000000000001</v>
+        <v>0.2122</v>
       </c>
       <c r="U8">
-        <v>1082</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" t="s">
         <v>211</v>
@@ -40740,95 +40789,118 @@
       <c r="D9" t="s">
         <v>211</v>
       </c>
-      <c r="M9" t="s">
+      <c r="L9" t="s">
         <v>211</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N9" s="93" t="s">
         <v>211</v>
       </c>
+      <c r="O9" s="61"/>
+      <c r="P9" s="66"/>
+      <c r="Q9" s="66"/>
       <c r="R9" t="s">
         <v>211</v>
       </c>
       <c r="S9">
-        <v>18.89</v>
+        <v>46.67</v>
       </c>
       <c r="T9">
-        <v>0.1711</v>
+        <v>0.14990000000000001</v>
       </c>
       <c r="U9">
-        <v>628</v>
-      </c>
-    </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.35">
+        <v>1082</v>
+      </c>
+      <c r="W9">
+        <v>48.83</v>
+      </c>
+      <c r="X9">
+        <v>0.12720000000000001</v>
+      </c>
+      <c r="Y9">
+        <v>1386</v>
+      </c>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
         <v>211</v>
       </c>
-      <c r="G10" t="s">
+      <c r="D10" s="61"/>
+      <c r="E10" s="93" t="s">
         <v>211</v>
       </c>
-      <c r="M10" t="s">
+      <c r="H10" s="93" t="s">
         <v>211</v>
       </c>
+      <c r="I10" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="M10" s="61"/>
       <c r="N10" t="s">
         <v>211</v>
       </c>
+      <c r="P10" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q10" s="93" t="s">
+        <v>211</v>
+      </c>
       <c r="R10" t="s">
         <v>211</v>
       </c>
       <c r="S10">
-        <v>16.059999999999999</v>
+        <v>18.89</v>
       </c>
       <c r="T10">
-        <v>0.1303</v>
+        <v>0.1711</v>
       </c>
       <c r="U10">
-        <v>525</v>
-      </c>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.35">
+        <v>628</v>
+      </c>
+      <c r="W10">
+        <v>18.77</v>
+      </c>
+      <c r="X10">
+        <v>0.1855</v>
+      </c>
+      <c r="Y10">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>35</v>
       </c>
       <c r="B11" t="s">
         <v>211</v>
       </c>
-      <c r="D11" t="s">
-        <v>211</v>
-      </c>
-      <c r="H11" t="s">
+      <c r="G11" t="s">
         <v>211</v>
       </c>
       <c r="M11" t="s">
         <v>211</v>
       </c>
-      <c r="O11" t="s">
-        <v>211</v>
-      </c>
-      <c r="P11" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="N11" t="s">
         <v>211</v>
       </c>
       <c r="R11" t="s">
         <v>211</v>
       </c>
       <c r="S11">
-        <v>20.85</v>
+        <v>16.059999999999999</v>
       </c>
       <c r="T11">
-        <v>0.32519999999999999</v>
+        <v>0.1303</v>
       </c>
       <c r="U11">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.35">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>156</v>
+        <v>21</v>
       </c>
       <c r="B12" t="s">
         <v>211</v>
@@ -40839,10 +40911,10 @@
       <c r="H12" t="s">
         <v>211</v>
       </c>
-      <c r="I12" t="s">
+      <c r="M12" t="s">
         <v>211</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>211</v>
       </c>
       <c r="P12" t="s">
@@ -40855,18 +40927,18 @@
         <v>211</v>
       </c>
       <c r="S12">
-        <v>33.68</v>
+        <v>20.85</v>
       </c>
       <c r="T12">
-        <v>0.11020000000000001</v>
+        <v>0.32519999999999999</v>
       </c>
       <c r="U12">
-        <v>778</v>
-      </c>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.35">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>156</v>
       </c>
       <c r="B13" t="s">
         <v>211</v>
@@ -40874,103 +40946,109 @@
       <c r="D13" t="s">
         <v>211</v>
       </c>
+      <c r="H13" t="s">
+        <v>211</v>
+      </c>
       <c r="I13" t="s">
         <v>211</v>
       </c>
-      <c r="O13" t="s">
+      <c r="N13" t="s">
+        <v>211</v>
+      </c>
+      <c r="P13" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q13" t="s">
         <v>211</v>
       </c>
       <c r="R13" t="s">
         <v>211</v>
       </c>
       <c r="S13">
-        <v>13.17</v>
+        <v>33.68</v>
       </c>
       <c r="T13">
-        <v>0.2238</v>
+        <v>0.11020000000000001</v>
       </c>
       <c r="U13">
-        <v>514</v>
-      </c>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.35">
+        <v>778</v>
+      </c>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
         <v>211</v>
       </c>
-      <c r="F14" t="s">
+      <c r="D14" t="s">
         <v>211</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>211</v>
       </c>
-      <c r="J14" t="s">
-        <v>211</v>
-      </c>
-      <c r="N14" t="s">
-        <v>211</v>
-      </c>
-      <c r="P14" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="O14" t="s">
         <v>211</v>
       </c>
       <c r="R14" t="s">
         <v>211</v>
       </c>
       <c r="S14">
-        <v>19.57</v>
+        <v>13.17</v>
       </c>
       <c r="T14">
-        <v>0.23630000000000001</v>
+        <v>0.2238</v>
       </c>
       <c r="U14">
-        <v>663</v>
-      </c>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.35">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
-        <v>28</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
         <v>211</v>
       </c>
-      <c r="E15" t="s">
+      <c r="F15" t="s">
         <v>211</v>
       </c>
-      <c r="M15" t="s">
+      <c r="H15" t="s">
         <v>211</v>
       </c>
-      <c r="O15" t="s">
+      <c r="J15" t="s">
+        <v>211</v>
+      </c>
+      <c r="N15" t="s">
+        <v>211</v>
+      </c>
+      <c r="P15" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q15" t="s">
         <v>211</v>
       </c>
       <c r="R15" t="s">
         <v>211</v>
       </c>
       <c r="S15">
-        <v>52.53</v>
+        <v>19.57</v>
       </c>
       <c r="T15">
-        <v>4.9299999999999997E-2</v>
+        <v>0.23630000000000001</v>
       </c>
       <c r="U15">
-        <v>716</v>
-      </c>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.35">
+        <v>663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B16" t="s">
         <v>211</v>
       </c>
-      <c r="D16" t="s">
-        <v>211</v>
-      </c>
-      <c r="H16" t="s">
+      <c r="E16" t="s">
         <v>211</v>
       </c>
       <c r="M16" t="s">
@@ -40979,33 +41057,27 @@
       <c r="O16" t="s">
         <v>211</v>
       </c>
-      <c r="P16" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>211</v>
-      </c>
       <c r="R16" t="s">
         <v>211</v>
       </c>
       <c r="S16">
-        <v>31.77</v>
+        <v>52.53</v>
       </c>
       <c r="T16">
-        <v>0.18279999999999999</v>
+        <v>4.9299999999999997E-2</v>
       </c>
       <c r="U16">
-        <v>231</v>
+        <v>716</v>
       </c>
     </row>
     <row r="17" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
-        <v>7</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
         <v>211</v>
       </c>
-      <c r="F17" t="s">
+      <c r="D17" t="s">
         <v>211</v>
       </c>
       <c r="H17" t="s">
@@ -41027,29 +41099,29 @@
         <v>211</v>
       </c>
       <c r="S17">
-        <v>13.96</v>
+        <v>31.77</v>
       </c>
       <c r="T17">
-        <v>0.1061</v>
+        <v>0.2361</v>
       </c>
       <c r="U17">
-        <v>343</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B18" t="s">
         <v>211</v>
       </c>
-      <c r="G18" t="s">
+      <c r="F18" t="s">
         <v>211</v>
       </c>
       <c r="H18" t="s">
         <v>211</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>211</v>
       </c>
       <c r="O18" t="s">
@@ -41065,47 +41137,56 @@
         <v>211</v>
       </c>
       <c r="S18">
-        <v>22.79</v>
+        <v>13.96</v>
       </c>
       <c r="T18">
-        <v>0.28999999999999998</v>
+        <v>0.1061</v>
       </c>
       <c r="U18">
-        <v>320</v>
+        <v>343</v>
       </c>
     </row>
     <row r="19" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
-        <v>39</v>
+        <v>8</v>
       </c>
       <c r="B19" t="s">
         <v>211</v>
       </c>
-      <c r="E19" t="s">
+      <c r="G19" t="s">
         <v>211</v>
       </c>
-      <c r="J19" t="s">
+      <c r="H19" t="s">
         <v>211</v>
       </c>
-      <c r="N19" t="s">
+      <c r="L19" t="s">
+        <v>211</v>
+      </c>
+      <c r="O19" t="s">
+        <v>211</v>
+      </c>
+      <c r="P19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q19" t="s">
         <v>211</v>
       </c>
       <c r="R19" t="s">
         <v>211</v>
       </c>
       <c r="S19">
-        <v>63.69</v>
+        <v>22.79</v>
       </c>
       <c r="T19">
-        <v>0.1002</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="U19">
-        <v>283</v>
+        <v>320</v>
       </c>
     </row>
     <row r="20" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>39</v>
       </c>
       <c r="B20" t="s">
         <v>211</v>
@@ -41113,48 +41194,39 @@
       <c r="E20" t="s">
         <v>211</v>
       </c>
-      <c r="H20" t="s">
+      <c r="J20" t="s">
         <v>211</v>
       </c>
-      <c r="M20" t="s">
-        <v>211</v>
-      </c>
-      <c r="O20" t="s">
-        <v>211</v>
-      </c>
-      <c r="P20" t="s">
-        <v>211</v>
-      </c>
-      <c r="Q20" t="s">
+      <c r="N20" t="s">
         <v>211</v>
       </c>
       <c r="R20" t="s">
         <v>211</v>
       </c>
       <c r="S20">
-        <v>11.31</v>
+        <v>63.69</v>
       </c>
       <c r="T20">
-        <v>0.11219999999999999</v>
+        <v>0.1002</v>
       </c>
       <c r="U20">
-        <v>646</v>
+        <v>283</v>
       </c>
     </row>
     <row r="21" spans="1:21" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>211</v>
       </c>
-      <c r="G21" t="s">
+      <c r="E21" t="s">
         <v>211</v>
       </c>
       <c r="H21" t="s">
         <v>211</v>
       </c>
-      <c r="J21" t="s">
+      <c r="M21" t="s">
         <v>211</v>
       </c>
       <c r="O21" t="s">
@@ -41170,21 +41242,795 @@
         <v>211</v>
       </c>
       <c r="S21">
+        <v>11.31</v>
+      </c>
+      <c r="T21">
+        <v>0.11219999999999999</v>
+      </c>
+      <c r="U21">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22" t="s">
+        <v>211</v>
+      </c>
+      <c r="H22" t="s">
+        <v>211</v>
+      </c>
+      <c r="J22" t="s">
+        <v>211</v>
+      </c>
+      <c r="O22" t="s">
+        <v>211</v>
+      </c>
+      <c r="P22" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q22" t="s">
+        <v>211</v>
+      </c>
+      <c r="R22" t="s">
+        <v>211</v>
+      </c>
+      <c r="S22">
         <v>10.199999999999999</v>
       </c>
-      <c r="T21">
+      <c r="T22">
         <v>0.37130000000000002</v>
       </c>
-      <c r="U21">
+      <c r="U22">
         <v>236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>12</v>
+      </c>
+      <c r="B23" t="s">
+        <v>211</v>
+      </c>
+      <c r="E23" t="s">
+        <v>211</v>
+      </c>
+      <c r="J23" t="s">
+        <v>211</v>
+      </c>
+      <c r="O23" t="s">
+        <v>211</v>
+      </c>
+      <c r="R23" t="s">
+        <v>211</v>
+      </c>
+      <c r="S23">
+        <v>14.93</v>
+      </c>
+      <c r="T23">
+        <v>0.1002</v>
+      </c>
+      <c r="U23">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>191</v>
+      </c>
+      <c r="B24" t="s">
+        <v>211</v>
+      </c>
+      <c r="D24" t="s">
+        <v>211</v>
+      </c>
+      <c r="J24" t="s">
+        <v>211</v>
+      </c>
+      <c r="N24" t="s">
+        <v>211</v>
+      </c>
+      <c r="R24" t="s">
+        <v>211</v>
+      </c>
+      <c r="S24">
+        <v>23.49</v>
+      </c>
+      <c r="T24">
+        <v>0.1487</v>
+      </c>
+      <c r="U24">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>37</v>
+      </c>
+      <c r="B25" t="s">
+        <v>211</v>
+      </c>
+      <c r="G25" t="s">
+        <v>211</v>
+      </c>
+      <c r="H25" t="s">
+        <v>211</v>
+      </c>
+      <c r="J25" t="s">
+        <v>211</v>
+      </c>
+      <c r="N25" t="s">
+        <v>211</v>
+      </c>
+      <c r="P25" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q25" t="s">
+        <v>211</v>
+      </c>
+      <c r="R25" t="s">
+        <v>211</v>
+      </c>
+      <c r="S25">
+        <v>17.02</v>
+      </c>
+      <c r="T25">
+        <v>0.21240000000000001</v>
+      </c>
+      <c r="U25">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" t="s">
+        <v>211</v>
+      </c>
+      <c r="F26" t="s">
+        <v>211</v>
+      </c>
+      <c r="H26" t="s">
+        <v>211</v>
+      </c>
+      <c r="I26" t="s">
+        <v>211</v>
+      </c>
+      <c r="O26" t="s">
+        <v>211</v>
+      </c>
+      <c r="P26" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>211</v>
+      </c>
+      <c r="R26" t="s">
+        <v>211</v>
+      </c>
+      <c r="S26">
+        <v>10.1</v>
+      </c>
+      <c r="T26">
+        <v>0.3599</v>
+      </c>
+      <c r="U26">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" t="s">
+        <v>211</v>
+      </c>
+      <c r="F27" t="s">
+        <v>211</v>
+      </c>
+      <c r="H27" t="s">
+        <v>211</v>
+      </c>
+      <c r="M27" t="s">
+        <v>211</v>
+      </c>
+      <c r="N27" t="s">
+        <v>211</v>
+      </c>
+      <c r="P27" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>211</v>
+      </c>
+      <c r="R27" t="s">
+        <v>211</v>
+      </c>
+      <c r="S27">
+        <v>22.76</v>
+      </c>
+      <c r="T27">
+        <v>0.27900000000000003</v>
+      </c>
+      <c r="U27">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>211</v>
+      </c>
+      <c r="G28" t="s">
+        <v>211</v>
+      </c>
+      <c r="H28" t="s">
+        <v>211</v>
+      </c>
+      <c r="I28" t="s">
+        <v>211</v>
+      </c>
+      <c r="N28" t="s">
+        <v>211</v>
+      </c>
+      <c r="P28" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>211</v>
+      </c>
+      <c r="R28" t="s">
+        <v>211</v>
+      </c>
+      <c r="S28">
+        <v>30.57</v>
+      </c>
+      <c r="T28">
+        <v>0.26269999999999999</v>
+      </c>
+      <c r="U28">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B29" t="s">
+        <v>211</v>
+      </c>
+      <c r="F29" t="s">
+        <v>211</v>
+      </c>
+      <c r="H29" t="s">
+        <v>211</v>
+      </c>
+      <c r="I29" t="s">
+        <v>211</v>
+      </c>
+      <c r="N29" t="s">
+        <v>211</v>
+      </c>
+      <c r="P29" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>211</v>
+      </c>
+      <c r="R29" t="s">
+        <v>211</v>
+      </c>
+      <c r="S29">
+        <v>19.22</v>
+      </c>
+      <c r="T29">
+        <v>0.3029</v>
+      </c>
+      <c r="U29">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>211</v>
+      </c>
+      <c r="F30" t="s">
+        <v>211</v>
+      </c>
+      <c r="H30" t="s">
+        <v>211</v>
+      </c>
+      <c r="M30" t="s">
+        <v>211</v>
+      </c>
+      <c r="O30" t="s">
+        <v>211</v>
+      </c>
+      <c r="P30" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>211</v>
+      </c>
+      <c r="R30" t="s">
+        <v>211</v>
+      </c>
+      <c r="S30">
+        <v>11.61</v>
+      </c>
+      <c r="T30">
+        <v>6.8199999999999997E-2</v>
+      </c>
+      <c r="U30">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" t="s">
+        <v>211</v>
+      </c>
+      <c r="D31" t="s">
+        <v>211</v>
+      </c>
+      <c r="H31" t="s">
+        <v>211</v>
+      </c>
+      <c r="J31" t="s">
+        <v>211</v>
+      </c>
+      <c r="N31" t="s">
+        <v>211</v>
+      </c>
+      <c r="P31" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q31" t="s">
+        <v>211</v>
+      </c>
+      <c r="R31" t="s">
+        <v>211</v>
+      </c>
+      <c r="S31">
+        <v>16.989999999999998</v>
+      </c>
+      <c r="T31">
+        <v>0.20349999999999999</v>
+      </c>
+      <c r="U31">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" t="s">
+        <v>211</v>
+      </c>
+      <c r="E32" t="s">
+        <v>211</v>
+      </c>
+      <c r="H32" t="s">
+        <v>211</v>
+      </c>
+      <c r="M32" t="s">
+        <v>211</v>
+      </c>
+      <c r="O32" t="s">
+        <v>211</v>
+      </c>
+      <c r="P32" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>211</v>
+      </c>
+      <c r="R32" t="s">
+        <v>211</v>
+      </c>
+      <c r="S32">
+        <v>14.08</v>
+      </c>
+      <c r="T32">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="U32">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B33" t="s">
+        <v>211</v>
+      </c>
+      <c r="D33" s="61"/>
+      <c r="F33" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="H33" t="s">
+        <v>211</v>
+      </c>
+      <c r="L33" t="s">
+        <v>211</v>
+      </c>
+      <c r="O33" t="s">
+        <v>211</v>
+      </c>
+      <c r="P33" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q33" s="93" t="s">
+        <v>211</v>
+      </c>
+      <c r="R33" t="s">
+        <v>211</v>
+      </c>
+      <c r="S33">
+        <v>27.43</v>
+      </c>
+      <c r="T33">
+        <v>0.1033</v>
+      </c>
+      <c r="U33">
+        <v>477</v>
+      </c>
+      <c r="W33">
+        <v>27.26</v>
+      </c>
+      <c r="X33">
+        <v>10.7</v>
+      </c>
+      <c r="Y33">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" t="s">
+        <v>211</v>
+      </c>
+      <c r="E34" t="s">
+        <v>211</v>
+      </c>
+      <c r="I34" t="s">
+        <v>211</v>
+      </c>
+      <c r="N34" t="s">
+        <v>211</v>
+      </c>
+      <c r="R34" t="s">
+        <v>211</v>
+      </c>
+      <c r="S34">
+        <v>11.52</v>
+      </c>
+      <c r="T34">
+        <v>0.24110000000000001</v>
+      </c>
+      <c r="U34">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>190</v>
+      </c>
+      <c r="B35" t="s">
+        <v>211</v>
+      </c>
+      <c r="E35" t="s">
+        <v>211</v>
+      </c>
+      <c r="J35" t="s">
+        <v>211</v>
+      </c>
+      <c r="N35" t="s">
+        <v>211</v>
+      </c>
+      <c r="R35" t="s">
+        <v>211</v>
+      </c>
+      <c r="S35">
+        <v>8.57</v>
+      </c>
+      <c r="T35">
+        <v>0.2122</v>
+      </c>
+      <c r="U35">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" t="s">
+        <v>211</v>
+      </c>
+      <c r="G36" t="s">
+        <v>211</v>
+      </c>
+      <c r="H36" t="s">
+        <v>211</v>
+      </c>
+      <c r="M36" t="s">
+        <v>211</v>
+      </c>
+      <c r="O36" t="s">
+        <v>211</v>
+      </c>
+      <c r="P36" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>211</v>
+      </c>
+      <c r="R36" t="s">
+        <v>211</v>
+      </c>
+      <c r="S36">
+        <v>26.52</v>
+      </c>
+      <c r="T36">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="U36">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>157</v>
+      </c>
+      <c r="B37" t="s">
+        <v>211</v>
+      </c>
+      <c r="G37" t="s">
+        <v>211</v>
+      </c>
+      <c r="H37" t="s">
+        <v>211</v>
+      </c>
+      <c r="I37" t="s">
+        <v>211</v>
+      </c>
+      <c r="O37" t="s">
+        <v>211</v>
+      </c>
+      <c r="P37" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>211</v>
+      </c>
+      <c r="R37" t="s">
+        <v>211</v>
+      </c>
+      <c r="S37">
+        <v>39.68</v>
+      </c>
+      <c r="T37">
+        <v>0.1246</v>
+      </c>
+      <c r="U37">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>159</v>
+      </c>
+      <c r="B38" t="s">
+        <v>211</v>
+      </c>
+      <c r="D38" t="s">
+        <v>211</v>
+      </c>
+      <c r="H38" t="s">
+        <v>211</v>
+      </c>
+      <c r="I38" t="s">
+        <v>211</v>
+      </c>
+      <c r="O38" t="s">
+        <v>211</v>
+      </c>
+      <c r="P38" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>211</v>
+      </c>
+      <c r="R38" t="s">
+        <v>211</v>
+      </c>
+      <c r="S38">
+        <v>22.22</v>
+      </c>
+      <c r="T38">
+        <v>0.30280000000000001</v>
+      </c>
+      <c r="U38">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>160</v>
+      </c>
+      <c r="B39" t="s">
+        <v>211</v>
+      </c>
+      <c r="E39" t="s">
+        <v>211</v>
+      </c>
+      <c r="H39" t="s">
+        <v>211</v>
+      </c>
+      <c r="I39" t="s">
+        <v>211</v>
+      </c>
+      <c r="O39" t="s">
+        <v>211</v>
+      </c>
+      <c r="P39" t="s">
+        <v>211</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>211</v>
+      </c>
+      <c r="R39" t="s">
+        <v>211</v>
+      </c>
+      <c r="S39">
+        <v>26.34</v>
+      </c>
+      <c r="T39">
+        <v>0.22470000000000001</v>
+      </c>
+      <c r="U39">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>187</v>
+      </c>
+      <c r="B40" t="s">
+        <v>211</v>
+      </c>
+      <c r="F40" t="s">
+        <v>211</v>
+      </c>
+      <c r="M40" t="s">
+        <v>211</v>
+      </c>
+      <c r="O40" t="s">
+        <v>211</v>
+      </c>
+      <c r="R40" t="s">
+        <v>211</v>
+      </c>
+      <c r="S40">
+        <v>20.14</v>
+      </c>
+      <c r="T40">
+        <v>0.17030000000000001</v>
+      </c>
+      <c r="U40">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>188</v>
+      </c>
+      <c r="B41" t="s">
+        <v>211</v>
+      </c>
+      <c r="F41" t="s">
+        <v>211</v>
+      </c>
+      <c r="M41" t="s">
+        <v>211</v>
+      </c>
+      <c r="O41" t="s">
+        <v>211</v>
+      </c>
+      <c r="R41" t="s">
+        <v>211</v>
+      </c>
+      <c r="S41">
+        <v>9.7100000000000009</v>
+      </c>
+      <c r="T41">
+        <v>0.187</v>
+      </c>
+      <c r="U41">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>192</v>
+      </c>
+      <c r="B42" t="s">
+        <v>211</v>
+      </c>
+      <c r="F42" t="s">
+        <v>211</v>
+      </c>
+      <c r="L42" t="s">
+        <v>211</v>
+      </c>
+      <c r="O42" t="s">
+        <v>211</v>
+      </c>
+      <c r="R42" t="s">
+        <v>211</v>
+      </c>
+      <c r="S42">
+        <v>12.46</v>
+      </c>
+      <c r="T42">
+        <v>0.19750000000000001</v>
+      </c>
+      <c r="U42">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>186</v>
+      </c>
+      <c r="B43" t="s">
+        <v>211</v>
+      </c>
+      <c r="F43" t="s">
+        <v>211</v>
+      </c>
+      <c r="J43" t="s">
+        <v>211</v>
+      </c>
+      <c r="N43" t="s">
+        <v>211</v>
+      </c>
+      <c r="R43" t="s">
+        <v>211</v>
+      </c>
+      <c r="S43">
+        <v>33.28</v>
+      </c>
+      <c r="T43">
+        <v>0.2903</v>
+      </c>
+      <c r="U43">
+        <v>117</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B2:C2"/>
-    <mergeCell ref="D2:G2"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="N2:O2"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="D3:G3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:O3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Loaded updated StockSMART data. Error with merge due to Species column
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2229" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="217">
   <si>
     <t>Species</t>
   </si>
@@ -1732,7 +1732,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1941,6 +1941,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="40" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -1989,20 +2003,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -29096,35 +29097,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="74" t="s">
+      <c r="B2" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="76"/>
+      <c r="C2" s="81"/>
+      <c r="D2" s="81"/>
+      <c r="E2" s="81"/>
+      <c r="F2" s="81"/>
+      <c r="G2" s="81"/>
+      <c r="H2" s="81"/>
+      <c r="I2" s="81"/>
+      <c r="J2" s="81"/>
+      <c r="K2" s="81"/>
+      <c r="L2" s="81"/>
+      <c r="M2" s="82"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="74" t="s">
+      <c r="R2" s="80" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="75"/>
-      <c r="T2" s="75"/>
-      <c r="U2" s="75"/>
-      <c r="V2" s="75"/>
-      <c r="W2" s="75"/>
-      <c r="X2" s="75"/>
-      <c r="Y2" s="75"/>
-      <c r="Z2" s="75"/>
-      <c r="AA2" s="76"/>
+      <c r="S2" s="81"/>
+      <c r="T2" s="81"/>
+      <c r="U2" s="81"/>
+      <c r="V2" s="81"/>
+      <c r="W2" s="81"/>
+      <c r="X2" s="81"/>
+      <c r="Y2" s="81"/>
+      <c r="Z2" s="81"/>
+      <c r="AA2" s="82"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -29137,50 +29138,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="80" t="s">
+      <c r="C3" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="82" t="s">
+      <c r="D3" s="88" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="80" t="s">
+      <c r="E3" s="86" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="77" t="s">
+      <c r="F3" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="78"/>
-      <c r="H3" s="77" t="s">
+      <c r="G3" s="84"/>
+      <c r="H3" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="79"/>
-      <c r="J3" s="78"/>
-      <c r="K3" s="77" t="s">
+      <c r="I3" s="85"/>
+      <c r="J3" s="84"/>
+      <c r="K3" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="79"/>
-      <c r="M3" s="78"/>
+      <c r="L3" s="85"/>
+      <c r="M3" s="84"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="80" t="s">
+      <c r="S3" s="86" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="77" t="s">
+      <c r="T3" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="78"/>
-      <c r="V3" s="77" t="s">
+      <c r="U3" s="84"/>
+      <c r="V3" s="83" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="79"/>
-      <c r="X3" s="78"/>
-      <c r="Y3" s="77" t="s">
+      <c r="W3" s="85"/>
+      <c r="X3" s="84"/>
+      <c r="Y3" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="79"/>
-      <c r="AA3" s="78"/>
+      <c r="Z3" s="85"/>
+      <c r="AA3" s="84"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -29194,9 +29195,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="81"/>
-      <c r="D4" s="83"/>
-      <c r="E4" s="81"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="89"/>
+      <c r="E4" s="87"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -29231,7 +29232,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="81"/>
+      <c r="S4" s="87"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -39243,30 +39244,30 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="85" t="s">
+      <c r="W2" s="91" t="s">
         <v>178</v>
       </c>
-      <c r="X2" s="86"/>
-      <c r="Y2" s="84" t="s">
+      <c r="X2" s="92"/>
+      <c r="Y2" s="90" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="84"/>
-      <c r="AA2" s="84"/>
-      <c r="AB2" s="84"/>
+      <c r="Z2" s="90"/>
+      <c r="AA2" s="90"/>
+      <c r="AB2" s="90"/>
       <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="84" t="s">
+      <c r="AD2" s="90" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" s="84"/>
-      <c r="AF2" s="84"/>
-      <c r="AG2" s="84"/>
-      <c r="AH2" s="84"/>
-      <c r="AI2" s="84" t="s">
+      <c r="AE2" s="90"/>
+      <c r="AF2" s="90"/>
+      <c r="AG2" s="90"/>
+      <c r="AH2" s="90"/>
+      <c r="AI2" s="90" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="84"/>
+      <c r="AJ2" s="90"/>
       <c r="AK2" s="63" t="s">
         <v>183</v>
       </c>
@@ -40483,8 +40484,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="P1" sqref="P1:Q1048576"/>
+    <sheetView tabSelected="1" topLeftCell="O3" workbookViewId="0">
+      <selection activeCell="X30" sqref="X30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40504,13 +40505,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:25" s="69" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
       <c r="C1" s="72"/>
       <c r="D1" s="73"/>
       <c r="E1" s="73"/>
-      <c r="F1" s="95" t="s">
+      <c r="F1" s="79" t="s">
         <v>214</v>
       </c>
       <c r="G1" s="73"/>
@@ -40522,14 +40523,14 @@
       <c r="M1" s="73"/>
       <c r="N1" s="73"/>
       <c r="O1" s="73"/>
-      <c r="P1" s="92" t="s">
+      <c r="P1" s="76" t="s">
         <v>215</v>
       </c>
       <c r="R1" s="73"/>
-      <c r="S1" s="90" t="s">
+      <c r="S1" s="74" t="s">
         <v>212</v>
       </c>
-      <c r="W1" s="91" t="s">
+      <c r="W1" s="75" t="s">
         <v>213</v>
       </c>
     </row>
@@ -40539,30 +40540,30 @@
       </c>
     </row>
     <row r="3" spans="1:25" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="87" t="s">
+      <c r="B3" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="88"/>
-      <c r="D3" s="89" t="s">
+      <c r="C3" s="94"/>
+      <c r="D3" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="89"/>
-      <c r="F3" s="89"/>
-      <c r="G3" s="89"/>
+      <c r="E3" s="95"/>
+      <c r="F3" s="95"/>
+      <c r="G3" s="95"/>
       <c r="H3" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="89" t="s">
+      <c r="I3" s="95" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="89"/>
-      <c r="K3" s="89"/>
-      <c r="L3" s="89"/>
-      <c r="M3" s="89"/>
-      <c r="N3" s="89" t="s">
+      <c r="J3" s="95"/>
+      <c r="K3" s="95"/>
+      <c r="L3" s="95"/>
+      <c r="M3" s="95"/>
+      <c r="N3" s="95" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="89"/>
+      <c r="O3" s="95"/>
       <c r="P3" s="70" t="s">
         <v>183</v>
       </c>
@@ -40651,16 +40652,19 @@
       <c r="B5" t="s">
         <v>211</v>
       </c>
-      <c r="G5" t="s">
+      <c r="F5" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="G5" s="61"/>
       <c r="H5" t="s">
         <v>211</v>
       </c>
-      <c r="L5" t="s">
+      <c r="L5" s="61"/>
+      <c r="M5" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="N5" t="s">
+      <c r="N5" s="61"/>
+      <c r="O5" s="77" t="s">
         <v>211</v>
       </c>
       <c r="P5" t="s">
@@ -40680,6 +40684,15 @@
       </c>
       <c r="U5">
         <v>722</v>
+      </c>
+      <c r="W5">
+        <v>24.324999999999999</v>
+      </c>
+      <c r="X5">
+        <v>9.6600000000000005E-2</v>
+      </c>
+      <c r="Y5">
+        <v>777</v>
       </c>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.35">
@@ -40792,7 +40805,7 @@
       <c r="L9" t="s">
         <v>211</v>
       </c>
-      <c r="N9" s="93" t="s">
+      <c r="N9" s="77" t="s">
         <v>211</v>
       </c>
       <c r="O9" s="61"/>
@@ -40828,23 +40841,23 @@
         <v>211</v>
       </c>
       <c r="D10" s="61"/>
-      <c r="E10" s="93" t="s">
+      <c r="E10" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="H10" s="93" t="s">
+      <c r="H10" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="I10" s="93" t="s">
+      <c r="I10" s="77" t="s">
         <v>211</v>
       </c>
       <c r="M10" s="61"/>
       <c r="N10" t="s">
         <v>211</v>
       </c>
-      <c r="P10" s="93" t="s">
+      <c r="P10" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="Q10" s="93" t="s">
+      <c r="Q10" s="77" t="s">
         <v>211</v>
       </c>
       <c r="R10" t="s">
@@ -40952,7 +40965,8 @@
       <c r="I13" t="s">
         <v>211</v>
       </c>
-      <c r="N13" t="s">
+      <c r="N13" s="61"/>
+      <c r="O13" s="77" t="s">
         <v>211</v>
       </c>
       <c r="P13" t="s">
@@ -40972,6 +40986,15 @@
       </c>
       <c r="U13">
         <v>778</v>
+      </c>
+      <c r="W13">
+        <v>33.869999999999997</v>
+      </c>
+      <c r="X13">
+        <v>0.12609999999999999</v>
+      </c>
+      <c r="Y13">
+        <v>799</v>
       </c>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.35">
@@ -41070,7 +41093,7 @@
         <v>716</v>
       </c>
     </row>
-    <row r="17" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -41107,8 +41130,17 @@
       <c r="U17">
         <v>231</v>
       </c>
-    </row>
-    <row r="18" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W17">
+        <v>33.69</v>
+      </c>
+      <c r="X17">
+        <v>0.2351</v>
+      </c>
+      <c r="Y17">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -41145,8 +41177,17 @@
       <c r="U18">
         <v>343</v>
       </c>
-    </row>
-    <row r="19" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W18">
+        <v>14.15</v>
+      </c>
+      <c r="X18">
+        <v>0.13669999999999999</v>
+      </c>
+      <c r="Y18">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -41159,7 +41200,8 @@
       <c r="H19" t="s">
         <v>211</v>
       </c>
-      <c r="L19" t="s">
+      <c r="L19" s="61"/>
+      <c r="M19" s="77" t="s">
         <v>211</v>
       </c>
       <c r="O19" t="s">
@@ -41184,7 +41226,7 @@
         <v>320</v>
       </c>
     </row>
-    <row r="20" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -41213,25 +41255,28 @@
         <v>283</v>
       </c>
     </row>
-    <row r="21" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>211</v>
       </c>
-      <c r="E21" t="s">
+      <c r="E21" s="61"/>
+      <c r="F21" s="77" t="s">
         <v>211</v>
       </c>
       <c r="H21" t="s">
         <v>211</v>
       </c>
-      <c r="M21" t="s">
+      <c r="I21" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="O21" t="s">
+      <c r="M21" s="61"/>
+      <c r="N21" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="O21" s="61"/>
       <c r="P21" t="s">
         <v>211</v>
       </c>
@@ -41250,8 +41295,17 @@
       <c r="U21">
         <v>646</v>
       </c>
-    </row>
-    <row r="22" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W21">
+        <v>12.422000000000001</v>
+      </c>
+      <c r="X21">
+        <v>0.17219999999999999</v>
+      </c>
+      <c r="Y21">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -41289,7 +41343,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="23" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -41318,7 +41372,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="24" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -41347,16 +41401,17 @@
         <v>283</v>
       </c>
     </row>
-    <row r="25" spans="1:21" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
       <c r="B25" t="s">
         <v>211</v>
       </c>
-      <c r="G25" t="s">
+      <c r="E25" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="G25" s="61"/>
       <c r="H25" t="s">
         <v>211</v>
       </c>
@@ -41384,21 +41439,32 @@
       <c r="U25">
         <v>204</v>
       </c>
-    </row>
-    <row r="26" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W25">
+        <v>20.657</v>
+      </c>
+      <c r="X25">
+        <v>0.27250000000000002</v>
+      </c>
+      <c r="Y25">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
       <c r="B26" t="s">
         <v>211</v>
       </c>
-      <c r="F26" t="s">
+      <c r="E26" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="F26" s="61"/>
       <c r="H26" t="s">
         <v>211</v>
       </c>
-      <c r="I26" t="s">
+      <c r="I26" s="61"/>
+      <c r="J26" s="77" t="s">
         <v>211</v>
       </c>
       <c r="O26" t="s">
@@ -41422,8 +41488,17 @@
       <c r="U26">
         <v>220</v>
       </c>
-    </row>
-    <row r="27" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W26">
+        <v>14.15</v>
+      </c>
+      <c r="X26">
+        <v>0.26519999999999999</v>
+      </c>
+      <c r="Y26">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -41436,9 +41511,10 @@
       <c r="H27" t="s">
         <v>211</v>
       </c>
-      <c r="M27" t="s">
+      <c r="J27" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="M27" s="61"/>
       <c r="N27" t="s">
         <v>211</v>
       </c>
@@ -41460,21 +41536,32 @@
       <c r="U27">
         <v>174</v>
       </c>
-    </row>
-    <row r="28" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W27">
+        <v>20.295200000000001</v>
+      </c>
+      <c r="X27">
+        <v>0.36109999999999998</v>
+      </c>
+      <c r="Y27">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
       <c r="B28" t="s">
         <v>211</v>
       </c>
-      <c r="G28" t="s">
+      <c r="F28" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="G28" s="61"/>
       <c r="H28" t="s">
         <v>211</v>
       </c>
-      <c r="I28" t="s">
+      <c r="I28" s="96"/>
+      <c r="M28" s="77" t="s">
         <v>211</v>
       </c>
       <c r="N28" t="s">
@@ -41498,21 +41585,32 @@
       <c r="U28">
         <v>165</v>
       </c>
-    </row>
-    <row r="29" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W28">
+        <v>30.59</v>
+      </c>
+      <c r="X28">
+        <v>0.24249999999999999</v>
+      </c>
+      <c r="Y28">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
       <c r="B29" t="s">
         <v>211</v>
       </c>
-      <c r="F29" t="s">
+      <c r="D29" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="F29" s="61"/>
       <c r="H29" t="s">
         <v>211</v>
       </c>
-      <c r="I29" t="s">
+      <c r="I29" s="61"/>
+      <c r="M29" s="77" t="s">
         <v>211</v>
       </c>
       <c r="N29" t="s">
@@ -41536,23 +41634,34 @@
       <c r="U29">
         <v>324</v>
       </c>
-    </row>
-    <row r="30" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W29">
+        <v>20.582799999999999</v>
+      </c>
+      <c r="X29">
+        <v>0.26569999999999999</v>
+      </c>
+      <c r="Y29">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
       <c r="B30" t="s">
         <v>211</v>
       </c>
-      <c r="F30" t="s">
+      <c r="D30" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="F30" s="61"/>
       <c r="H30" t="s">
         <v>211</v>
       </c>
-      <c r="M30" t="s">
+      <c r="J30" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="M30" s="96"/>
       <c r="O30" t="s">
         <v>211</v>
       </c>
@@ -41574,8 +41683,17 @@
       <c r="U30">
         <v>233</v>
       </c>
-    </row>
-    <row r="31" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W30">
+        <v>12.86</v>
+      </c>
+      <c r="X30">
+        <v>5.0200000000000002E-2</v>
+      </c>
+      <c r="Y30">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -41612,8 +41730,17 @@
       <c r="U31">
         <v>140</v>
       </c>
-    </row>
-    <row r="32" spans="1:21" x14ac:dyDescent="0.35">
+      <c r="W31">
+        <v>19.125900000000001</v>
+      </c>
+      <c r="X31">
+        <v>0.22359999999999999</v>
+      </c>
+      <c r="Y31">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -41626,9 +41753,10 @@
       <c r="H32" t="s">
         <v>211</v>
       </c>
-      <c r="M32" t="s">
+      <c r="L32" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="M32" s="61"/>
       <c r="O32" t="s">
         <v>211</v>
       </c>
@@ -41649,6 +41777,15 @@
       </c>
       <c r="U32">
         <v>318</v>
+      </c>
+      <c r="W32">
+        <v>14.58</v>
+      </c>
+      <c r="X32">
+        <v>0.24709999999999999</v>
+      </c>
+      <c r="Y32">
+        <v>397</v>
       </c>
     </row>
     <row r="33" spans="1:25" x14ac:dyDescent="0.35">
@@ -41659,7 +41796,7 @@
         <v>211</v>
       </c>
       <c r="D33" s="61"/>
-      <c r="F33" s="93" t="s">
+      <c r="F33" s="77" t="s">
         <v>211</v>
       </c>
       <c r="H33" t="s">
@@ -41671,10 +41808,10 @@
       <c r="O33" t="s">
         <v>211</v>
       </c>
-      <c r="P33" s="93" t="s">
+      <c r="P33" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="Q33" s="93" t="s">
+      <c r="Q33" s="77" t="s">
         <v>211</v>
       </c>
       <c r="R33" t="s">
@@ -41693,7 +41830,7 @@
         <v>27.26</v>
       </c>
       <c r="X33">
-        <v>10.7</v>
+        <v>0.107</v>
       </c>
       <c r="Y33">
         <v>477</v>
@@ -41794,6 +41931,15 @@
       <c r="U36">
         <v>159</v>
       </c>
+      <c r="W36">
+        <v>28.13</v>
+      </c>
+      <c r="X36">
+        <v>0.36980000000000002</v>
+      </c>
+      <c r="Y36">
+        <v>162</v>
+      </c>
     </row>
     <row r="37" spans="1:25" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
@@ -41802,15 +41948,15 @@
       <c r="B37" t="s">
         <v>211</v>
       </c>
-      <c r="G37" t="s">
+      <c r="D37" s="77" t="s">
         <v>211</v>
       </c>
+      <c r="G37" s="61"/>
       <c r="H37" t="s">
         <v>211</v>
       </c>
-      <c r="I37" t="s">
-        <v>211</v>
-      </c>
+      <c r="I37" s="61"/>
+      <c r="J37" s="77"/>
       <c r="O37" t="s">
         <v>211</v>
       </c>
@@ -41831,6 +41977,15 @@
       </c>
       <c r="U37">
         <v>250</v>
+      </c>
+      <c r="W37">
+        <v>41.597000000000001</v>
+      </c>
+      <c r="X37">
+        <v>0.10009999999999999</v>
+      </c>
+      <c r="Y37">
+        <v>388</v>
       </c>
     </row>
     <row r="38" spans="1:25" x14ac:dyDescent="0.35">
@@ -41840,13 +41995,15 @@
       <c r="B38" t="s">
         <v>211</v>
       </c>
-      <c r="D38" t="s">
+      <c r="D38" s="61"/>
+      <c r="G38" s="77" t="s">
         <v>211</v>
       </c>
       <c r="H38" t="s">
         <v>211</v>
       </c>
-      <c r="I38" t="s">
+      <c r="I38" s="61"/>
+      <c r="L38" s="77" t="s">
         <v>211</v>
       </c>
       <c r="O38" t="s">
@@ -41869,6 +42026,15 @@
       </c>
       <c r="U38">
         <v>263</v>
+      </c>
+      <c r="W38">
+        <v>22.66</v>
+      </c>
+      <c r="X38">
+        <v>0.29189999999999999</v>
+      </c>
+      <c r="Y38">
+        <v>273</v>
       </c>
     </row>
     <row r="39" spans="1:25" x14ac:dyDescent="0.35">
@@ -41907,6 +42073,15 @@
       </c>
       <c r="U39">
         <v>137</v>
+      </c>
+      <c r="W39">
+        <v>26.353999999999999</v>
+      </c>
+      <c r="X39">
+        <v>0.28310000000000002</v>
+      </c>
+      <c r="Y39">
+        <v>159</v>
       </c>
     </row>
     <row r="40" spans="1:25" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
5/28/2021 data pull has missing CommonName, so changing to StockName for merge with data
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2228" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="224">
   <si>
     <t>Species</t>
   </si>
@@ -677,6 +677,27 @@
   </si>
   <si>
     <t>Added after increased unit stock strata</t>
+  </si>
+  <si>
+    <t>Full strata for single stock species</t>
+  </si>
+  <si>
+    <t>GCV increased</t>
+  </si>
+  <si>
+    <t>Deviance Explained Increased</t>
+  </si>
+  <si>
+    <t>Updated StockSMART data</t>
+  </si>
+  <si>
+    <t>Stock areas expanded beyond EPUs</t>
+  </si>
+  <si>
+    <t>All data used from selected indices for GAMs</t>
+  </si>
+  <si>
+    <t>Updated plankton indices</t>
   </si>
 </sst>
 </file>
@@ -1955,6 +1976,7 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="45" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2003,7 +2025,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2049,7 +2070,51 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="126">
+  <dxfs count="131">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -16016,44 +16081,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="125" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="130" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="124" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="122" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="127" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="121" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="120" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="119" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="117" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18639,145 +18704,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="115" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="120" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="114" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="112" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="117" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="111" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="109" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="114" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="108" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="106" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="111" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="105" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="103" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="108" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="102" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="100" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="105" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="99" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="97" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="102" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="96" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="94" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="99" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="93" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="91" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="96" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="90" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="88" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="93" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="87" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="85" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="90" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="84" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20600,168 +20665,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="82" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="87" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17 B38:B119">
-    <cfRule type="cellIs" dxfId="81" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="79" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="78" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="77" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 J5 J10 J14 J17:J18 J21:J22 J24:J25 J27:J29">
-    <cfRule type="cellIs" dxfId="75" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31 L5 L10 L14 L17:L18 L21:L22 L27:L29 L24:L25">
-    <cfRule type="cellIs" dxfId="73" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="78" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L4 L6:L9 L11:L13 L15:L16 L19:L20 L23 L30:L31 L26">
-    <cfRule type="cellIs" dxfId="72" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="70" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="75" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="69" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26 P4:P9 P11 P13:P15 P19:P21 P24 P30">
-    <cfRule type="cellIs" dxfId="67" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="72" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P31 P18 P10 P12 P16 P22:P23 P25:P26">
-    <cfRule type="cellIs" dxfId="66" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="64" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="69" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="63" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13 R10 R12 R16:R18 R22:R23 R25:R29 R31 R3">
-    <cfRule type="cellIs" dxfId="61" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="66" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2 R19:R21 R6:R9 R11 R13 R24 R30 R4">
-    <cfRule type="cellIs" dxfId="60" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="58" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="63" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="57" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="55" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="60" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="54" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="52" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="51" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119 B31:B37">
-    <cfRule type="cellIs" dxfId="49" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="47" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="46" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="51" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 J3:J4 J6:J9 J11:J13 J15:J16 J19:J20 J23 J26 J30:J31">
-    <cfRule type="cellIs" dxfId="45" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28980,87 +29045,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="44" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="43" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="41" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="40" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="45" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="39" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="37" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="36" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="34" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="33" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="38" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="32" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="30" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="27" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="26" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29097,35 +29162,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="80" t="s">
+      <c r="B2" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="81"/>
-      <c r="D2" s="81"/>
-      <c r="E2" s="81"/>
-      <c r="F2" s="81"/>
-      <c r="G2" s="81"/>
-      <c r="H2" s="81"/>
-      <c r="I2" s="81"/>
-      <c r="J2" s="81"/>
-      <c r="K2" s="81"/>
-      <c r="L2" s="81"/>
-      <c r="M2" s="82"/>
+      <c r="C2" s="82"/>
+      <c r="D2" s="82"/>
+      <c r="E2" s="82"/>
+      <c r="F2" s="82"/>
+      <c r="G2" s="82"/>
+      <c r="H2" s="82"/>
+      <c r="I2" s="82"/>
+      <c r="J2" s="82"/>
+      <c r="K2" s="82"/>
+      <c r="L2" s="82"/>
+      <c r="M2" s="83"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="80" t="s">
+      <c r="R2" s="81" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="81"/>
-      <c r="X2" s="81"/>
-      <c r="Y2" s="81"/>
-      <c r="Z2" s="81"/>
-      <c r="AA2" s="82"/>
+      <c r="S2" s="82"/>
+      <c r="T2" s="82"/>
+      <c r="U2" s="82"/>
+      <c r="V2" s="82"/>
+      <c r="W2" s="82"/>
+      <c r="X2" s="82"/>
+      <c r="Y2" s="82"/>
+      <c r="Z2" s="82"/>
+      <c r="AA2" s="83"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -29138,50 +29203,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="86" t="s">
+      <c r="C3" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="88" t="s">
+      <c r="D3" s="89" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="86" t="s">
+      <c r="E3" s="87" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="83" t="s">
+      <c r="F3" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="84"/>
-      <c r="H3" s="83" t="s">
+      <c r="G3" s="85"/>
+      <c r="H3" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="85"/>
-      <c r="J3" s="84"/>
-      <c r="K3" s="83" t="s">
+      <c r="I3" s="86"/>
+      <c r="J3" s="85"/>
+      <c r="K3" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="85"/>
-      <c r="M3" s="84"/>
+      <c r="L3" s="86"/>
+      <c r="M3" s="85"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="86" t="s">
+      <c r="S3" s="87" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="83" t="s">
+      <c r="T3" s="84" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="84"/>
-      <c r="V3" s="83" t="s">
+      <c r="U3" s="85"/>
+      <c r="V3" s="84" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="85"/>
-      <c r="X3" s="84"/>
-      <c r="Y3" s="83" t="s">
+      <c r="W3" s="86"/>
+      <c r="X3" s="85"/>
+      <c r="Y3" s="84" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="85"/>
-      <c r="AA3" s="84"/>
+      <c r="Z3" s="86"/>
+      <c r="AA3" s="85"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -29195,9 +29260,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="87"/>
-      <c r="D4" s="89"/>
-      <c r="E4" s="87"/>
+      <c r="C4" s="88"/>
+      <c r="D4" s="90"/>
+      <c r="E4" s="88"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -29232,7 +29297,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="87"/>
+      <c r="S4" s="88"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -33083,67 +33148,67 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="25" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="23" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="28" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="22" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="27" priority="12" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="21" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="19" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="8" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="17" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ4:BJ27">
-    <cfRule type="cellIs" dxfId="16" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BH27">
-    <cfRule type="cellIs" dxfId="15" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ28:BJ32">
-    <cfRule type="cellIs" dxfId="13" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB28:BH32">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39062,28 +39127,28 @@
     <sortCondition ref="I2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="6" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39244,30 +39309,30 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="91" t="s">
+      <c r="W2" s="92" t="s">
         <v>178</v>
       </c>
-      <c r="X2" s="92"/>
-      <c r="Y2" s="90" t="s">
+      <c r="X2" s="93"/>
+      <c r="Y2" s="91" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="90"/>
-      <c r="AA2" s="90"/>
-      <c r="AB2" s="90"/>
+      <c r="Z2" s="91"/>
+      <c r="AA2" s="91"/>
+      <c r="AB2" s="91"/>
       <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="90" t="s">
+      <c r="AD2" s="91" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" s="90"/>
-      <c r="AF2" s="90"/>
-      <c r="AG2" s="90"/>
-      <c r="AH2" s="90"/>
-      <c r="AI2" s="90" t="s">
+      <c r="AE2" s="91"/>
+      <c r="AF2" s="91"/>
+      <c r="AG2" s="91"/>
+      <c r="AH2" s="91"/>
+      <c r="AI2" s="91" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="90"/>
+      <c r="AJ2" s="91"/>
       <c r="AK2" s="63" t="s">
         <v>183</v>
       </c>
@@ -40459,19 +40524,19 @@
     <mergeCell ref="AD2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40482,10 +40547,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Y43"/>
+  <dimension ref="A1:AU45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="O3" workbookViewId="0">
-      <selection activeCell="X30" sqref="X30"/>
+    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
+      <selection activeCell="AC4" sqref="AC4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40504,7 +40569,7 @@
     <col min="23" max="25" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:47" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40534,36 +40599,36 @@
         <v>213</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="3" spans="1:25" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="93" t="s">
+    <row r="3" spans="1:47" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="94" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="94"/>
-      <c r="D3" s="95" t="s">
+      <c r="C3" s="95"/>
+      <c r="D3" s="96" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="95"/>
-      <c r="F3" s="95"/>
-      <c r="G3" s="95"/>
+      <c r="E3" s="96"/>
+      <c r="F3" s="96"/>
+      <c r="G3" s="96"/>
       <c r="H3" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="95" t="s">
+      <c r="I3" s="96" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="95"/>
-      <c r="K3" s="95"/>
-      <c r="L3" s="95"/>
-      <c r="M3" s="95"/>
-      <c r="N3" s="95" t="s">
+      <c r="J3" s="96"/>
+      <c r="K3" s="96"/>
+      <c r="L3" s="96"/>
+      <c r="M3" s="96"/>
+      <c r="N3" s="96" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="95"/>
+      <c r="O3" s="96"/>
       <c r="P3" s="70" t="s">
         <v>183</v>
       </c>
@@ -40573,8 +40638,23 @@
       <c r="R3" s="70" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" s="69" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+      <c r="W3" s="75" t="s">
+        <v>217</v>
+      </c>
+      <c r="AC3" s="75" t="s">
+        <v>220</v>
+      </c>
+      <c r="AI3" s="75" t="s">
+        <v>221</v>
+      </c>
+      <c r="AO3" s="75" t="s">
+        <v>222</v>
+      </c>
+      <c r="AU3" s="75" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:47" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40644,8 +40724,14 @@
       <c r="Y4" s="69" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="AA4" s="69" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -40694,8 +40780,16 @@
       <c r="Y5">
         <v>777</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z5">
+        <f>W5-S5</f>
+        <v>0.66499999999999915</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" ref="AA5:AA43" si="0">X5-T5</f>
+        <v>2.8700000000000003E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -40724,8 +40818,16 @@
       <c r="U6">
         <v>918</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z6">
+        <f t="shared" ref="Z6:Z43" si="1">W6-S6</f>
+        <v>-19.489999999999998</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="0"/>
+        <v>-0.1578</v>
+      </c>
+    </row>
+    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -40753,8 +40855,16 @@
       <c r="U7">
         <v>514</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z7">
+        <f t="shared" si="1"/>
+        <v>-24.05</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="0"/>
+        <v>-0.17219999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -40791,8 +40901,16 @@
       <c r="U8">
         <v>434</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z8">
+        <f t="shared" si="1"/>
+        <v>-8.4600000000000009</v>
+      </c>
+      <c r="AA8">
+        <f t="shared" si="0"/>
+        <v>-0.2122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -40832,8 +40950,16 @@
       <c r="Y9">
         <v>1386</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z9">
+        <f t="shared" si="1"/>
+        <v>2.1599999999999966</v>
+      </c>
+      <c r="AA9">
+        <f t="shared" si="0"/>
+        <v>-2.2699999999999998E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -40881,8 +41007,16 @@
       <c r="Y10">
         <v>628</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z10">
+        <f t="shared" si="1"/>
+        <v>-0.12000000000000099</v>
+      </c>
+      <c r="AA10">
+        <f t="shared" si="0"/>
+        <v>1.4399999999999996E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -40910,8 +41044,16 @@
       <c r="U11">
         <v>525</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z11">
+        <f t="shared" si="1"/>
+        <v>-16.059999999999999</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" si="0"/>
+        <v>-0.1303</v>
+      </c>
+    </row>
+    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -40948,8 +41090,16 @@
       <c r="U12">
         <v>588</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z12">
+        <f t="shared" si="1"/>
+        <v>-20.85</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="0"/>
+        <v>-0.32519999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -40996,8 +41146,16 @@
       <c r="Y13">
         <v>799</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z13">
+        <f t="shared" si="1"/>
+        <v>0.18999999999999773</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="0"/>
+        <v>1.5899999999999984E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -41025,8 +41183,16 @@
       <c r="U14">
         <v>514</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z14">
+        <f t="shared" si="1"/>
+        <v>-13.17</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="0"/>
+        <v>-0.2238</v>
+      </c>
+    </row>
+    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -41063,8 +41229,16 @@
       <c r="U15">
         <v>663</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z15">
+        <f t="shared" si="1"/>
+        <v>-19.57</v>
+      </c>
+      <c r="AA15">
+        <f t="shared" si="0"/>
+        <v>-0.23630000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -41092,8 +41266,16 @@
       <c r="U16">
         <v>716</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z16">
+        <f t="shared" si="1"/>
+        <v>-52.53</v>
+      </c>
+      <c r="AA16">
+        <f t="shared" si="0"/>
+        <v>-4.9299999999999997E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -41139,8 +41321,16 @@
       <c r="Y17">
         <v>288</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z17">
+        <f t="shared" si="1"/>
+        <v>1.9199999999999982</v>
+      </c>
+      <c r="AA17">
+        <f t="shared" si="0"/>
+        <v>-1.0000000000000009E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -41186,8 +41376,16 @@
       <c r="Y18">
         <v>383</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z18">
+        <f t="shared" si="1"/>
+        <v>0.1899999999999995</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" si="0"/>
+        <v>3.0599999999999988E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -41225,8 +41423,16 @@
       <c r="U19">
         <v>320</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z19">
+        <f t="shared" si="1"/>
+        <v>-22.79</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="0"/>
+        <v>-0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -41254,8 +41460,16 @@
       <c r="U20">
         <v>283</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z20">
+        <f t="shared" si="1"/>
+        <v>-63.69</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="0"/>
+        <v>-0.1002</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -41304,8 +41518,16 @@
       <c r="Y21">
         <v>752</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z21">
+        <f t="shared" si="1"/>
+        <v>1.1120000000000001</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -41342,8 +41564,16 @@
       <c r="U22">
         <v>236</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z22">
+        <f t="shared" si="1"/>
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="AA22">
+        <f t="shared" si="0"/>
+        <v>-0.37130000000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -41371,8 +41601,16 @@
       <c r="U23">
         <v>323</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z23">
+        <f t="shared" si="1"/>
+        <v>-14.93</v>
+      </c>
+      <c r="AA23">
+        <f t="shared" si="0"/>
+        <v>-0.1002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -41400,8 +41638,16 @@
       <c r="U24">
         <v>283</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z24">
+        <f t="shared" si="1"/>
+        <v>-23.49</v>
+      </c>
+      <c r="AA24">
+        <f t="shared" si="0"/>
+        <v>-0.1487</v>
+      </c>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -41448,8 +41694,16 @@
       <c r="Y25">
         <v>286</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z25">
+        <f t="shared" si="1"/>
+        <v>3.6370000000000005</v>
+      </c>
+      <c r="AA25">
+        <f t="shared" si="0"/>
+        <v>6.0100000000000015E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -41497,8 +41751,16 @@
       <c r="Y26">
         <v>341</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z26">
+        <f t="shared" si="1"/>
+        <v>4.0500000000000007</v>
+      </c>
+      <c r="AA26">
+        <f t="shared" si="0"/>
+        <v>-9.4700000000000006E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -41545,8 +41807,16 @@
       <c r="Y27">
         <v>250</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z27">
+        <f t="shared" si="1"/>
+        <v>-2.4648000000000003</v>
+      </c>
+      <c r="AA27">
+        <f t="shared" si="0"/>
+        <v>8.2099999999999951E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -41560,7 +41830,7 @@
       <c r="H28" t="s">
         <v>211</v>
       </c>
-      <c r="I28" s="96"/>
+      <c r="I28" s="80"/>
       <c r="M28" s="77" t="s">
         <v>211</v>
       </c>
@@ -41594,8 +41864,16 @@
       <c r="Y28">
         <v>179</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z28">
+        <f t="shared" si="1"/>
+        <v>1.9999999999999574E-2</v>
+      </c>
+      <c r="AA28">
+        <f t="shared" si="0"/>
+        <v>-2.0199999999999996E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -41643,8 +41921,16 @@
       <c r="Y29">
         <v>384</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z29">
+        <f t="shared" si="1"/>
+        <v>1.3628</v>
+      </c>
+      <c r="AA29">
+        <f t="shared" si="0"/>
+        <v>-3.7200000000000011E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -41661,7 +41947,7 @@
       <c r="J30" s="77" t="s">
         <v>211</v>
       </c>
-      <c r="M30" s="96"/>
+      <c r="M30" s="80"/>
       <c r="O30" t="s">
         <v>211</v>
       </c>
@@ -41692,8 +41978,16 @@
       <c r="Y30">
         <v>284</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z30">
+        <f t="shared" si="1"/>
+        <v>1.25</v>
+      </c>
+      <c r="AA30">
+        <f t="shared" si="0"/>
+        <v>-1.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -41739,8 +42033,16 @@
       <c r="Y31">
         <v>164</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z31">
+        <f t="shared" si="1"/>
+        <v>2.135900000000003</v>
+      </c>
+      <c r="AA31">
+        <f t="shared" si="0"/>
+        <v>2.0100000000000007E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -41787,8 +42089,16 @@
       <c r="Y32">
         <v>397</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z32">
+        <f t="shared" si="1"/>
+        <v>0.5</v>
+      </c>
+      <c r="AA32">
+        <f t="shared" si="0"/>
+        <v>-1.6900000000000026E-2</v>
+      </c>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -41835,8 +42145,16 @@
       <c r="Y33">
         <v>477</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z33">
+        <f t="shared" si="1"/>
+        <v>-0.16999999999999815</v>
+      </c>
+      <c r="AA33">
+        <f t="shared" si="0"/>
+        <v>3.699999999999995E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -41864,8 +42182,16 @@
       <c r="U34">
         <v>530</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z34">
+        <f t="shared" si="1"/>
+        <v>-11.52</v>
+      </c>
+      <c r="AA34">
+        <f t="shared" si="0"/>
+        <v>-0.24110000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -41893,8 +42219,16 @@
       <c r="U35">
         <v>454</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z35">
+        <f t="shared" si="1"/>
+        <v>-8.57</v>
+      </c>
+      <c r="AA35">
+        <f t="shared" si="0"/>
+        <v>-0.2122</v>
+      </c>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -41940,8 +42274,16 @@
       <c r="Y36">
         <v>162</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z36">
+        <f t="shared" si="1"/>
+        <v>1.6099999999999994</v>
+      </c>
+      <c r="AA36">
+        <f t="shared" si="0"/>
+        <v>5.8000000000000274E-3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -41987,8 +42329,16 @@
       <c r="Y37">
         <v>388</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z37">
+        <f t="shared" si="1"/>
+        <v>1.9170000000000016</v>
+      </c>
+      <c r="AA37">
+        <f t="shared" si="0"/>
+        <v>-2.4500000000000008E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -42036,8 +42386,16 @@
       <c r="Y38">
         <v>273</v>
       </c>
-    </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z38">
+        <f t="shared" si="1"/>
+        <v>0.44000000000000128</v>
+      </c>
+      <c r="AA38">
+        <f t="shared" si="0"/>
+        <v>-1.0900000000000021E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -42083,8 +42441,16 @@
       <c r="Y39">
         <v>159</v>
       </c>
-    </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z39">
+        <f t="shared" si="1"/>
+        <v>1.3999999999999346E-2</v>
+      </c>
+      <c r="AA39">
+        <f t="shared" si="0"/>
+        <v>5.8400000000000007E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -42112,8 +42478,16 @@
       <c r="U40">
         <v>173</v>
       </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z40">
+        <f t="shared" si="1"/>
+        <v>-20.14</v>
+      </c>
+      <c r="AA40">
+        <f t="shared" si="0"/>
+        <v>-0.17030000000000001</v>
+      </c>
+    </row>
+    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -42141,8 +42515,16 @@
       <c r="U41">
         <v>248</v>
       </c>
-    </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z41">
+        <f t="shared" si="1"/>
+        <v>-9.7100000000000009</v>
+      </c>
+      <c r="AA41">
+        <f t="shared" si="0"/>
+        <v>-0.187</v>
+      </c>
+    </row>
+    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -42170,8 +42552,16 @@
       <c r="U42">
         <v>108</v>
       </c>
-    </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="Z42">
+        <f t="shared" si="1"/>
+        <v>-12.46</v>
+      </c>
+      <c r="AA42">
+        <f t="shared" si="0"/>
+        <v>-0.19750000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -42198,6 +42588,24 @@
       </c>
       <c r="U43">
         <v>117</v>
+      </c>
+      <c r="Z43">
+        <f t="shared" si="1"/>
+        <v>-33.28</v>
+      </c>
+      <c r="AA43">
+        <f t="shared" si="0"/>
+        <v>-0.2903</v>
+      </c>
+    </row>
+    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="Z45">
+        <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
+        <v>20.418899999999997</v>
+      </c>
+      <c r="AA45">
+        <f>SUM(AA5,AA9:AA10,AA13,AA17:AA18,AA21,AA25:AA33,AA36:AA39)</f>
+        <v>0.1336999999999999</v>
       </c>
     </row>
   </sheetData>
@@ -42207,6 +42615,31 @@
     <mergeCell ref="I3:M3"/>
     <mergeCell ref="N3:O3"/>
   </mergeCells>
+  <conditionalFormatting sqref="Z5:Z43">
+    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA5:AA43 AA45">
+    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z45">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AA46">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z46">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Formatting small/large copepods by strata
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="225">
   <si>
     <t>Species</t>
   </si>
@@ -698,6 +698,9 @@
   </si>
   <si>
     <t>Updated plankton indices</t>
+  </si>
+  <si>
+    <t>32,125 NEFSC survey records not assigned EPU out of 273,626</t>
   </si>
 </sst>
 </file>
@@ -33221,7 +33224,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T232"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="H1" workbookViewId="0">
       <selection activeCell="R14" sqref="R14"/>
     </sheetView>
   </sheetViews>
@@ -39160,8 +39163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AN20"/>
   <sheetViews>
-    <sheetView topLeftCell="U1" zoomScale="146" workbookViewId="0">
-      <selection activeCell="AM3" sqref="W1:AM3"/>
+    <sheetView topLeftCell="B1" zoomScale="114" workbookViewId="0">
+      <selection activeCell="AD7" sqref="AD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40549,8 +40552,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AU45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" workbookViewId="0">
-      <selection activeCell="AC4" sqref="AC4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AG4" sqref="AG4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40602,6 +40605,9 @@
     <row r="2" spans="1:47" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>224</v>
       </c>
     </row>
     <row r="3" spans="1:47" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Reinstalled survdata with extended EPUs, bringing in copepod small/large by strata instead of EPU
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2236" uniqueCount="225">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="232">
   <si>
     <t>Species</t>
   </si>
@@ -702,11 +702,35 @@
   <si>
     <t>32,125 NEFSC survey records not assigned EPU out of 273,626</t>
   </si>
+  <si>
+    <t>Completed 7/23/2021</t>
+  </si>
+  <si>
+    <t>n diff</t>
+  </si>
+  <si>
+    <t>need to change to ITIScodes?</t>
+  </si>
+  <si>
+    <t>Rexamine removing outliers: mean instead of 100 before removing 1std dev</t>
+  </si>
+  <si>
+    <t>Rexamine removing outliers: only remove extreme outliers</t>
+  </si>
+  <si>
+    <t>Outliers</t>
+  </si>
+  <si>
+    <t>Use EPU_expanded in survdat file (now 11,500 rows are missing EPU or 6,485/273,626 of final data without outliers):</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1756,7 +1780,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -1980,6 +2004,7 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2073,7 +2098,41 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="131">
+  <dxfs count="135">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -16084,44 +16143,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="130" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="134" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="129" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="127" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="131" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="126" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="129" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="124" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="123" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="122" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="121" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18707,145 +18766,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="120" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="124" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="119" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="117" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="121" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="116" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="114" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="118" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="113" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="111" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="115" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="110" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="109" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="108" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="112" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="107" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="106" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="105" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="109" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="104" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="102" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="106" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="101" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="99" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="103" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="98" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="97" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="96" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="100" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="95" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="93" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="97" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="92" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="90" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="94" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="89" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="88" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20668,168 +20727,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="87" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="91" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17 B38:B119">
-    <cfRule type="cellIs" dxfId="86" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="84" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="82" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 J5 J10 J14 J17:J18 J21:J22 J24:J25 J27:J29">
-    <cfRule type="cellIs" dxfId="80" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="79" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31 L5 L10 L14 L17:L18 L21:L22 L27:L29 L24:L25">
-    <cfRule type="cellIs" dxfId="78" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="82" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L4 L6:L9 L11:L13 L15:L16 L19:L20 L23 L30:L31 L26">
-    <cfRule type="cellIs" dxfId="77" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="76" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="80" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="75" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="79" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="74" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="77" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26 P4:P9 P11 P13:P15 P19:P21 P24 P30">
-    <cfRule type="cellIs" dxfId="72" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="76" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P31 P18 P10 P12 P16 P22:P23 P25:P26">
-    <cfRule type="cellIs" dxfId="71" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="70" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="69" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="73" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="68" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13 R10 R12 R16:R18 R22:R23 R25:R29 R31 R3">
-    <cfRule type="cellIs" dxfId="66" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="70" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2 R19:R21 R6:R9 R11 R13 R24 R30 R4">
-    <cfRule type="cellIs" dxfId="65" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="63" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="67" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="62" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="60" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="64" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="59" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="57" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="61" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="56" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="59" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119 B31:B37">
-    <cfRule type="cellIs" dxfId="54" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="58" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="53" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="57" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="52" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="51" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 J3:J4 J6:J9 J11:J13 J15:J16 J19:J20 J23 J26 J30:J31">
-    <cfRule type="cellIs" dxfId="50" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29048,87 +29107,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="49" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="53" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="48" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="51" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="46" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="50" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="45" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="49" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="44" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="47" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="42" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="46" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="41" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="44" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="39" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="43" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="38" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="37" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="40" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="35" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="39" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="34" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="31" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29165,35 +29224,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="81" t="s">
+      <c r="B2" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="82"/>
-      <c r="D2" s="82"/>
-      <c r="E2" s="82"/>
-      <c r="F2" s="82"/>
-      <c r="G2" s="82"/>
-      <c r="H2" s="82"/>
-      <c r="I2" s="82"/>
-      <c r="J2" s="82"/>
-      <c r="K2" s="82"/>
-      <c r="L2" s="82"/>
-      <c r="M2" s="83"/>
+      <c r="C2" s="83"/>
+      <c r="D2" s="83"/>
+      <c r="E2" s="83"/>
+      <c r="F2" s="83"/>
+      <c r="G2" s="83"/>
+      <c r="H2" s="83"/>
+      <c r="I2" s="83"/>
+      <c r="J2" s="83"/>
+      <c r="K2" s="83"/>
+      <c r="L2" s="83"/>
+      <c r="M2" s="84"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="81" t="s">
+      <c r="R2" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="82"/>
-      <c r="T2" s="82"/>
-      <c r="U2" s="82"/>
-      <c r="V2" s="82"/>
-      <c r="W2" s="82"/>
-      <c r="X2" s="82"/>
-      <c r="Y2" s="82"/>
-      <c r="Z2" s="82"/>
-      <c r="AA2" s="83"/>
+      <c r="S2" s="83"/>
+      <c r="T2" s="83"/>
+      <c r="U2" s="83"/>
+      <c r="V2" s="83"/>
+      <c r="W2" s="83"/>
+      <c r="X2" s="83"/>
+      <c r="Y2" s="83"/>
+      <c r="Z2" s="83"/>
+      <c r="AA2" s="84"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -29206,50 +29265,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="87" t="s">
+      <c r="C3" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="89" t="s">
+      <c r="D3" s="90" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="87" t="s">
+      <c r="E3" s="88" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="84" t="s">
+      <c r="F3" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="85"/>
-      <c r="H3" s="84" t="s">
+      <c r="G3" s="86"/>
+      <c r="H3" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="86"/>
-      <c r="J3" s="85"/>
-      <c r="K3" s="84" t="s">
+      <c r="I3" s="87"/>
+      <c r="J3" s="86"/>
+      <c r="K3" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="86"/>
-      <c r="M3" s="85"/>
+      <c r="L3" s="87"/>
+      <c r="M3" s="86"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="87" t="s">
+      <c r="S3" s="88" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="84" t="s">
+      <c r="T3" s="85" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="85"/>
-      <c r="V3" s="84" t="s">
+      <c r="U3" s="86"/>
+      <c r="V3" s="85" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="86"/>
-      <c r="X3" s="85"/>
-      <c r="Y3" s="84" t="s">
+      <c r="W3" s="87"/>
+      <c r="X3" s="86"/>
+      <c r="Y3" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="86"/>
-      <c r="AA3" s="85"/>
+      <c r="Z3" s="87"/>
+      <c r="AA3" s="86"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -29263,9 +29322,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="88"/>
-      <c r="D4" s="90"/>
-      <c r="E4" s="88"/>
+      <c r="C4" s="89"/>
+      <c r="D4" s="91"/>
+      <c r="E4" s="89"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -29300,7 +29359,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="88"/>
+      <c r="S4" s="89"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -33151,67 +33210,67 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="30" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="33" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="28" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="32" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="27" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="31" priority="12" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="26" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="30" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="24" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="8" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="22" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ4:BJ27">
-    <cfRule type="cellIs" dxfId="21" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BH27">
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="23" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ28:BJ32">
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB28:BH32">
-    <cfRule type="cellIs" dxfId="17" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="16" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39130,28 +39189,28 @@
     <sortCondition ref="I2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="15" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="12" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39312,30 +39371,30 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="92" t="s">
+      <c r="W2" s="93" t="s">
         <v>178</v>
       </c>
-      <c r="X2" s="93"/>
-      <c r="Y2" s="91" t="s">
+      <c r="X2" s="94"/>
+      <c r="Y2" s="92" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="91"/>
-      <c r="AA2" s="91"/>
-      <c r="AB2" s="91"/>
+      <c r="Z2" s="92"/>
+      <c r="AA2" s="92"/>
+      <c r="AB2" s="92"/>
       <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="91" t="s">
+      <c r="AD2" s="92" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" s="91"/>
-      <c r="AF2" s="91"/>
-      <c r="AG2" s="91"/>
-      <c r="AH2" s="91"/>
-      <c r="AI2" s="91" t="s">
+      <c r="AE2" s="92"/>
+      <c r="AF2" s="92"/>
+      <c r="AG2" s="92"/>
+      <c r="AH2" s="92"/>
+      <c r="AI2" s="92" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="91"/>
+      <c r="AJ2" s="92"/>
       <c r="AK2" s="63" t="s">
         <v>183</v>
       </c>
@@ -40527,19 +40586,19 @@
     <mergeCell ref="AD2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
-    <cfRule type="cellIs" dxfId="9" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40550,10 +40609,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AU45"/>
+  <dimension ref="A1:BN45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AG4" sqref="AG4"/>
+    <sheetView tabSelected="1" topLeftCell="Y4" workbookViewId="0">
+      <selection activeCell="Z7" sqref="Z7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40572,7 +40631,7 @@
     <col min="23" max="25" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:47" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:66" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40601,40 +40660,56 @@
       <c r="W1" s="75" t="s">
         <v>213</v>
       </c>
-    </row>
-    <row r="2" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AV1" t="s">
+        <v>224</v>
+      </c>
+      <c r="BH1"/>
+    </row>
+    <row r="2" spans="1:66" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
-      <c r="AI2" t="s">
-        <v>224</v>
-      </c>
-    </row>
-    <row r="3" spans="1:47" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="94" t="s">
+      <c r="AD2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>227</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>231</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:66" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="B3" s="95" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="95"/>
-      <c r="D3" s="96" t="s">
+      <c r="C3" s="96"/>
+      <c r="D3" s="97" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="96"/>
-      <c r="F3" s="96"/>
-      <c r="G3" s="96"/>
+      <c r="E3" s="97"/>
+      <c r="F3" s="97"/>
+      <c r="G3" s="97"/>
       <c r="H3" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="96" t="s">
+      <c r="I3" s="97" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="96"/>
-      <c r="K3" s="96"/>
-      <c r="L3" s="96"/>
-      <c r="M3" s="96"/>
-      <c r="N3" s="96" t="s">
+      <c r="J3" s="97"/>
+      <c r="K3" s="97"/>
+      <c r="L3" s="97"/>
+      <c r="M3" s="97"/>
+      <c r="N3" s="97" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="96"/>
+      <c r="O3" s="97"/>
       <c r="P3" s="70" t="s">
         <v>183</v>
       </c>
@@ -40647,20 +40722,27 @@
       <c r="W3" s="75" t="s">
         <v>217</v>
       </c>
-      <c r="AC3" s="75" t="s">
+      <c r="AD3" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="AJ3" s="75" t="s">
+        <v>230</v>
+      </c>
+      <c r="AP3" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="AI3" s="75" t="s">
+      <c r="AV3" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="AO3" s="75" t="s">
+      <c r="BC3" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="AU3" s="75" t="s">
+      <c r="BH3"/>
+      <c r="BJ3" s="75" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:47" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:66" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40736,8 +40818,107 @@
       <c r="AA4" s="69" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="5" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="AD4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="AE4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="AF4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="AG4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="AH4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="AJ4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="AK4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="AM4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="AN4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="AP4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="AQ4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="AR4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="AS4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="AT4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="AV4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="AW4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="AX4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="AY4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="AZ4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="BA4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="BC4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="BD4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="BE4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="BF4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="BG4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="BH4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="BJ4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="BK4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="BL4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="BM4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="BN4" s="69" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="5" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -40794,8 +40975,45 @@
         <f t="shared" ref="AA5:AA43" si="0">X5-T5</f>
         <v>2.8700000000000003E-2</v>
       </c>
-    </row>
-    <row r="6" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB5">
+        <f>Y5-U5</f>
+        <v>55</v>
+      </c>
+      <c r="AV5">
+        <v>21.826599999999999</v>
+      </c>
+      <c r="AW5">
+        <v>0.15859999999999999</v>
+      </c>
+      <c r="AX5">
+        <v>564</v>
+      </c>
+      <c r="AY5">
+        <f>AV5-S5</f>
+        <v>-1.833400000000001</v>
+      </c>
+      <c r="AZ5">
+        <f>AW5-T5</f>
+        <v>9.0699999999999989E-2</v>
+      </c>
+      <c r="BA5">
+        <f>AX5-U5</f>
+        <v>-158</v>
+      </c>
+      <c r="BF5">
+        <f t="shared" ref="BF5:BF43" si="1">BC5-S5</f>
+        <v>-23.66</v>
+      </c>
+      <c r="BG5">
+        <f t="shared" ref="BG5:BG43" si="2">BD5-T5</f>
+        <v>-6.7900000000000002E-2</v>
+      </c>
+      <c r="BH5">
+        <f t="shared" ref="BH5:BH43" si="3">BE5-U5</f>
+        <v>-722</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -40825,15 +41043,61 @@
         <v>918</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z43" si="1">W6-S6</f>
+        <f t="shared" ref="Z6:Z43" si="4">W6-S6</f>
         <v>-19.489999999999998</v>
       </c>
       <c r="AA6">
         <f t="shared" si="0"/>
         <v>-0.1578</v>
       </c>
-    </row>
-    <row r="7" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB6">
+        <f t="shared" ref="AB6:AB43" si="5">Y6-U6</f>
+        <v>-918</v>
+      </c>
+      <c r="AV6">
+        <v>21.686299999999999</v>
+      </c>
+      <c r="AW6">
+        <v>0.12389799999999999</v>
+      </c>
+      <c r="AX6">
+        <v>1184</v>
+      </c>
+      <c r="AY6">
+        <f t="shared" ref="AY6:AY17" si="6">AV6-S6</f>
+        <v>2.1963000000000008</v>
+      </c>
+      <c r="AZ6">
+        <f t="shared" ref="AZ6:AZ17" si="7">AW6-T6</f>
+        <v>-3.3902000000000002E-2</v>
+      </c>
+      <c r="BA6">
+        <f t="shared" ref="BA6:BA17" si="8">AX6-U6</f>
+        <v>266</v>
+      </c>
+      <c r="BC6">
+        <v>21.29806</v>
+      </c>
+      <c r="BD6">
+        <v>0.12659999999999999</v>
+      </c>
+      <c r="BE6">
+        <v>2039</v>
+      </c>
+      <c r="BF6">
+        <f t="shared" si="1"/>
+        <v>1.8080600000000011</v>
+      </c>
+      <c r="BG6">
+        <f t="shared" si="2"/>
+        <v>-3.1200000000000006E-2</v>
+      </c>
+      <c r="BH6">
+        <f t="shared" si="3"/>
+        <v>1121</v>
+      </c>
+    </row>
+    <row r="7" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -40862,15 +41126,61 @@
         <v>514</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-24.05</v>
       </c>
       <c r="AA7">
         <f t="shared" si="0"/>
         <v>-0.17219999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB7">
+        <f t="shared" si="5"/>
+        <v>-514</v>
+      </c>
+      <c r="AV7">
+        <v>24.4513</v>
+      </c>
+      <c r="AW7">
+        <v>0.17283699999999999</v>
+      </c>
+      <c r="AX7">
+        <v>529</v>
+      </c>
+      <c r="AY7">
+        <f t="shared" si="6"/>
+        <v>0.4012999999999991</v>
+      </c>
+      <c r="AZ7">
+        <f t="shared" si="7"/>
+        <v>6.3699999999999868E-4</v>
+      </c>
+      <c r="BA7">
+        <f t="shared" si="8"/>
+        <v>15</v>
+      </c>
+      <c r="BC7" s="81">
+        <v>27.037700000000001</v>
+      </c>
+      <c r="BD7">
+        <v>0.13519999999999999</v>
+      </c>
+      <c r="BE7">
+        <v>913</v>
+      </c>
+      <c r="BF7">
+        <f t="shared" si="1"/>
+        <v>2.9877000000000002</v>
+      </c>
+      <c r="BG7">
+        <f t="shared" si="2"/>
+        <v>-3.7000000000000005E-2</v>
+      </c>
+      <c r="BH7">
+        <f t="shared" si="3"/>
+        <v>399</v>
+      </c>
+    </row>
+    <row r="8" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -40908,15 +41218,52 @@
         <v>434</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-8.4600000000000009</v>
       </c>
       <c r="AA8">
         <f t="shared" si="0"/>
         <v>-0.2122</v>
       </c>
-    </row>
-    <row r="9" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB8">
+        <f t="shared" si="5"/>
+        <v>-434</v>
+      </c>
+      <c r="AV8">
+        <v>9.6183999999999994</v>
+      </c>
+      <c r="AW8">
+        <v>0.20796999999999999</v>
+      </c>
+      <c r="AX8">
+        <v>677</v>
+      </c>
+      <c r="AY8">
+        <f t="shared" si="6"/>
+        <v>1.1583999999999985</v>
+      </c>
+      <c r="AZ8">
+        <f t="shared" si="7"/>
+        <v>-4.2300000000000115E-3</v>
+      </c>
+      <c r="BA8">
+        <f t="shared" si="8"/>
+        <v>243</v>
+      </c>
+      <c r="BF8">
+        <f t="shared" si="1"/>
+        <v>-8.4600000000000009</v>
+      </c>
+      <c r="BG8">
+        <f t="shared" si="2"/>
+        <v>-0.2122</v>
+      </c>
+      <c r="BH8">
+        <f t="shared" si="3"/>
+        <v>-434</v>
+      </c>
+    </row>
+    <row r="9" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -40957,15 +41304,61 @@
         <v>1386</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.1599999999999966</v>
       </c>
       <c r="AA9">
         <f t="shared" si="0"/>
         <v>-2.2699999999999998E-2</v>
       </c>
-    </row>
-    <row r="10" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB9">
+        <f t="shared" si="5"/>
+        <v>304</v>
+      </c>
+      <c r="AV9">
+        <v>49.6509</v>
+      </c>
+      <c r="AW9">
+        <v>0.14335000000000001</v>
+      </c>
+      <c r="AX9">
+        <v>1756</v>
+      </c>
+      <c r="AY9">
+        <f t="shared" si="6"/>
+        <v>2.9808999999999983</v>
+      </c>
+      <c r="AZ9">
+        <f t="shared" si="7"/>
+        <v>-6.5500000000000003E-3</v>
+      </c>
+      <c r="BA9">
+        <f t="shared" si="8"/>
+        <v>674</v>
+      </c>
+      <c r="BC9">
+        <v>52.134480000000003</v>
+      </c>
+      <c r="BD9">
+        <v>7.7249999999999999E-2</v>
+      </c>
+      <c r="BE9">
+        <v>2549</v>
+      </c>
+      <c r="BF9">
+        <f t="shared" si="1"/>
+        <v>5.4644800000000018</v>
+      </c>
+      <c r="BG9">
+        <f t="shared" si="2"/>
+        <v>-7.2650000000000006E-2</v>
+      </c>
+      <c r="BH9">
+        <f t="shared" si="3"/>
+        <v>1467</v>
+      </c>
+    </row>
+    <row r="10" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -41014,15 +41407,52 @@
         <v>628</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.12000000000000099</v>
       </c>
       <c r="AA10">
         <f t="shared" si="0"/>
         <v>1.4399999999999996E-2</v>
       </c>
-    </row>
-    <row r="11" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="AV10">
+        <v>20.887740000000001</v>
+      </c>
+      <c r="AW10">
+        <v>0.10326</v>
+      </c>
+      <c r="AX10">
+        <v>857</v>
+      </c>
+      <c r="AY10">
+        <f t="shared" si="6"/>
+        <v>1.9977400000000003</v>
+      </c>
+      <c r="AZ10">
+        <f t="shared" si="7"/>
+        <v>-6.7839999999999998E-2</v>
+      </c>
+      <c r="BA10">
+        <f t="shared" si="8"/>
+        <v>229</v>
+      </c>
+      <c r="BF10">
+        <f t="shared" si="1"/>
+        <v>-18.89</v>
+      </c>
+      <c r="BG10">
+        <f t="shared" si="2"/>
+        <v>-0.1711</v>
+      </c>
+      <c r="BH10">
+        <f t="shared" si="3"/>
+        <v>-628</v>
+      </c>
+    </row>
+    <row r="11" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -41051,15 +41481,61 @@
         <v>525</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-16.059999999999999</v>
       </c>
       <c r="AA11">
         <f t="shared" si="0"/>
         <v>-0.1303</v>
       </c>
-    </row>
-    <row r="12" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB11">
+        <f t="shared" si="5"/>
+        <v>-525</v>
+      </c>
+      <c r="AV11">
+        <v>16.619240000000001</v>
+      </c>
+      <c r="AW11">
+        <v>0.1237</v>
+      </c>
+      <c r="AX11">
+        <v>542</v>
+      </c>
+      <c r="AY11">
+        <f t="shared" si="6"/>
+        <v>0.55924000000000262</v>
+      </c>
+      <c r="AZ11">
+        <f t="shared" si="7"/>
+        <v>-6.5999999999999948E-3</v>
+      </c>
+      <c r="BA11">
+        <f t="shared" si="8"/>
+        <v>17</v>
+      </c>
+      <c r="BC11">
+        <v>19.383800000000001</v>
+      </c>
+      <c r="BD11">
+        <v>8.1460000000000005E-2</v>
+      </c>
+      <c r="BE11">
+        <v>862</v>
+      </c>
+      <c r="BF11">
+        <f t="shared" si="1"/>
+        <v>3.3238000000000021</v>
+      </c>
+      <c r="BG11">
+        <f t="shared" si="2"/>
+        <v>-4.8839999999999995E-2</v>
+      </c>
+      <c r="BH11">
+        <f t="shared" si="3"/>
+        <v>337</v>
+      </c>
+    </row>
+    <row r="12" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -41097,15 +41573,43 @@
         <v>588</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-20.85</v>
       </c>
       <c r="AA12">
         <f t="shared" si="0"/>
         <v>-0.32519999999999999</v>
       </c>
-    </row>
-    <row r="13" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB12">
+        <f t="shared" si="5"/>
+        <v>-588</v>
+      </c>
+      <c r="AY12">
+        <f t="shared" si="6"/>
+        <v>-20.85</v>
+      </c>
+      <c r="AZ12">
+        <f t="shared" si="7"/>
+        <v>-0.32519999999999999</v>
+      </c>
+      <c r="BA12">
+        <f t="shared" si="8"/>
+        <v>-588</v>
+      </c>
+      <c r="BF12">
+        <f t="shared" si="1"/>
+        <v>-20.85</v>
+      </c>
+      <c r="BG12">
+        <f t="shared" si="2"/>
+        <v>-0.32519999999999999</v>
+      </c>
+      <c r="BH12">
+        <f t="shared" si="3"/>
+        <v>-588</v>
+      </c>
+    </row>
+    <row r="13" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -41153,15 +41657,43 @@
         <v>799</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.18999999999999773</v>
       </c>
       <c r="AA13">
         <f t="shared" si="0"/>
         <v>1.5899999999999984E-2</v>
       </c>
-    </row>
-    <row r="14" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB13">
+        <f t="shared" si="5"/>
+        <v>21</v>
+      </c>
+      <c r="AY13">
+        <f t="shared" si="6"/>
+        <v>-33.68</v>
+      </c>
+      <c r="AZ13">
+        <f t="shared" si="7"/>
+        <v>-0.11020000000000001</v>
+      </c>
+      <c r="BA13">
+        <f t="shared" si="8"/>
+        <v>-778</v>
+      </c>
+      <c r="BF13">
+        <f t="shared" si="1"/>
+        <v>-33.68</v>
+      </c>
+      <c r="BG13">
+        <f t="shared" si="2"/>
+        <v>-0.11020000000000001</v>
+      </c>
+      <c r="BH13">
+        <f t="shared" si="3"/>
+        <v>-778</v>
+      </c>
+    </row>
+    <row r="14" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -41190,15 +41722,61 @@
         <v>514</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-13.17</v>
       </c>
       <c r="AA14">
         <f t="shared" si="0"/>
         <v>-0.2238</v>
       </c>
-    </row>
-    <row r="15" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB14">
+        <f t="shared" si="5"/>
+        <v>-514</v>
+      </c>
+      <c r="AV14">
+        <v>13.399900000000001</v>
+      </c>
+      <c r="AW14">
+        <v>0.215</v>
+      </c>
+      <c r="AX14">
+        <v>527</v>
+      </c>
+      <c r="AY14">
+        <f t="shared" si="6"/>
+        <v>0.22990000000000066</v>
+      </c>
+      <c r="AZ14">
+        <f t="shared" si="7"/>
+        <v>-8.8000000000000023E-3</v>
+      </c>
+      <c r="BA14">
+        <f t="shared" si="8"/>
+        <v>13</v>
+      </c>
+      <c r="BC14">
+        <v>13.7043</v>
+      </c>
+      <c r="BD14">
+        <v>0.17480000000000001</v>
+      </c>
+      <c r="BE14">
+        <v>1022</v>
+      </c>
+      <c r="BF14">
+        <f t="shared" si="1"/>
+        <v>0.5343</v>
+      </c>
+      <c r="BG14">
+        <f t="shared" si="2"/>
+        <v>-4.8999999999999988E-2</v>
+      </c>
+      <c r="BH14">
+        <f t="shared" si="3"/>
+        <v>508</v>
+      </c>
+    </row>
+    <row r="15" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -41236,15 +41814,43 @@
         <v>663</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-19.57</v>
       </c>
       <c r="AA15">
         <f t="shared" si="0"/>
         <v>-0.23630000000000001</v>
       </c>
-    </row>
-    <row r="16" spans="1:47" x14ac:dyDescent="0.35">
+      <c r="AB15">
+        <f t="shared" si="5"/>
+        <v>-663</v>
+      </c>
+      <c r="AY15">
+        <f t="shared" si="6"/>
+        <v>-19.57</v>
+      </c>
+      <c r="AZ15">
+        <f t="shared" si="7"/>
+        <v>-0.23630000000000001</v>
+      </c>
+      <c r="BA15">
+        <f t="shared" si="8"/>
+        <v>-663</v>
+      </c>
+      <c r="BF15">
+        <f t="shared" si="1"/>
+        <v>-19.57</v>
+      </c>
+      <c r="BG15">
+        <f t="shared" si="2"/>
+        <v>-0.23630000000000001</v>
+      </c>
+      <c r="BH15">
+        <f t="shared" si="3"/>
+        <v>-663</v>
+      </c>
+    </row>
+    <row r="16" spans="1:66" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -41273,15 +41879,52 @@
         <v>716</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-52.53</v>
       </c>
       <c r="AA16">
         <f t="shared" si="0"/>
         <v>-4.9299999999999997E-2</v>
       </c>
-    </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB16">
+        <f t="shared" si="5"/>
+        <v>-716</v>
+      </c>
+      <c r="AY16">
+        <f t="shared" si="6"/>
+        <v>-52.53</v>
+      </c>
+      <c r="AZ16">
+        <f t="shared" si="7"/>
+        <v>-4.9299999999999997E-2</v>
+      </c>
+      <c r="BA16">
+        <f t="shared" si="8"/>
+        <v>-716</v>
+      </c>
+      <c r="BC16">
+        <v>53.034950000000002</v>
+      </c>
+      <c r="BD16">
+        <v>5.9695999999999999E-2</v>
+      </c>
+      <c r="BE16">
+        <v>1133</v>
+      </c>
+      <c r="BF16">
+        <f t="shared" si="1"/>
+        <v>0.5049500000000009</v>
+      </c>
+      <c r="BG16">
+        <f t="shared" si="2"/>
+        <v>1.0396000000000002E-2</v>
+      </c>
+      <c r="BH16">
+        <f t="shared" si="3"/>
+        <v>417</v>
+      </c>
+    </row>
+    <row r="17" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -41328,15 +41971,43 @@
         <v>288</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9199999999999982</v>
       </c>
       <c r="AA17">
         <f t="shared" si="0"/>
         <v>-1.0000000000000009E-3</v>
       </c>
-    </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB17">
+        <f t="shared" si="5"/>
+        <v>57</v>
+      </c>
+      <c r="AY17">
+        <f t="shared" si="6"/>
+        <v>-31.77</v>
+      </c>
+      <c r="AZ17">
+        <f t="shared" si="7"/>
+        <v>-0.2361</v>
+      </c>
+      <c r="BA17">
+        <f t="shared" si="8"/>
+        <v>-231</v>
+      </c>
+      <c r="BF17">
+        <f t="shared" si="1"/>
+        <v>-31.77</v>
+      </c>
+      <c r="BG17">
+        <f t="shared" si="2"/>
+        <v>-0.2361</v>
+      </c>
+      <c r="BH17">
+        <f t="shared" si="3"/>
+        <v>-231</v>
+      </c>
+    </row>
+    <row r="18" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -41383,15 +42054,31 @@
         <v>383</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.1899999999999995</v>
       </c>
       <c r="AA18">
         <f t="shared" si="0"/>
         <v>3.0599999999999988E-2</v>
       </c>
-    </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB18">
+        <f t="shared" si="5"/>
+        <v>40</v>
+      </c>
+      <c r="BF18">
+        <f t="shared" si="1"/>
+        <v>-13.96</v>
+      </c>
+      <c r="BG18">
+        <f t="shared" si="2"/>
+        <v>-0.1061</v>
+      </c>
+      <c r="BH18">
+        <f t="shared" si="3"/>
+        <v>-343</v>
+      </c>
+    </row>
+    <row r="19" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -41430,15 +42117,31 @@
         <v>320</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-22.79</v>
       </c>
       <c r="AA19">
         <f t="shared" si="0"/>
         <v>-0.28999999999999998</v>
       </c>
-    </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB19">
+        <f t="shared" si="5"/>
+        <v>-320</v>
+      </c>
+      <c r="BF19">
+        <f t="shared" si="1"/>
+        <v>-22.79</v>
+      </c>
+      <c r="BG19">
+        <f t="shared" si="2"/>
+        <v>-0.28999999999999998</v>
+      </c>
+      <c r="BH19">
+        <f t="shared" si="3"/>
+        <v>-320</v>
+      </c>
+    </row>
+    <row r="20" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -41467,15 +42170,40 @@
         <v>283</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-63.69</v>
       </c>
       <c r="AA20">
         <f t="shared" si="0"/>
         <v>-0.1002</v>
       </c>
-    </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB20">
+        <f t="shared" si="5"/>
+        <v>-283</v>
+      </c>
+      <c r="BC20">
+        <v>68.383750000000006</v>
+      </c>
+      <c r="BD20">
+        <v>0.11585139999999999</v>
+      </c>
+      <c r="BE20">
+        <v>454</v>
+      </c>
+      <c r="BF20">
+        <f t="shared" si="1"/>
+        <v>4.6937500000000085</v>
+      </c>
+      <c r="BG20">
+        <f t="shared" si="2"/>
+        <v>1.5651399999999996E-2</v>
+      </c>
+      <c r="BH20">
+        <f t="shared" si="3"/>
+        <v>171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -41525,15 +42253,31 @@
         <v>752</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.1120000000000001</v>
       </c>
       <c r="AA21">
         <f t="shared" si="0"/>
         <v>0.06</v>
       </c>
-    </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB21">
+        <f t="shared" si="5"/>
+        <v>106</v>
+      </c>
+      <c r="BF21">
+        <f t="shared" si="1"/>
+        <v>-11.31</v>
+      </c>
+      <c r="BG21">
+        <f t="shared" si="2"/>
+        <v>-0.11219999999999999</v>
+      </c>
+      <c r="BH21">
+        <f t="shared" si="3"/>
+        <v>-646</v>
+      </c>
+    </row>
+    <row r="22" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -41571,15 +42315,31 @@
         <v>236</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-10.199999999999999</v>
       </c>
       <c r="AA22">
         <f t="shared" si="0"/>
         <v>-0.37130000000000002</v>
       </c>
-    </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB22">
+        <f t="shared" si="5"/>
+        <v>-236</v>
+      </c>
+      <c r="BF22">
+        <f t="shared" si="1"/>
+        <v>-10.199999999999999</v>
+      </c>
+      <c r="BG22">
+        <f t="shared" si="2"/>
+        <v>-0.37130000000000002</v>
+      </c>
+      <c r="BH22">
+        <f t="shared" si="3"/>
+        <v>-236</v>
+      </c>
+    </row>
+    <row r="23" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -41608,15 +42368,40 @@
         <v>323</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-14.93</v>
       </c>
       <c r="AA23">
         <f t="shared" si="0"/>
         <v>-0.1002</v>
       </c>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB23">
+        <f t="shared" si="5"/>
+        <v>-323</v>
+      </c>
+      <c r="BC23">
+        <v>15.04355</v>
+      </c>
+      <c r="BD23">
+        <v>9.3257999999999994E-2</v>
+      </c>
+      <c r="BE23">
+        <v>829</v>
+      </c>
+      <c r="BF23">
+        <f t="shared" si="1"/>
+        <v>0.11355000000000004</v>
+      </c>
+      <c r="BG23">
+        <f t="shared" si="2"/>
+        <v>-6.9420000000000037E-3</v>
+      </c>
+      <c r="BH23">
+        <f t="shared" si="3"/>
+        <v>506</v>
+      </c>
+    </row>
+    <row r="24" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -41645,15 +42430,40 @@
         <v>283</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-23.49</v>
       </c>
       <c r="AA24">
         <f t="shared" si="0"/>
         <v>-0.1487</v>
       </c>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB24">
+        <f t="shared" si="5"/>
+        <v>-283</v>
+      </c>
+      <c r="BC24">
+        <v>21.397960000000001</v>
+      </c>
+      <c r="BD24">
+        <v>0.14054</v>
+      </c>
+      <c r="BE24">
+        <v>602</v>
+      </c>
+      <c r="BF24">
+        <f t="shared" si="1"/>
+        <v>-2.0920399999999972</v>
+      </c>
+      <c r="BG24">
+        <f t="shared" si="2"/>
+        <v>-8.1600000000000006E-3</v>
+      </c>
+      <c r="BH24">
+        <f t="shared" si="3"/>
+        <v>319</v>
+      </c>
+    </row>
+    <row r="25" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -41701,15 +42511,31 @@
         <v>286</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>3.6370000000000005</v>
       </c>
       <c r="AA25">
         <f t="shared" si="0"/>
         <v>6.0100000000000015E-2</v>
       </c>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB25">
+        <f t="shared" si="5"/>
+        <v>82</v>
+      </c>
+      <c r="BF25">
+        <f t="shared" si="1"/>
+        <v>-17.02</v>
+      </c>
+      <c r="BG25">
+        <f t="shared" si="2"/>
+        <v>-0.21240000000000001</v>
+      </c>
+      <c r="BH25">
+        <f t="shared" si="3"/>
+        <v>-204</v>
+      </c>
+    </row>
+    <row r="26" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -41758,15 +42584,31 @@
         <v>341</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>4.0500000000000007</v>
       </c>
       <c r="AA26">
         <f t="shared" si="0"/>
         <v>-9.4700000000000006E-2</v>
       </c>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB26">
+        <f t="shared" si="5"/>
+        <v>121</v>
+      </c>
+      <c r="BF26">
+        <f t="shared" si="1"/>
+        <v>-10.1</v>
+      </c>
+      <c r="BG26">
+        <f t="shared" si="2"/>
+        <v>-0.3599</v>
+      </c>
+      <c r="BH26">
+        <f t="shared" si="3"/>
+        <v>-220</v>
+      </c>
+    </row>
+    <row r="27" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -41814,15 +42656,31 @@
         <v>250</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-2.4648000000000003</v>
       </c>
       <c r="AA27">
         <f t="shared" si="0"/>
         <v>8.2099999999999951E-2</v>
       </c>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB27">
+        <f t="shared" si="5"/>
+        <v>76</v>
+      </c>
+      <c r="BF27">
+        <f t="shared" si="1"/>
+        <v>-22.76</v>
+      </c>
+      <c r="BG27">
+        <f t="shared" si="2"/>
+        <v>-0.27900000000000003</v>
+      </c>
+      <c r="BH27">
+        <f t="shared" si="3"/>
+        <v>-174</v>
+      </c>
+    </row>
+    <row r="28" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -41871,15 +42729,31 @@
         <v>179</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9999999999999574E-2</v>
       </c>
       <c r="AA28">
         <f t="shared" si="0"/>
         <v>-2.0199999999999996E-2</v>
       </c>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB28">
+        <f t="shared" si="5"/>
+        <v>14</v>
+      </c>
+      <c r="BF28">
+        <f t="shared" si="1"/>
+        <v>-30.57</v>
+      </c>
+      <c r="BG28">
+        <f t="shared" si="2"/>
+        <v>-0.26269999999999999</v>
+      </c>
+      <c r="BH28">
+        <f t="shared" si="3"/>
+        <v>-165</v>
+      </c>
+    </row>
+    <row r="29" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -41928,15 +42802,31 @@
         <v>384</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.3628</v>
       </c>
       <c r="AA29">
         <f t="shared" si="0"/>
         <v>-3.7200000000000011E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB29">
+        <f t="shared" si="5"/>
+        <v>60</v>
+      </c>
+      <c r="BF29">
+        <f t="shared" si="1"/>
+        <v>-19.22</v>
+      </c>
+      <c r="BG29">
+        <f t="shared" si="2"/>
+        <v>-0.3029</v>
+      </c>
+      <c r="BH29">
+        <f t="shared" si="3"/>
+        <v>-324</v>
+      </c>
+    </row>
+    <row r="30" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -41985,15 +42875,31 @@
         <v>284</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.25</v>
       </c>
       <c r="AA30">
         <f t="shared" si="0"/>
         <v>-1.7999999999999995E-2</v>
       </c>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB30">
+        <f t="shared" si="5"/>
+        <v>51</v>
+      </c>
+      <c r="BF30">
+        <f t="shared" si="1"/>
+        <v>-11.61</v>
+      </c>
+      <c r="BG30">
+        <f t="shared" si="2"/>
+        <v>-6.8199999999999997E-2</v>
+      </c>
+      <c r="BH30">
+        <f t="shared" si="3"/>
+        <v>-233</v>
+      </c>
+    </row>
+    <row r="31" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -42040,15 +42946,31 @@
         <v>164</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2.135900000000003</v>
       </c>
       <c r="AA31">
         <f t="shared" si="0"/>
         <v>2.0100000000000007E-2</v>
       </c>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB31">
+        <f t="shared" si="5"/>
+        <v>24</v>
+      </c>
+      <c r="BF31">
+        <f t="shared" si="1"/>
+        <v>-16.989999999999998</v>
+      </c>
+      <c r="BG31">
+        <f t="shared" si="2"/>
+        <v>-0.20349999999999999</v>
+      </c>
+      <c r="BH31">
+        <f t="shared" si="3"/>
+        <v>-140</v>
+      </c>
+    </row>
+    <row r="32" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -42096,15 +43018,31 @@
         <v>397</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.5</v>
       </c>
       <c r="AA32">
         <f t="shared" si="0"/>
         <v>-1.6900000000000026E-2</v>
       </c>
-    </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB32">
+        <f t="shared" si="5"/>
+        <v>79</v>
+      </c>
+      <c r="BF32">
+        <f t="shared" si="1"/>
+        <v>-14.08</v>
+      </c>
+      <c r="BG32">
+        <f t="shared" si="2"/>
+        <v>-0.26400000000000001</v>
+      </c>
+      <c r="BH32">
+        <f t="shared" si="3"/>
+        <v>-318</v>
+      </c>
+    </row>
+    <row r="33" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -42152,15 +43090,31 @@
         <v>477</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-0.16999999999999815</v>
       </c>
       <c r="AA33">
         <f t="shared" si="0"/>
         <v>3.699999999999995E-3</v>
       </c>
-    </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB33">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="BF33">
+        <f t="shared" si="1"/>
+        <v>-27.43</v>
+      </c>
+      <c r="BG33">
+        <f t="shared" si="2"/>
+        <v>-0.1033</v>
+      </c>
+      <c r="BH33">
+        <f t="shared" si="3"/>
+        <v>-477</v>
+      </c>
+    </row>
+    <row r="34" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -42189,15 +43143,40 @@
         <v>530</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-11.52</v>
       </c>
       <c r="AA34">
         <f t="shared" si="0"/>
         <v>-0.24110000000000001</v>
       </c>
-    </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB34">
+        <f t="shared" si="5"/>
+        <v>-530</v>
+      </c>
+      <c r="BC34">
+        <v>14.0328</v>
+      </c>
+      <c r="BD34">
+        <v>0.1895</v>
+      </c>
+      <c r="BE34">
+        <v>764</v>
+      </c>
+      <c r="BF34">
+        <f t="shared" si="1"/>
+        <v>2.5128000000000004</v>
+      </c>
+      <c r="BG34">
+        <f t="shared" si="2"/>
+        <v>-5.1600000000000007E-2</v>
+      </c>
+      <c r="BH34">
+        <f t="shared" si="3"/>
+        <v>234</v>
+      </c>
+    </row>
+    <row r="35" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -42226,15 +43205,40 @@
         <v>454</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-8.57</v>
       </c>
       <c r="AA35">
         <f t="shared" si="0"/>
         <v>-0.2122</v>
       </c>
-    </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB35">
+        <f t="shared" si="5"/>
+        <v>-454</v>
+      </c>
+      <c r="BC35">
+        <v>8.6080649999999999</v>
+      </c>
+      <c r="BD35">
+        <v>0.2099</v>
+      </c>
+      <c r="BE35">
+        <v>477</v>
+      </c>
+      <c r="BF35">
+        <f t="shared" si="1"/>
+        <v>3.8064999999999571E-2</v>
+      </c>
+      <c r="BG35">
+        <f t="shared" si="2"/>
+        <v>-2.2999999999999965E-3</v>
+      </c>
+      <c r="BH35">
+        <f t="shared" si="3"/>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -42281,15 +43285,31 @@
         <v>162</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.6099999999999994</v>
       </c>
       <c r="AA36">
         <f t="shared" si="0"/>
         <v>5.8000000000000274E-3</v>
       </c>
-    </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB36">
+        <f t="shared" si="5"/>
+        <v>3</v>
+      </c>
+      <c r="BF36">
+        <f t="shared" si="1"/>
+        <v>-26.52</v>
+      </c>
+      <c r="BG36">
+        <f t="shared" si="2"/>
+        <v>-0.36399999999999999</v>
+      </c>
+      <c r="BH36">
+        <f t="shared" si="3"/>
+        <v>-159</v>
+      </c>
+    </row>
+    <row r="37" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -42336,15 +43356,31 @@
         <v>388</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.9170000000000016</v>
       </c>
       <c r="AA37">
         <f t="shared" si="0"/>
         <v>-2.4500000000000008E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB37">
+        <f t="shared" si="5"/>
+        <v>138</v>
+      </c>
+      <c r="BF37">
+        <f t="shared" si="1"/>
+        <v>-39.68</v>
+      </c>
+      <c r="BG37">
+        <f t="shared" si="2"/>
+        <v>-0.1246</v>
+      </c>
+      <c r="BH37">
+        <f t="shared" si="3"/>
+        <v>-250</v>
+      </c>
+    </row>
+    <row r="38" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -42393,15 +43429,31 @@
         <v>273</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>0.44000000000000128</v>
       </c>
       <c r="AA38">
         <f t="shared" si="0"/>
         <v>-1.0900000000000021E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB38">
+        <f t="shared" si="5"/>
+        <v>10</v>
+      </c>
+      <c r="BF38">
+        <f t="shared" si="1"/>
+        <v>-22.22</v>
+      </c>
+      <c r="BG38">
+        <f t="shared" si="2"/>
+        <v>-0.30280000000000001</v>
+      </c>
+      <c r="BH38">
+        <f t="shared" si="3"/>
+        <v>-263</v>
+      </c>
+    </row>
+    <row r="39" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -42448,15 +43500,31 @@
         <v>159</v>
       </c>
       <c r="Z39">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>1.3999999999999346E-2</v>
       </c>
       <c r="AA39">
         <f t="shared" si="0"/>
         <v>5.8400000000000007E-2</v>
       </c>
-    </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB39">
+        <f t="shared" si="5"/>
+        <v>22</v>
+      </c>
+      <c r="BF39">
+        <f t="shared" si="1"/>
+        <v>-26.34</v>
+      </c>
+      <c r="BG39">
+        <f t="shared" si="2"/>
+        <v>-0.22470000000000001</v>
+      </c>
+      <c r="BH39">
+        <f t="shared" si="3"/>
+        <v>-137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -42485,15 +43553,40 @@
         <v>173</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-20.14</v>
       </c>
       <c r="AA40">
         <f t="shared" si="0"/>
         <v>-0.17030000000000001</v>
       </c>
-    </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB40">
+        <f t="shared" si="5"/>
+        <v>-173</v>
+      </c>
+      <c r="BC40">
+        <v>19.668900000000001</v>
+      </c>
+      <c r="BD40" s="81">
+        <v>0.33239999999999997</v>
+      </c>
+      <c r="BE40">
+        <v>211</v>
+      </c>
+      <c r="BF40">
+        <f t="shared" si="1"/>
+        <v>-0.47109999999999985</v>
+      </c>
+      <c r="BG40">
+        <f t="shared" si="2"/>
+        <v>0.16209999999999997</v>
+      </c>
+      <c r="BH40">
+        <f t="shared" si="3"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -42522,15 +43615,40 @@
         <v>248</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-9.7100000000000009</v>
       </c>
       <c r="AA41">
         <f t="shared" si="0"/>
         <v>-0.187</v>
       </c>
-    </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB41">
+        <f t="shared" si="5"/>
+        <v>-248</v>
+      </c>
+      <c r="BC41">
+        <v>9.7552000000000003</v>
+      </c>
+      <c r="BD41">
+        <v>0.16739999999999999</v>
+      </c>
+      <c r="BE41">
+        <v>260</v>
+      </c>
+      <c r="BF41">
+        <f t="shared" si="1"/>
+        <v>4.5199999999999463E-2</v>
+      </c>
+      <c r="BG41">
+        <f t="shared" si="2"/>
+        <v>-1.9600000000000006E-2</v>
+      </c>
+      <c r="BH41">
+        <f t="shared" si="3"/>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="42" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -42559,15 +43677,40 @@
         <v>108</v>
       </c>
       <c r="Z42">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-12.46</v>
       </c>
       <c r="AA42">
         <f t="shared" si="0"/>
         <v>-0.19750000000000001</v>
       </c>
-    </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB42">
+        <f t="shared" si="5"/>
+        <v>-108</v>
+      </c>
+      <c r="BC42">
+        <v>12.31058</v>
+      </c>
+      <c r="BD42">
+        <v>0.19095999999999999</v>
+      </c>
+      <c r="BE42">
+        <v>115</v>
+      </c>
+      <c r="BF42">
+        <f t="shared" si="1"/>
+        <v>-0.149420000000001</v>
+      </c>
+      <c r="BG42">
+        <f t="shared" si="2"/>
+        <v>-6.540000000000018E-3</v>
+      </c>
+      <c r="BH42">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:60" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -42596,15 +43739,40 @@
         <v>117</v>
       </c>
       <c r="Z43">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>-33.28</v>
       </c>
       <c r="AA43">
         <f t="shared" si="0"/>
         <v>-0.2903</v>
       </c>
-    </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.35">
+      <c r="AB43">
+        <f t="shared" si="5"/>
+        <v>-117</v>
+      </c>
+      <c r="BC43">
+        <v>41.243749999999999</v>
+      </c>
+      <c r="BD43">
+        <v>0.32723000000000002</v>
+      </c>
+      <c r="BE43">
+        <v>145</v>
+      </c>
+      <c r="BF43">
+        <f t="shared" si="1"/>
+        <v>7.9637499999999974</v>
+      </c>
+      <c r="BG43">
+        <f t="shared" si="2"/>
+        <v>3.6930000000000018E-2</v>
+      </c>
+      <c r="BH43">
+        <f t="shared" si="3"/>
+        <v>28</v>
+      </c>
+    </row>
+    <row r="45" spans="1:60" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -42612,6 +43780,14 @@
       <c r="AA45">
         <f>SUM(AA5,AA9:AA10,AA13,AA17:AA18,AA21,AA25:AA33,AA36:AA39)</f>
         <v>0.1336999999999999</v>
+      </c>
+      <c r="BF45">
+        <f>SUM(BF6:BF7,BF9,BF11,BF14,BF16,BF20,BF23:BF24,BF34:BF35,BF40:BF43)</f>
+        <v>27.277845000000013</v>
+      </c>
+      <c r="BG45">
+        <f>SUM(BG6:BG7,BG9,BG11,BG14,BG16,BG20,BG23:BG24,BG34:BG35,BG40:BG43)</f>
+        <v>-0.10875460000000006</v>
       </c>
     </row>
   </sheetData>
@@ -42622,26 +43798,46 @@
     <mergeCell ref="N3:O3"/>
   </mergeCells>
   <conditionalFormatting sqref="Z5:Z43">
-    <cfRule type="cellIs" dxfId="4" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA5:AA43 AA45">
-    <cfRule type="cellIs" dxfId="3" priority="6" operator="greaterThan">
+  <conditionalFormatting sqref="AA45:AB45 AA5:AB43">
+    <cfRule type="cellIs" dxfId="7" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45">
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="6" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA46">
+  <conditionalFormatting sqref="AA46:AB46">
+    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z46">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BF5:BF43">
+    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BG5:BG43">
+    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="BF45:BG45">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="Z46">
+  <conditionalFormatting sqref="BH1:BH3 BH5:BH43">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Removed outliers based on 1 stdev from mean (instead of from 100)
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2276" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="232">
   <si>
     <t>Species</t>
   </si>
@@ -40609,10 +40609,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BN45"/>
+  <dimension ref="A1:BO45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y4" workbookViewId="0">
-      <selection activeCell="Z7" sqref="Z7"/>
+    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
+      <selection activeCell="AK2" sqref="AK2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40631,7 +40631,7 @@
     <col min="23" max="25" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:66" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:67" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40660,32 +40660,32 @@
       <c r="W1" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="AV1" t="s">
+      <c r="AW1" t="s">
         <v>224</v>
       </c>
-      <c r="BH1"/>
-    </row>
-    <row r="2" spans="1:66" x14ac:dyDescent="0.35">
+      <c r="BI1"/>
+    </row>
+    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
       <c r="AD2" t="s">
         <v>228</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>229</v>
       </c>
-      <c r="AP2" t="s">
+      <c r="AQ2" t="s">
         <v>227</v>
       </c>
-      <c r="AV2" t="s">
+      <c r="AW2" t="s">
         <v>231</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BD2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:66" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:67" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="95" t="s">
         <v>178</v>
       </c>
@@ -40725,24 +40725,24 @@
       <c r="AD3" s="75" t="s">
         <v>230</v>
       </c>
-      <c r="AJ3" s="75" t="s">
+      <c r="AK3" s="75" t="s">
         <v>230</v>
       </c>
-      <c r="AP3" s="75" t="s">
+      <c r="AQ3" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="AV3" s="75" t="s">
+      <c r="AW3" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="BC3" s="75" t="s">
+      <c r="BD3" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="BH3"/>
-      <c r="BJ3" s="75" t="s">
+      <c r="BI3"/>
+      <c r="BK3" s="75" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:66" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:67" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40836,89 +40836,92 @@
       <c r="AH4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="AJ4" s="69" t="s">
+      <c r="AI4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="AK4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AK4" s="69" t="s">
+      <c r="AL4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AL4" s="69" t="s">
+      <c r="AM4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AM4" s="69" t="s">
+      <c r="AN4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="AN4" s="69" t="s">
+      <c r="AO4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="AP4" s="69" t="s">
+      <c r="AQ4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AQ4" s="69" t="s">
+      <c r="AR4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AR4" s="69" t="s">
+      <c r="AS4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AS4" s="69" t="s">
+      <c r="AT4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="AT4" s="69" t="s">
+      <c r="AU4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="AV4" s="69" t="s">
+      <c r="AW4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AW4" s="69" t="s">
+      <c r="AX4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AX4" s="69" t="s">
+      <c r="AY4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AY4" s="69" t="s">
+      <c r="AZ4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="AZ4" s="69" t="s">
+      <c r="BA4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="BA4" s="69" t="s">
+      <c r="BB4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="BC4" s="69" t="s">
+      <c r="BD4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BD4" s="69" t="s">
+      <c r="BE4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BE4" s="69" t="s">
+      <c r="BF4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BF4" s="69" t="s">
+      <c r="BG4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BG4" s="69" t="s">
+      <c r="BH4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="BH4" s="69" t="s">
+      <c r="BI4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="BJ4" s="69" t="s">
+      <c r="BK4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BK4" s="69" t="s">
+      <c r="BL4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BL4" s="69" t="s">
+      <c r="BM4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BM4" s="69" t="s">
+      <c r="BN4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BN4" s="69" t="s">
+      <c r="BO4" s="69" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -40972,48 +40975,69 @@
         <v>0.66499999999999915</v>
       </c>
       <c r="AA5">
-        <f t="shared" ref="AA5:AA43" si="0">X5-T5</f>
+        <f>X5-T5</f>
         <v>2.8700000000000003E-2</v>
       </c>
       <c r="AB5">
         <f>Y5-U5</f>
         <v>55</v>
       </c>
-      <c r="AV5">
+      <c r="AD5">
+        <v>28.1629</v>
+      </c>
+      <c r="AE5">
+        <v>9.0800000000000006E-2</v>
+      </c>
+      <c r="AF5">
+        <v>1149</v>
+      </c>
+      <c r="AG5">
+        <f>AD5-AW5</f>
+        <v>6.3363000000000014</v>
+      </c>
+      <c r="AH5">
+        <f t="shared" ref="AH5:AI5" si="0">AE5-AX5</f>
+        <v>-6.7799999999999985E-2</v>
+      </c>
+      <c r="AI5">
+        <f t="shared" si="0"/>
+        <v>585</v>
+      </c>
+      <c r="AW5">
         <v>21.826599999999999</v>
       </c>
-      <c r="AW5">
+      <c r="AX5">
         <v>0.15859999999999999</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>564</v>
       </c>
-      <c r="AY5">
-        <f>AV5-S5</f>
-        <v>-1.833400000000001</v>
-      </c>
       <c r="AZ5">
-        <f>AW5-T5</f>
-        <v>9.0699999999999989E-2</v>
+        <f>AW5-BD5</f>
+        <v>21.826599999999999</v>
       </c>
       <c r="BA5">
-        <f>AX5-U5</f>
-        <v>-158</v>
-      </c>
-      <c r="BF5">
-        <f t="shared" ref="BF5:BF43" si="1">BC5-S5</f>
+        <f>AX5-BE5</f>
+        <v>0.15859999999999999</v>
+      </c>
+      <c r="BB5">
+        <f>AY5-BF5</f>
+        <v>564</v>
+      </c>
+      <c r="BG5">
+        <f t="shared" ref="BG5:BG43" si="1">BD5-S5</f>
         <v>-23.66</v>
       </c>
-      <c r="BG5">
-        <f t="shared" ref="BG5:BG43" si="2">BD5-T5</f>
+      <c r="BH5">
+        <f t="shared" ref="BH5:BH43" si="2">BE5-T5</f>
         <v>-6.7900000000000002E-2</v>
       </c>
-      <c r="BH5">
-        <f t="shared" ref="BH5:BH43" si="3">BE5-U5</f>
+      <c r="BI5">
+        <f t="shared" ref="BI5:BI43" si="3">BF5-U5</f>
         <v>-722</v>
       </c>
     </row>
-    <row r="6" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -41047,57 +41071,78 @@
         <v>-19.489999999999998</v>
       </c>
       <c r="AA6">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="AA6:AA43" si="5">X6-T6</f>
         <v>-0.1578</v>
       </c>
       <c r="AB6">
-        <f t="shared" ref="AB6:AB43" si="5">Y6-U6</f>
+        <f t="shared" ref="AB6:AB43" si="6">Y6-U6</f>
         <v>-918</v>
       </c>
-      <c r="AV6">
+      <c r="AD6">
+        <v>24.764700000000001</v>
+      </c>
+      <c r="AE6">
+        <v>9.1875999999999999E-2</v>
+      </c>
+      <c r="AF6">
+        <v>2298</v>
+      </c>
+      <c r="AG6">
+        <f t="shared" ref="AG6:AG22" si="7">AD6-AW6</f>
+        <v>3.078400000000002</v>
+      </c>
+      <c r="AH6">
+        <f t="shared" ref="AH6:AH22" si="8">AE6-AX6</f>
+        <v>-3.2021999999999995E-2</v>
+      </c>
+      <c r="AI6">
+        <f t="shared" ref="AI6:AI22" si="9">AF6-AY6</f>
+        <v>1114</v>
+      </c>
+      <c r="AW6">
         <v>21.686299999999999</v>
       </c>
-      <c r="AW6">
+      <c r="AX6">
         <v>0.12389799999999999</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>1184</v>
       </c>
-      <c r="AY6">
-        <f t="shared" ref="AY6:AY17" si="6">AV6-S6</f>
-        <v>2.1963000000000008</v>
-      </c>
       <c r="AZ6">
-        <f t="shared" ref="AZ6:AZ17" si="7">AW6-T6</f>
-        <v>-3.3902000000000002E-2</v>
+        <f t="shared" ref="AZ6:AZ17" si="10">AW6-BD6</f>
+        <v>0.3882399999999997</v>
       </c>
       <c r="BA6">
-        <f t="shared" ref="BA6:BA17" si="8">AX6-U6</f>
-        <v>266</v>
-      </c>
-      <c r="BC6">
+        <f t="shared" ref="BA6:BA17" si="11">AX6-BE6</f>
+        <v>-2.7019999999999961E-3</v>
+      </c>
+      <c r="BB6">
+        <f t="shared" ref="BB6:BB17" si="12">AY6-BF6</f>
+        <v>-855</v>
+      </c>
+      <c r="BD6">
         <v>21.29806</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <v>0.12659999999999999</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <v>2039</v>
       </c>
-      <c r="BF6">
+      <c r="BG6">
         <f t="shared" si="1"/>
         <v>1.8080600000000011</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <f t="shared" si="2"/>
         <v>-3.1200000000000006E-2</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <f t="shared" si="3"/>
         <v>1121</v>
       </c>
     </row>
-    <row r="7" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -41130,57 +41175,78 @@
         <v>-24.05</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.17219999999999999</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-514</v>
       </c>
-      <c r="AV7">
+      <c r="AD7">
+        <v>25.19595</v>
+      </c>
+      <c r="AE7">
+        <v>0.16868</v>
+      </c>
+      <c r="AF7">
+        <v>630</v>
+      </c>
+      <c r="AG7">
+        <f t="shared" si="7"/>
+        <v>0.74465000000000003</v>
+      </c>
+      <c r="AH7">
+        <f t="shared" si="8"/>
+        <v>-4.156999999999994E-3</v>
+      </c>
+      <c r="AI7">
+        <f t="shared" si="9"/>
+        <v>101</v>
+      </c>
+      <c r="AW7">
         <v>24.4513</v>
       </c>
-      <c r="AW7">
+      <c r="AX7">
         <v>0.17283699999999999</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <v>529</v>
       </c>
-      <c r="AY7">
-        <f t="shared" si="6"/>
-        <v>0.4012999999999991</v>
-      </c>
       <c r="AZ7">
-        <f t="shared" si="7"/>
-        <v>6.3699999999999868E-4</v>
+        <f t="shared" si="10"/>
+        <v>-2.5864000000000011</v>
       </c>
       <c r="BA7">
-        <f t="shared" si="8"/>
-        <v>15</v>
-      </c>
-      <c r="BC7" s="81">
+        <f t="shared" si="11"/>
+        <v>3.7637000000000004E-2</v>
+      </c>
+      <c r="BB7">
+        <f t="shared" si="12"/>
+        <v>-384</v>
+      </c>
+      <c r="BD7" s="81">
         <v>27.037700000000001</v>
       </c>
-      <c r="BD7">
+      <c r="BE7">
         <v>0.13519999999999999</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <v>913</v>
       </c>
-      <c r="BF7">
+      <c r="BG7">
         <f t="shared" si="1"/>
         <v>2.9877000000000002</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <f t="shared" si="2"/>
         <v>-3.7000000000000005E-2</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <f t="shared" si="3"/>
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -41222,48 +41288,69 @@
         <v>-8.4600000000000009</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.2122</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-434</v>
       </c>
-      <c r="AV8">
+      <c r="AD8">
+        <v>12.230399999999999</v>
+      </c>
+      <c r="AE8">
+        <v>0.16598199999999999</v>
+      </c>
+      <c r="AF8">
+        <v>868</v>
+      </c>
+      <c r="AG8">
+        <f>AD8-AW8</f>
+        <v>2.6120000000000001</v>
+      </c>
+      <c r="AH8">
+        <f t="shared" si="8"/>
+        <v>-4.1987999999999998E-2</v>
+      </c>
+      <c r="AI8">
+        <f t="shared" si="9"/>
+        <v>191</v>
+      </c>
+      <c r="AW8">
         <v>9.6183999999999994</v>
       </c>
-      <c r="AW8">
+      <c r="AX8">
         <v>0.20796999999999999</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <v>677</v>
       </c>
-      <c r="AY8">
-        <f t="shared" si="6"/>
-        <v>1.1583999999999985</v>
-      </c>
       <c r="AZ8">
-        <f t="shared" si="7"/>
-        <v>-4.2300000000000115E-3</v>
+        <f t="shared" si="10"/>
+        <v>9.6183999999999994</v>
       </c>
       <c r="BA8">
-        <f t="shared" si="8"/>
-        <v>243</v>
-      </c>
-      <c r="BF8">
+        <f t="shared" si="11"/>
+        <v>0.20796999999999999</v>
+      </c>
+      <c r="BB8">
+        <f t="shared" si="12"/>
+        <v>677</v>
+      </c>
+      <c r="BG8">
         <f t="shared" si="1"/>
         <v>-8.4600000000000009</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <f t="shared" si="2"/>
         <v>-0.2122</v>
       </c>
-      <c r="BH8">
+      <c r="BI8">
         <f t="shared" si="3"/>
         <v>-434</v>
       </c>
     </row>
-    <row r="9" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -41308,57 +41395,78 @@
         <v>2.1599999999999966</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-2.2699999999999998E-2</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>304</v>
       </c>
-      <c r="AV9">
+      <c r="AD9">
+        <v>74.304000000000002</v>
+      </c>
+      <c r="AE9">
+        <v>0.12945000000000001</v>
+      </c>
+      <c r="AF9">
+        <v>2004</v>
+      </c>
+      <c r="AG9">
+        <f t="shared" si="7"/>
+        <v>24.653100000000002</v>
+      </c>
+      <c r="AH9">
+        <f t="shared" si="8"/>
+        <v>-1.3899999999999996E-2</v>
+      </c>
+      <c r="AI9">
+        <f t="shared" si="9"/>
+        <v>248</v>
+      </c>
+      <c r="AW9">
         <v>49.6509</v>
       </c>
-      <c r="AW9">
+      <c r="AX9">
         <v>0.14335000000000001</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <v>1756</v>
       </c>
-      <c r="AY9">
-        <f t="shared" si="6"/>
-        <v>2.9808999999999983</v>
-      </c>
       <c r="AZ9">
-        <f t="shared" si="7"/>
-        <v>-6.5500000000000003E-3</v>
+        <f t="shared" si="10"/>
+        <v>-2.4835800000000035</v>
       </c>
       <c r="BA9">
-        <f t="shared" si="8"/>
-        <v>674</v>
-      </c>
-      <c r="BC9">
+        <f t="shared" si="11"/>
+        <v>6.6100000000000006E-2</v>
+      </c>
+      <c r="BB9">
+        <f t="shared" si="12"/>
+        <v>-793</v>
+      </c>
+      <c r="BD9">
         <v>52.134480000000003</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <v>7.7249999999999999E-2</v>
       </c>
-      <c r="BE9">
+      <c r="BF9">
         <v>2549</v>
       </c>
-      <c r="BF9">
+      <c r="BG9">
         <f t="shared" si="1"/>
         <v>5.4644800000000018</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <f t="shared" si="2"/>
         <v>-7.2650000000000006E-2</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <f t="shared" si="3"/>
         <v>1467</v>
       </c>
     </row>
-    <row r="10" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -41411,48 +41519,69 @@
         <v>-0.12000000000000099</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.4399999999999996E-2</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="AV10">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="AD10">
+        <v>29.107600000000001</v>
+      </c>
+      <c r="AE10">
+        <v>9.0768000000000001E-2</v>
+      </c>
+      <c r="AF10">
+        <v>883</v>
+      </c>
+      <c r="AG10">
+        <f t="shared" si="7"/>
+        <v>8.2198600000000006</v>
+      </c>
+      <c r="AH10">
+        <f t="shared" si="8"/>
+        <v>-1.2492000000000003E-2</v>
+      </c>
+      <c r="AI10">
+        <f t="shared" si="9"/>
+        <v>26</v>
+      </c>
+      <c r="AW10">
         <v>20.887740000000001</v>
       </c>
-      <c r="AW10">
+      <c r="AX10">
         <v>0.10326</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <v>857</v>
       </c>
-      <c r="AY10">
-        <f t="shared" si="6"/>
-        <v>1.9977400000000003</v>
-      </c>
       <c r="AZ10">
-        <f t="shared" si="7"/>
-        <v>-6.7839999999999998E-2</v>
+        <f t="shared" si="10"/>
+        <v>20.887740000000001</v>
       </c>
       <c r="BA10">
-        <f t="shared" si="8"/>
-        <v>229</v>
-      </c>
-      <c r="BF10">
+        <f t="shared" si="11"/>
+        <v>0.10326</v>
+      </c>
+      <c r="BB10">
+        <f t="shared" si="12"/>
+        <v>857</v>
+      </c>
+      <c r="BG10">
         <f t="shared" si="1"/>
         <v>-18.89</v>
       </c>
-      <c r="BG10">
+      <c r="BH10">
         <f t="shared" si="2"/>
         <v>-0.1711</v>
       </c>
-      <c r="BH10">
+      <c r="BI10">
         <f t="shared" si="3"/>
         <v>-628</v>
       </c>
     </row>
-    <row r="11" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -41485,57 +41614,78 @@
         <v>-16.059999999999999</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.1303</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-525</v>
       </c>
-      <c r="AV11">
+      <c r="AD11">
+        <v>20.465959999999999</v>
+      </c>
+      <c r="AE11">
+        <v>9.3369999999999995E-2</v>
+      </c>
+      <c r="AF11">
+        <v>988</v>
+      </c>
+      <c r="AG11">
+        <f t="shared" si="7"/>
+        <v>3.8467199999999977</v>
+      </c>
+      <c r="AH11">
+        <f t="shared" si="8"/>
+        <v>-3.033000000000001E-2</v>
+      </c>
+      <c r="AI11">
+        <f t="shared" si="9"/>
+        <v>446</v>
+      </c>
+      <c r="AW11">
         <v>16.619240000000001</v>
       </c>
-      <c r="AW11">
+      <c r="AX11">
         <v>0.1237</v>
       </c>
-      <c r="AX11">
+      <c r="AY11">
         <v>542</v>
       </c>
-      <c r="AY11">
-        <f t="shared" si="6"/>
-        <v>0.55924000000000262</v>
-      </c>
       <c r="AZ11">
-        <f t="shared" si="7"/>
-        <v>-6.5999999999999948E-3</v>
+        <f t="shared" si="10"/>
+        <v>-2.7645599999999995</v>
       </c>
       <c r="BA11">
-        <f t="shared" si="8"/>
-        <v>17</v>
-      </c>
-      <c r="BC11">
+        <f t="shared" si="11"/>
+        <v>4.224E-2</v>
+      </c>
+      <c r="BB11">
+        <f t="shared" si="12"/>
+        <v>-320</v>
+      </c>
+      <c r="BD11">
         <v>19.383800000000001</v>
       </c>
-      <c r="BD11">
+      <c r="BE11">
         <v>8.1460000000000005E-2</v>
       </c>
-      <c r="BE11">
+      <c r="BF11">
         <v>862</v>
       </c>
-      <c r="BF11">
+      <c r="BG11">
         <f t="shared" si="1"/>
         <v>3.3238000000000021</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <f t="shared" si="2"/>
         <v>-4.8839999999999995E-2</v>
       </c>
-      <c r="BH11">
+      <c r="BI11">
         <f t="shared" si="3"/>
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -41577,39 +41727,51 @@
         <v>-20.85</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.32519999999999999</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-588</v>
       </c>
-      <c r="AY12">
-        <f t="shared" si="6"/>
-        <v>-20.85</v>
+      <c r="AG12">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH12">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI12">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AZ12">
-        <f t="shared" si="7"/>
-        <v>-0.32519999999999999</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="BA12">
-        <f t="shared" si="8"/>
-        <v>-588</v>
-      </c>
-      <c r="BF12">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BB12">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BG12">
         <f t="shared" si="1"/>
         <v>-20.85</v>
       </c>
-      <c r="BG12">
+      <c r="BH12">
         <f t="shared" si="2"/>
         <v>-0.32519999999999999</v>
       </c>
-      <c r="BH12">
+      <c r="BI12">
         <f t="shared" si="3"/>
         <v>-588</v>
       </c>
     </row>
-    <row r="13" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -41661,39 +41823,51 @@
         <v>0.18999999999999773</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>1.5899999999999984E-2</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>21</v>
       </c>
-      <c r="AY13">
-        <f t="shared" si="6"/>
-        <v>-33.68</v>
+      <c r="AG13">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH13">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI13">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AZ13">
-        <f t="shared" si="7"/>
-        <v>-0.11020000000000001</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="BA13">
-        <f t="shared" si="8"/>
-        <v>-778</v>
-      </c>
-      <c r="BF13">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BB13">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BG13">
         <f t="shared" si="1"/>
         <v>-33.68</v>
       </c>
-      <c r="BG13">
+      <c r="BH13">
         <f t="shared" si="2"/>
         <v>-0.11020000000000001</v>
       </c>
-      <c r="BH13">
+      <c r="BI13">
         <f t="shared" si="3"/>
         <v>-778</v>
       </c>
     </row>
-    <row r="14" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -41726,57 +41900,78 @@
         <v>-13.17</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.2238</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-514</v>
       </c>
-      <c r="AV14">
+      <c r="AD14">
+        <v>18.104900000000001</v>
+      </c>
+      <c r="AE14">
+        <v>0.12770000000000001</v>
+      </c>
+      <c r="AF14">
+        <v>1064</v>
+      </c>
+      <c r="AG14">
+        <f t="shared" si="7"/>
+        <v>4.7050000000000001</v>
+      </c>
+      <c r="AH14">
+        <f t="shared" si="8"/>
+        <v>-8.7299999999999989E-2</v>
+      </c>
+      <c r="AI14">
+        <f t="shared" si="9"/>
+        <v>537</v>
+      </c>
+      <c r="AW14">
         <v>13.399900000000001</v>
       </c>
-      <c r="AW14">
+      <c r="AX14">
         <v>0.215</v>
       </c>
-      <c r="AX14">
+      <c r="AY14">
         <v>527</v>
       </c>
-      <c r="AY14">
-        <f t="shared" si="6"/>
-        <v>0.22990000000000066</v>
-      </c>
       <c r="AZ14">
-        <f t="shared" si="7"/>
-        <v>-8.8000000000000023E-3</v>
+        <f t="shared" si="10"/>
+        <v>-0.30439999999999934</v>
       </c>
       <c r="BA14">
-        <f t="shared" si="8"/>
-        <v>13</v>
-      </c>
-      <c r="BC14">
+        <f t="shared" si="11"/>
+        <v>4.0199999999999986E-2</v>
+      </c>
+      <c r="BB14">
+        <f t="shared" si="12"/>
+        <v>-495</v>
+      </c>
+      <c r="BD14">
         <v>13.7043</v>
       </c>
-      <c r="BD14">
+      <c r="BE14">
         <v>0.17480000000000001</v>
       </c>
-      <c r="BE14">
+      <c r="BF14">
         <v>1022</v>
       </c>
-      <c r="BF14">
+      <c r="BG14">
         <f t="shared" si="1"/>
         <v>0.5343</v>
       </c>
-      <c r="BG14">
+      <c r="BH14">
         <f t="shared" si="2"/>
         <v>-4.8999999999999988E-2</v>
       </c>
-      <c r="BH14">
+      <c r="BI14">
         <f t="shared" si="3"/>
         <v>508</v>
       </c>
     </row>
-    <row r="15" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -41818,39 +42013,51 @@
         <v>-19.57</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.23630000000000001</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-663</v>
       </c>
-      <c r="AY15">
-        <f t="shared" si="6"/>
-        <v>-19.57</v>
+      <c r="AG15">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH15">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI15">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AZ15">
-        <f t="shared" si="7"/>
-        <v>-0.23630000000000001</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="BA15">
-        <f t="shared" si="8"/>
-        <v>-663</v>
-      </c>
-      <c r="BF15">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BB15">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BG15">
         <f t="shared" si="1"/>
         <v>-19.57</v>
       </c>
-      <c r="BG15">
+      <c r="BH15">
         <f t="shared" si="2"/>
         <v>-0.23630000000000001</v>
       </c>
-      <c r="BH15">
+      <c r="BI15">
         <f t="shared" si="3"/>
         <v>-663</v>
       </c>
     </row>
-    <row r="16" spans="1:66" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:67" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -41883,48 +42090,60 @@
         <v>-52.53</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-4.9299999999999997E-2</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-716</v>
       </c>
-      <c r="AY16">
-        <f t="shared" si="6"/>
-        <v>-52.53</v>
+      <c r="AG16">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH16">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI16">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AZ16">
-        <f t="shared" si="7"/>
-        <v>-4.9299999999999997E-2</v>
+        <f t="shared" si="10"/>
+        <v>-53.034950000000002</v>
       </c>
       <c r="BA16">
-        <f t="shared" si="8"/>
-        <v>-716</v>
-      </c>
-      <c r="BC16">
+        <f t="shared" si="11"/>
+        <v>-5.9695999999999999E-2</v>
+      </c>
+      <c r="BB16">
+        <f t="shared" si="12"/>
+        <v>-1133</v>
+      </c>
+      <c r="BD16">
         <v>53.034950000000002</v>
       </c>
-      <c r="BD16">
+      <c r="BE16">
         <v>5.9695999999999999E-2</v>
       </c>
-      <c r="BE16">
+      <c r="BF16">
         <v>1133</v>
       </c>
-      <c r="BF16">
+      <c r="BG16">
         <f t="shared" si="1"/>
         <v>0.5049500000000009</v>
       </c>
-      <c r="BG16">
+      <c r="BH16">
         <f t="shared" si="2"/>
         <v>1.0396000000000002E-2</v>
       </c>
-      <c r="BH16">
+      <c r="BI16">
         <f t="shared" si="3"/>
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -41975,39 +42194,51 @@
         <v>1.9199999999999982</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-1.0000000000000009E-3</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>57</v>
       </c>
-      <c r="AY17">
-        <f t="shared" si="6"/>
-        <v>-31.77</v>
+      <c r="AG17">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH17">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI17">
+        <f t="shared" si="9"/>
+        <v>0</v>
       </c>
       <c r="AZ17">
-        <f t="shared" si="7"/>
-        <v>-0.2361</v>
+        <f t="shared" si="10"/>
+        <v>0</v>
       </c>
       <c r="BA17">
-        <f t="shared" si="8"/>
-        <v>-231</v>
-      </c>
-      <c r="BF17">
+        <f t="shared" si="11"/>
+        <v>0</v>
+      </c>
+      <c r="BB17">
+        <f t="shared" si="12"/>
+        <v>0</v>
+      </c>
+      <c r="BG17">
         <f t="shared" si="1"/>
         <v>-31.77</v>
       </c>
-      <c r="BG17">
+      <c r="BH17">
         <f t="shared" si="2"/>
         <v>-0.2361</v>
       </c>
-      <c r="BH17">
+      <c r="BI17">
         <f t="shared" si="3"/>
         <v>-231</v>
       </c>
     </row>
-    <row r="18" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -42058,27 +42289,39 @@
         <v>0.1899999999999995</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.0599999999999988E-2</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>40</v>
       </c>
-      <c r="BF18">
+      <c r="AG18">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH18">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI18">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="BG18">
         <f t="shared" si="1"/>
         <v>-13.96</v>
       </c>
-      <c r="BG18">
+      <c r="BH18">
         <f t="shared" si="2"/>
         <v>-0.1061</v>
       </c>
-      <c r="BH18">
+      <c r="BI18">
         <f t="shared" si="3"/>
         <v>-343</v>
       </c>
     </row>
-    <row r="19" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -42121,27 +42364,39 @@
         <v>-22.79</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.28999999999999998</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-320</v>
       </c>
-      <c r="BF19">
+      <c r="AG19">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH19">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI19">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="BG19">
         <f t="shared" si="1"/>
         <v>-22.79</v>
       </c>
-      <c r="BG19">
+      <c r="BH19">
         <f t="shared" si="2"/>
         <v>-0.28999999999999998</v>
       </c>
-      <c r="BH19">
+      <c r="BI19">
         <f t="shared" si="3"/>
         <v>-320</v>
       </c>
     </row>
-    <row r="20" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -42174,36 +42429,48 @@
         <v>-63.69</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.1002</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-283</v>
       </c>
-      <c r="BC20">
+      <c r="AG20">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH20">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI20">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="BD20">
         <v>68.383750000000006</v>
       </c>
-      <c r="BD20">
+      <c r="BE20">
         <v>0.11585139999999999</v>
       </c>
-      <c r="BE20">
+      <c r="BF20">
         <v>454</v>
       </c>
-      <c r="BF20">
+      <c r="BG20">
         <f t="shared" si="1"/>
         <v>4.6937500000000085</v>
       </c>
-      <c r="BG20">
+      <c r="BH20">
         <f t="shared" si="2"/>
         <v>1.5651399999999996E-2</v>
       </c>
-      <c r="BH20">
+      <c r="BI20">
         <f t="shared" si="3"/>
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -42257,27 +42524,39 @@
         <v>1.1120000000000001</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>0.06</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>106</v>
       </c>
-      <c r="BF21">
+      <c r="AG21">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH21">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI21">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="BG21">
         <f t="shared" si="1"/>
         <v>-11.31</v>
       </c>
-      <c r="BG21">
+      <c r="BH21">
         <f t="shared" si="2"/>
         <v>-0.11219999999999999</v>
       </c>
-      <c r="BH21">
+      <c r="BI21">
         <f t="shared" si="3"/>
         <v>-646</v>
       </c>
     </row>
-    <row r="22" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -42319,27 +42598,39 @@
         <v>-10.199999999999999</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.37130000000000002</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-236</v>
       </c>
-      <c r="BF22">
+      <c r="AG22">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="AH22">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AI22">
+        <f t="shared" si="9"/>
+        <v>0</v>
+      </c>
+      <c r="BG22">
         <f t="shared" si="1"/>
         <v>-10.199999999999999</v>
       </c>
-      <c r="BG22">
+      <c r="BH22">
         <f t="shared" si="2"/>
         <v>-0.37130000000000002</v>
       </c>
-      <c r="BH22">
+      <c r="BI22">
         <f t="shared" si="3"/>
         <v>-236</v>
       </c>
     </row>
-    <row r="23" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -42372,36 +42663,36 @@
         <v>-14.93</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.1002</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-323</v>
       </c>
-      <c r="BC23">
+      <c r="BD23">
         <v>15.04355</v>
       </c>
-      <c r="BD23">
+      <c r="BE23">
         <v>9.3257999999999994E-2</v>
       </c>
-      <c r="BE23">
+      <c r="BF23">
         <v>829</v>
       </c>
-      <c r="BF23">
+      <c r="BG23">
         <f t="shared" si="1"/>
         <v>0.11355000000000004</v>
       </c>
-      <c r="BG23">
+      <c r="BH23">
         <f t="shared" si="2"/>
         <v>-6.9420000000000037E-3</v>
       </c>
-      <c r="BH23">
+      <c r="BI23">
         <f t="shared" si="3"/>
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -42434,36 +42725,36 @@
         <v>-23.49</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.1487</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-283</v>
       </c>
-      <c r="BC24">
+      <c r="BD24">
         <v>21.397960000000001</v>
       </c>
-      <c r="BD24">
+      <c r="BE24">
         <v>0.14054</v>
       </c>
-      <c r="BE24">
+      <c r="BF24">
         <v>602</v>
       </c>
-      <c r="BF24">
+      <c r="BG24">
         <f t="shared" si="1"/>
         <v>-2.0920399999999972</v>
       </c>
-      <c r="BG24">
+      <c r="BH24">
         <f t="shared" si="2"/>
         <v>-8.1600000000000006E-3</v>
       </c>
-      <c r="BH24">
+      <c r="BI24">
         <f t="shared" si="3"/>
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -42515,27 +42806,27 @@
         <v>3.6370000000000005</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>6.0100000000000015E-2</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>82</v>
       </c>
-      <c r="BF25">
+      <c r="BG25">
         <f t="shared" si="1"/>
         <v>-17.02</v>
       </c>
-      <c r="BG25">
+      <c r="BH25">
         <f t="shared" si="2"/>
         <v>-0.21240000000000001</v>
       </c>
-      <c r="BH25">
+      <c r="BI25">
         <f t="shared" si="3"/>
         <v>-204</v>
       </c>
     </row>
-    <row r="26" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -42588,27 +42879,27 @@
         <v>4.0500000000000007</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-9.4700000000000006E-2</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>121</v>
       </c>
-      <c r="BF26">
+      <c r="BG26">
         <f t="shared" si="1"/>
         <v>-10.1</v>
       </c>
-      <c r="BG26">
+      <c r="BH26">
         <f t="shared" si="2"/>
         <v>-0.3599</v>
       </c>
-      <c r="BH26">
+      <c r="BI26">
         <f t="shared" si="3"/>
         <v>-220</v>
       </c>
     </row>
-    <row r="27" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -42660,27 +42951,27 @@
         <v>-2.4648000000000003</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>8.2099999999999951E-2</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>76</v>
       </c>
-      <c r="BF27">
+      <c r="BG27">
         <f t="shared" si="1"/>
         <v>-22.76</v>
       </c>
-      <c r="BG27">
+      <c r="BH27">
         <f t="shared" si="2"/>
         <v>-0.27900000000000003</v>
       </c>
-      <c r="BH27">
+      <c r="BI27">
         <f t="shared" si="3"/>
         <v>-174</v>
       </c>
     </row>
-    <row r="28" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -42733,27 +43024,27 @@
         <v>1.9999999999999574E-2</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-2.0199999999999996E-2</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="BF28">
+      <c r="BG28">
         <f t="shared" si="1"/>
         <v>-30.57</v>
       </c>
-      <c r="BG28">
+      <c r="BH28">
         <f t="shared" si="2"/>
         <v>-0.26269999999999999</v>
       </c>
-      <c r="BH28">
+      <c r="BI28">
         <f t="shared" si="3"/>
         <v>-165</v>
       </c>
     </row>
-    <row r="29" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -42806,27 +43097,27 @@
         <v>1.3628</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-3.7200000000000011E-2</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="BF29">
+      <c r="BG29">
         <f t="shared" si="1"/>
         <v>-19.22</v>
       </c>
-      <c r="BG29">
+      <c r="BH29">
         <f t="shared" si="2"/>
         <v>-0.3029</v>
       </c>
-      <c r="BH29">
+      <c r="BI29">
         <f t="shared" si="3"/>
         <v>-324</v>
       </c>
     </row>
-    <row r="30" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -42879,27 +43170,27 @@
         <v>1.25</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-1.7999999999999995E-2</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>51</v>
       </c>
-      <c r="BF30">
+      <c r="BG30">
         <f t="shared" si="1"/>
         <v>-11.61</v>
       </c>
-      <c r="BG30">
+      <c r="BH30">
         <f t="shared" si="2"/>
         <v>-6.8199999999999997E-2</v>
       </c>
-      <c r="BH30">
+      <c r="BI30">
         <f t="shared" si="3"/>
         <v>-233</v>
       </c>
     </row>
-    <row r="31" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -42950,27 +43241,27 @@
         <v>2.135900000000003</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>2.0100000000000007E-2</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="BF31">
+      <c r="BG31">
         <f t="shared" si="1"/>
         <v>-16.989999999999998</v>
       </c>
-      <c r="BG31">
+      <c r="BH31">
         <f t="shared" si="2"/>
         <v>-0.20349999999999999</v>
       </c>
-      <c r="BH31">
+      <c r="BI31">
         <f t="shared" si="3"/>
         <v>-140</v>
       </c>
     </row>
-    <row r="32" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -43022,27 +43313,27 @@
         <v>0.5</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-1.6900000000000026E-2</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>79</v>
       </c>
-      <c r="BF32">
+      <c r="BG32">
         <f t="shared" si="1"/>
         <v>-14.08</v>
       </c>
-      <c r="BG32">
+      <c r="BH32">
         <f t="shared" si="2"/>
         <v>-0.26400000000000001</v>
       </c>
-      <c r="BH32">
+      <c r="BI32">
         <f t="shared" si="3"/>
         <v>-318</v>
       </c>
     </row>
-    <row r="33" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -43094,27 +43385,27 @@
         <v>-0.16999999999999815</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>3.699999999999995E-3</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="BF33">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="BG33">
         <f t="shared" si="1"/>
         <v>-27.43</v>
       </c>
-      <c r="BG33">
+      <c r="BH33">
         <f t="shared" si="2"/>
         <v>-0.1033</v>
       </c>
-      <c r="BH33">
+      <c r="BI33">
         <f t="shared" si="3"/>
         <v>-477</v>
       </c>
     </row>
-    <row r="34" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -43147,36 +43438,36 @@
         <v>-11.52</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.24110000000000001</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-530</v>
       </c>
-      <c r="BC34">
+      <c r="BD34">
         <v>14.0328</v>
       </c>
-      <c r="BD34">
+      <c r="BE34">
         <v>0.1895</v>
       </c>
-      <c r="BE34">
+      <c r="BF34">
         <v>764</v>
       </c>
-      <c r="BF34">
+      <c r="BG34">
         <f t="shared" si="1"/>
         <v>2.5128000000000004</v>
       </c>
-      <c r="BG34">
+      <c r="BH34">
         <f t="shared" si="2"/>
         <v>-5.1600000000000007E-2</v>
       </c>
-      <c r="BH34">
+      <c r="BI34">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -43209,36 +43500,36 @@
         <v>-8.57</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.2122</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-454</v>
       </c>
-      <c r="BC35">
+      <c r="BD35">
         <v>8.6080649999999999</v>
       </c>
-      <c r="BD35">
+      <c r="BE35">
         <v>0.2099</v>
       </c>
-      <c r="BE35">
+      <c r="BF35">
         <v>477</v>
       </c>
-      <c r="BF35">
+      <c r="BG35">
         <f t="shared" si="1"/>
         <v>3.8064999999999571E-2</v>
       </c>
-      <c r="BG35">
+      <c r="BH35">
         <f t="shared" si="2"/>
         <v>-2.2999999999999965E-3</v>
       </c>
-      <c r="BH35">
+      <c r="BI35">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -43289,27 +43580,27 @@
         <v>1.6099999999999994</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5.8000000000000274E-3</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="BF36">
+      <c r="BG36">
         <f t="shared" si="1"/>
         <v>-26.52</v>
       </c>
-      <c r="BG36">
+      <c r="BH36">
         <f t="shared" si="2"/>
         <v>-0.36399999999999999</v>
       </c>
-      <c r="BH36">
+      <c r="BI36">
         <f t="shared" si="3"/>
         <v>-159</v>
       </c>
     </row>
-    <row r="37" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -43360,27 +43651,27 @@
         <v>1.9170000000000016</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-2.4500000000000008E-2</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>138</v>
       </c>
-      <c r="BF37">
+      <c r="BG37">
         <f t="shared" si="1"/>
         <v>-39.68</v>
       </c>
-      <c r="BG37">
+      <c r="BH37">
         <f t="shared" si="2"/>
         <v>-0.1246</v>
       </c>
-      <c r="BH37">
+      <c r="BI37">
         <f t="shared" si="3"/>
         <v>-250</v>
       </c>
     </row>
-    <row r="38" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -43433,27 +43724,27 @@
         <v>0.44000000000000128</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-1.0900000000000021E-2</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="BF38">
+      <c r="BG38">
         <f t="shared" si="1"/>
         <v>-22.22</v>
       </c>
-      <c r="BG38">
+      <c r="BH38">
         <f t="shared" si="2"/>
         <v>-0.30280000000000001</v>
       </c>
-      <c r="BH38">
+      <c r="BI38">
         <f t="shared" si="3"/>
         <v>-263</v>
       </c>
     </row>
-    <row r="39" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -43504,27 +43795,27 @@
         <v>1.3999999999999346E-2</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>5.8400000000000007E-2</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="BF39">
+      <c r="BG39">
         <f t="shared" si="1"/>
         <v>-26.34</v>
       </c>
-      <c r="BG39">
+      <c r="BH39">
         <f t="shared" si="2"/>
         <v>-0.22470000000000001</v>
       </c>
-      <c r="BH39">
+      <c r="BI39">
         <f t="shared" si="3"/>
         <v>-137</v>
       </c>
     </row>
-    <row r="40" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -43557,36 +43848,36 @@
         <v>-20.14</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.17030000000000001</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-173</v>
       </c>
-      <c r="BC40">
+      <c r="BD40">
         <v>19.668900000000001</v>
       </c>
-      <c r="BD40" s="81">
+      <c r="BE40" s="81">
         <v>0.33239999999999997</v>
       </c>
-      <c r="BE40">
+      <c r="BF40">
         <v>211</v>
       </c>
-      <c r="BF40">
+      <c r="BG40">
         <f t="shared" si="1"/>
         <v>-0.47109999999999985</v>
       </c>
-      <c r="BG40">
+      <c r="BH40">
         <f t="shared" si="2"/>
         <v>0.16209999999999997</v>
       </c>
-      <c r="BH40">
+      <c r="BI40">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -43619,36 +43910,36 @@
         <v>-9.7100000000000009</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.187</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-248</v>
       </c>
-      <c r="BC41">
+      <c r="BD41">
         <v>9.7552000000000003</v>
       </c>
-      <c r="BD41">
+      <c r="BE41">
         <v>0.16739999999999999</v>
       </c>
-      <c r="BE41">
+      <c r="BF41">
         <v>260</v>
       </c>
-      <c r="BF41">
+      <c r="BG41">
         <f t="shared" si="1"/>
         <v>4.5199999999999463E-2</v>
       </c>
-      <c r="BG41">
+      <c r="BH41">
         <f t="shared" si="2"/>
         <v>-1.9600000000000006E-2</v>
       </c>
-      <c r="BH41">
+      <c r="BI41">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -43681,36 +43972,36 @@
         <v>-12.46</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.19750000000000001</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-108</v>
       </c>
-      <c r="BC42">
+      <c r="BD42">
         <v>12.31058</v>
       </c>
-      <c r="BD42">
+      <c r="BE42">
         <v>0.19095999999999999</v>
       </c>
-      <c r="BE42">
+      <c r="BF42">
         <v>115</v>
       </c>
-      <c r="BF42">
+      <c r="BG42">
         <f t="shared" si="1"/>
         <v>-0.149420000000001</v>
       </c>
-      <c r="BG42">
+      <c r="BH42">
         <f t="shared" si="2"/>
         <v>-6.540000000000018E-3</v>
       </c>
-      <c r="BH42">
+      <c r="BI42">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:61" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -43743,36 +44034,36 @@
         <v>-33.28</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="5"/>
         <v>-0.2903</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-117</v>
       </c>
-      <c r="BC43">
+      <c r="BD43">
         <v>41.243749999999999</v>
       </c>
-      <c r="BD43">
+      <c r="BE43">
         <v>0.32723000000000002</v>
       </c>
-      <c r="BE43">
+      <c r="BF43">
         <v>145</v>
       </c>
-      <c r="BF43">
+      <c r="BG43">
         <f t="shared" si="1"/>
         <v>7.9637499999999974</v>
       </c>
-      <c r="BG43">
+      <c r="BH43">
         <f t="shared" si="2"/>
         <v>3.6930000000000018E-2</v>
       </c>
-      <c r="BH43">
+      <c r="BI43">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:60" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:61" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -43781,12 +44072,12 @@
         <f>SUM(AA5,AA9:AA10,AA13,AA17:AA18,AA21,AA25:AA33,AA36:AA39)</f>
         <v>0.1336999999999999</v>
       </c>
-      <c r="BF45">
-        <f>SUM(BF6:BF7,BF9,BF11,BF14,BF16,BF20,BF23:BF24,BF34:BF35,BF40:BF43)</f>
-        <v>27.277845000000013</v>
-      </c>
       <c r="BG45">
         <f>SUM(BG6:BG7,BG9,BG11,BG14,BG16,BG20,BG23:BG24,BG34:BG35,BG40:BG43)</f>
+        <v>27.277845000000013</v>
+      </c>
+      <c r="BH45">
+        <f>SUM(BH6:BH7,BH9,BH11,BH14,BH16,BH20,BH23:BH24,BH34:BH35,BH40:BH43)</f>
         <v>-0.10875460000000006</v>
       </c>
     </row>
@@ -43822,22 +44113,22 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BF5:BF43">
+  <conditionalFormatting sqref="BG5:BG43">
     <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG5:BG43">
+  <conditionalFormatting sqref="BH5:BH43">
     <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BF45:BG45">
+  <conditionalFormatting sqref="BG45:BH45">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH1:BH3 BH5:BH43">
+  <conditionalFormatting sqref="BI1:BI3 BI5:BI43">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Only eliminating very small fish and extreme condition (not 1 std dev)
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="5" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="7" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="Single Variable GAMs" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2277" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="232">
   <si>
     <t>Species</t>
   </si>
@@ -715,13 +715,13 @@
     <t>Rexamine removing outliers: mean instead of 100 before removing 1std dev</t>
   </si>
   <si>
-    <t>Rexamine removing outliers: only remove extreme outliers</t>
-  </si>
-  <si>
     <t>Outliers</t>
   </si>
   <si>
     <t>Use EPU_expanded in survdat file (now 11,500 rows are missing EPU or 6,485/273,626 of final data without outliers):</t>
+  </si>
+  <si>
+    <t>Rexamine removing outliers: only remove extreme outliers ( indwt &lt;0.005, length&lt;0, RelCond &gt;300)</t>
   </si>
 </sst>
 </file>
@@ -2098,24 +2098,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="135">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="133">
     <dxf>
       <fill>
         <patternFill>
@@ -16143,44 +16126,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="134" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="132" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="133" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="131" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="132" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="130" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="131" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="129" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="130" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="128" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="129" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="128" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="127" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="126" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18766,145 +18749,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="124" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="122" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="123" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="121" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="119" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="120" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="118" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="116" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="117" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="115" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="113" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="114" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="112" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="110" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="111" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="109" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="107" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="108" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="106" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="104" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="105" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="103" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="101" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="102" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="100" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="98" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="99" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="97" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="95" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="96" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="94" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="92" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="93" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -20727,168 +20710,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="91" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="89" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17 B38:B119">
-    <cfRule type="cellIs" dxfId="90" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="88" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="86" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="84" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="83" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 J5 J10 J14 J17:J18 J21:J22 J24:J25 J27:J29">
-    <cfRule type="cellIs" dxfId="84" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="82" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="81" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31 L5 L10 L14 L17:L18 L21:L22 L27:L29 L24:L25">
-    <cfRule type="cellIs" dxfId="82" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="80" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L4 L6:L9 L11:L13 L15:L16 L19:L20 L23 L30:L31 L26">
-    <cfRule type="cellIs" dxfId="81" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="79" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="78" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="79" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="77" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="78" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="75" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26 P4:P9 P11 P13:P15 P19:P21 P24 P30">
-    <cfRule type="cellIs" dxfId="76" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="74" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P31 P18 P10 P12 P16 P22:P23 P25:P26">
-    <cfRule type="cellIs" dxfId="75" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="72" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="73" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="71" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="72" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13 R10 R12 R16:R18 R22:R23 R25:R29 R31 R3">
-    <cfRule type="cellIs" dxfId="70" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="68" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2 R19:R21 R6:R9 R11 R13 R24 R30 R4">
-    <cfRule type="cellIs" dxfId="69" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="68" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="67" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="65" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="66" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="63" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="64" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="62" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="63" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="62" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="61" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="59" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="60" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119 B31:B37">
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="56" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="57" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="55" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="56" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="54" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="55" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="53" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 J3:J4 J6:J9 J11:J13 J15:J16 J19:J20 J23 J26 J30:J31">
-    <cfRule type="cellIs" dxfId="54" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="52" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29107,87 +29090,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="53" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="51" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="52" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="50" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="48" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="49" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="47" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="48" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="46" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="44" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="45" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="43" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="43" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="41" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="40" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="41" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="39" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="37" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="38" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="34" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="35" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="33" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33210,67 +33193,67 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="34" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="32" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="30" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="31" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="29" priority="12" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="30" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="28" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="26" priority="8" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="26" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="24" priority="7" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ4:BJ27">
-    <cfRule type="cellIs" dxfId="25" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="23" priority="6" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BH27">
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="23" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ28:BJ32">
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="20" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB28:BH32">
-    <cfRule type="cellIs" dxfId="21" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -39189,28 +39172,28 @@
     <sortCondition ref="I2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="19" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="16" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="15" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="16" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="15" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40586,19 +40569,19 @@
     <mergeCell ref="AD2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
-    <cfRule type="cellIs" dxfId="13" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="11" priority="1" operator="lessThan">
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="2" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="9" priority="3" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="7" priority="5" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -40609,10 +40592,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BO45"/>
+  <dimension ref="A1:BP45"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AK2" sqref="AK2"/>
+      <selection activeCell="AO6" sqref="AO6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40631,7 +40614,7 @@
     <col min="23" max="25" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:68" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40660,12 +40643,12 @@
       <c r="W1" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="AW1" t="s">
+      <c r="AX1" t="s">
         <v>224</v>
       </c>
-      <c r="BI1"/>
-    </row>
-    <row r="2" spans="1:67" x14ac:dyDescent="0.35">
+      <c r="BJ1"/>
+    </row>
+    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
@@ -40673,19 +40656,19 @@
         <v>228</v>
       </c>
       <c r="AK2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AQ2" t="s">
+        <v>231</v>
+      </c>
+      <c r="AR2" t="s">
         <v>227</v>
       </c>
-      <c r="AW2" t="s">
-        <v>231</v>
-      </c>
-      <c r="BD2" t="s">
+      <c r="AX2" t="s">
+        <v>230</v>
+      </c>
+      <c r="BE2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:67" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:68" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="95" t="s">
         <v>178</v>
       </c>
@@ -40723,26 +40706,26 @@
         <v>217</v>
       </c>
       <c r="AD3" s="75" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="AK3" s="75" t="s">
-        <v>230</v>
-      </c>
-      <c r="AQ3" s="75" t="s">
+        <v>229</v>
+      </c>
+      <c r="AR3" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="AW3" s="75" t="s">
+      <c r="AX3" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="BD3" s="75" t="s">
+      <c r="BE3" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="BI3"/>
-      <c r="BK3" s="75" t="s">
+      <c r="BJ3"/>
+      <c r="BL3" s="75" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:67" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:68" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40854,74 +40837,77 @@
       <c r="AO4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="AQ4" s="69" t="s">
+      <c r="AP4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="AR4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AR4" s="69" t="s">
+      <c r="AS4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AS4" s="69" t="s">
+      <c r="AT4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AT4" s="69" t="s">
+      <c r="AU4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="AU4" s="69" t="s">
+      <c r="AV4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="AW4" s="69" t="s">
+      <c r="AX4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AX4" s="69" t="s">
+      <c r="AY4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AY4" s="69" t="s">
+      <c r="AZ4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AZ4" s="69" t="s">
+      <c r="BA4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BA4" s="69" t="s">
+      <c r="BB4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="BB4" s="69" t="s">
+      <c r="BC4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="BD4" s="69" t="s">
+      <c r="BE4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BE4" s="69" t="s">
+      <c r="BF4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BF4" s="69" t="s">
+      <c r="BG4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BG4" s="69" t="s">
+      <c r="BH4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BH4" s="69" t="s">
+      <c r="BI4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="BI4" s="69" t="s">
+      <c r="BJ4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="BK4" s="69" t="s">
+      <c r="BL4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BL4" s="69" t="s">
+      <c r="BM4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BM4" s="69" t="s">
+      <c r="BN4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BN4" s="69" t="s">
+      <c r="BO4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BO4" s="69" t="s">
+      <c r="BP4" s="69" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -40992,52 +40978,73 @@
         <v>1149</v>
       </c>
       <c r="AG5">
-        <f>AD5-AW5</f>
+        <f>AD5-AX5</f>
         <v>6.3363000000000014</v>
       </c>
       <c r="AH5">
-        <f t="shared" ref="AH5:AI5" si="0">AE5-AX5</f>
+        <f>AE5-AY5</f>
         <v>-6.7799999999999985E-2</v>
       </c>
       <c r="AI5">
+        <f>AF5-AZ5</f>
+        <v>585</v>
+      </c>
+      <c r="AK5">
+        <v>113.81780000000001</v>
+      </c>
+      <c r="AL5">
+        <v>0.115518</v>
+      </c>
+      <c r="AM5">
+        <v>1259</v>
+      </c>
+      <c r="AN5">
+        <f>AK5-AD5</f>
+        <v>85.654899999999998</v>
+      </c>
+      <c r="AO5">
+        <f t="shared" ref="AO5:AP5" si="0">AL5-AE5</f>
+        <v>2.471799999999999E-2</v>
+      </c>
+      <c r="AP5">
         <f t="shared" si="0"/>
-        <v>585</v>
-      </c>
-      <c r="AW5">
+        <v>110</v>
+      </c>
+      <c r="AX5">
         <v>21.826599999999999</v>
       </c>
-      <c r="AX5">
+      <c r="AY5">
         <v>0.15859999999999999</v>
       </c>
-      <c r="AY5">
+      <c r="AZ5">
         <v>564</v>
-      </c>
-      <c r="AZ5">
-        <f>AW5-BD5</f>
-        <v>21.826599999999999</v>
       </c>
       <c r="BA5">
         <f>AX5-BE5</f>
-        <v>0.15859999999999999</v>
+        <v>21.826599999999999</v>
       </c>
       <c r="BB5">
         <f>AY5-BF5</f>
+        <v>0.15859999999999999</v>
+      </c>
+      <c r="BC5">
+        <f>AZ5-BG5</f>
         <v>564</v>
       </c>
-      <c r="BG5">
-        <f t="shared" ref="BG5:BG43" si="1">BD5-S5</f>
+      <c r="BH5">
+        <f t="shared" ref="BH5:BH43" si="1">BE5-S5</f>
         <v>-23.66</v>
       </c>
-      <c r="BH5">
-        <f t="shared" ref="BH5:BH43" si="2">BE5-T5</f>
+      <c r="BI5">
+        <f t="shared" ref="BI5:BI43" si="2">BF5-T5</f>
         <v>-6.7900000000000002E-2</v>
       </c>
-      <c r="BI5">
-        <f t="shared" ref="BI5:BI43" si="3">BF5-U5</f>
+      <c r="BJ5">
+        <f t="shared" ref="BJ5:BJ43" si="3">BG5-U5</f>
         <v>-722</v>
       </c>
     </row>
-    <row r="6" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -41088,61 +41095,82 @@
         <v>2298</v>
       </c>
       <c r="AG6">
-        <f t="shared" ref="AG6:AG22" si="7">AD6-AW6</f>
+        <f>AD6-AX6</f>
         <v>3.078400000000002</v>
       </c>
       <c r="AH6">
-        <f t="shared" ref="AH6:AH22" si="8">AE6-AX6</f>
+        <f t="shared" ref="AH6:AH22" si="7">AE6-AY6</f>
         <v>-3.2021999999999995E-2</v>
       </c>
       <c r="AI6">
-        <f t="shared" ref="AI6:AI22" si="9">AF6-AY6</f>
+        <f t="shared" ref="AI6:AI22" si="8">AF6-AZ6</f>
         <v>1114</v>
       </c>
-      <c r="AW6">
+      <c r="AK6">
+        <v>99.863500000000002</v>
+      </c>
+      <c r="AL6">
+        <v>9.5115000000000005E-2</v>
+      </c>
+      <c r="AM6">
+        <v>2448</v>
+      </c>
+      <c r="AN6">
+        <f t="shared" ref="AN6:AN9" si="9">AK6-AD6</f>
+        <v>75.098799999999997</v>
+      </c>
+      <c r="AO6">
+        <f t="shared" ref="AO6:AO9" si="10">AL6-AE6</f>
+        <v>3.2390000000000058E-3</v>
+      </c>
+      <c r="AP6">
+        <f t="shared" ref="AP6:AP9" si="11">AM6-AF6</f>
+        <v>150</v>
+      </c>
+      <c r="AX6">
         <v>21.686299999999999</v>
       </c>
-      <c r="AX6">
+      <c r="AY6">
         <v>0.12389799999999999</v>
       </c>
-      <c r="AY6">
+      <c r="AZ6">
         <v>1184</v>
       </c>
-      <c r="AZ6">
-        <f t="shared" ref="AZ6:AZ17" si="10">AW6-BD6</f>
+      <c r="BA6">
+        <f t="shared" ref="BA6:BA17" si="12">AX6-BE6</f>
         <v>0.3882399999999997</v>
       </c>
-      <c r="BA6">
-        <f t="shared" ref="BA6:BA17" si="11">AX6-BE6</f>
+      <c r="BB6">
+        <f t="shared" ref="BB6:BB17" si="13">AY6-BF6</f>
         <v>-2.7019999999999961E-3</v>
       </c>
-      <c r="BB6">
-        <f t="shared" ref="BB6:BB17" si="12">AY6-BF6</f>
+      <c r="BC6">
+        <f t="shared" ref="BC6:BC17" si="14">AZ6-BG6</f>
         <v>-855</v>
       </c>
-      <c r="BD6">
+      <c r="BE6">
         <v>21.29806</v>
       </c>
-      <c r="BE6">
+      <c r="BF6">
         <v>0.12659999999999999</v>
       </c>
-      <c r="BF6">
+      <c r="BG6">
         <v>2039</v>
       </c>
-      <c r="BG6">
+      <c r="BH6">
         <f t="shared" si="1"/>
         <v>1.8080600000000011</v>
       </c>
-      <c r="BH6">
+      <c r="BI6">
         <f t="shared" si="2"/>
         <v>-3.1200000000000006E-2</v>
       </c>
-      <c r="BI6">
+      <c r="BJ6">
         <f t="shared" si="3"/>
         <v>1121</v>
       </c>
     </row>
-    <row r="7" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -41192,61 +41220,82 @@
         <v>630</v>
       </c>
       <c r="AG7">
+        <f>AD7-AX7</f>
+        <v>0.74465000000000003</v>
+      </c>
+      <c r="AH7">
         <f t="shared" si="7"/>
-        <v>0.74465000000000003</v>
-      </c>
-      <c r="AH7">
+        <v>-4.156999999999994E-3</v>
+      </c>
+      <c r="AI7">
         <f t="shared" si="8"/>
-        <v>-4.156999999999994E-3</v>
-      </c>
-      <c r="AI7">
+        <v>101</v>
+      </c>
+      <c r="AK7">
+        <v>81.785700000000006</v>
+      </c>
+      <c r="AL7">
+        <v>0.30153999999999997</v>
+      </c>
+      <c r="AM7">
+        <v>716</v>
+      </c>
+      <c r="AN7">
         <f t="shared" si="9"/>
-        <v>101</v>
-      </c>
-      <c r="AW7">
+        <v>56.589750000000009</v>
+      </c>
+      <c r="AO7">
+        <f t="shared" si="10"/>
+        <v>0.13285999999999998</v>
+      </c>
+      <c r="AP7">
+        <f t="shared" si="11"/>
+        <v>86</v>
+      </c>
+      <c r="AX7">
         <v>24.4513</v>
       </c>
-      <c r="AX7">
+      <c r="AY7">
         <v>0.17283699999999999</v>
       </c>
-      <c r="AY7">
+      <c r="AZ7">
         <v>529</v>
       </c>
-      <c r="AZ7">
-        <f t="shared" si="10"/>
+      <c r="BA7">
+        <f t="shared" si="12"/>
         <v>-2.5864000000000011</v>
       </c>
-      <c r="BA7">
-        <f t="shared" si="11"/>
+      <c r="BB7">
+        <f t="shared" si="13"/>
         <v>3.7637000000000004E-2</v>
       </c>
-      <c r="BB7">
-        <f t="shared" si="12"/>
+      <c r="BC7">
+        <f t="shared" si="14"/>
         <v>-384</v>
       </c>
-      <c r="BD7" s="81">
+      <c r="BE7" s="81">
         <v>27.037700000000001</v>
       </c>
-      <c r="BE7">
+      <c r="BF7">
         <v>0.13519999999999999</v>
       </c>
-      <c r="BF7">
+      <c r="BG7">
         <v>913</v>
       </c>
-      <c r="BG7">
+      <c r="BH7">
         <f t="shared" si="1"/>
         <v>2.9877000000000002</v>
       </c>
-      <c r="BH7">
+      <c r="BI7">
         <f t="shared" si="2"/>
         <v>-3.7000000000000005E-2</v>
       </c>
-      <c r="BI7">
+      <c r="BJ7">
         <f t="shared" si="3"/>
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -41305,52 +41354,73 @@
         <v>868</v>
       </c>
       <c r="AG8">
-        <f>AD8-AW8</f>
+        <f>AD8-AX8</f>
         <v>2.6120000000000001</v>
       </c>
       <c r="AH8">
+        <f t="shared" si="7"/>
+        <v>-4.1987999999999998E-2</v>
+      </c>
+      <c r="AI8">
         <f t="shared" si="8"/>
-        <v>-4.1987999999999998E-2</v>
-      </c>
-      <c r="AI8">
+        <v>191</v>
+      </c>
+      <c r="AK8">
+        <v>41.561320000000002</v>
+      </c>
+      <c r="AL8">
+        <v>0.2364</v>
+      </c>
+      <c r="AM8">
+        <v>929</v>
+      </c>
+      <c r="AN8">
         <f t="shared" si="9"/>
-        <v>191</v>
-      </c>
-      <c r="AW8">
+        <v>29.330920000000003</v>
+      </c>
+      <c r="AO8">
+        <f t="shared" si="10"/>
+        <v>7.0418000000000008E-2</v>
+      </c>
+      <c r="AP8">
+        <f t="shared" si="11"/>
+        <v>61</v>
+      </c>
+      <c r="AX8">
         <v>9.6183999999999994</v>
       </c>
-      <c r="AX8">
+      <c r="AY8">
         <v>0.20796999999999999</v>
       </c>
-      <c r="AY8">
+      <c r="AZ8">
         <v>677</v>
       </c>
-      <c r="AZ8">
-        <f t="shared" si="10"/>
+      <c r="BA8">
+        <f t="shared" si="12"/>
         <v>9.6183999999999994</v>
       </c>
-      <c r="BA8">
-        <f t="shared" si="11"/>
+      <c r="BB8">
+        <f t="shared" si="13"/>
         <v>0.20796999999999999</v>
       </c>
-      <c r="BB8">
-        <f t="shared" si="12"/>
+      <c r="BC8">
+        <f t="shared" si="14"/>
         <v>677</v>
       </c>
-      <c r="BG8">
+      <c r="BH8">
         <f t="shared" si="1"/>
         <v>-8.4600000000000009</v>
       </c>
-      <c r="BH8">
+      <c r="BI8">
         <f t="shared" si="2"/>
         <v>-0.2122</v>
       </c>
-      <c r="BI8">
+      <c r="BJ8">
         <f t="shared" si="3"/>
         <v>-434</v>
       </c>
     </row>
-    <row r="9" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -41412,61 +41482,82 @@
         <v>2004</v>
       </c>
       <c r="AG9">
+        <f>AD9-AX9</f>
+        <v>24.653100000000002</v>
+      </c>
+      <c r="AH9">
         <f t="shared" si="7"/>
-        <v>24.653100000000002</v>
-      </c>
-      <c r="AH9">
+        <v>-1.3899999999999996E-2</v>
+      </c>
+      <c r="AI9">
         <f t="shared" si="8"/>
-        <v>-1.3899999999999996E-2</v>
-      </c>
-      <c r="AI9">
+        <v>248</v>
+      </c>
+      <c r="AK9">
+        <v>185.83799999999999</v>
+      </c>
+      <c r="AL9">
+        <v>0.21282999999999999</v>
+      </c>
+      <c r="AM9">
+        <v>2228</v>
+      </c>
+      <c r="AN9">
         <f t="shared" si="9"/>
-        <v>248</v>
-      </c>
-      <c r="AW9">
+        <v>111.53399999999999</v>
+      </c>
+      <c r="AO9">
+        <f t="shared" si="10"/>
+        <v>8.3379999999999982E-2</v>
+      </c>
+      <c r="AP9">
+        <f t="shared" si="11"/>
+        <v>224</v>
+      </c>
+      <c r="AX9">
         <v>49.6509</v>
       </c>
-      <c r="AX9">
+      <c r="AY9">
         <v>0.14335000000000001</v>
       </c>
-      <c r="AY9">
+      <c r="AZ9">
         <v>1756</v>
       </c>
-      <c r="AZ9">
-        <f t="shared" si="10"/>
+      <c r="BA9">
+        <f t="shared" si="12"/>
         <v>-2.4835800000000035</v>
       </c>
-      <c r="BA9">
-        <f t="shared" si="11"/>
+      <c r="BB9">
+        <f t="shared" si="13"/>
         <v>6.6100000000000006E-2</v>
       </c>
-      <c r="BB9">
-        <f t="shared" si="12"/>
+      <c r="BC9">
+        <f t="shared" si="14"/>
         <v>-793</v>
       </c>
-      <c r="BD9">
+      <c r="BE9">
         <v>52.134480000000003</v>
       </c>
-      <c r="BE9">
+      <c r="BF9">
         <v>7.7249999999999999E-2</v>
       </c>
-      <c r="BF9">
+      <c r="BG9">
         <v>2549</v>
       </c>
-      <c r="BG9">
+      <c r="BH9">
         <f t="shared" si="1"/>
         <v>5.4644800000000018</v>
       </c>
-      <c r="BH9">
+      <c r="BI9">
         <f t="shared" si="2"/>
         <v>-7.2650000000000006E-2</v>
       </c>
-      <c r="BI9">
+      <c r="BJ9">
         <f t="shared" si="3"/>
         <v>1467</v>
       </c>
     </row>
-    <row r="10" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -41536,52 +41627,73 @@
         <v>883</v>
       </c>
       <c r="AG10">
+        <f>AD10-AX10</f>
+        <v>8.2198600000000006</v>
+      </c>
+      <c r="AH10">
         <f t="shared" si="7"/>
-        <v>8.2198600000000006</v>
-      </c>
-      <c r="AH10">
+        <v>-1.2492000000000003E-2</v>
+      </c>
+      <c r="AI10">
         <f t="shared" si="8"/>
-        <v>-1.2492000000000003E-2</v>
-      </c>
-      <c r="AI10">
-        <f t="shared" si="9"/>
         <v>26</v>
       </c>
-      <c r="AW10">
+      <c r="AK10">
+        <v>72.706999999999994</v>
+      </c>
+      <c r="AL10">
+        <v>0.21526000000000001</v>
+      </c>
+      <c r="AM10">
+        <v>1015</v>
+      </c>
+      <c r="AN10">
+        <f t="shared" ref="AN10:AN13" si="15">AK10-AD10</f>
+        <v>43.599399999999989</v>
+      </c>
+      <c r="AO10">
+        <f t="shared" ref="AO10:AO13" si="16">AL10-AE10</f>
+        <v>0.12449200000000001</v>
+      </c>
+      <c r="AP10">
+        <f t="shared" ref="AP10:AP13" si="17">AM10-AF10</f>
+        <v>132</v>
+      </c>
+      <c r="AX10">
         <v>20.887740000000001</v>
       </c>
-      <c r="AX10">
+      <c r="AY10">
         <v>0.10326</v>
       </c>
-      <c r="AY10">
+      <c r="AZ10">
         <v>857</v>
       </c>
-      <c r="AZ10">
-        <f t="shared" si="10"/>
+      <c r="BA10">
+        <f t="shared" si="12"/>
         <v>20.887740000000001</v>
       </c>
-      <c r="BA10">
-        <f t="shared" si="11"/>
+      <c r="BB10">
+        <f t="shared" si="13"/>
         <v>0.10326</v>
       </c>
-      <c r="BB10">
-        <f t="shared" si="12"/>
+      <c r="BC10">
+        <f t="shared" si="14"/>
         <v>857</v>
       </c>
-      <c r="BG10">
+      <c r="BH10">
         <f t="shared" si="1"/>
         <v>-18.89</v>
       </c>
-      <c r="BH10">
+      <c r="BI10">
         <f t="shared" si="2"/>
         <v>-0.1711</v>
       </c>
-      <c r="BI10">
+      <c r="BJ10">
         <f t="shared" si="3"/>
         <v>-628</v>
       </c>
     </row>
-    <row r="11" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -41631,61 +41743,82 @@
         <v>988</v>
       </c>
       <c r="AG11">
+        <f>AD11-AX11</f>
+        <v>3.8467199999999977</v>
+      </c>
+      <c r="AH11">
         <f t="shared" si="7"/>
-        <v>3.8467199999999977</v>
-      </c>
-      <c r="AH11">
+        <v>-3.033000000000001E-2</v>
+      </c>
+      <c r="AI11">
         <f t="shared" si="8"/>
-        <v>-3.033000000000001E-2</v>
-      </c>
-      <c r="AI11">
-        <f t="shared" si="9"/>
         <v>446</v>
       </c>
-      <c r="AW11">
+      <c r="AK11">
+        <v>68.496600000000001</v>
+      </c>
+      <c r="AL11">
+        <v>0.16120000000000001</v>
+      </c>
+      <c r="AM11">
+        <v>1133</v>
+      </c>
+      <c r="AN11">
+        <f t="shared" si="15"/>
+        <v>48.030640000000005</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="16"/>
+        <v>6.7830000000000015E-2</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" si="17"/>
+        <v>145</v>
+      </c>
+      <c r="AX11">
         <v>16.619240000000001</v>
       </c>
-      <c r="AX11">
+      <c r="AY11">
         <v>0.1237</v>
       </c>
-      <c r="AY11">
+      <c r="AZ11">
         <v>542</v>
       </c>
-      <c r="AZ11">
-        <f t="shared" si="10"/>
+      <c r="BA11">
+        <f t="shared" si="12"/>
         <v>-2.7645599999999995</v>
       </c>
-      <c r="BA11">
-        <f t="shared" si="11"/>
+      <c r="BB11">
+        <f t="shared" si="13"/>
         <v>4.224E-2</v>
       </c>
-      <c r="BB11">
-        <f t="shared" si="12"/>
+      <c r="BC11">
+        <f t="shared" si="14"/>
         <v>-320</v>
       </c>
-      <c r="BD11">
+      <c r="BE11">
         <v>19.383800000000001</v>
       </c>
-      <c r="BE11">
+      <c r="BF11">
         <v>8.1460000000000005E-2</v>
       </c>
-      <c r="BF11">
+      <c r="BG11">
         <v>862</v>
       </c>
-      <c r="BG11">
+      <c r="BH11">
         <f t="shared" si="1"/>
         <v>3.3238000000000021</v>
       </c>
-      <c r="BH11">
+      <c r="BI11">
         <f t="shared" si="2"/>
         <v>-4.8839999999999995E-2</v>
       </c>
-      <c r="BI11">
+      <c r="BJ11">
         <f t="shared" si="3"/>
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -41735,43 +41868,64 @@
         <v>-588</v>
       </c>
       <c r="AG12">
+        <f>AD12-AX12</f>
+        <v>0</v>
+      </c>
+      <c r="AH12">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH12">
+      <c r="AI12">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI12">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AZ12">
-        <f t="shared" si="10"/>
-        <v>0</v>
+      <c r="AK12">
+        <v>95.403899999999993</v>
+      </c>
+      <c r="AL12">
+        <v>0.29437999999999998</v>
+      </c>
+      <c r="AM12">
+        <v>1157</v>
+      </c>
+      <c r="AN12">
+        <f t="shared" si="15"/>
+        <v>95.403899999999993</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="16"/>
+        <v>0.29437999999999998</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="17"/>
+        <v>1157</v>
       </c>
       <c r="BA12">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BB12">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BG12">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BC12">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BH12">
         <f t="shared" si="1"/>
         <v>-20.85</v>
       </c>
-      <c r="BH12">
+      <c r="BI12">
         <f t="shared" si="2"/>
         <v>-0.32519999999999999</v>
       </c>
-      <c r="BI12">
+      <c r="BJ12">
         <f t="shared" si="3"/>
         <v>-588</v>
       </c>
     </row>
-    <row r="13" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -41831,43 +41985,64 @@
         <v>21</v>
       </c>
       <c r="AG13">
+        <f>AD13-AX13</f>
+        <v>0</v>
+      </c>
+      <c r="AH13">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH13">
+      <c r="AI13">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI13">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AZ13">
-        <f t="shared" si="10"/>
-        <v>0</v>
+      <c r="AK13">
+        <v>114.5904</v>
+      </c>
+      <c r="AL13">
+        <v>0.16016</v>
+      </c>
+      <c r="AM13">
+        <v>1375</v>
+      </c>
+      <c r="AN13">
+        <f t="shared" si="15"/>
+        <v>114.5904</v>
+      </c>
+      <c r="AO13">
+        <f t="shared" si="16"/>
+        <v>0.16016</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="17"/>
+        <v>1375</v>
       </c>
       <c r="BA13">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BB13">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BG13">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BC13">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BH13">
         <f t="shared" si="1"/>
         <v>-33.68</v>
       </c>
-      <c r="BH13">
+      <c r="BI13">
         <f t="shared" si="2"/>
         <v>-0.11020000000000001</v>
       </c>
-      <c r="BI13">
+      <c r="BJ13">
         <f t="shared" si="3"/>
         <v>-778</v>
       </c>
     </row>
-    <row r="14" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -41917,61 +42092,82 @@
         <v>1064</v>
       </c>
       <c r="AG14">
+        <f>AD14-AX14</f>
+        <v>4.7050000000000001</v>
+      </c>
+      <c r="AH14">
         <f t="shared" si="7"/>
-        <v>4.7050000000000001</v>
-      </c>
-      <c r="AH14">
+        <v>-8.7299999999999989E-2</v>
+      </c>
+      <c r="AI14">
         <f t="shared" si="8"/>
-        <v>-8.7299999999999989E-2</v>
-      </c>
-      <c r="AI14">
-        <f t="shared" si="9"/>
         <v>537</v>
       </c>
-      <c r="AW14">
+      <c r="AK14">
+        <v>71.672600000000003</v>
+      </c>
+      <c r="AL14">
+        <v>0.15629999999999999</v>
+      </c>
+      <c r="AM14">
+        <v>1154</v>
+      </c>
+      <c r="AN14">
+        <f t="shared" ref="AN14:AN43" si="18">AK14-AD14</f>
+        <v>53.567700000000002</v>
+      </c>
+      <c r="AO14">
+        <f t="shared" ref="AO14:AO43" si="19">AL14-AE14</f>
+        <v>2.8599999999999987E-2</v>
+      </c>
+      <c r="AP14">
+        <f t="shared" ref="AP14:AP43" si="20">AM14-AF14</f>
+        <v>90</v>
+      </c>
+      <c r="AX14">
         <v>13.399900000000001</v>
       </c>
-      <c r="AX14">
+      <c r="AY14">
         <v>0.215</v>
       </c>
-      <c r="AY14">
+      <c r="AZ14">
         <v>527</v>
       </c>
-      <c r="AZ14">
-        <f t="shared" si="10"/>
+      <c r="BA14">
+        <f t="shared" si="12"/>
         <v>-0.30439999999999934</v>
       </c>
-      <c r="BA14">
-        <f t="shared" si="11"/>
+      <c r="BB14">
+        <f t="shared" si="13"/>
         <v>4.0199999999999986E-2</v>
       </c>
-      <c r="BB14">
-        <f t="shared" si="12"/>
+      <c r="BC14">
+        <f t="shared" si="14"/>
         <v>-495</v>
       </c>
-      <c r="BD14">
+      <c r="BE14">
         <v>13.7043</v>
       </c>
-      <c r="BE14">
+      <c r="BF14">
         <v>0.17480000000000001</v>
       </c>
-      <c r="BF14">
+      <c r="BG14">
         <v>1022</v>
       </c>
-      <c r="BG14">
+      <c r="BH14">
         <f t="shared" si="1"/>
         <v>0.5343</v>
       </c>
-      <c r="BH14">
+      <c r="BI14">
         <f t="shared" si="2"/>
         <v>-4.8999999999999988E-2</v>
       </c>
-      <c r="BI14">
+      <c r="BJ14">
         <f t="shared" si="3"/>
         <v>508</v>
       </c>
     </row>
-    <row r="15" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -42021,43 +42217,64 @@
         <v>-663</v>
       </c>
       <c r="AG15">
+        <f>AD15-AX15</f>
+        <v>0</v>
+      </c>
+      <c r="AH15">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH15">
+      <c r="AI15">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI15">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AZ15">
-        <f t="shared" si="10"/>
-        <v>0</v>
+      <c r="AK15">
+        <v>90.829400000000007</v>
+      </c>
+      <c r="AL15">
+        <v>0.1797</v>
+      </c>
+      <c r="AM15">
+        <v>1656</v>
+      </c>
+      <c r="AN15">
+        <f t="shared" si="18"/>
+        <v>90.829400000000007</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="19"/>
+        <v>0.1797</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="20"/>
+        <v>1656</v>
       </c>
       <c r="BA15">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BB15">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BG15">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BC15">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BH15">
         <f t="shared" si="1"/>
         <v>-19.57</v>
       </c>
-      <c r="BH15">
+      <c r="BI15">
         <f t="shared" si="2"/>
         <v>-0.23630000000000001</v>
       </c>
-      <c r="BI15">
+      <c r="BJ15">
         <f t="shared" si="3"/>
         <v>-663</v>
       </c>
     </row>
-    <row r="16" spans="1:67" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:68" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -42098,52 +42315,73 @@
         <v>-716</v>
       </c>
       <c r="AG16">
+        <f>AD16-AX16</f>
+        <v>0</v>
+      </c>
+      <c r="AH16">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH16">
+      <c r="AI16">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI16">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AZ16">
-        <f t="shared" si="10"/>
+      <c r="AK16">
+        <v>240.0746</v>
+      </c>
+      <c r="AL16">
+        <v>8.5360000000000005E-2</v>
+      </c>
+      <c r="AM16">
+        <v>1396</v>
+      </c>
+      <c r="AN16">
+        <f t="shared" si="18"/>
+        <v>240.0746</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" si="19"/>
+        <v>8.5360000000000005E-2</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="20"/>
+        <v>1396</v>
+      </c>
+      <c r="BA16">
+        <f t="shared" si="12"/>
         <v>-53.034950000000002</v>
       </c>
-      <c r="BA16">
-        <f t="shared" si="11"/>
+      <c r="BB16">
+        <f t="shared" si="13"/>
         <v>-5.9695999999999999E-2</v>
       </c>
-      <c r="BB16">
-        <f t="shared" si="12"/>
+      <c r="BC16">
+        <f t="shared" si="14"/>
         <v>-1133</v>
       </c>
-      <c r="BD16">
+      <c r="BE16">
         <v>53.034950000000002</v>
       </c>
-      <c r="BE16">
+      <c r="BF16">
         <v>5.9695999999999999E-2</v>
       </c>
-      <c r="BF16">
+      <c r="BG16">
         <v>1133</v>
       </c>
-      <c r="BG16">
+      <c r="BH16">
         <f t="shared" si="1"/>
         <v>0.5049500000000009</v>
       </c>
-      <c r="BH16">
+      <c r="BI16">
         <f t="shared" si="2"/>
         <v>1.0396000000000002E-2</v>
       </c>
-      <c r="BI16">
+      <c r="BJ16">
         <f t="shared" si="3"/>
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -42202,43 +42440,64 @@
         <v>57</v>
       </c>
       <c r="AG17">
+        <f>AD17-AX17</f>
+        <v>0</v>
+      </c>
+      <c r="AH17">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH17">
+      <c r="AI17">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI17">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="AZ17">
-        <f t="shared" si="10"/>
-        <v>0</v>
+      <c r="AK17">
+        <v>151.08240000000001</v>
+      </c>
+      <c r="AL17">
+        <v>0.36549999999999999</v>
+      </c>
+      <c r="AM17">
+        <v>527</v>
+      </c>
+      <c r="AN17">
+        <f t="shared" si="18"/>
+        <v>151.08240000000001</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="19"/>
+        <v>0.36549999999999999</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="20"/>
+        <v>527</v>
       </c>
       <c r="BA17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0</v>
       </c>
       <c r="BB17">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BG17">
+        <f t="shared" si="13"/>
+        <v>0</v>
+      </c>
+      <c r="BC17">
+        <f t="shared" si="14"/>
+        <v>0</v>
+      </c>
+      <c r="BH17">
         <f t="shared" si="1"/>
         <v>-31.77</v>
       </c>
-      <c r="BH17">
+      <c r="BI17">
         <f t="shared" si="2"/>
         <v>-0.2361</v>
       </c>
-      <c r="BI17">
+      <c r="BJ17">
         <f t="shared" si="3"/>
         <v>-231</v>
       </c>
     </row>
-    <row r="18" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -42297,31 +42556,52 @@
         <v>40</v>
       </c>
       <c r="AG18">
-        <f t="shared" si="7"/>
+        <f>AD18-AX18</f>
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="AH18" si="21">AE18-AY18</f>
         <v>0</v>
       </c>
       <c r="AI18">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BG18">
+        <f t="shared" ref="AI18" si="22">AF18-AZ18</f>
+        <v>0</v>
+      </c>
+      <c r="AK18">
+        <v>76.399000000000001</v>
+      </c>
+      <c r="AL18">
+        <v>0.15029999999999999</v>
+      </c>
+      <c r="AM18">
+        <v>947</v>
+      </c>
+      <c r="AN18">
+        <f t="shared" ref="AN18" si="23">AK18-AD18</f>
+        <v>76.399000000000001</v>
+      </c>
+      <c r="AO18">
+        <f t="shared" ref="AO18" si="24">AL18-AE18</f>
+        <v>0.15029999999999999</v>
+      </c>
+      <c r="AP18">
+        <f t="shared" ref="AP18" si="25">AM18-AF18</f>
+        <v>947</v>
+      </c>
+      <c r="BH18">
         <f t="shared" si="1"/>
         <v>-13.96</v>
       </c>
-      <c r="BH18">
+      <c r="BI18">
         <f t="shared" si="2"/>
         <v>-0.1061</v>
       </c>
-      <c r="BI18">
+      <c r="BJ18">
         <f t="shared" si="3"/>
         <v>-343</v>
       </c>
     </row>
-    <row r="19" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -42372,31 +42652,52 @@
         <v>-320</v>
       </c>
       <c r="AG19">
+        <f>AD19-AX19</f>
+        <v>0</v>
+      </c>
+      <c r="AH19">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH19">
+      <c r="AI19">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI19">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BG19">
+      <c r="AK19">
+        <v>80.852900000000005</v>
+      </c>
+      <c r="AL19">
+        <v>0.24697</v>
+      </c>
+      <c r="AM19">
+        <v>734</v>
+      </c>
+      <c r="AN19">
+        <f t="shared" si="18"/>
+        <v>80.852900000000005</v>
+      </c>
+      <c r="AO19">
+        <f t="shared" si="19"/>
+        <v>0.24697</v>
+      </c>
+      <c r="AP19">
+        <f t="shared" si="20"/>
+        <v>734</v>
+      </c>
+      <c r="BH19">
         <f t="shared" si="1"/>
         <v>-22.79</v>
       </c>
-      <c r="BH19">
+      <c r="BI19">
         <f t="shared" si="2"/>
         <v>-0.28999999999999998</v>
       </c>
-      <c r="BI19">
+      <c r="BJ19">
         <f t="shared" si="3"/>
         <v>-320</v>
       </c>
     </row>
-    <row r="20" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -42437,40 +42738,61 @@
         <v>-283</v>
       </c>
       <c r="AG20">
+        <f>AD20-AX20</f>
+        <v>0</v>
+      </c>
+      <c r="AH20">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH20">
+      <c r="AI20">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI20">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BD20">
+      <c r="AK20">
+        <v>225.16650000000001</v>
+      </c>
+      <c r="AL20">
+        <v>0.1212</v>
+      </c>
+      <c r="AM20">
+        <v>651</v>
+      </c>
+      <c r="AN20">
+        <f t="shared" si="18"/>
+        <v>225.16650000000001</v>
+      </c>
+      <c r="AO20">
+        <f t="shared" si="19"/>
+        <v>0.1212</v>
+      </c>
+      <c r="AP20">
+        <f t="shared" si="20"/>
+        <v>651</v>
+      </c>
+      <c r="BE20">
         <v>68.383750000000006</v>
       </c>
-      <c r="BE20">
+      <c r="BF20">
         <v>0.11585139999999999</v>
       </c>
-      <c r="BF20">
+      <c r="BG20">
         <v>454</v>
       </c>
-      <c r="BG20">
+      <c r="BH20">
         <f t="shared" si="1"/>
         <v>4.6937500000000085</v>
       </c>
-      <c r="BH20">
+      <c r="BI20">
         <f t="shared" si="2"/>
         <v>1.5651399999999996E-2</v>
       </c>
-      <c r="BI20">
+      <c r="BJ20">
         <f t="shared" si="3"/>
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -42532,31 +42854,52 @@
         <v>106</v>
       </c>
       <c r="AG21">
+        <f>AD21-AX21</f>
+        <v>0</v>
+      </c>
+      <c r="AH21">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH21">
+      <c r="AI21">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI21">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BG21">
+      <c r="AK21">
+        <v>48.740499999999997</v>
+      </c>
+      <c r="AL21">
+        <v>0.1769</v>
+      </c>
+      <c r="AM21">
+        <v>1742</v>
+      </c>
+      <c r="AN21">
+        <f t="shared" si="18"/>
+        <v>48.740499999999997</v>
+      </c>
+      <c r="AO21">
+        <f t="shared" si="19"/>
+        <v>0.1769</v>
+      </c>
+      <c r="AP21">
+        <f t="shared" si="20"/>
+        <v>1742</v>
+      </c>
+      <c r="BH21">
         <f t="shared" si="1"/>
         <v>-11.31</v>
       </c>
-      <c r="BH21">
+      <c r="BI21">
         <f t="shared" si="2"/>
         <v>-0.11219999999999999</v>
       </c>
-      <c r="BI21">
+      <c r="BJ21">
         <f t="shared" si="3"/>
         <v>-646</v>
       </c>
     </row>
-    <row r="22" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -42606,31 +42949,52 @@
         <v>-236</v>
       </c>
       <c r="AG22">
+        <f>AD22-AX22</f>
+        <v>0</v>
+      </c>
+      <c r="AH22">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="AH22">
+      <c r="AI22">
         <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AI22">
-        <f t="shared" si="9"/>
-        <v>0</v>
-      </c>
-      <c r="BG22">
+      <c r="AK22">
+        <v>56.912999999999997</v>
+      </c>
+      <c r="AL22">
+        <v>0.26650000000000001</v>
+      </c>
+      <c r="AM22">
+        <v>963</v>
+      </c>
+      <c r="AN22">
+        <f t="shared" si="18"/>
+        <v>56.912999999999997</v>
+      </c>
+      <c r="AO22">
+        <f t="shared" si="19"/>
+        <v>0.26650000000000001</v>
+      </c>
+      <c r="AP22">
+        <f t="shared" si="20"/>
+        <v>963</v>
+      </c>
+      <c r="BH22">
         <f t="shared" si="1"/>
         <v>-10.199999999999999</v>
       </c>
-      <c r="BH22">
+      <c r="BI22">
         <f t="shared" si="2"/>
         <v>-0.37130000000000002</v>
       </c>
-      <c r="BI22">
+      <c r="BJ22">
         <f t="shared" si="3"/>
         <v>-236</v>
       </c>
     </row>
-    <row r="23" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -42670,29 +43034,50 @@
         <f t="shared" si="6"/>
         <v>-323</v>
       </c>
-      <c r="BD23">
+      <c r="AK23">
+        <v>74.535600000000002</v>
+      </c>
+      <c r="AL23">
+        <v>0.13339999999999999</v>
+      </c>
+      <c r="AM23">
+        <v>579</v>
+      </c>
+      <c r="AN23">
+        <f t="shared" si="18"/>
+        <v>74.535600000000002</v>
+      </c>
+      <c r="AO23">
+        <f t="shared" si="19"/>
+        <v>0.13339999999999999</v>
+      </c>
+      <c r="AP23">
+        <f t="shared" si="20"/>
+        <v>579</v>
+      </c>
+      <c r="BE23">
         <v>15.04355</v>
       </c>
-      <c r="BE23">
+      <c r="BF23">
         <v>9.3257999999999994E-2</v>
       </c>
-      <c r="BF23">
+      <c r="BG23">
         <v>829</v>
       </c>
-      <c r="BG23">
+      <c r="BH23">
         <f t="shared" si="1"/>
         <v>0.11355000000000004</v>
       </c>
-      <c r="BH23">
+      <c r="BI23">
         <f t="shared" si="2"/>
         <v>-6.9420000000000037E-3</v>
       </c>
-      <c r="BI23">
+      <c r="BJ23">
         <f t="shared" si="3"/>
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -42732,29 +43117,50 @@
         <f t="shared" si="6"/>
         <v>-283</v>
       </c>
-      <c r="BD24">
+      <c r="AK24">
+        <v>121.116</v>
+      </c>
+      <c r="AL24">
+        <v>0.2165</v>
+      </c>
+      <c r="AM24">
+        <v>462</v>
+      </c>
+      <c r="AN24">
+        <f t="shared" si="18"/>
+        <v>121.116</v>
+      </c>
+      <c r="AO24">
+        <f t="shared" si="19"/>
+        <v>0.2165</v>
+      </c>
+      <c r="AP24">
+        <f t="shared" si="20"/>
+        <v>462</v>
+      </c>
+      <c r="BE24">
         <v>21.397960000000001</v>
       </c>
-      <c r="BE24">
+      <c r="BF24">
         <v>0.14054</v>
       </c>
-      <c r="BF24">
+      <c r="BG24">
         <v>602</v>
       </c>
-      <c r="BG24">
+      <c r="BH24">
         <f t="shared" si="1"/>
         <v>-2.0920399999999972</v>
       </c>
-      <c r="BH24">
+      <c r="BI24">
         <f t="shared" si="2"/>
         <v>-8.1600000000000006E-3</v>
       </c>
-      <c r="BI24">
+      <c r="BJ24">
         <f t="shared" si="3"/>
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -42813,20 +43219,41 @@
         <f t="shared" si="6"/>
         <v>82</v>
       </c>
-      <c r="BG25">
+      <c r="AK25">
+        <v>98.161590000000004</v>
+      </c>
+      <c r="AL25">
+        <v>0.26608999999999999</v>
+      </c>
+      <c r="AM25">
+        <v>599</v>
+      </c>
+      <c r="AN25">
+        <f t="shared" si="18"/>
+        <v>98.161590000000004</v>
+      </c>
+      <c r="AO25">
+        <f t="shared" si="19"/>
+        <v>0.26608999999999999</v>
+      </c>
+      <c r="AP25">
+        <f t="shared" si="20"/>
+        <v>599</v>
+      </c>
+      <c r="BH25">
         <f t="shared" si="1"/>
         <v>-17.02</v>
       </c>
-      <c r="BH25">
+      <c r="BI25">
         <f t="shared" si="2"/>
         <v>-0.21240000000000001</v>
       </c>
-      <c r="BI25">
+      <c r="BJ25">
         <f t="shared" si="3"/>
         <v>-204</v>
       </c>
     </row>
-    <row r="26" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -42886,20 +43313,41 @@
         <f t="shared" si="6"/>
         <v>121</v>
       </c>
-      <c r="BG26">
+      <c r="AK26">
+        <v>72.231539999999995</v>
+      </c>
+      <c r="AL26">
+        <v>0.2412</v>
+      </c>
+      <c r="AM26">
+        <v>795</v>
+      </c>
+      <c r="AN26">
+        <f t="shared" si="18"/>
+        <v>72.231539999999995</v>
+      </c>
+      <c r="AO26">
+        <f t="shared" si="19"/>
+        <v>0.2412</v>
+      </c>
+      <c r="AP26">
+        <f t="shared" si="20"/>
+        <v>795</v>
+      </c>
+      <c r="BH26">
         <f t="shared" si="1"/>
         <v>-10.1</v>
       </c>
-      <c r="BH26">
+      <c r="BI26">
         <f t="shared" si="2"/>
         <v>-0.3599</v>
       </c>
-      <c r="BI26">
+      <c r="BJ26">
         <f t="shared" si="3"/>
         <v>-220</v>
       </c>
     </row>
-    <row r="27" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -42958,20 +43406,41 @@
         <f t="shared" si="6"/>
         <v>76</v>
       </c>
-      <c r="BG27">
+      <c r="AK27">
+        <v>83.323599999999999</v>
+      </c>
+      <c r="AL27">
+        <v>0.31533</v>
+      </c>
+      <c r="AM27">
+        <v>421</v>
+      </c>
+      <c r="AN27">
+        <f t="shared" si="18"/>
+        <v>83.323599999999999</v>
+      </c>
+      <c r="AO27">
+        <f t="shared" si="19"/>
+        <v>0.31533</v>
+      </c>
+      <c r="AP27">
+        <f t="shared" si="20"/>
+        <v>421</v>
+      </c>
+      <c r="BH27">
         <f t="shared" si="1"/>
         <v>-22.76</v>
       </c>
-      <c r="BH27">
+      <c r="BI27">
         <f t="shared" si="2"/>
         <v>-0.27900000000000003</v>
       </c>
-      <c r="BI27">
+      <c r="BJ27">
         <f t="shared" si="3"/>
         <v>-174</v>
       </c>
     </row>
-    <row r="28" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -43031,20 +43500,41 @@
         <f t="shared" si="6"/>
         <v>14</v>
       </c>
-      <c r="BG28">
+      <c r="AK28">
+        <v>119.6892</v>
+      </c>
+      <c r="AL28">
+        <v>0.22966</v>
+      </c>
+      <c r="AM28">
+        <v>408</v>
+      </c>
+      <c r="AN28">
+        <f t="shared" si="18"/>
+        <v>119.6892</v>
+      </c>
+      <c r="AO28">
+        <f t="shared" si="19"/>
+        <v>0.22966</v>
+      </c>
+      <c r="AP28">
+        <f t="shared" si="20"/>
+        <v>408</v>
+      </c>
+      <c r="BH28">
         <f t="shared" si="1"/>
         <v>-30.57</v>
       </c>
-      <c r="BH28">
+      <c r="BI28">
         <f t="shared" si="2"/>
         <v>-0.26269999999999999</v>
       </c>
-      <c r="BI28">
+      <c r="BJ28">
         <f t="shared" si="3"/>
         <v>-165</v>
       </c>
     </row>
-    <row r="29" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -43104,20 +43594,41 @@
         <f t="shared" si="6"/>
         <v>60</v>
       </c>
-      <c r="BG29">
+      <c r="AK29">
+        <v>91.474900000000005</v>
+      </c>
+      <c r="AL29">
+        <v>0.34320000000000001</v>
+      </c>
+      <c r="AM29">
+        <v>712</v>
+      </c>
+      <c r="AN29">
+        <f t="shared" si="18"/>
+        <v>91.474900000000005</v>
+      </c>
+      <c r="AO29">
+        <f t="shared" si="19"/>
+        <v>0.34320000000000001</v>
+      </c>
+      <c r="AP29">
+        <f t="shared" si="20"/>
+        <v>712</v>
+      </c>
+      <c r="BH29">
         <f t="shared" si="1"/>
         <v>-19.22</v>
       </c>
-      <c r="BH29">
+      <c r="BI29">
         <f t="shared" si="2"/>
         <v>-0.3029</v>
       </c>
-      <c r="BI29">
+      <c r="BJ29">
         <f t="shared" si="3"/>
         <v>-324</v>
       </c>
     </row>
-    <row r="30" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -43177,20 +43688,41 @@
         <f t="shared" si="6"/>
         <v>51</v>
       </c>
-      <c r="BG30">
+      <c r="AK30">
+        <v>88.2821</v>
+      </c>
+      <c r="AL30">
+        <v>8.9889999999999998E-2</v>
+      </c>
+      <c r="AM30">
+        <v>454</v>
+      </c>
+      <c r="AN30">
+        <f t="shared" si="18"/>
+        <v>88.2821</v>
+      </c>
+      <c r="AO30">
+        <f t="shared" si="19"/>
+        <v>8.9889999999999998E-2</v>
+      </c>
+      <c r="AP30">
+        <f t="shared" si="20"/>
+        <v>454</v>
+      </c>
+      <c r="BH30">
         <f t="shared" si="1"/>
         <v>-11.61</v>
       </c>
-      <c r="BH30">
+      <c r="BI30">
         <f t="shared" si="2"/>
         <v>-6.8199999999999997E-2</v>
       </c>
-      <c r="BI30">
+      <c r="BJ30">
         <f t="shared" si="3"/>
         <v>-233</v>
       </c>
     </row>
-    <row r="31" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -43248,20 +43780,41 @@
         <f t="shared" si="6"/>
         <v>24</v>
       </c>
-      <c r="BG31">
+      <c r="AK31">
+        <v>67.405699999999996</v>
+      </c>
+      <c r="AL31">
+        <v>0.19688</v>
+      </c>
+      <c r="AM31">
+        <v>327</v>
+      </c>
+      <c r="AN31">
+        <f t="shared" si="18"/>
+        <v>67.405699999999996</v>
+      </c>
+      <c r="AO31">
+        <f t="shared" si="19"/>
+        <v>0.19688</v>
+      </c>
+      <c r="AP31">
+        <f t="shared" si="20"/>
+        <v>327</v>
+      </c>
+      <c r="BH31">
         <f t="shared" si="1"/>
         <v>-16.989999999999998</v>
       </c>
-      <c r="BH31">
+      <c r="BI31">
         <f t="shared" si="2"/>
         <v>-0.20349999999999999</v>
       </c>
-      <c r="BI31">
+      <c r="BJ31">
         <f t="shared" si="3"/>
         <v>-140</v>
       </c>
     </row>
-    <row r="32" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -43320,20 +43873,41 @@
         <f t="shared" si="6"/>
         <v>79</v>
       </c>
-      <c r="BG32">
+      <c r="AK32">
+        <v>84.632999999999996</v>
+      </c>
+      <c r="AL32">
+        <v>0.2198</v>
+      </c>
+      <c r="AM32">
+        <v>828</v>
+      </c>
+      <c r="AN32">
+        <f t="shared" si="18"/>
+        <v>84.632999999999996</v>
+      </c>
+      <c r="AO32">
+        <f t="shared" si="19"/>
+        <v>0.2198</v>
+      </c>
+      <c r="AP32">
+        <f t="shared" si="20"/>
+        <v>828</v>
+      </c>
+      <c r="BH32">
         <f t="shared" si="1"/>
         <v>-14.08</v>
       </c>
-      <c r="BH32">
+      <c r="BI32">
         <f t="shared" si="2"/>
         <v>-0.26400000000000001</v>
       </c>
-      <c r="BI32">
+      <c r="BJ32">
         <f t="shared" si="3"/>
         <v>-318</v>
       </c>
     </row>
-    <row r="33" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -43392,20 +43966,41 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="BG33">
+      <c r="AK33">
+        <v>113.6572</v>
+      </c>
+      <c r="AL33">
+        <v>0.13764999999999999</v>
+      </c>
+      <c r="AM33">
+        <v>1052</v>
+      </c>
+      <c r="AN33">
+        <f t="shared" si="18"/>
+        <v>113.6572</v>
+      </c>
+      <c r="AO33">
+        <f t="shared" si="19"/>
+        <v>0.13764999999999999</v>
+      </c>
+      <c r="AP33">
+        <f t="shared" si="20"/>
+        <v>1052</v>
+      </c>
+      <c r="BH33">
         <f t="shared" si="1"/>
         <v>-27.43</v>
       </c>
-      <c r="BH33">
+      <c r="BI33">
         <f t="shared" si="2"/>
         <v>-0.1033</v>
       </c>
-      <c r="BI33">
+      <c r="BJ33">
         <f t="shared" si="3"/>
         <v>-477</v>
       </c>
     </row>
-    <row r="34" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -43445,29 +44040,50 @@
         <f t="shared" si="6"/>
         <v>-530</v>
       </c>
-      <c r="BD34">
+      <c r="AK34">
+        <v>46.363799999999998</v>
+      </c>
+      <c r="AL34">
+        <v>0.27146999999999999</v>
+      </c>
+      <c r="AM34">
+        <v>840</v>
+      </c>
+      <c r="AN34">
+        <f t="shared" si="18"/>
+        <v>46.363799999999998</v>
+      </c>
+      <c r="AO34">
+        <f t="shared" si="19"/>
+        <v>0.27146999999999999</v>
+      </c>
+      <c r="AP34">
+        <f t="shared" si="20"/>
+        <v>840</v>
+      </c>
+      <c r="BE34">
         <v>14.0328</v>
       </c>
-      <c r="BE34">
+      <c r="BF34">
         <v>0.1895</v>
       </c>
-      <c r="BF34">
+      <c r="BG34">
         <v>764</v>
       </c>
-      <c r="BG34">
+      <c r="BH34">
         <f t="shared" si="1"/>
         <v>2.5128000000000004</v>
       </c>
-      <c r="BH34">
+      <c r="BI34">
         <f t="shared" si="2"/>
         <v>-5.1600000000000007E-2</v>
       </c>
-      <c r="BI34">
+      <c r="BJ34">
         <f t="shared" si="3"/>
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -43507,29 +44123,50 @@
         <f t="shared" si="6"/>
         <v>-454</v>
       </c>
-      <c r="BD35">
+      <c r="AK35">
+        <v>30.443850000000001</v>
+      </c>
+      <c r="AL35">
+        <v>0.28094999999999998</v>
+      </c>
+      <c r="AM35">
+        <v>610</v>
+      </c>
+      <c r="AN35">
+        <f t="shared" si="18"/>
+        <v>30.443850000000001</v>
+      </c>
+      <c r="AO35">
+        <f t="shared" si="19"/>
+        <v>0.28094999999999998</v>
+      </c>
+      <c r="AP35">
+        <f t="shared" si="20"/>
+        <v>610</v>
+      </c>
+      <c r="BE35">
         <v>8.6080649999999999</v>
       </c>
-      <c r="BE35">
+      <c r="BF35">
         <v>0.2099</v>
       </c>
-      <c r="BF35">
+      <c r="BG35">
         <v>477</v>
       </c>
-      <c r="BG35">
+      <c r="BH35">
         <f t="shared" si="1"/>
         <v>3.8064999999999571E-2</v>
       </c>
-      <c r="BH35">
+      <c r="BI35">
         <f t="shared" si="2"/>
         <v>-2.2999999999999965E-3</v>
       </c>
-      <c r="BI35">
+      <c r="BJ35">
         <f t="shared" si="3"/>
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -43587,20 +44224,41 @@
         <f t="shared" si="6"/>
         <v>3</v>
       </c>
-      <c r="BG36">
+      <c r="AK36">
+        <v>66.238900000000001</v>
+      </c>
+      <c r="AL36">
+        <v>0.42817</v>
+      </c>
+      <c r="AM36">
+        <v>307</v>
+      </c>
+      <c r="AN36">
+        <f t="shared" si="18"/>
+        <v>66.238900000000001</v>
+      </c>
+      <c r="AO36">
+        <f t="shared" si="19"/>
+        <v>0.42817</v>
+      </c>
+      <c r="AP36">
+        <f t="shared" si="20"/>
+        <v>307</v>
+      </c>
+      <c r="BH36">
         <f t="shared" si="1"/>
         <v>-26.52</v>
       </c>
-      <c r="BH36">
+      <c r="BI36">
         <f t="shared" si="2"/>
         <v>-0.36399999999999999</v>
       </c>
-      <c r="BI36">
+      <c r="BJ36">
         <f t="shared" si="3"/>
         <v>-159</v>
       </c>
     </row>
-    <row r="37" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -43658,20 +44316,41 @@
         <f t="shared" si="6"/>
         <v>138</v>
       </c>
-      <c r="BG37">
+      <c r="AK37">
+        <v>157.17169999999999</v>
+      </c>
+      <c r="AL37">
+        <v>9.6170000000000005E-2</v>
+      </c>
+      <c r="AM37">
+        <v>464</v>
+      </c>
+      <c r="AN37">
+        <f t="shared" si="18"/>
+        <v>157.17169999999999</v>
+      </c>
+      <c r="AO37">
+        <f t="shared" si="19"/>
+        <v>9.6170000000000005E-2</v>
+      </c>
+      <c r="AP37">
+        <f t="shared" si="20"/>
+        <v>464</v>
+      </c>
+      <c r="BH37">
         <f t="shared" si="1"/>
         <v>-39.68</v>
       </c>
-      <c r="BH37">
+      <c r="BI37">
         <f t="shared" si="2"/>
         <v>-0.1246</v>
       </c>
-      <c r="BI37">
+      <c r="BJ37">
         <f t="shared" si="3"/>
         <v>-250</v>
       </c>
     </row>
-    <row r="38" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -43731,20 +44410,41 @@
         <f t="shared" si="6"/>
         <v>10</v>
       </c>
-      <c r="BG38">
+      <c r="AK38">
+        <v>98.72</v>
+      </c>
+      <c r="AL38">
+        <v>0.21548</v>
+      </c>
+      <c r="AM38">
+        <v>508</v>
+      </c>
+      <c r="AN38">
+        <f t="shared" si="18"/>
+        <v>98.72</v>
+      </c>
+      <c r="AO38">
+        <f t="shared" si="19"/>
+        <v>0.21548</v>
+      </c>
+      <c r="AP38">
+        <f t="shared" si="20"/>
+        <v>508</v>
+      </c>
+      <c r="BH38">
         <f t="shared" si="1"/>
         <v>-22.22</v>
       </c>
-      <c r="BH38">
+      <c r="BI38">
         <f t="shared" si="2"/>
         <v>-0.30280000000000001</v>
       </c>
-      <c r="BI38">
+      <c r="BJ38">
         <f t="shared" si="3"/>
         <v>-263</v>
       </c>
     </row>
-    <row r="39" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -43802,20 +44502,41 @@
         <f t="shared" si="6"/>
         <v>22</v>
       </c>
-      <c r="BG39">
+      <c r="AK39">
+        <v>102.0086</v>
+      </c>
+      <c r="AL39">
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="AM39">
+        <v>230</v>
+      </c>
+      <c r="AN39">
+        <f t="shared" si="18"/>
+        <v>102.0086</v>
+      </c>
+      <c r="AO39">
+        <f t="shared" si="19"/>
+        <v>7.3599999999999999E-2</v>
+      </c>
+      <c r="AP39">
+        <f t="shared" si="20"/>
+        <v>230</v>
+      </c>
+      <c r="BH39">
         <f t="shared" si="1"/>
         <v>-26.34</v>
       </c>
-      <c r="BH39">
+      <c r="BI39">
         <f t="shared" si="2"/>
         <v>-0.22470000000000001</v>
       </c>
-      <c r="BI39">
+      <c r="BJ39">
         <f t="shared" si="3"/>
         <v>-137</v>
       </c>
     </row>
-    <row r="40" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -43855,29 +44576,50 @@
         <f t="shared" si="6"/>
         <v>-173</v>
       </c>
-      <c r="BD40">
+      <c r="AK40">
+        <v>90.071899999999999</v>
+      </c>
+      <c r="AL40">
+        <v>0.2913</v>
+      </c>
+      <c r="AM40">
+        <v>301</v>
+      </c>
+      <c r="AN40">
+        <f t="shared" si="18"/>
+        <v>90.071899999999999</v>
+      </c>
+      <c r="AO40">
+        <f t="shared" si="19"/>
+        <v>0.2913</v>
+      </c>
+      <c r="AP40">
+        <f t="shared" si="20"/>
+        <v>301</v>
+      </c>
+      <c r="BE40">
         <v>19.668900000000001</v>
       </c>
-      <c r="BE40" s="81">
+      <c r="BF40" s="81">
         <v>0.33239999999999997</v>
       </c>
-      <c r="BF40">
+      <c r="BG40">
         <v>211</v>
       </c>
-      <c r="BG40">
+      <c r="BH40">
         <f t="shared" si="1"/>
         <v>-0.47109999999999985</v>
       </c>
-      <c r="BH40">
+      <c r="BI40">
         <f t="shared" si="2"/>
         <v>0.16209999999999997</v>
       </c>
-      <c r="BI40">
+      <c r="BJ40">
         <f t="shared" si="3"/>
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -43917,29 +44659,50 @@
         <f t="shared" si="6"/>
         <v>-248</v>
       </c>
-      <c r="BD41">
+      <c r="AK41">
+        <v>46.406399999999998</v>
+      </c>
+      <c r="AL41">
+        <v>0.15325</v>
+      </c>
+      <c r="AM41">
+        <v>404</v>
+      </c>
+      <c r="AN41">
+        <f t="shared" si="18"/>
+        <v>46.406399999999998</v>
+      </c>
+      <c r="AO41">
+        <f t="shared" si="19"/>
+        <v>0.15325</v>
+      </c>
+      <c r="AP41">
+        <f t="shared" si="20"/>
+        <v>404</v>
+      </c>
+      <c r="BE41">
         <v>9.7552000000000003</v>
       </c>
-      <c r="BE41">
+      <c r="BF41">
         <v>0.16739999999999999</v>
       </c>
-      <c r="BF41">
+      <c r="BG41">
         <v>260</v>
       </c>
-      <c r="BG41">
+      <c r="BH41">
         <f t="shared" si="1"/>
         <v>4.5199999999999463E-2</v>
       </c>
-      <c r="BH41">
+      <c r="BI41">
         <f t="shared" si="2"/>
         <v>-1.9600000000000006E-2</v>
       </c>
-      <c r="BI41">
+      <c r="BJ41">
         <f t="shared" si="3"/>
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -43979,29 +44742,50 @@
         <f t="shared" si="6"/>
         <v>-108</v>
       </c>
-      <c r="BD42">
+      <c r="AK42">
+        <v>83.256900000000002</v>
+      </c>
+      <c r="AL42">
+        <v>0.30740000000000001</v>
+      </c>
+      <c r="AM42">
+        <v>212</v>
+      </c>
+      <c r="AN42">
+        <f t="shared" si="18"/>
+        <v>83.256900000000002</v>
+      </c>
+      <c r="AO42">
+        <f t="shared" si="19"/>
+        <v>0.30740000000000001</v>
+      </c>
+      <c r="AP42">
+        <f t="shared" si="20"/>
+        <v>212</v>
+      </c>
+      <c r="BE42">
         <v>12.31058</v>
       </c>
-      <c r="BE42">
+      <c r="BF42">
         <v>0.19095999999999999</v>
       </c>
-      <c r="BF42">
+      <c r="BG42">
         <v>115</v>
       </c>
-      <c r="BG42">
+      <c r="BH42">
         <f t="shared" si="1"/>
         <v>-0.149420000000001</v>
       </c>
-      <c r="BH42">
+      <c r="BI42">
         <f t="shared" si="2"/>
         <v>-6.540000000000018E-3</v>
       </c>
-      <c r="BI42">
+      <c r="BJ42">
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:62" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -44041,29 +44825,50 @@
         <f t="shared" si="6"/>
         <v>-117</v>
       </c>
-      <c r="BD43">
+      <c r="AK43">
+        <v>215.42920000000001</v>
+      </c>
+      <c r="AL43">
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="AM43">
+        <v>202</v>
+      </c>
+      <c r="AN43">
+        <f t="shared" si="18"/>
+        <v>215.42920000000001</v>
+      </c>
+      <c r="AO43">
+        <f t="shared" si="19"/>
+        <v>0.25890000000000002</v>
+      </c>
+      <c r="AP43">
+        <f t="shared" si="20"/>
+        <v>202</v>
+      </c>
+      <c r="BE43">
         <v>41.243749999999999</v>
       </c>
-      <c r="BE43">
+      <c r="BF43">
         <v>0.32723000000000002</v>
       </c>
-      <c r="BF43">
+      <c r="BG43">
         <v>145</v>
       </c>
-      <c r="BG43">
+      <c r="BH43">
         <f t="shared" si="1"/>
         <v>7.9637499999999974</v>
       </c>
-      <c r="BH43">
+      <c r="BI43">
         <f t="shared" si="2"/>
         <v>3.6930000000000018E-2</v>
       </c>
-      <c r="BI43">
+      <c r="BJ43">
         <f t="shared" si="3"/>
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:61" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:62" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -44072,12 +44877,12 @@
         <f>SUM(AA5,AA9:AA10,AA13,AA17:AA18,AA21,AA25:AA33,AA36:AA39)</f>
         <v>0.1336999999999999</v>
       </c>
-      <c r="BG45">
-        <f>SUM(BG6:BG7,BG9,BG11,BG14,BG16,BG20,BG23:BG24,BG34:BG35,BG40:BG43)</f>
-        <v>27.277845000000013</v>
-      </c>
       <c r="BH45">
         <f>SUM(BH6:BH7,BH9,BH11,BH14,BH16,BH20,BH23:BH24,BH34:BH35,BH40:BH43)</f>
+        <v>27.277845000000013</v>
+      </c>
+      <c r="BI45">
+        <f>SUM(BI6:BI7,BI9,BI11,BI14,BI16,BI20,BI23:BI24,BI34:BI35,BI40:BI43)</f>
         <v>-0.10875460000000006</v>
       </c>
     </row>
@@ -44088,47 +44893,37 @@
     <mergeCell ref="I3:M3"/>
     <mergeCell ref="N3:O3"/>
   </mergeCells>
-  <conditionalFormatting sqref="Z5:Z43">
-    <cfRule type="cellIs" dxfId="8" priority="12" operator="greaterThan">
+  <conditionalFormatting sqref="Z5:Z43 BH5:BH43">
+    <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA45:AB45 AA5:AB43">
-    <cfRule type="cellIs" dxfId="7" priority="11" operator="greaterThan">
+  <conditionalFormatting sqref="AA45:AB45 AA5:AB43 BI5:BJ43">
+    <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45">
-    <cfRule type="cellIs" dxfId="6" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="4" priority="10" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AB46">
-    <cfRule type="cellIs" dxfId="5" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="7" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46">
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="2" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BG5:BG43">
-    <cfRule type="cellIs" dxfId="3" priority="5" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BH5:BH43">
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="greaterThan">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="BG45:BH45">
+  <conditionalFormatting sqref="BH45:BI45">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BI1:BI3 BI5:BI43">
+  <conditionalFormatting sqref="BJ1:BJ3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Removed condition outliers outside of 2 Std Dev
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2278" uniqueCount="232">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="234">
   <si>
     <t>Species</t>
   </si>
@@ -722,6 +722,12 @@
   </si>
   <si>
     <t>Rexamine removing outliers: only remove extreme outliers ( indwt &lt;0.005, length&lt;0, RelCond &gt;300)</t>
+  </si>
+  <si>
+    <t>% n diff</t>
+  </si>
+  <si>
+    <t>Removing outliers: same as AK2, plus remove outside of 2*Std Dev</t>
   </si>
 </sst>
 </file>
@@ -40592,10 +40598,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BP45"/>
+  <dimension ref="A1:BX45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AJ1" workbookViewId="0">
-      <selection activeCell="AO6" sqref="AO6"/>
+    <sheetView tabSelected="1" topLeftCell="AR11" workbookViewId="0">
+      <selection activeCell="AT22" sqref="AT22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40614,7 +40620,7 @@
     <col min="23" max="25" width="8.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:68" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:76" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40643,12 +40649,12 @@
       <c r="W1" s="75" t="s">
         <v>213</v>
       </c>
-      <c r="AX1" t="s">
+      <c r="BF1" t="s">
         <v>224</v>
       </c>
-      <c r="BJ1"/>
-    </row>
-    <row r="2" spans="1:68" x14ac:dyDescent="0.35">
+      <c r="BR1"/>
+    </row>
+    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
@@ -40658,17 +40664,20 @@
       <c r="AK2" t="s">
         <v>231</v>
       </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
+        <v>233</v>
+      </c>
+      <c r="AZ2" t="s">
         <v>227</v>
       </c>
-      <c r="AX2" t="s">
+      <c r="BF2" t="s">
         <v>230</v>
       </c>
-      <c r="BE2" t="s">
+      <c r="BM2" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:68" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:76" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="95" t="s">
         <v>178</v>
       </c>
@@ -40711,21 +40720,24 @@
       <c r="AK3" s="75" t="s">
         <v>229</v>
       </c>
-      <c r="AR3" s="75" t="s">
+      <c r="AS3" s="75" t="s">
+        <v>229</v>
+      </c>
+      <c r="AZ3" s="75" t="s">
         <v>220</v>
       </c>
-      <c r="AX3" s="75" t="s">
+      <c r="BF3" s="75" t="s">
         <v>221</v>
       </c>
-      <c r="BE3" s="75" t="s">
+      <c r="BM3" s="75" t="s">
         <v>222</v>
       </c>
-      <c r="BJ3"/>
-      <c r="BL3" s="75" t="s">
+      <c r="BR3"/>
+      <c r="BT3" s="75" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:68" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:76" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40840,74 +40852,98 @@
       <c r="AP4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="AR4" s="69" t="s">
+      <c r="AQ4" s="69" t="s">
+        <v>232</v>
+      </c>
+      <c r="AS4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AS4" s="69" t="s">
+      <c r="AT4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AT4" s="69" t="s">
+      <c r="AU4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="AU4" s="69" t="s">
+      <c r="AV4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="AV4" s="69" t="s">
+      <c r="AW4" s="69" t="s">
         <v>219</v>
       </c>
       <c r="AX4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="AY4" s="69" t="s">
+        <v>232</v>
+      </c>
+      <c r="AZ4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="AY4" s="69" t="s">
+      <c r="BA4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="AZ4" s="69" t="s">
+      <c r="BB4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BA4" s="69" t="s">
+      <c r="BC4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BB4" s="69" t="s">
+      <c r="BD4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="BC4" s="69" t="s">
+      <c r="BF4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="BG4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="BH4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="BI4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="BJ4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="BK4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="BE4" s="69" t="s">
+      <c r="BM4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BF4" s="69" t="s">
+      <c r="BN4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BG4" s="69" t="s">
+      <c r="BO4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BH4" s="69" t="s">
+      <c r="BP4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BI4" s="69" t="s">
+      <c r="BQ4" s="69" t="s">
         <v>219</v>
       </c>
-      <c r="BJ4" s="69" t="s">
+      <c r="BR4" s="69" t="s">
         <v>226</v>
       </c>
-      <c r="BL4" s="69" t="s">
+      <c r="BT4" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="BM4" s="69" t="s">
+      <c r="BU4" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="BN4" s="69" t="s">
+      <c r="BV4" s="69" t="s">
         <v>5</v>
       </c>
-      <c r="BO4" s="69" t="s">
+      <c r="BW4" s="69" t="s">
         <v>218</v>
       </c>
-      <c r="BP4" s="69" t="s">
+      <c r="BX4" s="69" t="s">
         <v>219</v>
       </c>
     </row>
-    <row r="5" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -40978,15 +41014,15 @@
         <v>1149</v>
       </c>
       <c r="AG5">
-        <f>AD5-AX5</f>
+        <f>AD5-BF5</f>
         <v>6.3363000000000014</v>
       </c>
       <c r="AH5">
-        <f>AE5-AY5</f>
+        <f>AE5-BG5</f>
         <v>-6.7799999999999985E-2</v>
       </c>
       <c r="AI5">
-        <f>AF5-AZ5</f>
+        <f>AF5-BH5</f>
         <v>585</v>
       </c>
       <c r="AK5">
@@ -41003,48 +41039,77 @@
         <v>85.654899999999998</v>
       </c>
       <c r="AO5">
-        <f t="shared" ref="AO5:AP5" si="0">AL5-AE5</f>
+        <f t="shared" ref="AO5" si="0">AL5-AE5</f>
         <v>2.471799999999999E-2</v>
       </c>
       <c r="AP5">
-        <f t="shared" si="0"/>
+        <f>AM5-AF5</f>
         <v>110</v>
       </c>
+      <c r="AQ5">
+        <f>AP5/AF5</f>
+        <v>9.5735422106179288E-2</v>
+      </c>
+      <c r="AS5">
+        <v>72.116399999999999</v>
+      </c>
+      <c r="AT5">
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="AU5">
+        <v>635</v>
+      </c>
+      <c r="AV5">
+        <f>AS5-AK5</f>
+        <v>-41.701400000000007</v>
+      </c>
+      <c r="AW5">
+        <f t="shared" ref="AW5:AW43" si="1">AT5-AL5</f>
+        <v>5.2482000000000015E-2</v>
+      </c>
       <c r="AX5">
+        <f>AM5-AU5</f>
+        <v>624</v>
+      </c>
+      <c r="AY5">
+        <f>AX5/AM5</f>
+        <v>0.49563145353455124</v>
+      </c>
+      <c r="BF5">
         <v>21.826599999999999</v>
       </c>
-      <c r="AY5">
+      <c r="BG5">
         <v>0.15859999999999999</v>
       </c>
-      <c r="AZ5">
+      <c r="BH5">
         <v>564</v>
       </c>
-      <c r="BA5">
-        <f>AX5-BE5</f>
+      <c r="BI5">
+        <f>BF5-BM5</f>
         <v>21.826599999999999</v>
       </c>
-      <c r="BB5">
-        <f>AY5-BF5</f>
+      <c r="BJ5">
+        <f>BG5-BN5</f>
         <v>0.15859999999999999</v>
       </c>
-      <c r="BC5">
-        <f>AZ5-BG5</f>
+      <c r="BK5">
+        <f>BH5-BO5</f>
         <v>564</v>
       </c>
-      <c r="BH5">
-        <f t="shared" ref="BH5:BH43" si="1">BE5-S5</f>
+      <c r="BP5">
+        <f t="shared" ref="BP5:BP43" si="2">BM5-S5</f>
         <v>-23.66</v>
       </c>
-      <c r="BI5">
-        <f t="shared" ref="BI5:BI43" si="2">BF5-T5</f>
+      <c r="BQ5">
+        <f t="shared" ref="BQ5:BQ43" si="3">BN5-T5</f>
         <v>-6.7900000000000002E-2</v>
       </c>
-      <c r="BJ5">
-        <f t="shared" ref="BJ5:BJ43" si="3">BG5-U5</f>
+      <c r="BR5">
+        <f t="shared" ref="BR5:BR43" si="4">BO5-U5</f>
         <v>-722</v>
       </c>
     </row>
-    <row r="6" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -41074,15 +41139,15 @@
         <v>918</v>
       </c>
       <c r="Z6">
-        <f t="shared" ref="Z6:Z43" si="4">W6-S6</f>
+        <f t="shared" ref="Z6:Z43" si="5">W6-S6</f>
         <v>-19.489999999999998</v>
       </c>
       <c r="AA6">
-        <f t="shared" ref="AA6:AA43" si="5">X6-T6</f>
+        <f t="shared" ref="AA6:AA43" si="6">X6-T6</f>
         <v>-0.1578</v>
       </c>
       <c r="AB6">
-        <f t="shared" ref="AB6:AB43" si="6">Y6-U6</f>
+        <f t="shared" ref="AB6:AB43" si="7">Y6-U6</f>
         <v>-918</v>
       </c>
       <c r="AD6">
@@ -41095,15 +41160,15 @@
         <v>2298</v>
       </c>
       <c r="AG6">
-        <f>AD6-AX6</f>
+        <f t="shared" ref="AG6:AG22" si="8">AD6-BF6</f>
         <v>3.078400000000002</v>
       </c>
       <c r="AH6">
-        <f t="shared" ref="AH6:AH22" si="7">AE6-AY6</f>
+        <f t="shared" ref="AH6:AH22" si="9">AE6-BG6</f>
         <v>-3.2021999999999995E-2</v>
       </c>
       <c r="AI6">
-        <f t="shared" ref="AI6:AI22" si="8">AF6-AZ6</f>
+        <f t="shared" ref="AI6:AI22" si="10">AF6-BH6</f>
         <v>1114</v>
       </c>
       <c r="AK6">
@@ -41116,61 +41181,90 @@
         <v>2448</v>
       </c>
       <c r="AN6">
-        <f t="shared" ref="AN6:AN9" si="9">AK6-AD6</f>
+        <f t="shared" ref="AN6:AN9" si="11">AK6-AD6</f>
         <v>75.098799999999997</v>
       </c>
       <c r="AO6">
-        <f t="shared" ref="AO6:AO9" si="10">AL6-AE6</f>
+        <f t="shared" ref="AO6:AO9" si="12">AL6-AE6</f>
         <v>3.2390000000000058E-3</v>
       </c>
       <c r="AP6">
-        <f t="shared" ref="AP6:AP9" si="11">AM6-AF6</f>
+        <f t="shared" ref="AP6:AP9" si="13">AM6-AF6</f>
         <v>150</v>
       </c>
+      <c r="AQ6">
+        <f t="shared" ref="AQ6:AQ43" si="14">AP6/AF6</f>
+        <v>6.5274151436031339E-2</v>
+      </c>
+      <c r="AS6">
+        <v>98.552000000000007</v>
+      </c>
+      <c r="AT6">
+        <v>0.11679</v>
+      </c>
+      <c r="AU6">
+        <v>1296</v>
+      </c>
+      <c r="AV6">
+        <f t="shared" ref="AV6:AV43" si="15">AS6-AK6</f>
+        <v>-1.3114999999999952</v>
+      </c>
+      <c r="AW6">
+        <f t="shared" si="1"/>
+        <v>2.1675E-2</v>
+      </c>
       <c r="AX6">
+        <f t="shared" ref="AX6:AX43" si="16">AM6-AU6</f>
+        <v>1152</v>
+      </c>
+      <c r="AY6">
+        <f t="shared" ref="AY6:AY43" si="17">AX6/AM6</f>
+        <v>0.47058823529411764</v>
+      </c>
+      <c r="BF6">
         <v>21.686299999999999</v>
       </c>
-      <c r="AY6">
+      <c r="BG6">
         <v>0.12389799999999999</v>
       </c>
-      <c r="AZ6">
+      <c r="BH6">
         <v>1184</v>
       </c>
-      <c r="BA6">
-        <f t="shared" ref="BA6:BA17" si="12">AX6-BE6</f>
+      <c r="BI6">
+        <f t="shared" ref="BI6:BI17" si="18">BF6-BM6</f>
         <v>0.3882399999999997</v>
       </c>
-      <c r="BB6">
-        <f t="shared" ref="BB6:BB17" si="13">AY6-BF6</f>
+      <c r="BJ6">
+        <f t="shared" ref="BJ6:BJ17" si="19">BG6-BN6</f>
         <v>-2.7019999999999961E-3</v>
       </c>
-      <c r="BC6">
-        <f t="shared" ref="BC6:BC17" si="14">AZ6-BG6</f>
+      <c r="BK6">
+        <f t="shared" ref="BK6:BK17" si="20">BH6-BO6</f>
         <v>-855</v>
       </c>
-      <c r="BE6">
+      <c r="BM6">
         <v>21.29806</v>
       </c>
-      <c r="BF6">
+      <c r="BN6">
         <v>0.12659999999999999</v>
       </c>
-      <c r="BG6">
+      <c r="BO6">
         <v>2039</v>
       </c>
-      <c r="BH6">
-        <f t="shared" si="1"/>
+      <c r="BP6">
+        <f t="shared" si="2"/>
         <v>1.8080600000000011</v>
       </c>
-      <c r="BI6">
-        <f t="shared" si="2"/>
+      <c r="BQ6">
+        <f t="shared" si="3"/>
         <v>-3.1200000000000006E-2</v>
       </c>
-      <c r="BJ6">
-        <f t="shared" si="3"/>
+      <c r="BR6">
+        <f t="shared" si="4"/>
         <v>1121</v>
       </c>
     </row>
-    <row r="7" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -41199,15 +41293,15 @@
         <v>514</v>
       </c>
       <c r="Z7">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-24.05</v>
       </c>
       <c r="AA7">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.17219999999999999</v>
       </c>
       <c r="AB7">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-514</v>
       </c>
       <c r="AD7">
@@ -41220,15 +41314,15 @@
         <v>630</v>
       </c>
       <c r="AG7">
-        <f>AD7-AX7</f>
+        <f t="shared" si="8"/>
         <v>0.74465000000000003</v>
       </c>
       <c r="AH7">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-4.156999999999994E-3</v>
       </c>
       <c r="AI7">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>101</v>
       </c>
       <c r="AK7">
@@ -41241,61 +41335,90 @@
         <v>716</v>
       </c>
       <c r="AN7">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>56.589750000000009</v>
       </c>
       <c r="AO7">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.13285999999999998</v>
       </c>
       <c r="AP7">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>86</v>
       </c>
+      <c r="AQ7">
+        <f t="shared" si="14"/>
+        <v>0.13650793650793649</v>
+      </c>
+      <c r="AS7">
+        <v>86.528989999999993</v>
+      </c>
+      <c r="AT7">
+        <v>0.3301268</v>
+      </c>
+      <c r="AU7">
+        <v>587</v>
+      </c>
+      <c r="AV7">
+        <f t="shared" si="15"/>
+        <v>4.7432899999999876</v>
+      </c>
+      <c r="AW7">
+        <f t="shared" si="1"/>
+        <v>2.8586800000000023E-2</v>
+      </c>
       <c r="AX7">
+        <f t="shared" si="16"/>
+        <v>129</v>
+      </c>
+      <c r="AY7">
+        <f t="shared" si="17"/>
+        <v>0.18016759776536312</v>
+      </c>
+      <c r="BF7">
         <v>24.4513</v>
       </c>
-      <c r="AY7">
+      <c r="BG7">
         <v>0.17283699999999999</v>
       </c>
-      <c r="AZ7">
+      <c r="BH7">
         <v>529</v>
       </c>
-      <c r="BA7">
-        <f t="shared" si="12"/>
+      <c r="BI7">
+        <f t="shared" si="18"/>
         <v>-2.5864000000000011</v>
       </c>
-      <c r="BB7">
-        <f t="shared" si="13"/>
+      <c r="BJ7">
+        <f t="shared" si="19"/>
         <v>3.7637000000000004E-2</v>
       </c>
-      <c r="BC7">
-        <f t="shared" si="14"/>
+      <c r="BK7">
+        <f t="shared" si="20"/>
         <v>-384</v>
       </c>
-      <c r="BE7" s="81">
+      <c r="BM7" s="81">
         <v>27.037700000000001</v>
       </c>
-      <c r="BF7">
+      <c r="BN7">
         <v>0.13519999999999999</v>
       </c>
-      <c r="BG7">
+      <c r="BO7">
         <v>913</v>
       </c>
-      <c r="BH7">
-        <f t="shared" si="1"/>
+      <c r="BP7">
+        <f t="shared" si="2"/>
         <v>2.9877000000000002</v>
       </c>
-      <c r="BI7">
-        <f t="shared" si="2"/>
+      <c r="BQ7">
+        <f t="shared" si="3"/>
         <v>-3.7000000000000005E-2</v>
       </c>
-      <c r="BJ7">
-        <f t="shared" si="3"/>
+      <c r="BR7">
+        <f t="shared" si="4"/>
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -41333,15 +41456,15 @@
         <v>434</v>
       </c>
       <c r="Z8">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-8.4600000000000009</v>
       </c>
       <c r="AA8">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.2122</v>
       </c>
       <c r="AB8">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-434</v>
       </c>
       <c r="AD8">
@@ -41354,15 +41477,15 @@
         <v>868</v>
       </c>
       <c r="AG8">
-        <f>AD8-AX8</f>
+        <f t="shared" si="8"/>
         <v>2.6120000000000001</v>
       </c>
       <c r="AH8">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-4.1987999999999998E-2</v>
       </c>
       <c r="AI8">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>191</v>
       </c>
       <c r="AK8">
@@ -41375,52 +41498,81 @@
         <v>929</v>
       </c>
       <c r="AN8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>29.330920000000003</v>
       </c>
       <c r="AO8">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>7.0418000000000008E-2</v>
       </c>
       <c r="AP8">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>61</v>
       </c>
+      <c r="AQ8">
+        <f t="shared" si="14"/>
+        <v>7.0276497695852536E-2</v>
+      </c>
+      <c r="AS8">
+        <v>42.622</v>
+      </c>
+      <c r="AT8">
+        <v>0.24540000000000001</v>
+      </c>
+      <c r="AU8">
+        <v>735</v>
+      </c>
+      <c r="AV8">
+        <f t="shared" si="15"/>
+        <v>1.0606799999999978</v>
+      </c>
+      <c r="AW8">
+        <f t="shared" si="1"/>
+        <v>9.000000000000008E-3</v>
+      </c>
       <c r="AX8">
+        <f t="shared" si="16"/>
+        <v>194</v>
+      </c>
+      <c r="AY8">
+        <f t="shared" si="17"/>
+        <v>0.20882669537136705</v>
+      </c>
+      <c r="BF8">
         <v>9.6183999999999994</v>
       </c>
-      <c r="AY8">
+      <c r="BG8">
         <v>0.20796999999999999</v>
       </c>
-      <c r="AZ8">
+      <c r="BH8">
         <v>677</v>
       </c>
-      <c r="BA8">
-        <f t="shared" si="12"/>
+      <c r="BI8">
+        <f t="shared" si="18"/>
         <v>9.6183999999999994</v>
       </c>
-      <c r="BB8">
-        <f t="shared" si="13"/>
+      <c r="BJ8">
+        <f t="shared" si="19"/>
         <v>0.20796999999999999</v>
       </c>
-      <c r="BC8">
-        <f t="shared" si="14"/>
+      <c r="BK8">
+        <f t="shared" si="20"/>
         <v>677</v>
       </c>
-      <c r="BH8">
-        <f t="shared" si="1"/>
+      <c r="BP8">
+        <f t="shared" si="2"/>
         <v>-8.4600000000000009</v>
       </c>
-      <c r="BI8">
-        <f t="shared" si="2"/>
+      <c r="BQ8">
+        <f t="shared" si="3"/>
         <v>-0.2122</v>
       </c>
-      <c r="BJ8">
-        <f t="shared" si="3"/>
+      <c r="BR8">
+        <f t="shared" si="4"/>
         <v>-434</v>
       </c>
     </row>
-    <row r="9" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -41461,15 +41613,15 @@
         <v>1386</v>
       </c>
       <c r="Z9">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.1599999999999966</v>
       </c>
       <c r="AA9">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.2699999999999998E-2</v>
       </c>
       <c r="AB9">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>304</v>
       </c>
       <c r="AD9">
@@ -41482,15 +41634,15 @@
         <v>2004</v>
       </c>
       <c r="AG9">
-        <f>AD9-AX9</f>
+        <f t="shared" si="8"/>
         <v>24.653100000000002</v>
       </c>
       <c r="AH9">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-1.3899999999999996E-2</v>
       </c>
       <c r="AI9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>248</v>
       </c>
       <c r="AK9">
@@ -41503,61 +41655,90 @@
         <v>2228</v>
       </c>
       <c r="AN9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>111.53399999999999</v>
       </c>
       <c r="AO9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>8.3379999999999982E-2</v>
       </c>
       <c r="AP9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>224</v>
       </c>
+      <c r="AQ9">
+        <f t="shared" si="14"/>
+        <v>0.11177644710578842</v>
+      </c>
+      <c r="AS9">
+        <v>179.22739999999999</v>
+      </c>
+      <c r="AT9">
+        <v>0.22117870000000001</v>
+      </c>
+      <c r="AU9">
+        <v>1950</v>
+      </c>
+      <c r="AV9">
+        <f t="shared" si="15"/>
+        <v>-6.6106000000000051</v>
+      </c>
+      <c r="AW9">
+        <f t="shared" si="1"/>
+        <v>8.3487000000000144E-3</v>
+      </c>
       <c r="AX9">
+        <f t="shared" si="16"/>
+        <v>278</v>
+      </c>
+      <c r="AY9">
+        <f t="shared" si="17"/>
+        <v>0.12477558348294435</v>
+      </c>
+      <c r="BF9">
         <v>49.6509</v>
       </c>
-      <c r="AY9">
+      <c r="BG9">
         <v>0.14335000000000001</v>
       </c>
-      <c r="AZ9">
+      <c r="BH9">
         <v>1756</v>
       </c>
-      <c r="BA9">
-        <f t="shared" si="12"/>
+      <c r="BI9">
+        <f t="shared" si="18"/>
         <v>-2.4835800000000035</v>
       </c>
-      <c r="BB9">
-        <f t="shared" si="13"/>
+      <c r="BJ9">
+        <f t="shared" si="19"/>
         <v>6.6100000000000006E-2</v>
       </c>
-      <c r="BC9">
-        <f t="shared" si="14"/>
+      <c r="BK9">
+        <f t="shared" si="20"/>
         <v>-793</v>
       </c>
-      <c r="BE9">
+      <c r="BM9">
         <v>52.134480000000003</v>
       </c>
-      <c r="BF9">
+      <c r="BN9">
         <v>7.7249999999999999E-2</v>
       </c>
-      <c r="BG9">
+      <c r="BO9">
         <v>2549</v>
       </c>
-      <c r="BH9">
-        <f t="shared" si="1"/>
+      <c r="BP9">
+        <f t="shared" si="2"/>
         <v>5.4644800000000018</v>
       </c>
-      <c r="BI9">
-        <f t="shared" si="2"/>
+      <c r="BQ9">
+        <f t="shared" si="3"/>
         <v>-7.2650000000000006E-2</v>
       </c>
-      <c r="BJ9">
-        <f t="shared" si="3"/>
+      <c r="BR9">
+        <f t="shared" si="4"/>
         <v>1467</v>
       </c>
     </row>
-    <row r="10" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -41606,15 +41787,15 @@
         <v>628</v>
       </c>
       <c r="Z10">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.12000000000000099</v>
       </c>
       <c r="AA10">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.4399999999999996E-2</v>
       </c>
       <c r="AB10">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AD10">
@@ -41627,15 +41808,15 @@
         <v>883</v>
       </c>
       <c r="AG10">
-        <f>AD10-AX10</f>
+        <f t="shared" si="8"/>
         <v>8.2198600000000006</v>
       </c>
       <c r="AH10">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-1.2492000000000003E-2</v>
       </c>
       <c r="AI10">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26</v>
       </c>
       <c r="AK10">
@@ -41648,52 +41829,81 @@
         <v>1015</v>
       </c>
       <c r="AN10">
-        <f t="shared" ref="AN10:AN13" si="15">AK10-AD10</f>
+        <f t="shared" ref="AN10:AN13" si="21">AK10-AD10</f>
         <v>43.599399999999989</v>
       </c>
       <c r="AO10">
-        <f t="shared" ref="AO10:AO13" si="16">AL10-AE10</f>
+        <f t="shared" ref="AO10:AO13" si="22">AL10-AE10</f>
         <v>0.12449200000000001</v>
       </c>
       <c r="AP10">
-        <f t="shared" ref="AP10:AP13" si="17">AM10-AF10</f>
+        <f t="shared" ref="AP10:AP13" si="23">AM10-AF10</f>
         <v>132</v>
       </c>
+      <c r="AQ10">
+        <f t="shared" si="14"/>
+        <v>0.14949037372593432</v>
+      </c>
+      <c r="AS10">
+        <v>72.649799999999999</v>
+      </c>
+      <c r="AT10">
+        <v>0.2135</v>
+      </c>
+      <c r="AU10">
+        <v>1015</v>
+      </c>
+      <c r="AV10">
+        <f>AS18-AK10</f>
+        <v>-15.236599999999996</v>
+      </c>
+      <c r="AW10">
+        <f>AT18-AL10</f>
+        <v>0.11343999999999999</v>
+      </c>
       <c r="AX10">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AY10">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BF10">
         <v>20.887740000000001</v>
       </c>
-      <c r="AY10">
+      <c r="BG10">
         <v>0.10326</v>
       </c>
-      <c r="AZ10">
+      <c r="BH10">
         <v>857</v>
       </c>
-      <c r="BA10">
-        <f t="shared" si="12"/>
+      <c r="BI10">
+        <f t="shared" si="18"/>
         <v>20.887740000000001</v>
       </c>
-      <c r="BB10">
-        <f t="shared" si="13"/>
+      <c r="BJ10">
+        <f t="shared" si="19"/>
         <v>0.10326</v>
       </c>
-      <c r="BC10">
-        <f t="shared" si="14"/>
+      <c r="BK10">
+        <f t="shared" si="20"/>
         <v>857</v>
       </c>
-      <c r="BH10">
-        <f t="shared" si="1"/>
+      <c r="BP10">
+        <f t="shared" si="2"/>
         <v>-18.89</v>
       </c>
-      <c r="BI10">
-        <f t="shared" si="2"/>
+      <c r="BQ10">
+        <f t="shared" si="3"/>
         <v>-0.1711</v>
       </c>
-      <c r="BJ10">
-        <f t="shared" si="3"/>
+      <c r="BR10">
+        <f t="shared" si="4"/>
         <v>-628</v>
       </c>
     </row>
-    <row r="11" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -41722,15 +41932,15 @@
         <v>525</v>
       </c>
       <c r="Z11">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-16.059999999999999</v>
       </c>
       <c r="AA11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.1303</v>
       </c>
       <c r="AB11">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-525</v>
       </c>
       <c r="AD11">
@@ -41743,15 +41953,15 @@
         <v>988</v>
       </c>
       <c r="AG11">
-        <f>AD11-AX11</f>
+        <f t="shared" si="8"/>
         <v>3.8467199999999977</v>
       </c>
       <c r="AH11">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-3.033000000000001E-2</v>
       </c>
       <c r="AI11">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>446</v>
       </c>
       <c r="AK11">
@@ -41764,61 +41974,90 @@
         <v>1133</v>
       </c>
       <c r="AN11">
+        <f t="shared" si="21"/>
+        <v>48.030640000000005</v>
+      </c>
+      <c r="AO11">
+        <f t="shared" si="22"/>
+        <v>6.7830000000000015E-2</v>
+      </c>
+      <c r="AP11">
+        <f t="shared" si="23"/>
+        <v>145</v>
+      </c>
+      <c r="AQ11">
+        <f t="shared" si="14"/>
+        <v>0.14676113360323886</v>
+      </c>
+      <c r="AS11">
+        <v>54.328000000000003</v>
+      </c>
+      <c r="AT11">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="AU11">
+        <v>582</v>
+      </c>
+      <c r="AV11">
         <f t="shared" si="15"/>
-        <v>48.030640000000005</v>
-      </c>
-      <c r="AO11">
+        <v>-14.168599999999998</v>
+      </c>
+      <c r="AW11">
+        <f t="shared" si="1"/>
+        <v>3.2799999999999996E-2</v>
+      </c>
+      <c r="AX11">
         <f t="shared" si="16"/>
-        <v>6.7830000000000015E-2</v>
-      </c>
-      <c r="AP11">
+        <v>551</v>
+      </c>
+      <c r="AY11">
         <f t="shared" si="17"/>
-        <v>145</v>
-      </c>
-      <c r="AX11">
+        <v>0.48631950573698146</v>
+      </c>
+      <c r="BF11">
         <v>16.619240000000001</v>
       </c>
-      <c r="AY11">
+      <c r="BG11">
         <v>0.1237</v>
       </c>
-      <c r="AZ11">
+      <c r="BH11">
         <v>542</v>
       </c>
-      <c r="BA11">
-        <f t="shared" si="12"/>
+      <c r="BI11">
+        <f t="shared" si="18"/>
         <v>-2.7645599999999995</v>
       </c>
-      <c r="BB11">
-        <f t="shared" si="13"/>
+      <c r="BJ11">
+        <f t="shared" si="19"/>
         <v>4.224E-2</v>
       </c>
-      <c r="BC11">
-        <f t="shared" si="14"/>
+      <c r="BK11">
+        <f t="shared" si="20"/>
         <v>-320</v>
       </c>
-      <c r="BE11">
+      <c r="BM11">
         <v>19.383800000000001</v>
       </c>
-      <c r="BF11">
+      <c r="BN11">
         <v>8.1460000000000005E-2</v>
       </c>
-      <c r="BG11">
+      <c r="BO11">
         <v>862</v>
       </c>
-      <c r="BH11">
-        <f t="shared" si="1"/>
+      <c r="BP11">
+        <f t="shared" si="2"/>
         <v>3.3238000000000021</v>
       </c>
-      <c r="BI11">
-        <f t="shared" si="2"/>
+      <c r="BQ11">
+        <f t="shared" si="3"/>
         <v>-4.8839999999999995E-2</v>
       </c>
-      <c r="BJ11">
-        <f t="shared" si="3"/>
+      <c r="BR11">
+        <f t="shared" si="4"/>
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -41856,27 +42095,27 @@
         <v>588</v>
       </c>
       <c r="Z12">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-20.85</v>
       </c>
       <c r="AA12">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.32519999999999999</v>
       </c>
       <c r="AB12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-588</v>
       </c>
       <c r="AG12">
-        <f>AD12-AX12</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK12">
@@ -41889,43 +42128,72 @@
         <v>1157</v>
       </c>
       <c r="AN12">
+        <f t="shared" si="21"/>
+        <v>95.403899999999993</v>
+      </c>
+      <c r="AO12">
+        <f t="shared" si="22"/>
+        <v>0.29437999999999998</v>
+      </c>
+      <c r="AP12">
+        <f t="shared" si="23"/>
+        <v>1157</v>
+      </c>
+      <c r="AQ12" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS12">
+        <v>92.150899999999993</v>
+      </c>
+      <c r="AT12">
+        <v>0.335756</v>
+      </c>
+      <c r="AU12">
+        <v>1041</v>
+      </c>
+      <c r="AV12">
         <f t="shared" si="15"/>
-        <v>95.403899999999993</v>
-      </c>
-      <c r="AO12">
+        <v>-3.2530000000000001</v>
+      </c>
+      <c r="AW12">
+        <f t="shared" si="1"/>
+        <v>4.1376000000000024E-2</v>
+      </c>
+      <c r="AX12">
         <f t="shared" si="16"/>
-        <v>0.29437999999999998</v>
-      </c>
-      <c r="AP12">
+        <v>116</v>
+      </c>
+      <c r="AY12">
         <f t="shared" si="17"/>
-        <v>1157</v>
-      </c>
-      <c r="BA12">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BB12">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="BC12">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="BH12">
-        <f t="shared" si="1"/>
+        <v>0.10025929127052723</v>
+      </c>
+      <c r="BI12">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="BJ12">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="BK12">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="BP12">
+        <f t="shared" si="2"/>
         <v>-20.85</v>
       </c>
-      <c r="BI12">
-        <f t="shared" si="2"/>
+      <c r="BQ12">
+        <f t="shared" si="3"/>
         <v>-0.32519999999999999</v>
       </c>
-      <c r="BJ12">
-        <f t="shared" si="3"/>
+      <c r="BR12">
+        <f t="shared" si="4"/>
         <v>-588</v>
       </c>
     </row>
-    <row r="13" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -41973,27 +42241,27 @@
         <v>799</v>
       </c>
       <c r="Z13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.18999999999999773</v>
       </c>
       <c r="AA13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1.5899999999999984E-2</v>
       </c>
       <c r="AB13">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>21</v>
       </c>
       <c r="AG13">
-        <f>AD13-AX13</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH13">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK13">
@@ -42006,43 +42274,72 @@
         <v>1375</v>
       </c>
       <c r="AN13">
+        <f t="shared" si="21"/>
+        <v>114.5904</v>
+      </c>
+      <c r="AO13">
+        <f t="shared" si="22"/>
+        <v>0.16016</v>
+      </c>
+      <c r="AP13">
+        <f t="shared" si="23"/>
+        <v>1375</v>
+      </c>
+      <c r="AQ13" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS13">
+        <v>116.435</v>
+      </c>
+      <c r="AT13">
+        <v>0.16267999999999999</v>
+      </c>
+      <c r="AU13">
+        <v>1264</v>
+      </c>
+      <c r="AV13">
         <f t="shared" si="15"/>
-        <v>114.5904</v>
-      </c>
-      <c r="AO13">
+        <v>1.8445999999999998</v>
+      </c>
+      <c r="AW13">
+        <f t="shared" si="1"/>
+        <v>2.5199999999999945E-3</v>
+      </c>
+      <c r="AX13">
         <f t="shared" si="16"/>
-        <v>0.16016</v>
-      </c>
-      <c r="AP13">
+        <v>111</v>
+      </c>
+      <c r="AY13">
         <f t="shared" si="17"/>
-        <v>1375</v>
-      </c>
-      <c r="BA13">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BB13">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="BC13">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="BH13">
-        <f t="shared" si="1"/>
+        <v>8.0727272727272731E-2</v>
+      </c>
+      <c r="BI13">
+        <f t="shared" si="18"/>
+        <v>0</v>
+      </c>
+      <c r="BJ13">
+        <f t="shared" si="19"/>
+        <v>0</v>
+      </c>
+      <c r="BK13">
+        <f t="shared" si="20"/>
+        <v>0</v>
+      </c>
+      <c r="BP13">
+        <f t="shared" si="2"/>
         <v>-33.68</v>
       </c>
-      <c r="BI13">
-        <f t="shared" si="2"/>
+      <c r="BQ13">
+        <f t="shared" si="3"/>
         <v>-0.11020000000000001</v>
       </c>
-      <c r="BJ13">
-        <f t="shared" si="3"/>
+      <c r="BR13">
+        <f t="shared" si="4"/>
         <v>-778</v>
       </c>
     </row>
-    <row r="14" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -42071,15 +42368,15 @@
         <v>514</v>
       </c>
       <c r="Z14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-13.17</v>
       </c>
       <c r="AA14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.2238</v>
       </c>
       <c r="AB14">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-514</v>
       </c>
       <c r="AD14">
@@ -42092,15 +42389,15 @@
         <v>1064</v>
       </c>
       <c r="AG14">
-        <f>AD14-AX14</f>
+        <f t="shared" si="8"/>
         <v>4.7050000000000001</v>
       </c>
       <c r="AH14">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>-8.7299999999999989E-2</v>
       </c>
       <c r="AI14">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>537</v>
       </c>
       <c r="AK14">
@@ -42113,61 +42410,90 @@
         <v>1154</v>
       </c>
       <c r="AN14">
-        <f t="shared" ref="AN14:AN43" si="18">AK14-AD14</f>
+        <f t="shared" ref="AN14:AN43" si="24">AK14-AD14</f>
         <v>53.567700000000002</v>
       </c>
       <c r="AO14">
-        <f t="shared" ref="AO14:AO43" si="19">AL14-AE14</f>
+        <f t="shared" ref="AO14:AO43" si="25">AL14-AE14</f>
         <v>2.8599999999999987E-2</v>
       </c>
       <c r="AP14">
-        <f t="shared" ref="AP14:AP43" si="20">AM14-AF14</f>
+        <f t="shared" ref="AP14:AP43" si="26">AM14-AF14</f>
         <v>90</v>
       </c>
+      <c r="AQ14">
+        <f t="shared" si="14"/>
+        <v>8.4586466165413529E-2</v>
+      </c>
+      <c r="AS14">
+        <v>62.015000000000001</v>
+      </c>
+      <c r="AT14">
+        <v>0.26795999999999998</v>
+      </c>
+      <c r="AU14">
+        <v>586</v>
+      </c>
+      <c r="AV14">
+        <f t="shared" si="15"/>
+        <v>-9.6576000000000022</v>
+      </c>
+      <c r="AW14">
+        <f t="shared" si="1"/>
+        <v>0.11165999999999998</v>
+      </c>
       <c r="AX14">
+        <f t="shared" si="16"/>
+        <v>568</v>
+      </c>
+      <c r="AY14">
+        <f t="shared" si="17"/>
+        <v>0.49220103986135183</v>
+      </c>
+      <c r="BF14">
         <v>13.399900000000001</v>
       </c>
-      <c r="AY14">
+      <c r="BG14">
         <v>0.215</v>
       </c>
-      <c r="AZ14">
+      <c r="BH14">
         <v>527</v>
       </c>
-      <c r="BA14">
-        <f t="shared" si="12"/>
+      <c r="BI14">
+        <f t="shared" si="18"/>
         <v>-0.30439999999999934</v>
       </c>
-      <c r="BB14">
-        <f t="shared" si="13"/>
+      <c r="BJ14">
+        <f t="shared" si="19"/>
         <v>4.0199999999999986E-2</v>
       </c>
-      <c r="BC14">
-        <f t="shared" si="14"/>
+      <c r="BK14">
+        <f t="shared" si="20"/>
         <v>-495</v>
       </c>
-      <c r="BE14">
+      <c r="BM14">
         <v>13.7043</v>
       </c>
-      <c r="BF14">
+      <c r="BN14">
         <v>0.17480000000000001</v>
       </c>
-      <c r="BG14">
+      <c r="BO14">
         <v>1022</v>
       </c>
-      <c r="BH14">
-        <f t="shared" si="1"/>
+      <c r="BP14">
+        <f t="shared" si="2"/>
         <v>0.5343</v>
       </c>
-      <c r="BI14">
-        <f t="shared" si="2"/>
+      <c r="BQ14">
+        <f t="shared" si="3"/>
         <v>-4.8999999999999988E-2</v>
       </c>
-      <c r="BJ14">
-        <f t="shared" si="3"/>
+      <c r="BR14">
+        <f t="shared" si="4"/>
         <v>508</v>
       </c>
     </row>
-    <row r="15" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -42205,27 +42531,27 @@
         <v>663</v>
       </c>
       <c r="Z15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-19.57</v>
       </c>
       <c r="AA15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.23630000000000001</v>
       </c>
       <c r="AB15">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-663</v>
       </c>
       <c r="AG15">
-        <f>AD15-AX15</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH15">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI15">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK15">
@@ -42238,43 +42564,72 @@
         <v>1656</v>
       </c>
       <c r="AN15">
+        <f t="shared" si="24"/>
+        <v>90.829400000000007</v>
+      </c>
+      <c r="AO15">
+        <f t="shared" si="25"/>
+        <v>0.1797</v>
+      </c>
+      <c r="AP15">
+        <f t="shared" si="26"/>
+        <v>1656</v>
+      </c>
+      <c r="AQ15" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS15">
+        <v>88.235200000000006</v>
+      </c>
+      <c r="AT15">
+        <v>0.22417000000000001</v>
+      </c>
+      <c r="AU15">
+        <v>900</v>
+      </c>
+      <c r="AV15">
+        <f t="shared" si="15"/>
+        <v>-2.5942000000000007</v>
+      </c>
+      <c r="AW15">
+        <f t="shared" si="1"/>
+        <v>4.447000000000001E-2</v>
+      </c>
+      <c r="AX15">
+        <f t="shared" si="16"/>
+        <v>756</v>
+      </c>
+      <c r="AY15">
+        <f t="shared" si="17"/>
+        <v>0.45652173913043476</v>
+      </c>
+      <c r="BI15">
         <f t="shared" si="18"/>
-        <v>90.829400000000007</v>
-      </c>
-      <c r="AO15">
+        <v>0</v>
+      </c>
+      <c r="BJ15">
         <f t="shared" si="19"/>
-        <v>0.1797</v>
-      </c>
-      <c r="AP15">
+        <v>0</v>
+      </c>
+      <c r="BK15">
         <f t="shared" si="20"/>
-        <v>1656</v>
-      </c>
-      <c r="BA15">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BB15">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="BC15">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="BH15">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BP15">
+        <f t="shared" si="2"/>
         <v>-19.57</v>
       </c>
-      <c r="BI15">
-        <f t="shared" si="2"/>
+      <c r="BQ15">
+        <f t="shared" si="3"/>
         <v>-0.23630000000000001</v>
       </c>
-      <c r="BJ15">
-        <f t="shared" si="3"/>
+      <c r="BR15">
+        <f t="shared" si="4"/>
         <v>-663</v>
       </c>
     </row>
-    <row r="16" spans="1:68" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:76" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -42303,27 +42658,27 @@
         <v>716</v>
       </c>
       <c r="Z16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-52.53</v>
       </c>
       <c r="AA16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-4.9299999999999997E-2</v>
       </c>
       <c r="AB16">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-716</v>
       </c>
       <c r="AG16">
-        <f>AD16-AX16</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH16">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI16">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK16">
@@ -42336,52 +42691,81 @@
         <v>1396</v>
       </c>
       <c r="AN16">
+        <f t="shared" si="24"/>
+        <v>240.0746</v>
+      </c>
+      <c r="AO16">
+        <f t="shared" si="25"/>
+        <v>8.5360000000000005E-2</v>
+      </c>
+      <c r="AP16">
+        <f t="shared" si="26"/>
+        <v>1396</v>
+      </c>
+      <c r="AQ16" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS16">
+        <v>247.203</v>
+      </c>
+      <c r="AT16">
+        <v>0.104228</v>
+      </c>
+      <c r="AU16">
+        <v>876</v>
+      </c>
+      <c r="AV16">
+        <f t="shared" si="15"/>
+        <v>7.1283999999999992</v>
+      </c>
+      <c r="AW16">
+        <f t="shared" si="1"/>
+        <v>1.8867999999999996E-2</v>
+      </c>
+      <c r="AX16">
+        <f t="shared" si="16"/>
+        <v>520</v>
+      </c>
+      <c r="AY16">
+        <f t="shared" si="17"/>
+        <v>0.37249283667621774</v>
+      </c>
+      <c r="BI16">
         <f t="shared" si="18"/>
-        <v>240.0746</v>
-      </c>
-      <c r="AO16">
+        <v>-53.034950000000002</v>
+      </c>
+      <c r="BJ16">
         <f t="shared" si="19"/>
-        <v>8.5360000000000005E-2</v>
-      </c>
-      <c r="AP16">
+        <v>-5.9695999999999999E-2</v>
+      </c>
+      <c r="BK16">
         <f t="shared" si="20"/>
-        <v>1396</v>
-      </c>
-      <c r="BA16">
-        <f t="shared" si="12"/>
-        <v>-53.034950000000002</v>
-      </c>
-      <c r="BB16">
-        <f t="shared" si="13"/>
-        <v>-5.9695999999999999E-2</v>
-      </c>
-      <c r="BC16">
-        <f t="shared" si="14"/>
         <v>-1133</v>
       </c>
-      <c r="BE16">
+      <c r="BM16">
         <v>53.034950000000002</v>
       </c>
-      <c r="BF16">
+      <c r="BN16">
         <v>5.9695999999999999E-2</v>
       </c>
-      <c r="BG16">
+      <c r="BO16">
         <v>1133</v>
       </c>
-      <c r="BH16">
-        <f t="shared" si="1"/>
+      <c r="BP16">
+        <f t="shared" si="2"/>
         <v>0.5049500000000009</v>
       </c>
-      <c r="BI16">
-        <f t="shared" si="2"/>
+      <c r="BQ16">
+        <f t="shared" si="3"/>
         <v>1.0396000000000002E-2</v>
       </c>
-      <c r="BJ16">
-        <f t="shared" si="3"/>
+      <c r="BR16">
+        <f t="shared" si="4"/>
         <v>417</v>
       </c>
     </row>
-    <row r="17" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -42428,27 +42812,27 @@
         <v>288</v>
       </c>
       <c r="Z17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9199999999999982</v>
       </c>
       <c r="AA17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.0000000000000009E-3</v>
       </c>
       <c r="AB17">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>57</v>
       </c>
       <c r="AG17">
-        <f>AD17-AX17</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH17">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI17">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK17">
@@ -42461,43 +42845,72 @@
         <v>527</v>
       </c>
       <c r="AN17">
+        <f t="shared" si="24"/>
+        <v>151.08240000000001</v>
+      </c>
+      <c r="AO17">
+        <f t="shared" si="25"/>
+        <v>0.36549999999999999</v>
+      </c>
+      <c r="AP17">
+        <f t="shared" si="26"/>
+        <v>527</v>
+      </c>
+      <c r="AQ17" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS17">
+        <v>164.26859999999999</v>
+      </c>
+      <c r="AT17">
+        <v>0.31039</v>
+      </c>
+      <c r="AU17">
+        <v>380</v>
+      </c>
+      <c r="AV17">
+        <f t="shared" si="15"/>
+        <v>13.186199999999985</v>
+      </c>
+      <c r="AW17">
+        <f t="shared" si="1"/>
+        <v>-5.5109999999999992E-2</v>
+      </c>
+      <c r="AX17">
+        <f t="shared" si="16"/>
+        <v>147</v>
+      </c>
+      <c r="AY17">
+        <f t="shared" si="17"/>
+        <v>0.27893738140417457</v>
+      </c>
+      <c r="BI17">
         <f t="shared" si="18"/>
-        <v>151.08240000000001</v>
-      </c>
-      <c r="AO17">
+        <v>0</v>
+      </c>
+      <c r="BJ17">
         <f t="shared" si="19"/>
-        <v>0.36549999999999999</v>
-      </c>
-      <c r="AP17">
+        <v>0</v>
+      </c>
+      <c r="BK17">
         <f t="shared" si="20"/>
-        <v>527</v>
-      </c>
-      <c r="BA17">
-        <f t="shared" si="12"/>
-        <v>0</v>
-      </c>
-      <c r="BB17">
-        <f t="shared" si="13"/>
-        <v>0</v>
-      </c>
-      <c r="BC17">
-        <f t="shared" si="14"/>
-        <v>0</v>
-      </c>
-      <c r="BH17">
-        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="BP17">
+        <f t="shared" si="2"/>
         <v>-31.77</v>
       </c>
-      <c r="BI17">
-        <f t="shared" si="2"/>
+      <c r="BQ17">
+        <f t="shared" si="3"/>
         <v>-0.2361</v>
       </c>
-      <c r="BJ17">
-        <f t="shared" si="3"/>
+      <c r="BR17">
+        <f t="shared" si="4"/>
         <v>-231</v>
       </c>
     </row>
-    <row r="18" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -42544,27 +42957,27 @@
         <v>383</v>
       </c>
       <c r="Z18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.1899999999999995</v>
       </c>
       <c r="AA18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.0599999999999988E-2</v>
       </c>
       <c r="AB18">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>40</v>
       </c>
       <c r="AG18">
-        <f>AD18-AX18</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" ref="AH18" si="21">AE18-AY18</f>
+        <f t="shared" ref="AH18" si="27">AE18-BG18</f>
         <v>0</v>
       </c>
       <c r="AI18">
-        <f t="shared" ref="AI18" si="22">AF18-AZ18</f>
+        <f t="shared" ref="AI18" si="28">AF18-BH18</f>
         <v>0</v>
       </c>
       <c r="AK18">
@@ -42577,31 +42990,60 @@
         <v>947</v>
       </c>
       <c r="AN18">
-        <f t="shared" ref="AN18" si="23">AK18-AD18</f>
+        <f t="shared" ref="AN18" si="29">AK18-AD18</f>
         <v>76.399000000000001</v>
       </c>
       <c r="AO18">
-        <f t="shared" ref="AO18" si="24">AL18-AE18</f>
+        <f t="shared" ref="AO18" si="30">AL18-AE18</f>
         <v>0.15029999999999999</v>
       </c>
       <c r="AP18">
-        <f t="shared" ref="AP18" si="25">AM18-AF18</f>
+        <f t="shared" ref="AP18" si="31">AM18-AF18</f>
         <v>947</v>
       </c>
-      <c r="BH18">
-        <f t="shared" si="1"/>
+      <c r="AQ18" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS18">
+        <v>57.470399999999998</v>
+      </c>
+      <c r="AT18">
+        <v>0.32869999999999999</v>
+      </c>
+      <c r="AU18">
+        <v>477</v>
+      </c>
+      <c r="AV18">
+        <f t="shared" ref="AV18" si="32">AS18-AK18</f>
+        <v>-18.928600000000003</v>
+      </c>
+      <c r="AW18">
+        <f t="shared" ref="AW18" si="33">AT18-AL18</f>
+        <v>0.1784</v>
+      </c>
+      <c r="AX18">
+        <f t="shared" si="16"/>
+        <v>470</v>
+      </c>
+      <c r="AY18">
+        <f t="shared" si="17"/>
+        <v>0.49630411826821541</v>
+      </c>
+      <c r="BP18">
+        <f t="shared" si="2"/>
         <v>-13.96</v>
       </c>
-      <c r="BI18">
-        <f t="shared" si="2"/>
+      <c r="BQ18">
+        <f t="shared" si="3"/>
         <v>-0.1061</v>
       </c>
-      <c r="BJ18">
-        <f t="shared" si="3"/>
+      <c r="BR18">
+        <f t="shared" si="4"/>
         <v>-343</v>
       </c>
     </row>
-    <row r="19" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -42640,27 +43082,27 @@
         <v>320</v>
       </c>
       <c r="Z19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-22.79</v>
       </c>
       <c r="AA19">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.28999999999999998</v>
       </c>
       <c r="AB19">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-320</v>
       </c>
       <c r="AG19">
-        <f>AD19-AX19</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH19">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK19">
@@ -42673,31 +43115,60 @@
         <v>734</v>
       </c>
       <c r="AN19">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>80.852900000000005</v>
       </c>
       <c r="AO19">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.24697</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>734</v>
       </c>
-      <c r="BH19">
+      <c r="AQ19" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS19">
+        <v>79.593800000000002</v>
+      </c>
+      <c r="AT19">
+        <v>0.25069999999999998</v>
+      </c>
+      <c r="AU19">
+        <v>599</v>
+      </c>
+      <c r="AV19">
+        <f t="shared" si="15"/>
+        <v>-1.2591000000000037</v>
+      </c>
+      <c r="AW19">
         <f t="shared" si="1"/>
+        <v>3.7299999999999833E-3</v>
+      </c>
+      <c r="AX19">
+        <f t="shared" si="16"/>
+        <v>135</v>
+      </c>
+      <c r="AY19">
+        <f t="shared" si="17"/>
+        <v>0.18392370572207084</v>
+      </c>
+      <c r="BP19">
+        <f t="shared" si="2"/>
         <v>-22.79</v>
       </c>
-      <c r="BI19">
-        <f t="shared" si="2"/>
+      <c r="BQ19">
+        <f t="shared" si="3"/>
         <v>-0.28999999999999998</v>
       </c>
-      <c r="BJ19">
-        <f t="shared" si="3"/>
+      <c r="BR19">
+        <f t="shared" si="4"/>
         <v>-320</v>
       </c>
     </row>
-    <row r="20" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -42726,27 +43197,27 @@
         <v>283</v>
       </c>
       <c r="Z20">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-63.69</v>
       </c>
       <c r="AA20">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.1002</v>
       </c>
       <c r="AB20">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-283</v>
       </c>
       <c r="AG20">
-        <f>AD20-AX20</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK20">
@@ -42759,40 +43230,69 @@
         <v>651</v>
       </c>
       <c r="AN20">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>225.16650000000001</v>
       </c>
       <c r="AO20">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.1212</v>
       </c>
       <c r="AP20">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>651</v>
       </c>
-      <c r="BE20">
+      <c r="AQ20" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS20">
+        <v>210.01519999999999</v>
+      </c>
+      <c r="AT20">
+        <v>0.1356</v>
+      </c>
+      <c r="AU20">
+        <v>377</v>
+      </c>
+      <c r="AV20">
+        <f t="shared" si="15"/>
+        <v>-15.15130000000002</v>
+      </c>
+      <c r="AW20">
+        <f t="shared" si="1"/>
+        <v>1.4399999999999996E-2</v>
+      </c>
+      <c r="AX20">
+        <f t="shared" si="16"/>
+        <v>274</v>
+      </c>
+      <c r="AY20">
+        <f t="shared" si="17"/>
+        <v>0.42089093701996927</v>
+      </c>
+      <c r="BM20">
         <v>68.383750000000006</v>
       </c>
-      <c r="BF20">
+      <c r="BN20">
         <v>0.11585139999999999</v>
       </c>
-      <c r="BG20">
+      <c r="BO20">
         <v>454</v>
       </c>
-      <c r="BH20">
-        <f t="shared" si="1"/>
+      <c r="BP20">
+        <f t="shared" si="2"/>
         <v>4.6937500000000085</v>
       </c>
-      <c r="BI20">
-        <f t="shared" si="2"/>
+      <c r="BQ20">
+        <f t="shared" si="3"/>
         <v>1.5651399999999996E-2</v>
       </c>
-      <c r="BJ20">
-        <f t="shared" si="3"/>
+      <c r="BR20">
+        <f t="shared" si="4"/>
         <v>171</v>
       </c>
     </row>
-    <row r="21" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -42842,27 +43342,27 @@
         <v>752</v>
       </c>
       <c r="Z21">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.1120000000000001</v>
       </c>
       <c r="AA21">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0.06</v>
       </c>
       <c r="AB21">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>106</v>
       </c>
       <c r="AG21">
-        <f>AD21-AX21</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK21">
@@ -42875,31 +43375,60 @@
         <v>1742</v>
       </c>
       <c r="AN21">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>48.740499999999997</v>
       </c>
       <c r="AO21">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.1769</v>
       </c>
       <c r="AP21">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>1742</v>
       </c>
-      <c r="BH21">
+      <c r="AQ21" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS21">
+        <v>41.736699999999999</v>
+      </c>
+      <c r="AT21">
+        <v>0.21586</v>
+      </c>
+      <c r="AU21">
+        <v>1132</v>
+      </c>
+      <c r="AV21">
+        <f t="shared" si="15"/>
+        <v>-7.0037999999999982</v>
+      </c>
+      <c r="AW21">
         <f t="shared" si="1"/>
+        <v>3.8959999999999995E-2</v>
+      </c>
+      <c r="AX21">
+        <f t="shared" si="16"/>
+        <v>610</v>
+      </c>
+      <c r="AY21">
+        <f t="shared" si="17"/>
+        <v>0.35017221584385766</v>
+      </c>
+      <c r="BP21">
+        <f t="shared" si="2"/>
         <v>-11.31</v>
       </c>
-      <c r="BI21">
-        <f t="shared" si="2"/>
+      <c r="BQ21">
+        <f t="shared" si="3"/>
         <v>-0.11219999999999999</v>
       </c>
-      <c r="BJ21">
-        <f t="shared" si="3"/>
+      <c r="BR21">
+        <f t="shared" si="4"/>
         <v>-646</v>
       </c>
     </row>
-    <row r="22" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -42937,27 +43466,27 @@
         <v>236</v>
       </c>
       <c r="Z22">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-10.199999999999999</v>
       </c>
       <c r="AA22">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.37130000000000002</v>
       </c>
       <c r="AB22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-236</v>
       </c>
       <c r="AG22">
-        <f>AD22-AX22</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AH22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="AI22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="AK22">
@@ -42970,31 +43499,60 @@
         <v>963</v>
       </c>
       <c r="AN22">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>56.912999999999997</v>
       </c>
       <c r="AO22">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.26650000000000001</v>
       </c>
       <c r="AP22">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>963</v>
       </c>
-      <c r="BH22">
+      <c r="AQ22" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS22">
+        <v>41.099600000000002</v>
+      </c>
+      <c r="AT22">
+        <v>0.36631999999999998</v>
+      </c>
+      <c r="AU22">
+        <v>559</v>
+      </c>
+      <c r="AV22">
+        <f t="shared" si="15"/>
+        <v>-15.813399999999994</v>
+      </c>
+      <c r="AW22">
         <f t="shared" si="1"/>
+        <v>9.9819999999999964E-2</v>
+      </c>
+      <c r="AX22">
+        <f t="shared" si="16"/>
+        <v>404</v>
+      </c>
+      <c r="AY22">
+        <f t="shared" si="17"/>
+        <v>0.41952232606438211</v>
+      </c>
+      <c r="BP22">
+        <f t="shared" si="2"/>
         <v>-10.199999999999999</v>
       </c>
-      <c r="BI22">
-        <f t="shared" si="2"/>
+      <c r="BQ22">
+        <f t="shared" si="3"/>
         <v>-0.37130000000000002</v>
       </c>
-      <c r="BJ22">
-        <f t="shared" si="3"/>
+      <c r="BR22">
+        <f t="shared" si="4"/>
         <v>-236</v>
       </c>
     </row>
-    <row r="23" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -43023,15 +43581,15 @@
         <v>323</v>
       </c>
       <c r="Z23">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-14.93</v>
       </c>
       <c r="AA23">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.1002</v>
       </c>
       <c r="AB23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-323</v>
       </c>
       <c r="AK23">
@@ -43044,40 +43602,69 @@
         <v>579</v>
       </c>
       <c r="AN23">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>74.535600000000002</v>
       </c>
       <c r="AO23">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.13339999999999999</v>
       </c>
       <c r="AP23">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>579</v>
       </c>
-      <c r="BE23">
+      <c r="AQ23" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS23">
+        <v>86.693399999999997</v>
+      </c>
+      <c r="AT23">
+        <v>7.6909000000000005E-2</v>
+      </c>
+      <c r="AU23">
+        <v>418</v>
+      </c>
+      <c r="AV23">
+        <f t="shared" si="15"/>
+        <v>12.157799999999995</v>
+      </c>
+      <c r="AW23">
+        <f t="shared" si="1"/>
+        <v>-5.6490999999999986E-2</v>
+      </c>
+      <c r="AX23">
+        <f t="shared" si="16"/>
+        <v>161</v>
+      </c>
+      <c r="AY23">
+        <f t="shared" si="17"/>
+        <v>0.27806563039723664</v>
+      </c>
+      <c r="BM23">
         <v>15.04355</v>
       </c>
-      <c r="BF23">
+      <c r="BN23">
         <v>9.3257999999999994E-2</v>
       </c>
-      <c r="BG23">
+      <c r="BO23">
         <v>829</v>
       </c>
-      <c r="BH23">
-        <f t="shared" si="1"/>
+      <c r="BP23">
+        <f t="shared" si="2"/>
         <v>0.11355000000000004</v>
       </c>
-      <c r="BI23">
-        <f t="shared" si="2"/>
+      <c r="BQ23">
+        <f t="shared" si="3"/>
         <v>-6.9420000000000037E-3</v>
       </c>
-      <c r="BJ23">
-        <f t="shared" si="3"/>
+      <c r="BR23">
+        <f t="shared" si="4"/>
         <v>506</v>
       </c>
     </row>
-    <row r="24" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -43106,15 +43693,15 @@
         <v>283</v>
       </c>
       <c r="Z24">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-23.49</v>
       </c>
       <c r="AA24">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.1487</v>
       </c>
       <c r="AB24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-283</v>
       </c>
       <c r="AK24">
@@ -43127,40 +43714,69 @@
         <v>462</v>
       </c>
       <c r="AN24">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>121.116</v>
       </c>
       <c r="AO24">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.2165</v>
       </c>
       <c r="AP24">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>462</v>
       </c>
-      <c r="BE24">
+      <c r="AQ24" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS24">
+        <v>126.21339999999999</v>
+      </c>
+      <c r="AT24">
+        <v>0.23744999999999999</v>
+      </c>
+      <c r="AU24">
+        <v>385</v>
+      </c>
+      <c r="AV24">
+        <f t="shared" si="15"/>
+        <v>5.0973999999999933</v>
+      </c>
+      <c r="AW24">
+        <f t="shared" si="1"/>
+        <v>2.0949999999999996E-2</v>
+      </c>
+      <c r="AX24">
+        <f t="shared" si="16"/>
+        <v>77</v>
+      </c>
+      <c r="AY24">
+        <f t="shared" si="17"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="BM24">
         <v>21.397960000000001</v>
       </c>
-      <c r="BF24">
+      <c r="BN24">
         <v>0.14054</v>
       </c>
-      <c r="BG24">
+      <c r="BO24">
         <v>602</v>
       </c>
-      <c r="BH24">
-        <f t="shared" si="1"/>
+      <c r="BP24">
+        <f t="shared" si="2"/>
         <v>-2.0920399999999972</v>
       </c>
-      <c r="BI24">
-        <f t="shared" si="2"/>
+      <c r="BQ24">
+        <f t="shared" si="3"/>
         <v>-8.1600000000000006E-3</v>
       </c>
-      <c r="BJ24">
-        <f t="shared" si="3"/>
+      <c r="BR24">
+        <f t="shared" si="4"/>
         <v>319</v>
       </c>
     </row>
-    <row r="25" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -43208,15 +43824,15 @@
         <v>286</v>
       </c>
       <c r="Z25">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>3.6370000000000005</v>
       </c>
       <c r="AA25">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>6.0100000000000015E-2</v>
       </c>
       <c r="AB25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>82</v>
       </c>
       <c r="AK25">
@@ -43229,31 +43845,60 @@
         <v>599</v>
       </c>
       <c r="AN25">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>98.161590000000004</v>
       </c>
       <c r="AO25">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.26608999999999999</v>
       </c>
       <c r="AP25">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>599</v>
       </c>
-      <c r="BH25">
+      <c r="AQ25" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS25">
+        <v>112.77500000000001</v>
+      </c>
+      <c r="AT25">
+        <v>0.25979999999999998</v>
+      </c>
+      <c r="AU25">
+        <v>341</v>
+      </c>
+      <c r="AV25">
+        <f t="shared" si="15"/>
+        <v>14.613410000000002</v>
+      </c>
+      <c r="AW25">
         <f t="shared" si="1"/>
+        <v>-6.2900000000000178E-3</v>
+      </c>
+      <c r="AX25">
+        <f t="shared" si="16"/>
+        <v>258</v>
+      </c>
+      <c r="AY25">
+        <f t="shared" si="17"/>
+        <v>0.43071786310517529</v>
+      </c>
+      <c r="BP25">
+        <f t="shared" si="2"/>
         <v>-17.02</v>
       </c>
-      <c r="BI25">
-        <f t="shared" si="2"/>
+      <c r="BQ25">
+        <f t="shared" si="3"/>
         <v>-0.21240000000000001</v>
       </c>
-      <c r="BJ25">
-        <f t="shared" si="3"/>
+      <c r="BR25">
+        <f t="shared" si="4"/>
         <v>-204</v>
       </c>
     </row>
-    <row r="26" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -43302,15 +43947,15 @@
         <v>341</v>
       </c>
       <c r="Z26">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4.0500000000000007</v>
       </c>
       <c r="AA26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-9.4700000000000006E-2</v>
       </c>
       <c r="AB26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>121</v>
       </c>
       <c r="AK26">
@@ -43323,31 +43968,60 @@
         <v>795</v>
       </c>
       <c r="AN26">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>72.231539999999995</v>
       </c>
       <c r="AO26">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.2412</v>
       </c>
       <c r="AP26">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>795</v>
       </c>
-      <c r="BH26">
+      <c r="AQ26" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS26">
+        <v>65.240600000000001</v>
+      </c>
+      <c r="AT26">
+        <v>0.2424</v>
+      </c>
+      <c r="AU26">
+        <v>442</v>
+      </c>
+      <c r="AV26">
+        <f t="shared" si="15"/>
+        <v>-6.9909399999999948</v>
+      </c>
+      <c r="AW26">
         <f t="shared" si="1"/>
+        <v>1.2000000000000066E-3</v>
+      </c>
+      <c r="AX26">
+        <f t="shared" si="16"/>
+        <v>353</v>
+      </c>
+      <c r="AY26">
+        <f t="shared" si="17"/>
+        <v>0.44402515723270441</v>
+      </c>
+      <c r="BP26">
+        <f t="shared" si="2"/>
         <v>-10.1</v>
       </c>
-      <c r="BI26">
-        <f t="shared" si="2"/>
+      <c r="BQ26">
+        <f t="shared" si="3"/>
         <v>-0.3599</v>
       </c>
-      <c r="BJ26">
-        <f t="shared" si="3"/>
+      <c r="BR26">
+        <f t="shared" si="4"/>
         <v>-220</v>
       </c>
     </row>
-    <row r="27" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -43395,15 +44069,15 @@
         <v>250</v>
       </c>
       <c r="Z27">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-2.4648000000000003</v>
       </c>
       <c r="AA27">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8.2099999999999951E-2</v>
       </c>
       <c r="AB27">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>76</v>
       </c>
       <c r="AK27">
@@ -43416,31 +44090,60 @@
         <v>421</v>
       </c>
       <c r="AN27">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>83.323599999999999</v>
       </c>
       <c r="AO27">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.31533</v>
       </c>
       <c r="AP27">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>421</v>
       </c>
-      <c r="BH27">
+      <c r="AQ27" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS27">
+        <v>85.118799999999993</v>
+      </c>
+      <c r="AT27">
+        <v>0.35922999999999999</v>
+      </c>
+      <c r="AU27">
+        <v>354</v>
+      </c>
+      <c r="AV27">
+        <f t="shared" si="15"/>
+        <v>1.7951999999999941</v>
+      </c>
+      <c r="AW27">
         <f t="shared" si="1"/>
+        <v>4.3899999999999995E-2</v>
+      </c>
+      <c r="AX27">
+        <f t="shared" si="16"/>
+        <v>67</v>
+      </c>
+      <c r="AY27">
+        <f t="shared" si="17"/>
+        <v>0.15914489311163896</v>
+      </c>
+      <c r="BP27">
+        <f t="shared" si="2"/>
         <v>-22.76</v>
       </c>
-      <c r="BI27">
-        <f t="shared" si="2"/>
+      <c r="BQ27">
+        <f t="shared" si="3"/>
         <v>-0.27900000000000003</v>
       </c>
-      <c r="BJ27">
-        <f t="shared" si="3"/>
+      <c r="BR27">
+        <f t="shared" si="4"/>
         <v>-174</v>
       </c>
     </row>
-    <row r="28" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -43489,15 +44192,15 @@
         <v>179</v>
       </c>
       <c r="Z28">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9999999999999574E-2</v>
       </c>
       <c r="AA28">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.0199999999999996E-2</v>
       </c>
       <c r="AB28">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>14</v>
       </c>
       <c r="AK28">
@@ -43510,31 +44213,60 @@
         <v>408</v>
       </c>
       <c r="AN28">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>119.6892</v>
       </c>
       <c r="AO28">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.22966</v>
       </c>
       <c r="AP28">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>408</v>
       </c>
-      <c r="BH28">
+      <c r="AQ28" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS28">
+        <v>119.3027</v>
+      </c>
+      <c r="AT28">
+        <v>0.22609000000000001</v>
+      </c>
+      <c r="AU28">
+        <v>211</v>
+      </c>
+      <c r="AV28">
+        <f t="shared" si="15"/>
+        <v>-0.38649999999999807</v>
+      </c>
+      <c r="AW28">
         <f t="shared" si="1"/>
+        <v>-3.5699999999999898E-3</v>
+      </c>
+      <c r="AX28">
+        <f t="shared" si="16"/>
+        <v>197</v>
+      </c>
+      <c r="AY28">
+        <f t="shared" si="17"/>
+        <v>0.48284313725490197</v>
+      </c>
+      <c r="BP28">
+        <f t="shared" si="2"/>
         <v>-30.57</v>
       </c>
-      <c r="BI28">
-        <f t="shared" si="2"/>
+      <c r="BQ28">
+        <f t="shared" si="3"/>
         <v>-0.26269999999999999</v>
       </c>
-      <c r="BJ28">
-        <f t="shared" si="3"/>
+      <c r="BR28">
+        <f t="shared" si="4"/>
         <v>-165</v>
       </c>
     </row>
-    <row r="29" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -43583,15 +44315,15 @@
         <v>384</v>
       </c>
       <c r="Z29">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3628</v>
       </c>
       <c r="AA29">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-3.7200000000000011E-2</v>
       </c>
       <c r="AB29">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>60</v>
       </c>
       <c r="AK29">
@@ -43604,31 +44336,60 @@
         <v>712</v>
       </c>
       <c r="AN29">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>91.474900000000005</v>
       </c>
       <c r="AO29">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.34320000000000001</v>
       </c>
       <c r="AP29">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>712</v>
       </c>
-      <c r="BH29">
+      <c r="AQ29" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS29">
+        <v>55.037999999999997</v>
+      </c>
+      <c r="AT29">
+        <v>0.49536000000000002</v>
+      </c>
+      <c r="AU29">
+        <v>426</v>
+      </c>
+      <c r="AV29">
+        <f t="shared" si="15"/>
+        <v>-36.436900000000009</v>
+      </c>
+      <c r="AW29">
         <f t="shared" si="1"/>
+        <v>0.15216000000000002</v>
+      </c>
+      <c r="AX29">
+        <f t="shared" si="16"/>
+        <v>286</v>
+      </c>
+      <c r="AY29">
+        <f t="shared" si="17"/>
+        <v>0.40168539325842695</v>
+      </c>
+      <c r="BP29">
+        <f t="shared" si="2"/>
         <v>-19.22</v>
       </c>
-      <c r="BI29">
-        <f t="shared" si="2"/>
+      <c r="BQ29">
+        <f t="shared" si="3"/>
         <v>-0.3029</v>
       </c>
-      <c r="BJ29">
-        <f t="shared" si="3"/>
+      <c r="BR29">
+        <f t="shared" si="4"/>
         <v>-324</v>
       </c>
     </row>
-    <row r="30" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -43677,15 +44438,15 @@
         <v>284</v>
       </c>
       <c r="Z30">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.25</v>
       </c>
       <c r="AA30">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.7999999999999995E-2</v>
       </c>
       <c r="AB30">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>51</v>
       </c>
       <c r="AK30">
@@ -43698,31 +44459,60 @@
         <v>454</v>
       </c>
       <c r="AN30">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>88.2821</v>
       </c>
       <c r="AO30">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>8.9889999999999998E-2</v>
       </c>
       <c r="AP30">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>454</v>
       </c>
-      <c r="BH30">
+      <c r="AQ30" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS30">
+        <v>58.882599999999996</v>
+      </c>
+      <c r="AT30">
+        <v>0.11037</v>
+      </c>
+      <c r="AU30">
+        <v>313</v>
+      </c>
+      <c r="AV30">
+        <f t="shared" si="15"/>
+        <v>-29.399500000000003</v>
+      </c>
+      <c r="AW30">
         <f t="shared" si="1"/>
+        <v>2.0479999999999998E-2</v>
+      </c>
+      <c r="AX30">
+        <f t="shared" si="16"/>
+        <v>141</v>
+      </c>
+      <c r="AY30">
+        <f t="shared" si="17"/>
+        <v>0.31057268722466963</v>
+      </c>
+      <c r="BP30">
+        <f t="shared" si="2"/>
         <v>-11.61</v>
       </c>
-      <c r="BI30">
-        <f t="shared" si="2"/>
+      <c r="BQ30">
+        <f t="shared" si="3"/>
         <v>-6.8199999999999997E-2</v>
       </c>
-      <c r="BJ30">
-        <f t="shared" si="3"/>
+      <c r="BR30">
+        <f t="shared" si="4"/>
         <v>-233</v>
       </c>
     </row>
-    <row r="31" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -43769,15 +44559,15 @@
         <v>164</v>
       </c>
       <c r="Z31">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2.135900000000003</v>
       </c>
       <c r="AA31">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>2.0100000000000007E-2</v>
       </c>
       <c r="AB31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>24</v>
       </c>
       <c r="AK31">
@@ -43790,31 +44580,60 @@
         <v>327</v>
       </c>
       <c r="AN31">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>67.405699999999996</v>
       </c>
       <c r="AO31">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.19688</v>
       </c>
       <c r="AP31">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>327</v>
       </c>
-      <c r="BH31">
+      <c r="AQ31" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS31">
+        <v>66.93459</v>
+      </c>
+      <c r="AT31">
+        <v>0.40788999999999997</v>
+      </c>
+      <c r="AU31">
+        <v>211</v>
+      </c>
+      <c r="AV31">
+        <f t="shared" si="15"/>
+        <v>-0.47110999999999592</v>
+      </c>
+      <c r="AW31">
         <f t="shared" si="1"/>
+        <v>0.21100999999999998</v>
+      </c>
+      <c r="AX31">
+        <f>AM31-AU31</f>
+        <v>116</v>
+      </c>
+      <c r="AY31">
+        <f t="shared" si="17"/>
+        <v>0.35474006116207951</v>
+      </c>
+      <c r="BP31">
+        <f t="shared" si="2"/>
         <v>-16.989999999999998</v>
       </c>
-      <c r="BI31">
-        <f t="shared" si="2"/>
+      <c r="BQ31">
+        <f t="shared" si="3"/>
         <v>-0.20349999999999999</v>
       </c>
-      <c r="BJ31">
-        <f t="shared" si="3"/>
+      <c r="BR31">
+        <f t="shared" si="4"/>
         <v>-140</v>
       </c>
     </row>
-    <row r="32" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -43862,15 +44681,15 @@
         <v>397</v>
       </c>
       <c r="Z32">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.5</v>
       </c>
       <c r="AA32">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.6900000000000026E-2</v>
       </c>
       <c r="AB32">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>79</v>
       </c>
       <c r="AK32">
@@ -43883,31 +44702,60 @@
         <v>828</v>
       </c>
       <c r="AN32">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>84.632999999999996</v>
       </c>
       <c r="AO32">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.2198</v>
       </c>
       <c r="AP32">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>828</v>
       </c>
-      <c r="BH32">
+      <c r="AQ32" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS32">
+        <v>80.6875</v>
+      </c>
+      <c r="AT32">
+        <v>0.32166800000000001</v>
+      </c>
+      <c r="AU32">
+        <v>535</v>
+      </c>
+      <c r="AV32">
+        <f t="shared" si="15"/>
+        <v>-3.9454999999999956</v>
+      </c>
+      <c r="AW32">
         <f t="shared" si="1"/>
+        <v>0.10186800000000001</v>
+      </c>
+      <c r="AX32">
+        <f t="shared" si="16"/>
+        <v>293</v>
+      </c>
+      <c r="AY32">
+        <f t="shared" si="17"/>
+        <v>0.35386473429951693</v>
+      </c>
+      <c r="BP32">
+        <f t="shared" si="2"/>
         <v>-14.08</v>
       </c>
-      <c r="BI32">
-        <f t="shared" si="2"/>
+      <c r="BQ32">
+        <f t="shared" si="3"/>
         <v>-0.26400000000000001</v>
       </c>
-      <c r="BJ32">
-        <f t="shared" si="3"/>
+      <c r="BR32">
+        <f t="shared" si="4"/>
         <v>-318</v>
       </c>
     </row>
-    <row r="33" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -43955,15 +44803,15 @@
         <v>477</v>
       </c>
       <c r="Z33">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-0.16999999999999815</v>
       </c>
       <c r="AA33">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3.699999999999995E-3</v>
       </c>
       <c r="AB33">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
       </c>
       <c r="AK33">
@@ -43976,31 +44824,60 @@
         <v>1052</v>
       </c>
       <c r="AN33">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>113.6572</v>
       </c>
       <c r="AO33">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.13764999999999999</v>
       </c>
       <c r="AP33">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>1052</v>
       </c>
-      <c r="BH33">
+      <c r="AQ33" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS33">
+        <v>92.608599999999996</v>
+      </c>
+      <c r="AT33">
+        <v>0.1507</v>
+      </c>
+      <c r="AU33">
+        <v>739</v>
+      </c>
+      <c r="AV33">
+        <f t="shared" si="15"/>
+        <v>-21.048600000000008</v>
+      </c>
+      <c r="AW33">
         <f t="shared" si="1"/>
+        <v>1.3050000000000006E-2</v>
+      </c>
+      <c r="AX33">
+        <f t="shared" si="16"/>
+        <v>313</v>
+      </c>
+      <c r="AY33">
+        <f t="shared" si="17"/>
+        <v>0.29752851711026618</v>
+      </c>
+      <c r="BP33">
+        <f t="shared" si="2"/>
         <v>-27.43</v>
       </c>
-      <c r="BI33">
-        <f t="shared" si="2"/>
+      <c r="BQ33">
+        <f t="shared" si="3"/>
         <v>-0.1033</v>
       </c>
-      <c r="BJ33">
-        <f t="shared" si="3"/>
+      <c r="BR33">
+        <f t="shared" si="4"/>
         <v>-477</v>
       </c>
     </row>
-    <row r="34" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -44029,15 +44906,15 @@
         <v>530</v>
       </c>
       <c r="Z34">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-11.52</v>
       </c>
       <c r="AA34">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.24110000000000001</v>
       </c>
       <c r="AB34">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-530</v>
       </c>
       <c r="AK34">
@@ -44050,40 +44927,69 @@
         <v>840</v>
       </c>
       <c r="AN34">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>46.363799999999998</v>
       </c>
       <c r="AO34">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.27146999999999999</v>
       </c>
       <c r="AP34">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>840</v>
       </c>
-      <c r="BE34">
+      <c r="AQ34" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS34">
+        <v>46.128700000000002</v>
+      </c>
+      <c r="AT34">
+        <v>0.27218999999999999</v>
+      </c>
+      <c r="AU34">
+        <v>840</v>
+      </c>
+      <c r="AV34">
+        <f t="shared" si="15"/>
+        <v>-0.23509999999999565</v>
+      </c>
+      <c r="AW34">
+        <f t="shared" si="1"/>
+        <v>7.1999999999999842E-4</v>
+      </c>
+      <c r="AX34">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AY34">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BM34">
         <v>14.0328</v>
       </c>
-      <c r="BF34">
+      <c r="BN34">
         <v>0.1895</v>
       </c>
-      <c r="BG34">
+      <c r="BO34">
         <v>764</v>
       </c>
-      <c r="BH34">
-        <f t="shared" si="1"/>
+      <c r="BP34">
+        <f t="shared" si="2"/>
         <v>2.5128000000000004</v>
       </c>
-      <c r="BI34">
-        <f t="shared" si="2"/>
+      <c r="BQ34">
+        <f t="shared" si="3"/>
         <v>-5.1600000000000007E-2</v>
       </c>
-      <c r="BJ34">
-        <f t="shared" si="3"/>
+      <c r="BR34">
+        <f t="shared" si="4"/>
         <v>234</v>
       </c>
     </row>
-    <row r="35" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -44112,15 +45018,15 @@
         <v>454</v>
       </c>
       <c r="Z35">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-8.57</v>
       </c>
       <c r="AA35">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.2122</v>
       </c>
       <c r="AB35">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-454</v>
       </c>
       <c r="AK35">
@@ -44133,40 +45039,69 @@
         <v>610</v>
       </c>
       <c r="AN35">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>30.443850000000001</v>
       </c>
       <c r="AO35">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.28094999999999998</v>
       </c>
       <c r="AP35">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>610</v>
       </c>
-      <c r="BE35">
+      <c r="AQ35" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS35">
+        <v>30.3323</v>
+      </c>
+      <c r="AT35">
+        <v>0.28177000000000002</v>
+      </c>
+      <c r="AU35">
+        <v>610</v>
+      </c>
+      <c r="AV35">
+        <f t="shared" si="15"/>
+        <v>-0.11155000000000115</v>
+      </c>
+      <c r="AW35">
+        <f t="shared" si="1"/>
+        <v>8.2000000000004292E-4</v>
+      </c>
+      <c r="AX35">
+        <f t="shared" si="16"/>
+        <v>0</v>
+      </c>
+      <c r="AY35">
+        <f t="shared" si="17"/>
+        <v>0</v>
+      </c>
+      <c r="BM35">
         <v>8.6080649999999999</v>
       </c>
-      <c r="BF35">
+      <c r="BN35">
         <v>0.2099</v>
       </c>
-      <c r="BG35">
+      <c r="BO35">
         <v>477</v>
       </c>
-      <c r="BH35">
-        <f t="shared" si="1"/>
+      <c r="BP35">
+        <f t="shared" si="2"/>
         <v>3.8064999999999571E-2</v>
       </c>
-      <c r="BI35">
-        <f t="shared" si="2"/>
+      <c r="BQ35">
+        <f t="shared" si="3"/>
         <v>-2.2999999999999965E-3</v>
       </c>
-      <c r="BJ35">
-        <f t="shared" si="3"/>
+      <c r="BR35">
+        <f t="shared" si="4"/>
         <v>23</v>
       </c>
     </row>
-    <row r="36" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -44213,15 +45148,15 @@
         <v>162</v>
       </c>
       <c r="Z36">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.6099999999999994</v>
       </c>
       <c r="AA36">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.8000000000000274E-3</v>
       </c>
       <c r="AB36">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="AK36">
@@ -44234,31 +45169,60 @@
         <v>307</v>
       </c>
       <c r="AN36">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>66.238900000000001</v>
       </c>
       <c r="AO36">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.42817</v>
       </c>
       <c r="AP36">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>307</v>
       </c>
-      <c r="BH36">
+      <c r="AQ36" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS36">
+        <v>64.559700000000007</v>
+      </c>
+      <c r="AT36">
+        <v>0.35189999999999999</v>
+      </c>
+      <c r="AU36">
+        <v>174</v>
+      </c>
+      <c r="AV36">
+        <f t="shared" si="15"/>
+        <v>-1.6791999999999945</v>
+      </c>
+      <c r="AW36">
         <f t="shared" si="1"/>
+        <v>-7.6270000000000004E-2</v>
+      </c>
+      <c r="AX36">
+        <f t="shared" si="16"/>
+        <v>133</v>
+      </c>
+      <c r="AY36">
+        <f t="shared" si="17"/>
+        <v>0.43322475570032576</v>
+      </c>
+      <c r="BP36">
+        <f t="shared" si="2"/>
         <v>-26.52</v>
       </c>
-      <c r="BI36">
-        <f t="shared" si="2"/>
+      <c r="BQ36">
+        <f t="shared" si="3"/>
         <v>-0.36399999999999999</v>
       </c>
-      <c r="BJ36">
-        <f t="shared" si="3"/>
+      <c r="BR36">
+        <f t="shared" si="4"/>
         <v>-159</v>
       </c>
     </row>
-    <row r="37" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -44305,15 +45269,15 @@
         <v>388</v>
       </c>
       <c r="Z37">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.9170000000000016</v>
       </c>
       <c r="AA37">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-2.4500000000000008E-2</v>
       </c>
       <c r="AB37">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>138</v>
       </c>
       <c r="AK37">
@@ -44326,31 +45290,60 @@
         <v>464</v>
       </c>
       <c r="AN37">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>157.17169999999999</v>
       </c>
       <c r="AO37">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>9.6170000000000005E-2</v>
       </c>
       <c r="AP37">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>464</v>
       </c>
-      <c r="BH37">
+      <c r="AQ37" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS37">
+        <v>160.20500000000001</v>
+      </c>
+      <c r="AT37">
+        <v>0.11346000000000001</v>
+      </c>
+      <c r="AU37">
+        <v>434</v>
+      </c>
+      <c r="AV37">
+        <f t="shared" si="15"/>
+        <v>3.0333000000000254</v>
+      </c>
+      <c r="AW37">
         <f t="shared" si="1"/>
+        <v>1.729E-2</v>
+      </c>
+      <c r="AX37">
+        <f t="shared" si="16"/>
+        <v>30</v>
+      </c>
+      <c r="AY37">
+        <f t="shared" si="17"/>
+        <v>6.4655172413793108E-2</v>
+      </c>
+      <c r="BP37">
+        <f t="shared" si="2"/>
         <v>-39.68</v>
       </c>
-      <c r="BI37">
-        <f t="shared" si="2"/>
+      <c r="BQ37">
+        <f t="shared" si="3"/>
         <v>-0.1246</v>
       </c>
-      <c r="BJ37">
-        <f t="shared" si="3"/>
+      <c r="BR37">
+        <f t="shared" si="4"/>
         <v>-250</v>
       </c>
     </row>
-    <row r="38" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -44399,15 +45392,15 @@
         <v>273</v>
       </c>
       <c r="Z38">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>0.44000000000000128</v>
       </c>
       <c r="AA38">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-1.0900000000000021E-2</v>
       </c>
       <c r="AB38">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>10</v>
       </c>
       <c r="AK38">
@@ -44420,31 +45413,60 @@
         <v>508</v>
       </c>
       <c r="AN38">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>98.72</v>
       </c>
       <c r="AO38">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.21548</v>
       </c>
       <c r="AP38">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>508</v>
       </c>
-      <c r="BH38">
+      <c r="AQ38" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS38">
+        <v>87.449659999999994</v>
+      </c>
+      <c r="AT38">
+        <v>0.36652000000000001</v>
+      </c>
+      <c r="AU38">
+        <v>326</v>
+      </c>
+      <c r="AV38">
+        <f t="shared" si="15"/>
+        <v>-11.270340000000004</v>
+      </c>
+      <c r="AW38">
         <f t="shared" si="1"/>
+        <v>0.15104000000000001</v>
+      </c>
+      <c r="AX38">
+        <f t="shared" si="16"/>
+        <v>182</v>
+      </c>
+      <c r="AY38">
+        <f t="shared" si="17"/>
+        <v>0.35826771653543305</v>
+      </c>
+      <c r="BP38">
+        <f t="shared" si="2"/>
         <v>-22.22</v>
       </c>
-      <c r="BI38">
-        <f t="shared" si="2"/>
+      <c r="BQ38">
+        <f t="shared" si="3"/>
         <v>-0.30280000000000001</v>
       </c>
-      <c r="BJ38">
-        <f t="shared" si="3"/>
+      <c r="BR38">
+        <f t="shared" si="4"/>
         <v>-263</v>
       </c>
     </row>
-    <row r="39" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -44491,15 +45513,15 @@
         <v>159</v>
       </c>
       <c r="Z39">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1.3999999999999346E-2</v>
       </c>
       <c r="AA39">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>5.8400000000000007E-2</v>
       </c>
       <c r="AB39">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>22</v>
       </c>
       <c r="AK39">
@@ -44512,31 +45534,60 @@
         <v>230</v>
       </c>
       <c r="AN39">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>102.0086</v>
       </c>
       <c r="AO39">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>7.3599999999999999E-2</v>
       </c>
       <c r="AP39">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>230</v>
       </c>
-      <c r="BH39">
+      <c r="AQ39" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS39">
+        <v>103.3746</v>
+      </c>
+      <c r="AT39">
+        <v>0.15547800000000001</v>
+      </c>
+      <c r="AU39">
+        <v>174</v>
+      </c>
+      <c r="AV39">
+        <f t="shared" si="15"/>
+        <v>1.3659999999999997</v>
+      </c>
+      <c r="AW39">
         <f t="shared" si="1"/>
+        <v>8.1878000000000006E-2</v>
+      </c>
+      <c r="AX39">
+        <f t="shared" si="16"/>
+        <v>56</v>
+      </c>
+      <c r="AY39">
+        <f t="shared" si="17"/>
+        <v>0.24347826086956523</v>
+      </c>
+      <c r="BP39">
+        <f t="shared" si="2"/>
         <v>-26.34</v>
       </c>
-      <c r="BI39">
-        <f t="shared" si="2"/>
+      <c r="BQ39">
+        <f t="shared" si="3"/>
         <v>-0.22470000000000001</v>
       </c>
-      <c r="BJ39">
-        <f t="shared" si="3"/>
+      <c r="BR39">
+        <f t="shared" si="4"/>
         <v>-137</v>
       </c>
     </row>
-    <row r="40" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -44565,15 +45616,15 @@
         <v>173</v>
       </c>
       <c r="Z40">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-20.14</v>
       </c>
       <c r="AA40">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.17030000000000001</v>
       </c>
       <c r="AB40">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-173</v>
       </c>
       <c r="AK40">
@@ -44586,40 +45637,69 @@
         <v>301</v>
       </c>
       <c r="AN40">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>90.071899999999999</v>
       </c>
       <c r="AO40">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.2913</v>
       </c>
       <c r="AP40">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>301</v>
       </c>
-      <c r="BE40">
+      <c r="AQ40" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS40">
+        <v>85.150670000000005</v>
+      </c>
+      <c r="AT40">
+        <v>0.34103</v>
+      </c>
+      <c r="AU40">
+        <v>246</v>
+      </c>
+      <c r="AV40">
+        <f t="shared" si="15"/>
+        <v>-4.9212299999999942</v>
+      </c>
+      <c r="AW40">
+        <f t="shared" si="1"/>
+        <v>4.9729999999999996E-2</v>
+      </c>
+      <c r="AX40">
+        <f t="shared" si="16"/>
+        <v>55</v>
+      </c>
+      <c r="AY40">
+        <f t="shared" si="17"/>
+        <v>0.18272425249169436</v>
+      </c>
+      <c r="BM40">
         <v>19.668900000000001</v>
       </c>
-      <c r="BF40" s="81">
+      <c r="BN40" s="81">
         <v>0.33239999999999997</v>
       </c>
-      <c r="BG40">
+      <c r="BO40">
         <v>211</v>
       </c>
-      <c r="BH40">
-        <f t="shared" si="1"/>
+      <c r="BP40">
+        <f t="shared" si="2"/>
         <v>-0.47109999999999985</v>
       </c>
-      <c r="BI40">
-        <f t="shared" si="2"/>
+      <c r="BQ40">
+        <f t="shared" si="3"/>
         <v>0.16209999999999997</v>
       </c>
-      <c r="BJ40">
-        <f t="shared" si="3"/>
+      <c r="BR40">
+        <f t="shared" si="4"/>
         <v>38</v>
       </c>
     </row>
-    <row r="41" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -44648,15 +45728,15 @@
         <v>248</v>
       </c>
       <c r="Z41">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-9.7100000000000009</v>
       </c>
       <c r="AA41">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.187</v>
       </c>
       <c r="AB41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-248</v>
       </c>
       <c r="AK41">
@@ -44669,40 +45749,69 @@
         <v>404</v>
       </c>
       <c r="AN41">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>46.406399999999998</v>
       </c>
       <c r="AO41">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.15325</v>
       </c>
       <c r="AP41">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>404</v>
       </c>
-      <c r="BE41">
+      <c r="AQ41" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS41">
+        <v>47.331699999999998</v>
+      </c>
+      <c r="AT41">
+        <v>0.12736</v>
+      </c>
+      <c r="AU41">
+        <v>329</v>
+      </c>
+      <c r="AV41">
+        <f t="shared" si="15"/>
+        <v>0.92530000000000001</v>
+      </c>
+      <c r="AW41">
+        <f t="shared" si="1"/>
+        <v>-2.5889999999999996E-2</v>
+      </c>
+      <c r="AX41">
+        <f t="shared" si="16"/>
+        <v>75</v>
+      </c>
+      <c r="AY41">
+        <f t="shared" si="17"/>
+        <v>0.18564356435643564</v>
+      </c>
+      <c r="BM41">
         <v>9.7552000000000003</v>
       </c>
-      <c r="BF41">
+      <c r="BN41">
         <v>0.16739999999999999</v>
       </c>
-      <c r="BG41">
+      <c r="BO41">
         <v>260</v>
       </c>
-      <c r="BH41">
-        <f t="shared" si="1"/>
+      <c r="BP41">
+        <f t="shared" si="2"/>
         <v>4.5199999999999463E-2</v>
       </c>
-      <c r="BI41">
-        <f t="shared" si="2"/>
+      <c r="BQ41">
+        <f t="shared" si="3"/>
         <v>-1.9600000000000006E-2</v>
       </c>
-      <c r="BJ41">
-        <f t="shared" si="3"/>
+      <c r="BR41">
+        <f t="shared" si="4"/>
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -44731,15 +45840,15 @@
         <v>108</v>
       </c>
       <c r="Z42">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-12.46</v>
       </c>
       <c r="AA42">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.19750000000000001</v>
       </c>
       <c r="AB42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-108</v>
       </c>
       <c r="AK42">
@@ -44752,40 +45861,69 @@
         <v>212</v>
       </c>
       <c r="AN42">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>83.256900000000002</v>
       </c>
       <c r="AO42">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.30740000000000001</v>
       </c>
       <c r="AP42">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>212</v>
       </c>
-      <c r="BE42">
+      <c r="AQ42" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS42">
+        <v>68.259200000000007</v>
+      </c>
+      <c r="AT42">
+        <v>0.25735999999999998</v>
+      </c>
+      <c r="AU42">
+        <v>165</v>
+      </c>
+      <c r="AV42">
+        <f t="shared" si="15"/>
+        <v>-14.997699999999995</v>
+      </c>
+      <c r="AW42">
+        <f t="shared" si="1"/>
+        <v>-5.0040000000000029E-2</v>
+      </c>
+      <c r="AX42">
+        <f t="shared" si="16"/>
+        <v>47</v>
+      </c>
+      <c r="AY42">
+        <f t="shared" si="17"/>
+        <v>0.22169811320754718</v>
+      </c>
+      <c r="BM42">
         <v>12.31058</v>
       </c>
-      <c r="BF42">
+      <c r="BN42">
         <v>0.19095999999999999</v>
       </c>
-      <c r="BG42">
+      <c r="BO42">
         <v>115</v>
       </c>
-      <c r="BH42">
-        <f t="shared" si="1"/>
+      <c r="BP42">
+        <f t="shared" si="2"/>
         <v>-0.149420000000001</v>
       </c>
-      <c r="BI42">
-        <f t="shared" si="2"/>
+      <c r="BQ42">
+        <f t="shared" si="3"/>
         <v>-6.540000000000018E-3</v>
       </c>
-      <c r="BJ42">
-        <f t="shared" si="3"/>
+      <c r="BR42">
+        <f t="shared" si="4"/>
         <v>7</v>
       </c>
     </row>
-    <row r="43" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:70" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -44814,15 +45952,15 @@
         <v>117</v>
       </c>
       <c r="Z43">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>-33.28</v>
       </c>
       <c r="AA43">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>-0.2903</v>
       </c>
       <c r="AB43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>-117</v>
       </c>
       <c r="AK43">
@@ -44835,40 +45973,69 @@
         <v>202</v>
       </c>
       <c r="AN43">
-        <f t="shared" si="18"/>
+        <f t="shared" si="24"/>
         <v>215.42920000000001</v>
       </c>
       <c r="AO43">
-        <f t="shared" si="19"/>
+        <f t="shared" si="25"/>
         <v>0.25890000000000002</v>
       </c>
       <c r="AP43">
-        <f t="shared" si="20"/>
+        <f t="shared" si="26"/>
         <v>202</v>
       </c>
-      <c r="BE43">
+      <c r="AQ43" t="e">
+        <f t="shared" si="14"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="AS43">
+        <v>167.8339</v>
+      </c>
+      <c r="AT43">
+        <v>0.19420000000000001</v>
+      </c>
+      <c r="AU43">
+        <v>160</v>
+      </c>
+      <c r="AV43">
+        <f t="shared" si="15"/>
+        <v>-47.595300000000009</v>
+      </c>
+      <c r="AW43">
+        <f t="shared" si="1"/>
+        <v>-6.4700000000000008E-2</v>
+      </c>
+      <c r="AX43">
+        <f t="shared" si="16"/>
+        <v>42</v>
+      </c>
+      <c r="AY43">
+        <f t="shared" si="17"/>
+        <v>0.20792079207920791</v>
+      </c>
+      <c r="BM43">
         <v>41.243749999999999</v>
       </c>
-      <c r="BF43">
+      <c r="BN43">
         <v>0.32723000000000002</v>
       </c>
-      <c r="BG43">
+      <c r="BO43">
         <v>145</v>
       </c>
-      <c r="BH43">
-        <f t="shared" si="1"/>
+      <c r="BP43">
+        <f t="shared" si="2"/>
         <v>7.9637499999999974</v>
       </c>
-      <c r="BI43">
-        <f t="shared" si="2"/>
+      <c r="BQ43">
+        <f t="shared" si="3"/>
         <v>3.6930000000000018E-2</v>
       </c>
-      <c r="BJ43">
-        <f t="shared" si="3"/>
+      <c r="BR43">
+        <f t="shared" si="4"/>
         <v>28</v>
       </c>
     </row>
-    <row r="45" spans="1:62" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:70" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -44877,12 +46044,12 @@
         <f>SUM(AA5,AA9:AA10,AA13,AA17:AA18,AA21,AA25:AA33,AA36:AA39)</f>
         <v>0.1336999999999999</v>
       </c>
-      <c r="BH45">
-        <f>SUM(BH6:BH7,BH9,BH11,BH14,BH16,BH20,BH23:BH24,BH34:BH35,BH40:BH43)</f>
+      <c r="BP45">
+        <f>SUM(BP6:BP7,BP9,BP11,BP14,BP16,BP20,BP23:BP24,BP34:BP35,BP40:BP43)</f>
         <v>27.277845000000013</v>
       </c>
-      <c r="BI45">
-        <f>SUM(BI6:BI7,BI9,BI11,BI14,BI16,BI20,BI23:BI24,BI34:BI35,BI40:BI43)</f>
+      <c r="BQ45">
+        <f>SUM(BQ6:BQ7,BQ9,BQ11,BQ14,BQ16,BQ20,BQ23:BQ24,BQ34:BQ35,BQ40:BQ43)</f>
         <v>-0.10875460000000006</v>
       </c>
     </row>
@@ -44893,12 +46060,12 @@
     <mergeCell ref="I3:M3"/>
     <mergeCell ref="N3:O3"/>
   </mergeCells>
-  <conditionalFormatting sqref="Z5:Z43 BH5:BH43">
+  <conditionalFormatting sqref="Z5:Z43 BP5:BP43">
     <cfRule type="cellIs" dxfId="6" priority="12" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="AA45:AB45 AA5:AB43 BI5:BJ43">
+  <conditionalFormatting sqref="AA45:AB45 AA5:AB43 BQ5:BR43">
     <cfRule type="cellIs" dxfId="5" priority="11" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
@@ -44918,12 +46085,12 @@
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BH45:BI45">
+  <conditionalFormatting sqref="BP45:BQ45">
     <cfRule type="cellIs" dxfId="1" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="BJ1:BJ3">
+  <conditionalFormatting sqref="BR1:BR3">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>

</xml_diff>

<commit_message>
Added copepod small/large index by strata instead of EPU (for spring, fall and annual). Still includes copepod small/large index by EPU
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2288" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="237">
   <si>
     <t>Species</t>
   </si>
@@ -728,6 +728,15 @@
   </si>
   <si>
     <t>Removing outliers: same as AK2, plus remove outside of 2*Std Dev</t>
+  </si>
+  <si>
+    <t>8/2/2021 updated with small/large copeopod indices by strata for spring, fall and annual</t>
+  </si>
+  <si>
+    <t>small/large index used:</t>
+  </si>
+  <si>
+    <t>EPU</t>
   </si>
 </sst>
 </file>
@@ -40598,10 +40607,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BX45"/>
+  <dimension ref="A1:BZ45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR11" workbookViewId="0">
-      <selection activeCell="AT22" sqref="AT22"/>
+    <sheetView tabSelected="1" topLeftCell="AR10" workbookViewId="0">
+      <selection activeCell="AW16" sqref="AW16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -40618,9 +40627,10 @@
     <col min="16" max="16" width="9.81640625" customWidth="1"/>
     <col min="18" max="18" width="11.26953125" customWidth="1"/>
     <col min="23" max="25" width="8.81640625" customWidth="1"/>
+    <col min="78" max="78" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:78" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40653,8 +40663,11 @@
         <v>224</v>
       </c>
       <c r="BR1"/>
-    </row>
-    <row r="2" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="BT1" s="75" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
@@ -40677,7 +40690,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:76" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:78" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="95" t="s">
         <v>178</v>
       </c>
@@ -40737,7 +40750,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:76" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:78" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40942,8 +40955,14 @@
       <c r="BX4" s="69" t="s">
         <v>219</v>
       </c>
-    </row>
-    <row r="5" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="BY4" s="69" t="s">
+        <v>226</v>
+      </c>
+      <c r="BZ4" s="69" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -41108,8 +41127,32 @@
         <f t="shared" ref="BR5:BR43" si="4">BO5-U5</f>
         <v>-722</v>
       </c>
-    </row>
-    <row r="6" spans="1:76" x14ac:dyDescent="0.35">
+      <c r="BT5">
+        <v>34.229120000000002</v>
+      </c>
+      <c r="BU5">
+        <v>0.23117009999999999</v>
+      </c>
+      <c r="BV5">
+        <v>403</v>
+      </c>
+      <c r="BW5">
+        <f>BT5-AS5</f>
+        <v>-37.887279999999997</v>
+      </c>
+      <c r="BX5">
+        <f>BU5-AT5</f>
+        <v>6.3170099999999979E-2</v>
+      </c>
+      <c r="BY5">
+        <f>BV5-AU5</f>
+        <v>-232</v>
+      </c>
+      <c r="BZ5" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -41264,7 +41307,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="7" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -41418,7 +41461,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="8" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -41572,7 +41615,7 @@
         <v>-434</v>
       </c>
     </row>
-    <row r="9" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -41738,7 +41781,7 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="10" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -41903,7 +41946,7 @@
         <v>-628</v>
       </c>
     </row>
-    <row r="11" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -42057,7 +42100,7 @@
         <v>337</v>
       </c>
     </row>
-    <row r="12" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -42193,7 +42236,7 @@
         <v>-588</v>
       </c>
     </row>
-    <row r="13" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -42339,7 +42382,7 @@
         <v>-778</v>
       </c>
     </row>
-    <row r="14" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -42493,7 +42536,7 @@
         <v>508</v>
       </c>
     </row>
-    <row r="15" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -42629,7 +42672,7 @@
         <v>-663</v>
       </c>
     </row>
-    <row r="16" spans="1:76" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:78" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added ITIS codes to SVDBS data
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2292" uniqueCount="237">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2333" uniqueCount="246">
   <si>
     <t>Species</t>
   </si>
@@ -737,6 +737,33 @@
   </si>
   <si>
     <t>EPU</t>
+  </si>
+  <si>
+    <t>spring</t>
+  </si>
+  <si>
+    <t>fall</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>Annual</t>
+  </si>
+  <si>
+    <t>%n diff</t>
+  </si>
+  <si>
+    <t>6 spring</t>
+  </si>
+  <si>
+    <t>2 fall</t>
+  </si>
+  <si>
+    <t>5 annual</t>
+  </si>
+  <si>
+    <t>23 EPU</t>
   </si>
 </sst>
 </file>
@@ -40607,30 +40634,37 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BZ45"/>
+  <dimension ref="A1:CA48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AR10" workbookViewId="0">
-      <selection activeCell="AW16" sqref="AW16"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="BZ49" sqref="BZ49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="15.54296875" customWidth="1"/>
-    <col min="2" max="2" width="12.54296875" customWidth="1"/>
-    <col min="3" max="3" width="12" customWidth="1"/>
-    <col min="7" max="7" width="6.1796875" customWidth="1"/>
-    <col min="8" max="8" width="10.453125" customWidth="1"/>
-    <col min="9" max="9" width="11.54296875" customWidth="1"/>
-    <col min="10" max="10" width="9.7265625" customWidth="1"/>
-    <col min="12" max="12" width="10.26953125" customWidth="1"/>
-    <col min="15" max="15" width="10.26953125" customWidth="1"/>
-    <col min="16" max="16" width="9.81640625" customWidth="1"/>
-    <col min="18" max="18" width="11.26953125" customWidth="1"/>
-    <col min="23" max="25" width="8.81640625" customWidth="1"/>
+    <col min="2" max="2" width="12.54296875" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="12" hidden="1" customWidth="1"/>
+    <col min="4" max="6" width="0" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="6.1796875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.54296875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7265625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10.26953125" hidden="1" customWidth="1"/>
+    <col min="13" max="14" width="0" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="10.26953125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="9.81640625" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="0" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="11.26953125" hidden="1" customWidth="1"/>
+    <col min="19" max="22" width="0" hidden="1" customWidth="1"/>
+    <col min="23" max="25" width="8.81640625" hidden="1" customWidth="1"/>
+    <col min="26" max="44" width="0" hidden="1" customWidth="1"/>
+    <col min="52" max="70" width="0" hidden="1" customWidth="1"/>
     <col min="78" max="78" width="11.54296875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:78" s="69" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:79" s="69" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="78" t="s">
         <v>216</v>
       </c>
@@ -40667,7 +40701,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="2" spans="1:78" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:79" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
@@ -40690,7 +40724,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="3" spans="1:78" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:79" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="95" t="s">
         <v>178</v>
       </c>
@@ -40750,7 +40784,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="4" spans="1:78" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:79" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -40961,8 +40995,11 @@
       <c r="BZ4" s="69" t="s">
         <v>235</v>
       </c>
-    </row>
-    <row r="5" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="CA4" s="69" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="5" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -41151,8 +41188,12 @@
       <c r="BZ5" t="s">
         <v>236</v>
       </c>
-    </row>
-    <row r="6" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="CA5">
+        <f>BY5/AU5</f>
+        <v>-0.36535433070866141</v>
+      </c>
+    </row>
+    <row r="6" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -41306,8 +41347,36 @@
         <f t="shared" si="4"/>
         <v>1121</v>
       </c>
-    </row>
-    <row r="7" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT6">
+        <v>49.546399999999998</v>
+      </c>
+      <c r="BU6">
+        <v>0.22939999999999999</v>
+      </c>
+      <c r="BV6">
+        <v>854</v>
+      </c>
+      <c r="BW6">
+        <f t="shared" ref="BW6:BW43" si="21">BT6-AS6</f>
+        <v>-49.005600000000008</v>
+      </c>
+      <c r="BX6">
+        <f t="shared" ref="BX6:BX43" si="22">BU6-AT6</f>
+        <v>0.11260999999999999</v>
+      </c>
+      <c r="BY6">
+        <f t="shared" ref="BY6:BY43" si="23">BV6-AU6</f>
+        <v>-442</v>
+      </c>
+      <c r="BZ6" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA6">
+        <f t="shared" ref="CA6:CA43" si="24">BY6/AU6</f>
+        <v>-0.3410493827160494</v>
+      </c>
+    </row>
+    <row r="7" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -41460,8 +41529,36 @@
         <f t="shared" si="4"/>
         <v>399</v>
       </c>
-    </row>
-    <row r="8" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT7">
+        <v>58.832000000000001</v>
+      </c>
+      <c r="BU7">
+        <v>0.34878999999999999</v>
+      </c>
+      <c r="BV7">
+        <v>422</v>
+      </c>
+      <c r="BW7">
+        <f t="shared" si="21"/>
+        <v>-27.696989999999992</v>
+      </c>
+      <c r="BX7">
+        <f t="shared" si="22"/>
+        <v>1.8663199999999991E-2</v>
+      </c>
+      <c r="BY7">
+        <f t="shared" si="23"/>
+        <v>-165</v>
+      </c>
+      <c r="BZ7" t="s">
+        <v>237</v>
+      </c>
+      <c r="CA7">
+        <f t="shared" si="24"/>
+        <v>-0.28109028960817717</v>
+      </c>
+    </row>
+    <row r="8" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -41614,8 +41711,36 @@
         <f t="shared" si="4"/>
         <v>-434</v>
       </c>
-    </row>
-    <row r="9" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT8">
+        <v>23.154879999999999</v>
+      </c>
+      <c r="BU8">
+        <v>0.32857999999999998</v>
+      </c>
+      <c r="BV8">
+        <v>375</v>
+      </c>
+      <c r="BW8">
+        <f t="shared" si="21"/>
+        <v>-19.467120000000001</v>
+      </c>
+      <c r="BX8">
+        <f t="shared" si="22"/>
+        <v>8.3179999999999976E-2</v>
+      </c>
+      <c r="BY8">
+        <f t="shared" si="23"/>
+        <v>-360</v>
+      </c>
+      <c r="BZ8" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA8">
+        <f t="shared" si="24"/>
+        <v>-0.48979591836734693</v>
+      </c>
+    </row>
+    <row r="9" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -41780,8 +41905,36 @@
         <f t="shared" si="4"/>
         <v>1467</v>
       </c>
-    </row>
-    <row r="10" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT9">
+        <v>131.28</v>
+      </c>
+      <c r="BU9">
+        <v>0.22575999999999999</v>
+      </c>
+      <c r="BV9">
+        <v>1240</v>
+      </c>
+      <c r="BW9">
+        <f t="shared" si="21"/>
+        <v>-47.947399999999988</v>
+      </c>
+      <c r="BX9">
+        <f t="shared" si="22"/>
+        <v>4.5812999999999826E-3</v>
+      </c>
+      <c r="BY9">
+        <f t="shared" si="23"/>
+        <v>-710</v>
+      </c>
+      <c r="BZ9" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA9">
+        <f t="shared" si="24"/>
+        <v>-0.36410256410256409</v>
+      </c>
+    </row>
+    <row r="10" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -41872,15 +42025,15 @@
         <v>1015</v>
       </c>
       <c r="AN10">
-        <f t="shared" ref="AN10:AN13" si="21">AK10-AD10</f>
+        <f t="shared" ref="AN10:AN13" si="25">AK10-AD10</f>
         <v>43.599399999999989</v>
       </c>
       <c r="AO10">
-        <f t="shared" ref="AO10:AO13" si="22">AL10-AE10</f>
+        <f t="shared" ref="AO10:AO13" si="26">AL10-AE10</f>
         <v>0.12449200000000001</v>
       </c>
       <c r="AP10">
-        <f t="shared" ref="AP10:AP13" si="23">AM10-AF10</f>
+        <f t="shared" ref="AP10:AP13" si="27">AM10-AF10</f>
         <v>132</v>
       </c>
       <c r="AQ10">
@@ -41945,8 +42098,36 @@
         <f t="shared" si="4"/>
         <v>-628</v>
       </c>
-    </row>
-    <row r="11" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT10">
+        <v>56.933999999999997</v>
+      </c>
+      <c r="BU10">
+        <v>0.19596</v>
+      </c>
+      <c r="BV10">
+        <v>993</v>
+      </c>
+      <c r="BW10">
+        <f t="shared" si="21"/>
+        <v>-15.715800000000002</v>
+      </c>
+      <c r="BX10">
+        <f t="shared" si="22"/>
+        <v>-1.754E-2</v>
+      </c>
+      <c r="BY10">
+        <f t="shared" si="23"/>
+        <v>-22</v>
+      </c>
+      <c r="BZ10" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA10">
+        <f t="shared" si="24"/>
+        <v>-2.167487684729064E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -42017,15 +42198,15 @@
         <v>1133</v>
       </c>
       <c r="AN11">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>48.030640000000005</v>
       </c>
       <c r="AO11">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>6.7830000000000015E-2</v>
       </c>
       <c r="AP11">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>145</v>
       </c>
       <c r="AQ11">
@@ -42099,8 +42280,36 @@
         <f t="shared" si="4"/>
         <v>337</v>
       </c>
-    </row>
-    <row r="12" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT11">
+        <v>29.998999999999999</v>
+      </c>
+      <c r="BU11">
+        <v>0.22720000000000001</v>
+      </c>
+      <c r="BV11">
+        <v>418</v>
+      </c>
+      <c r="BW11">
+        <f t="shared" si="21"/>
+        <v>-24.329000000000004</v>
+      </c>
+      <c r="BX11">
+        <f t="shared" si="22"/>
+        <v>3.3200000000000007E-2</v>
+      </c>
+      <c r="BY11">
+        <f t="shared" si="23"/>
+        <v>-164</v>
+      </c>
+      <c r="BZ11" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA11">
+        <f t="shared" si="24"/>
+        <v>-0.28178694158075601</v>
+      </c>
+    </row>
+    <row r="12" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -42171,15 +42380,15 @@
         <v>1157</v>
       </c>
       <c r="AN12">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>95.403899999999993</v>
       </c>
       <c r="AO12">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.29437999999999998</v>
       </c>
       <c r="AP12">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>1157</v>
       </c>
       <c r="AQ12" t="e">
@@ -42235,8 +42444,36 @@
         <f t="shared" si="4"/>
         <v>-588</v>
       </c>
-    </row>
-    <row r="13" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT12">
+        <v>65.5839</v>
+      </c>
+      <c r="BU12">
+        <v>0.35551719999999998</v>
+      </c>
+      <c r="BV12">
+        <v>628</v>
+      </c>
+      <c r="BW12">
+        <f t="shared" si="21"/>
+        <v>-26.566999999999993</v>
+      </c>
+      <c r="BX12">
+        <f t="shared" si="22"/>
+        <v>1.9761199999999979E-2</v>
+      </c>
+      <c r="BY12">
+        <f t="shared" si="23"/>
+        <v>-413</v>
+      </c>
+      <c r="BZ12" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA12">
+        <f t="shared" si="24"/>
+        <v>-0.3967339097022094</v>
+      </c>
+    </row>
+    <row r="13" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -42317,15 +42554,15 @@
         <v>1375</v>
       </c>
       <c r="AN13">
-        <f t="shared" si="21"/>
+        <f t="shared" si="25"/>
         <v>114.5904</v>
       </c>
       <c r="AO13">
-        <f t="shared" si="22"/>
+        <f t="shared" si="26"/>
         <v>0.16016</v>
       </c>
       <c r="AP13">
-        <f t="shared" si="23"/>
+        <f t="shared" si="27"/>
         <v>1375</v>
       </c>
       <c r="AQ13" t="e">
@@ -42381,8 +42618,36 @@
         <f t="shared" si="4"/>
         <v>-778</v>
       </c>
-    </row>
-    <row r="14" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT13">
+        <v>73.141499999999994</v>
+      </c>
+      <c r="BU13">
+        <v>0.15959999999999999</v>
+      </c>
+      <c r="BV13">
+        <v>1239</v>
+      </c>
+      <c r="BW13">
+        <f t="shared" si="21"/>
+        <v>-43.293500000000009</v>
+      </c>
+      <c r="BX13">
+        <f t="shared" si="22"/>
+        <v>-3.0799999999999994E-3</v>
+      </c>
+      <c r="BY13">
+        <f t="shared" si="23"/>
+        <v>-25</v>
+      </c>
+      <c r="BZ13" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA13">
+        <f t="shared" si="24"/>
+        <v>-1.9778481012658229E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -42453,15 +42718,15 @@
         <v>1154</v>
       </c>
       <c r="AN14">
-        <f t="shared" ref="AN14:AN43" si="24">AK14-AD14</f>
+        <f t="shared" ref="AN14:AN43" si="28">AK14-AD14</f>
         <v>53.567700000000002</v>
       </c>
       <c r="AO14">
-        <f t="shared" ref="AO14:AO43" si="25">AL14-AE14</f>
+        <f t="shared" ref="AO14:AO43" si="29">AL14-AE14</f>
         <v>2.8599999999999987E-2</v>
       </c>
       <c r="AP14">
-        <f t="shared" ref="AP14:AP43" si="26">AM14-AF14</f>
+        <f t="shared" ref="AP14:AP43" si="30">AM14-AF14</f>
         <v>90</v>
       </c>
       <c r="AQ14">
@@ -42535,8 +42800,36 @@
         <f t="shared" si="4"/>
         <v>508</v>
       </c>
-    </row>
-    <row r="15" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT14">
+        <v>45.511699999999998</v>
+      </c>
+      <c r="BU14">
+        <v>0.20265</v>
+      </c>
+      <c r="BV14">
+        <v>456</v>
+      </c>
+      <c r="BW14">
+        <f t="shared" si="21"/>
+        <v>-16.503300000000003</v>
+      </c>
+      <c r="BX14">
+        <f t="shared" si="22"/>
+        <v>-6.5309999999999979E-2</v>
+      </c>
+      <c r="BY14">
+        <f t="shared" si="23"/>
+        <v>-130</v>
+      </c>
+      <c r="BZ14" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA14">
+        <f t="shared" si="24"/>
+        <v>-0.22184300341296928</v>
+      </c>
+    </row>
+    <row r="15" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -42607,15 +42900,15 @@
         <v>1656</v>
       </c>
       <c r="AN15">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>90.829400000000007</v>
       </c>
       <c r="AO15">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.1797</v>
       </c>
       <c r="AP15">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1656</v>
       </c>
       <c r="AQ15" t="e">
@@ -42671,8 +42964,36 @@
         <f t="shared" si="4"/>
         <v>-663</v>
       </c>
-    </row>
-    <row r="16" spans="1:78" x14ac:dyDescent="0.35">
+      <c r="BT15">
+        <v>58.681800000000003</v>
+      </c>
+      <c r="BU15">
+        <v>0.26729999999999998</v>
+      </c>
+      <c r="BV15">
+        <v>622</v>
+      </c>
+      <c r="BW15">
+        <f t="shared" si="21"/>
+        <v>-29.553400000000003</v>
+      </c>
+      <c r="BX15">
+        <f t="shared" si="22"/>
+        <v>4.3129999999999974E-2</v>
+      </c>
+      <c r="BY15">
+        <f t="shared" si="23"/>
+        <v>-278</v>
+      </c>
+      <c r="BZ15" t="s">
+        <v>238</v>
+      </c>
+      <c r="CA15">
+        <f t="shared" si="24"/>
+        <v>-0.30888888888888888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>
@@ -42734,15 +43055,15 @@
         <v>1396</v>
       </c>
       <c r="AN16">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>240.0746</v>
       </c>
       <c r="AO16">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>8.5360000000000005E-2</v>
       </c>
       <c r="AP16">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1396</v>
       </c>
       <c r="AQ16" t="e">
@@ -42807,8 +43128,36 @@
         <f t="shared" si="4"/>
         <v>417</v>
       </c>
-    </row>
-    <row r="17" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT16">
+        <v>132.70410000000001</v>
+      </c>
+      <c r="BU16">
+        <v>0.14002999999999999</v>
+      </c>
+      <c r="BV16">
+        <v>620</v>
+      </c>
+      <c r="BW16">
+        <f t="shared" si="21"/>
+        <v>-114.49889999999999</v>
+      </c>
+      <c r="BX16">
+        <f t="shared" si="22"/>
+        <v>3.5801999999999987E-2</v>
+      </c>
+      <c r="BY16">
+        <f t="shared" si="23"/>
+        <v>-256</v>
+      </c>
+      <c r="BZ16" t="s">
+        <v>239</v>
+      </c>
+      <c r="CA16">
+        <f t="shared" si="24"/>
+        <v>-0.29223744292237441</v>
+      </c>
+    </row>
+    <row r="17" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -42888,15 +43237,15 @@
         <v>527</v>
       </c>
       <c r="AN17">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>151.08240000000001</v>
       </c>
       <c r="AO17">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.36549999999999999</v>
       </c>
       <c r="AP17">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>527</v>
       </c>
       <c r="AQ17" t="e">
@@ -42952,8 +43301,36 @@
         <f t="shared" si="4"/>
         <v>-231</v>
       </c>
-    </row>
-    <row r="18" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT17">
+        <v>87.540300000000002</v>
+      </c>
+      <c r="BU17">
+        <v>0.44679999999999997</v>
+      </c>
+      <c r="BV17">
+        <v>285</v>
+      </c>
+      <c r="BW17">
+        <f t="shared" si="21"/>
+        <v>-76.72829999999999</v>
+      </c>
+      <c r="BX17">
+        <f t="shared" si="22"/>
+        <v>0.13640999999999998</v>
+      </c>
+      <c r="BY17">
+        <f t="shared" si="23"/>
+        <v>-95</v>
+      </c>
+      <c r="BZ17" t="s">
+        <v>237</v>
+      </c>
+      <c r="CA17">
+        <f t="shared" si="24"/>
+        <v>-0.25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -43016,11 +43393,11 @@
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" ref="AH18" si="27">AE18-BG18</f>
+        <f t="shared" ref="AH18" si="31">AE18-BG18</f>
         <v>0</v>
       </c>
       <c r="AI18">
-        <f t="shared" ref="AI18" si="28">AF18-BH18</f>
+        <f t="shared" ref="AI18" si="32">AF18-BH18</f>
         <v>0</v>
       </c>
       <c r="AK18">
@@ -43033,15 +43410,15 @@
         <v>947</v>
       </c>
       <c r="AN18">
-        <f t="shared" ref="AN18" si="29">AK18-AD18</f>
+        <f t="shared" ref="AN18" si="33">AK18-AD18</f>
         <v>76.399000000000001</v>
       </c>
       <c r="AO18">
-        <f t="shared" ref="AO18" si="30">AL18-AE18</f>
+        <f t="shared" ref="AO18" si="34">AL18-AE18</f>
         <v>0.15029999999999999</v>
       </c>
       <c r="AP18">
-        <f t="shared" ref="AP18" si="31">AM18-AF18</f>
+        <f t="shared" ref="AP18" si="35">AM18-AF18</f>
         <v>947</v>
       </c>
       <c r="AQ18" t="e">
@@ -43058,11 +43435,11 @@
         <v>477</v>
       </c>
       <c r="AV18">
-        <f t="shared" ref="AV18" si="32">AS18-AK18</f>
+        <f t="shared" ref="AV18" si="36">AS18-AK18</f>
         <v>-18.928600000000003</v>
       </c>
       <c r="AW18">
-        <f t="shared" ref="AW18" si="33">AT18-AL18</f>
+        <f t="shared" ref="AW18" si="37">AT18-AL18</f>
         <v>0.1784</v>
       </c>
       <c r="AX18">
@@ -43085,8 +43462,36 @@
         <f t="shared" si="4"/>
         <v>-343</v>
       </c>
-    </row>
-    <row r="19" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT18">
+        <v>25.470300000000002</v>
+      </c>
+      <c r="BU18">
+        <v>0.35639999999999999</v>
+      </c>
+      <c r="BV18">
+        <v>358</v>
+      </c>
+      <c r="BW18">
+        <f t="shared" si="21"/>
+        <v>-32.000099999999996</v>
+      </c>
+      <c r="BX18">
+        <f t="shared" si="22"/>
+        <v>2.7700000000000002E-2</v>
+      </c>
+      <c r="BY18">
+        <f t="shared" si="23"/>
+        <v>-119</v>
+      </c>
+      <c r="BZ18" t="s">
+        <v>238</v>
+      </c>
+      <c r="CA18">
+        <f t="shared" si="24"/>
+        <v>-0.24947589098532494</v>
+      </c>
+    </row>
+    <row r="19" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -43158,15 +43563,15 @@
         <v>734</v>
       </c>
       <c r="AN19">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>80.852900000000005</v>
       </c>
       <c r="AO19">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.24697</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>734</v>
       </c>
       <c r="AQ19" t="e">
@@ -43210,8 +43615,36 @@
         <f t="shared" si="4"/>
         <v>-320</v>
       </c>
-    </row>
-    <row r="20" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT19">
+        <v>54.324300000000001</v>
+      </c>
+      <c r="BU19">
+        <v>0.32273000000000002</v>
+      </c>
+      <c r="BV19">
+        <v>339</v>
+      </c>
+      <c r="BW19">
+        <f t="shared" si="21"/>
+        <v>-25.269500000000001</v>
+      </c>
+      <c r="BX19">
+        <f t="shared" si="22"/>
+        <v>7.2030000000000038E-2</v>
+      </c>
+      <c r="BY19">
+        <f t="shared" si="23"/>
+        <v>-260</v>
+      </c>
+      <c r="BZ19" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA19">
+        <f t="shared" si="24"/>
+        <v>-0.43405676126878129</v>
+      </c>
+    </row>
+    <row r="20" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -43273,15 +43706,15 @@
         <v>651</v>
       </c>
       <c r="AN20">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>225.16650000000001</v>
       </c>
       <c r="AO20">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.1212</v>
       </c>
       <c r="AP20">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>651</v>
       </c>
       <c r="AQ20" t="e">
@@ -43334,8 +43767,36 @@
         <f t="shared" si="4"/>
         <v>171</v>
       </c>
-    </row>
-    <row r="21" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT20">
+        <v>162.7996</v>
+      </c>
+      <c r="BU20">
+        <v>0.25974999999999998</v>
+      </c>
+      <c r="BV20">
+        <v>288</v>
+      </c>
+      <c r="BW20">
+        <f t="shared" si="21"/>
+        <v>-47.215599999999995</v>
+      </c>
+      <c r="BX20">
+        <f t="shared" si="22"/>
+        <v>0.12414999999999998</v>
+      </c>
+      <c r="BY20">
+        <f t="shared" si="23"/>
+        <v>-89</v>
+      </c>
+      <c r="BZ20" t="s">
+        <v>239</v>
+      </c>
+      <c r="CA20">
+        <f t="shared" si="24"/>
+        <v>-0.23607427055702918</v>
+      </c>
+    </row>
+    <row r="21" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -43418,15 +43879,15 @@
         <v>1742</v>
       </c>
       <c r="AN21">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>48.740499999999997</v>
       </c>
       <c r="AO21">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.1769</v>
       </c>
       <c r="AP21">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1742</v>
       </c>
       <c r="AQ21" t="e">
@@ -43470,8 +43931,36 @@
         <f t="shared" si="4"/>
         <v>-646</v>
       </c>
-    </row>
-    <row r="22" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT21">
+        <v>31.584800000000001</v>
+      </c>
+      <c r="BU21">
+        <v>0.21837000000000001</v>
+      </c>
+      <c r="BV21">
+        <v>1119</v>
+      </c>
+      <c r="BW21">
+        <f t="shared" si="21"/>
+        <v>-10.151899999999998</v>
+      </c>
+      <c r="BX21">
+        <f t="shared" si="22"/>
+        <v>2.5100000000000122E-3</v>
+      </c>
+      <c r="BY21">
+        <f t="shared" si="23"/>
+        <v>-13</v>
+      </c>
+      <c r="BZ21" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA21">
+        <f t="shared" si="24"/>
+        <v>-1.1484098939929329E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -43542,15 +44031,15 @@
         <v>963</v>
       </c>
       <c r="AN22">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>56.912999999999997</v>
       </c>
       <c r="AO22">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.26650000000000001</v>
       </c>
       <c r="AP22">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>963</v>
       </c>
       <c r="AQ22" t="e">
@@ -43594,8 +44083,36 @@
         <f t="shared" si="4"/>
         <v>-236</v>
       </c>
-    </row>
-    <row r="23" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT22">
+        <v>32.496400000000001</v>
+      </c>
+      <c r="BU22">
+        <v>0.37403999999999998</v>
+      </c>
+      <c r="BV22">
+        <v>360</v>
+      </c>
+      <c r="BW22">
+        <f t="shared" si="21"/>
+        <v>-8.6032000000000011</v>
+      </c>
+      <c r="BX22">
+        <f t="shared" si="22"/>
+        <v>7.7200000000000046E-3</v>
+      </c>
+      <c r="BY22">
+        <f t="shared" si="23"/>
+        <v>-199</v>
+      </c>
+      <c r="BZ22" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA22">
+        <f t="shared" si="24"/>
+        <v>-0.35599284436493739</v>
+      </c>
+    </row>
+    <row r="23" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -43645,15 +44162,15 @@
         <v>579</v>
       </c>
       <c r="AN23">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>74.535600000000002</v>
       </c>
       <c r="AO23">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.13339999999999999</v>
       </c>
       <c r="AP23">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>579</v>
       </c>
       <c r="AQ23" t="e">
@@ -43706,8 +44223,36 @@
         <f t="shared" si="4"/>
         <v>506</v>
       </c>
-    </row>
-    <row r="24" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT23">
+        <v>49.6509</v>
+      </c>
+      <c r="BU23">
+        <v>8.6449999999999999E-2</v>
+      </c>
+      <c r="BV23">
+        <v>249</v>
+      </c>
+      <c r="BW23">
+        <f t="shared" si="21"/>
+        <v>-37.042499999999997</v>
+      </c>
+      <c r="BX23">
+        <f t="shared" si="22"/>
+        <v>9.5409999999999939E-3</v>
+      </c>
+      <c r="BY23">
+        <f t="shared" si="23"/>
+        <v>-169</v>
+      </c>
+      <c r="BZ23" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA23">
+        <f t="shared" si="24"/>
+        <v>-0.40430622009569378</v>
+      </c>
+    </row>
+    <row r="24" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -43757,15 +44302,15 @@
         <v>462</v>
       </c>
       <c r="AN24">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>121.116</v>
       </c>
       <c r="AO24">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.2165</v>
       </c>
       <c r="AP24">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>462</v>
       </c>
       <c r="AQ24" t="e">
@@ -43818,8 +44363,36 @@
         <f t="shared" si="4"/>
         <v>319</v>
       </c>
-    </row>
-    <row r="25" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT24">
+        <v>53.668999999999997</v>
+      </c>
+      <c r="BU24">
+        <v>0.3085</v>
+      </c>
+      <c r="BV24">
+        <v>268</v>
+      </c>
+      <c r="BW24">
+        <f t="shared" si="21"/>
+        <v>-72.544399999999996</v>
+      </c>
+      <c r="BX24">
+        <f t="shared" si="22"/>
+        <v>7.1050000000000002E-2</v>
+      </c>
+      <c r="BY24">
+        <f t="shared" si="23"/>
+        <v>-117</v>
+      </c>
+      <c r="BZ24" t="s">
+        <v>237</v>
+      </c>
+      <c r="CA24">
+        <f t="shared" si="24"/>
+        <v>-0.30389610389610389</v>
+      </c>
+    </row>
+    <row r="25" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -43888,15 +44461,15 @@
         <v>599</v>
       </c>
       <c r="AN25">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>98.161590000000004</v>
       </c>
       <c r="AO25">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.26608999999999999</v>
       </c>
       <c r="AP25">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>599</v>
       </c>
       <c r="AQ25" t="e">
@@ -43940,8 +44513,36 @@
         <f t="shared" si="4"/>
         <v>-204</v>
       </c>
-    </row>
-    <row r="26" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT25">
+        <v>58.146000000000001</v>
+      </c>
+      <c r="BU25">
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="BV25">
+        <v>250</v>
+      </c>
+      <c r="BW25">
+        <f t="shared" si="21"/>
+        <v>-54.629000000000005</v>
+      </c>
+      <c r="BX25">
+        <f t="shared" si="22"/>
+        <v>6.5200000000000036E-2</v>
+      </c>
+      <c r="BY25">
+        <f t="shared" si="23"/>
+        <v>-91</v>
+      </c>
+      <c r="BZ25" t="s">
+        <v>237</v>
+      </c>
+      <c r="CA25">
+        <f t="shared" si="24"/>
+        <v>-0.26686217008797652</v>
+      </c>
+    </row>
+    <row r="26" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -44011,15 +44612,15 @@
         <v>795</v>
       </c>
       <c r="AN26">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>72.231539999999995</v>
       </c>
       <c r="AO26">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.2412</v>
       </c>
       <c r="AP26">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>795</v>
       </c>
       <c r="AQ26" t="e">
@@ -44063,8 +44664,36 @@
         <f t="shared" si="4"/>
         <v>-220</v>
       </c>
-    </row>
-    <row r="27" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT26">
+        <v>37.952599999999997</v>
+      </c>
+      <c r="BU26">
+        <v>0.22056999999999999</v>
+      </c>
+      <c r="BV26">
+        <v>291</v>
+      </c>
+      <c r="BW26">
+        <f t="shared" si="21"/>
+        <v>-27.288000000000004</v>
+      </c>
+      <c r="BX26">
+        <f t="shared" si="22"/>
+        <v>-2.1830000000000016E-2</v>
+      </c>
+      <c r="BY26">
+        <f t="shared" si="23"/>
+        <v>-151</v>
+      </c>
+      <c r="BZ26" t="s">
+        <v>240</v>
+      </c>
+      <c r="CA26">
+        <f t="shared" si="24"/>
+        <v>-0.34162895927601811</v>
+      </c>
+    </row>
+    <row r="27" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -44133,15 +44762,15 @@
         <v>421</v>
       </c>
       <c r="AN27">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>83.323599999999999</v>
       </c>
       <c r="AO27">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.31533</v>
       </c>
       <c r="AP27">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>421</v>
       </c>
       <c r="AQ27" t="e">
@@ -44185,8 +44814,36 @@
         <f t="shared" si="4"/>
         <v>-174</v>
       </c>
-    </row>
-    <row r="28" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT27">
+        <v>67.499399999999994</v>
+      </c>
+      <c r="BU27">
+        <v>0.32174999999999998</v>
+      </c>
+      <c r="BV27">
+        <v>190</v>
+      </c>
+      <c r="BW27">
+        <f t="shared" si="21"/>
+        <v>-17.619399999999999</v>
+      </c>
+      <c r="BX27">
+        <f t="shared" si="22"/>
+        <v>-3.7480000000000013E-2</v>
+      </c>
+      <c r="BY27">
+        <f t="shared" si="23"/>
+        <v>-164</v>
+      </c>
+      <c r="BZ27" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA27">
+        <f t="shared" si="24"/>
+        <v>-0.4632768361581921</v>
+      </c>
+    </row>
+    <row r="28" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -44256,15 +44913,15 @@
         <v>408</v>
       </c>
       <c r="AN28">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>119.6892</v>
       </c>
       <c r="AO28">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.22966</v>
       </c>
       <c r="AP28">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>408</v>
       </c>
       <c r="AQ28" t="e">
@@ -44308,8 +44965,36 @@
         <f t="shared" si="4"/>
         <v>-165</v>
       </c>
-    </row>
-    <row r="29" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT28">
+        <v>74.373000000000005</v>
+      </c>
+      <c r="BU28">
+        <v>0.41049999999999998</v>
+      </c>
+      <c r="BV28">
+        <v>166</v>
+      </c>
+      <c r="BW28">
+        <f t="shared" si="21"/>
+        <v>-44.929699999999997</v>
+      </c>
+      <c r="BX28">
+        <f t="shared" si="22"/>
+        <v>0.18440999999999996</v>
+      </c>
+      <c r="BY28">
+        <f t="shared" si="23"/>
+        <v>-45</v>
+      </c>
+      <c r="BZ28" t="s">
+        <v>239</v>
+      </c>
+      <c r="CA28">
+        <f t="shared" si="24"/>
+        <v>-0.2132701421800948</v>
+      </c>
+    </row>
+    <row r="29" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -44379,15 +45064,15 @@
         <v>712</v>
       </c>
       <c r="AN29">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>91.474900000000005</v>
       </c>
       <c r="AO29">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.34320000000000001</v>
       </c>
       <c r="AP29">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>712</v>
       </c>
       <c r="AQ29" t="e">
@@ -44431,8 +45116,36 @@
         <f t="shared" si="4"/>
         <v>-324</v>
       </c>
-    </row>
-    <row r="30" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT29">
+        <v>38.115699999999997</v>
+      </c>
+      <c r="BU29">
+        <v>0.54688999999999999</v>
+      </c>
+      <c r="BV29">
+        <v>309</v>
+      </c>
+      <c r="BW29">
+        <f t="shared" si="21"/>
+        <v>-16.9223</v>
+      </c>
+      <c r="BX29">
+        <f t="shared" si="22"/>
+        <v>5.1529999999999965E-2</v>
+      </c>
+      <c r="BY29">
+        <f t="shared" si="23"/>
+        <v>-117</v>
+      </c>
+      <c r="BZ29" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA29">
+        <f t="shared" si="24"/>
+        <v>-0.27464788732394368</v>
+      </c>
+    </row>
+    <row r="30" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -44502,15 +45215,15 @@
         <v>454</v>
       </c>
       <c r="AN30">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>88.2821</v>
       </c>
       <c r="AO30">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>8.9889999999999998E-2</v>
       </c>
       <c r="AP30">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>454</v>
       </c>
       <c r="AQ30" t="e">
@@ -44554,8 +45267,36 @@
         <f t="shared" si="4"/>
         <v>-233</v>
       </c>
-    </row>
-    <row r="31" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT30">
+        <v>38.648000000000003</v>
+      </c>
+      <c r="BU30">
+        <v>0.15513399999999999</v>
+      </c>
+      <c r="BV30">
+        <v>251</v>
+      </c>
+      <c r="BW30">
+        <f t="shared" si="21"/>
+        <v>-20.234599999999993</v>
+      </c>
+      <c r="BX30">
+        <f t="shared" si="22"/>
+        <v>4.4763999999999998E-2</v>
+      </c>
+      <c r="BY30">
+        <f t="shared" si="23"/>
+        <v>-62</v>
+      </c>
+      <c r="BZ30" t="s">
+        <v>237</v>
+      </c>
+      <c r="CA30">
+        <f t="shared" si="24"/>
+        <v>-0.19808306709265175</v>
+      </c>
+    </row>
+    <row r="31" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -44623,15 +45364,15 @@
         <v>327</v>
       </c>
       <c r="AN31">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>67.405699999999996</v>
       </c>
       <c r="AO31">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.19688</v>
       </c>
       <c r="AP31">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>327</v>
       </c>
       <c r="AQ31" t="e">
@@ -44675,8 +45416,36 @@
         <f t="shared" si="4"/>
         <v>-140</v>
       </c>
-    </row>
-    <row r="32" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT31">
+        <v>42.404299999999999</v>
+      </c>
+      <c r="BU31">
+        <v>0.46196999999999999</v>
+      </c>
+      <c r="BV31">
+        <v>161</v>
+      </c>
+      <c r="BW31">
+        <f t="shared" si="21"/>
+        <v>-24.530290000000001</v>
+      </c>
+      <c r="BX31">
+        <f t="shared" si="22"/>
+        <v>5.4080000000000017E-2</v>
+      </c>
+      <c r="BY31">
+        <f t="shared" si="23"/>
+        <v>-50</v>
+      </c>
+      <c r="BZ31" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA31">
+        <f t="shared" si="24"/>
+        <v>-0.23696682464454977</v>
+      </c>
+    </row>
+    <row r="32" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -44745,15 +45514,15 @@
         <v>828</v>
       </c>
       <c r="AN32">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>84.632999999999996</v>
       </c>
       <c r="AO32">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.2198</v>
       </c>
       <c r="AP32">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>828</v>
       </c>
       <c r="AQ32" t="e">
@@ -44797,8 +45566,36 @@
         <f t="shared" si="4"/>
         <v>-318</v>
       </c>
-    </row>
-    <row r="33" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT32">
+        <v>45.908999999999999</v>
+      </c>
+      <c r="BU32">
+        <v>0.42104000000000003</v>
+      </c>
+      <c r="BV32">
+        <v>331</v>
+      </c>
+      <c r="BW32">
+        <f t="shared" si="21"/>
+        <v>-34.778500000000001</v>
+      </c>
+      <c r="BX32">
+        <f t="shared" si="22"/>
+        <v>9.9372000000000016E-2</v>
+      </c>
+      <c r="BY32">
+        <f t="shared" si="23"/>
+        <v>-204</v>
+      </c>
+      <c r="BZ32" t="s">
+        <v>238</v>
+      </c>
+      <c r="CA32">
+        <f t="shared" si="24"/>
+        <v>-0.38130841121495329</v>
+      </c>
+    </row>
+    <row r="33" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -44867,15 +45664,15 @@
         <v>1052</v>
       </c>
       <c r="AN33">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>113.6572</v>
       </c>
       <c r="AO33">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.13764999999999999</v>
       </c>
       <c r="AP33">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>1052</v>
       </c>
       <c r="AQ33" t="e">
@@ -44919,8 +45716,36 @@
         <f t="shared" si="4"/>
         <v>-477</v>
       </c>
-    </row>
-    <row r="34" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT33">
+        <v>71.806899999999999</v>
+      </c>
+      <c r="BU33">
+        <v>0.18079999999999999</v>
+      </c>
+      <c r="BV33">
+        <v>402</v>
+      </c>
+      <c r="BW33">
+        <f t="shared" si="21"/>
+        <v>-20.801699999999997</v>
+      </c>
+      <c r="BX33">
+        <f t="shared" si="22"/>
+        <v>3.0099999999999988E-2</v>
+      </c>
+      <c r="BY33">
+        <f t="shared" si="23"/>
+        <v>-337</v>
+      </c>
+      <c r="BZ33" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA33">
+        <f t="shared" si="24"/>
+        <v>-0.45602165087956698</v>
+      </c>
+    </row>
+    <row r="34" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -44970,15 +45795,15 @@
         <v>840</v>
       </c>
       <c r="AN34">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>46.363799999999998</v>
       </c>
       <c r="AO34">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.27146999999999999</v>
       </c>
       <c r="AP34">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>840</v>
       </c>
       <c r="AQ34" t="e">
@@ -45031,8 +45856,36 @@
         <f t="shared" si="4"/>
         <v>234</v>
       </c>
-    </row>
-    <row r="35" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT34">
+        <v>33.96752</v>
+      </c>
+      <c r="BU34">
+        <v>0.28151999999999999</v>
+      </c>
+      <c r="BV34">
+        <v>837</v>
+      </c>
+      <c r="BW34">
+        <f t="shared" si="21"/>
+        <v>-12.161180000000002</v>
+      </c>
+      <c r="BX34">
+        <f t="shared" si="22"/>
+        <v>9.330000000000005E-3</v>
+      </c>
+      <c r="BY34">
+        <f t="shared" si="23"/>
+        <v>-3</v>
+      </c>
+      <c r="BZ34" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA34">
+        <f t="shared" si="24"/>
+        <v>-3.5714285714285713E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -45082,15 +45935,15 @@
         <v>610</v>
       </c>
       <c r="AN35">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>30.443850000000001</v>
       </c>
       <c r="AO35">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.28094999999999998</v>
       </c>
       <c r="AP35">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>610</v>
       </c>
       <c r="AQ35" t="e">
@@ -45143,8 +45996,36 @@
         <f t="shared" si="4"/>
         <v>23</v>
       </c>
-    </row>
-    <row r="36" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT35">
+        <v>22.156400000000001</v>
+      </c>
+      <c r="BU35">
+        <v>0.28470000000000001</v>
+      </c>
+      <c r="BV35">
+        <v>608</v>
+      </c>
+      <c r="BW35">
+        <f t="shared" si="21"/>
+        <v>-8.1758999999999986</v>
+      </c>
+      <c r="BX35">
+        <f t="shared" si="22"/>
+        <v>2.9299999999999882E-3</v>
+      </c>
+      <c r="BY35">
+        <f t="shared" si="23"/>
+        <v>-2</v>
+      </c>
+      <c r="BZ35" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA35">
+        <f t="shared" si="24"/>
+        <v>-3.2786885245901639E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -45212,15 +46093,15 @@
         <v>307</v>
       </c>
       <c r="AN36">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>66.238900000000001</v>
       </c>
       <c r="AO36">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.42817</v>
       </c>
       <c r="AP36">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>307</v>
       </c>
       <c r="AQ36" t="e">
@@ -45264,8 +46145,36 @@
         <f t="shared" si="4"/>
         <v>-159</v>
       </c>
-    </row>
-    <row r="37" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT36">
+        <v>36.930500000000002</v>
+      </c>
+      <c r="BU36">
+        <v>0.74221999999999999</v>
+      </c>
+      <c r="BV36">
+        <v>145</v>
+      </c>
+      <c r="BW36">
+        <f>BU35-AS36</f>
+        <v>-64.275000000000006</v>
+      </c>
+      <c r="BX36">
+        <f t="shared" si="22"/>
+        <v>0.39032</v>
+      </c>
+      <c r="BY36">
+        <f t="shared" si="23"/>
+        <v>-29</v>
+      </c>
+      <c r="BZ36" t="s">
+        <v>239</v>
+      </c>
+      <c r="CA36">
+        <f t="shared" si="24"/>
+        <v>-0.16666666666666666</v>
+      </c>
+    </row>
+    <row r="37" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -45333,15 +46242,15 @@
         <v>464</v>
       </c>
       <c r="AN37">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>157.17169999999999</v>
       </c>
       <c r="AO37">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>9.6170000000000005E-2</v>
       </c>
       <c r="AP37">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>464</v>
       </c>
       <c r="AQ37" t="e">
@@ -45385,8 +46294,36 @@
         <f t="shared" si="4"/>
         <v>-250</v>
       </c>
-    </row>
-    <row r="38" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT37">
+        <v>80.925799999999995</v>
+      </c>
+      <c r="BU37">
+        <v>0.19917000000000001</v>
+      </c>
+      <c r="BV37">
+        <v>212</v>
+      </c>
+      <c r="BW37">
+        <f t="shared" si="21"/>
+        <v>-79.279200000000017</v>
+      </c>
+      <c r="BX37">
+        <f t="shared" si="22"/>
+        <v>8.5710000000000008E-2</v>
+      </c>
+      <c r="BY37">
+        <f t="shared" si="23"/>
+        <v>-222</v>
+      </c>
+      <c r="BZ37" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA37">
+        <f t="shared" si="24"/>
+        <v>-0.51152073732718895</v>
+      </c>
+    </row>
+    <row r="38" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -45456,15 +46393,15 @@
         <v>508</v>
       </c>
       <c r="AN38">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>98.72</v>
       </c>
       <c r="AO38">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.21548</v>
       </c>
       <c r="AP38">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>508</v>
       </c>
       <c r="AQ38" t="e">
@@ -45508,8 +46445,36 @@
         <f t="shared" si="4"/>
         <v>-263</v>
       </c>
-    </row>
-    <row r="39" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT38">
+        <v>49.030799999999999</v>
+      </c>
+      <c r="BU38">
+        <v>0.45689999999999997</v>
+      </c>
+      <c r="BV38">
+        <v>267</v>
+      </c>
+      <c r="BW38">
+        <f t="shared" si="21"/>
+        <v>-38.418859999999995</v>
+      </c>
+      <c r="BX38">
+        <f t="shared" si="22"/>
+        <v>9.037999999999996E-2</v>
+      </c>
+      <c r="BY38">
+        <f t="shared" si="23"/>
+        <v>-59</v>
+      </c>
+      <c r="BZ38" t="s">
+        <v>237</v>
+      </c>
+      <c r="CA38">
+        <f t="shared" si="24"/>
+        <v>-0.18098159509202455</v>
+      </c>
+    </row>
+    <row r="39" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -45577,15 +46542,15 @@
         <v>230</v>
       </c>
       <c r="AN39">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>102.0086</v>
       </c>
       <c r="AO39">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>7.3599999999999999E-2</v>
       </c>
       <c r="AP39">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>230</v>
       </c>
       <c r="AQ39" t="e">
@@ -45629,8 +46594,20 @@
         <f t="shared" si="4"/>
         <v>-137</v>
       </c>
-    </row>
-    <row r="40" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BW39">
+        <f t="shared" si="21"/>
+        <v>-103.3746</v>
+      </c>
+      <c r="BY39">
+        <f t="shared" si="23"/>
+        <v>-174</v>
+      </c>
+      <c r="CA39">
+        <f t="shared" si="24"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -45680,15 +46657,15 @@
         <v>301</v>
       </c>
       <c r="AN40">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>90.071899999999999</v>
       </c>
       <c r="AO40">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.2913</v>
       </c>
       <c r="AP40">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>301</v>
       </c>
       <c r="AQ40" t="e">
@@ -45741,8 +46718,36 @@
         <f t="shared" si="4"/>
         <v>38</v>
       </c>
-    </row>
-    <row r="41" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT40">
+        <v>42.081200000000003</v>
+      </c>
+      <c r="BU40">
+        <v>0.45569999999999999</v>
+      </c>
+      <c r="BV40">
+        <v>235</v>
+      </c>
+      <c r="BW40">
+        <f t="shared" si="21"/>
+        <v>-43.069470000000003</v>
+      </c>
+      <c r="BX40">
+        <f t="shared" si="22"/>
+        <v>0.11466999999999999</v>
+      </c>
+      <c r="BY40">
+        <f t="shared" si="23"/>
+        <v>-11</v>
+      </c>
+      <c r="BZ40" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA40">
+        <f t="shared" si="24"/>
+        <v>-4.4715447154471545E-2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -45792,15 +46797,15 @@
         <v>404</v>
       </c>
       <c r="AN41">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>46.406399999999998</v>
       </c>
       <c r="AO41">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.15325</v>
       </c>
       <c r="AP41">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>404</v>
       </c>
       <c r="AQ41" t="e">
@@ -45853,8 +46858,36 @@
         <f t="shared" si="4"/>
         <v>12</v>
       </c>
-    </row>
-    <row r="42" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT41">
+        <v>29.056999999999999</v>
+      </c>
+      <c r="BU41">
+        <v>0.20055999999999999</v>
+      </c>
+      <c r="BV41">
+        <v>324</v>
+      </c>
+      <c r="BW41">
+        <f t="shared" si="21"/>
+        <v>-18.274699999999999</v>
+      </c>
+      <c r="BX41">
+        <f t="shared" si="22"/>
+        <v>7.3199999999999987E-2</v>
+      </c>
+      <c r="BY41">
+        <f t="shared" si="23"/>
+        <v>-5</v>
+      </c>
+      <c r="BZ41" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA41">
+        <f t="shared" si="24"/>
+        <v>-1.5197568389057751E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -45904,15 +46937,15 @@
         <v>212</v>
       </c>
       <c r="AN42">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>83.256900000000002</v>
       </c>
       <c r="AO42">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.30740000000000001</v>
       </c>
       <c r="AP42">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>212</v>
       </c>
       <c r="AQ42" t="e">
@@ -45965,8 +46998,36 @@
         <f t="shared" si="4"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="43" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BT42">
+        <v>24.6417</v>
+      </c>
+      <c r="BU42">
+        <v>0.47789999999999999</v>
+      </c>
+      <c r="BV42">
+        <v>159</v>
+      </c>
+      <c r="BW42">
+        <f t="shared" si="21"/>
+        <v>-43.617500000000007</v>
+      </c>
+      <c r="BX42">
+        <f t="shared" si="22"/>
+        <v>0.22054000000000001</v>
+      </c>
+      <c r="BY42">
+        <f t="shared" si="23"/>
+        <v>-6</v>
+      </c>
+      <c r="BZ42" t="s">
+        <v>236</v>
+      </c>
+      <c r="CA42">
+        <f t="shared" si="24"/>
+        <v>-3.6363636363636362E-2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:79" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -46016,15 +47077,15 @@
         <v>202</v>
       </c>
       <c r="AN43">
-        <f t="shared" si="24"/>
+        <f t="shared" si="28"/>
         <v>215.42920000000001</v>
       </c>
       <c r="AO43">
-        <f t="shared" si="25"/>
+        <f t="shared" si="29"/>
         <v>0.25890000000000002</v>
       </c>
       <c r="AP43">
-        <f t="shared" si="26"/>
+        <f t="shared" si="30"/>
         <v>202</v>
       </c>
       <c r="AQ43" t="e">
@@ -46077,8 +47138,20 @@
         <f t="shared" si="4"/>
         <v>28</v>
       </c>
-    </row>
-    <row r="45" spans="1:70" x14ac:dyDescent="0.35">
+      <c r="BW43">
+        <f t="shared" si="21"/>
+        <v>-167.8339</v>
+      </c>
+      <c r="BY43">
+        <f t="shared" si="23"/>
+        <v>-160</v>
+      </c>
+      <c r="CA43">
+        <f t="shared" si="24"/>
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:79" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -46087,6 +47160,10 @@
         <f>SUM(AA5,AA9:AA10,AA13,AA17:AA18,AA21,AA25:AA33,AA36:AA39)</f>
         <v>0.1336999999999999</v>
       </c>
+      <c r="AW45">
+        <f>SUM(AW5:AW43)</f>
+        <v>1.3482715000000001</v>
+      </c>
       <c r="BP45">
         <f>SUM(BP6:BP7,BP9,BP11,BP14,BP16,BP20,BP23:BP24,BP34:BP35,BP40:BP43)</f>
         <v>27.277845000000013</v>
@@ -46094,6 +47171,28 @@
       <c r="BQ45">
         <f>SUM(BQ6:BQ7,BQ9,BQ11,BQ14,BQ16,BQ20,BQ23:BQ24,BQ34:BQ35,BQ40:BQ43)</f>
         <v>-0.10875460000000006</v>
+      </c>
+      <c r="BX45">
+        <f>SUM(BX5:BX43)</f>
+        <v>2.2365048000000005</v>
+      </c>
+      <c r="BZ45" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="46" spans="1:79" x14ac:dyDescent="0.35">
+      <c r="BZ46" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="47" spans="1:79" x14ac:dyDescent="0.35">
+      <c r="BZ47" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="48" spans="1:79" x14ac:dyDescent="0.35">
+      <c r="BZ48" t="s">
+        <v>245</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Brought in Harvey's zooplankton data by strata. Need to create new variables by season for merge. Replacing sm/lg copepods, total copepods and zoopl biomass anomalies by EPU
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -40907,9 +40907,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:DP49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="DG1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="DM44" sqref="DM44"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="88" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="DH1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="DN18" sqref="DN18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -51742,6 +51742,10 @@
       </c>
       <c r="CV45" t="s">
         <v>252</v>
+      </c>
+      <c r="DM45">
+        <f>SUM(DM5:DM43)</f>
+        <v>0.15523900000000007</v>
       </c>
     </row>
     <row r="46" spans="1:120" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
SOE plot including all sexes
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3605" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="309">
   <si>
     <t>Species</t>
   </si>
@@ -2606,7 +2606,49 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="213">
+  <dxfs count="217">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -5099,30 +5141,30 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B5:C41">
-    <cfRule type="containsBlanks" dxfId="212" priority="5">
+    <cfRule type="containsBlanks" dxfId="216" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="214" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="213" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H43">
-    <cfRule type="containsBlanks" dxfId="208" priority="1">
+    <cfRule type="containsBlanks" dxfId="212" priority="1">
       <formula>LEN(TRIM(G5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(G5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="211" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="210" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6951,16 +6993,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:AF7 F9:AF43 F8:P8 R8:AF8">
-    <cfRule type="containsBlanks" dxfId="58" priority="1">
+    <cfRule type="containsBlanks" dxfId="62" priority="1">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="61" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8987,16 +9029,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:Z43">
-    <cfRule type="containsBlanks" dxfId="55" priority="1">
+    <cfRule type="containsBlanks" dxfId="59" priority="1">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9396,16 +9438,16 @@
     <sortCondition ref="B5:B41"/>
   </sortState>
   <conditionalFormatting sqref="B5:C41">
-    <cfRule type="containsBlanks" dxfId="51" priority="1">
+    <cfRule type="containsBlanks" dxfId="55" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9653,16 +9695,16 @@
     <sortCondition ref="C5:C27"/>
   </sortState>
   <conditionalFormatting sqref="B5:C27">
-    <cfRule type="containsBlanks" dxfId="47" priority="1">
+    <cfRule type="containsBlanks" dxfId="51" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="50" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10188,16 +10230,16 @@
     <sortCondition ref="E5:E42"/>
   </sortState>
   <conditionalFormatting sqref="B5:E43">
-    <cfRule type="containsBlanks" dxfId="44" priority="1">
+    <cfRule type="containsBlanks" dxfId="48" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10840,30 +10882,30 @@
     <sortCondition ref="C5:C28"/>
   </sortState>
   <conditionalFormatting sqref="B5:E28">
-    <cfRule type="containsBlanks" dxfId="40" priority="5">
+    <cfRule type="containsBlanks" dxfId="44" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:K43">
-    <cfRule type="containsBlanks" dxfId="36" priority="1">
+    <cfRule type="containsBlanks" dxfId="40" priority="1">
       <formula>LEN(TRIM(H5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(H5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="39" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="34" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11160,16 +11202,16 @@
     <sortCondition ref="E5:E31"/>
   </sortState>
   <conditionalFormatting sqref="B5:E31">
-    <cfRule type="containsBlanks" dxfId="33" priority="1">
+    <cfRule type="containsBlanks" dxfId="37" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="36" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11843,16 +11885,16 @@
     <sortCondition ref="G5:G31"/>
   </sortState>
   <conditionalFormatting sqref="B5:G31 J5:M31">
-    <cfRule type="containsBlanks" dxfId="30" priority="5">
+    <cfRule type="containsBlanks" dxfId="34" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12353,16 +12395,16 @@
     <sortCondition ref="L5:L37"/>
   </sortState>
   <conditionalFormatting sqref="B5:L37">
-    <cfRule type="containsBlanks" dxfId="26" priority="1">
+    <cfRule type="containsBlanks" dxfId="30" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="29" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12764,16 +12806,16 @@
     <sortCondition ref="C6:C43"/>
   </sortState>
   <conditionalFormatting sqref="B5:C41">
-    <cfRule type="containsBlanks" dxfId="23" priority="1">
+    <cfRule type="containsBlanks" dxfId="27" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25436,44 +25478,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="205" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="209" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="204" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="208" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="207" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="202" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="206" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="201" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="205" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="204" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="199" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="203" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="198" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="202" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="197" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="201" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="196" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="200" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25661,16 +25703,16 @@
     <sortCondition ref="C5:C43"/>
   </sortState>
   <conditionalFormatting sqref="B5:C21">
-    <cfRule type="containsBlanks" dxfId="19" priority="1">
+    <cfRule type="containsBlanks" dxfId="23" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25896,16 +25938,16 @@
     <sortCondition ref="E5:E22"/>
   </sortState>
   <conditionalFormatting sqref="B5:C15 E5:E17 C16:C17">
-    <cfRule type="containsBlanks" dxfId="16" priority="1">
+    <cfRule type="containsBlanks" dxfId="20" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26615,28 +26657,28 @@
     <sortCondition descending="1" ref="F5:F43"/>
   </sortState>
   <conditionalFormatting sqref="B5:B43">
-    <cfRule type="containsBlanks" dxfId="12" priority="4">
+    <cfRule type="containsBlanks" dxfId="16" priority="4">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F43">
-    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
       <formula>0.25</formula>
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="3" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26955,16 +26997,16 @@
     <sortCondition ref="B3:B41"/>
   </sortState>
   <conditionalFormatting sqref="B3:B41">
-    <cfRule type="containsBlanks" dxfId="5" priority="1">
+    <cfRule type="containsBlanks" dxfId="9" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29261,15 +29303,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E40">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31854,145 +31896,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="195" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="199" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="194" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="198" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="193" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="197" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="192" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="196" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="191" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="195" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="190" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="194" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="189" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="193" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="188" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="192" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="191" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="186" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="190" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="185" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="189" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="184" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="188" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="183" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="187" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="182" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="186" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="181" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="185" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="180" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="184" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="179" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="183" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="178" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="182" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="177" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="181" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="176" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="180" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="175" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="179" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="174" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="178" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="173" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="177" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="172" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="176" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="171" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="175" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="170" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="174" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="173" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="168" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="172" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="167" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="171" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="166" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="170" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="165" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="169" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="164" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="168" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="167" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33815,168 +33857,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="162" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="166" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17 B38:B119">
-    <cfRule type="cellIs" dxfId="161" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="165" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="164" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="159" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="163" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="162" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="157" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="161" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="160" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 J5 J10 J14 J17:J18 J21:J22 J24:J25 J27:J29">
-    <cfRule type="cellIs" dxfId="155" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="159" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="154" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="158" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31 L5 L10 L14 L17:L18 L21:L22 L27:L29 L24:L25">
-    <cfRule type="cellIs" dxfId="153" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="157" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L4 L6:L9 L11:L13 L15:L16 L19:L20 L23 L30:L31 L26">
-    <cfRule type="cellIs" dxfId="152" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="156" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="151" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="155" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="150" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="154" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="149" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="153" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="152" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26 P4:P9 P11 P13:P15 P19:P21 P24 P30">
-    <cfRule type="cellIs" dxfId="147" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="151" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P31 P18 P10 P12 P16 P22:P23 P25:P26">
-    <cfRule type="cellIs" dxfId="146" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="150" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="145" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="149" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="144" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="148" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="143" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="147" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="142" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="146" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13 R10 R12 R16:R18 R22:R23 R25:R29 R31 R3">
-    <cfRule type="cellIs" dxfId="141" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="145" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2 R19:R21 R6:R9 R11 R13 R24 R30 R4">
-    <cfRule type="cellIs" dxfId="140" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="144" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="139" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="143" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="138" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="142" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="137" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="141" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="136" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="140" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="135" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="139" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="134" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="133" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="137" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="132" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="136" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="131" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="130" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="134" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119 B31:B37">
-    <cfRule type="cellIs" dxfId="129" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="133" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="128" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="132" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="127" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="131" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="126" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="130" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 J3:J4 J6:J9 J11:J13 J15:J16 J19:J20 J23 J26 J30:J31">
-    <cfRule type="cellIs" dxfId="125" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="129" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42195,87 +42237,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="124" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="128" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="123" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="127" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="126" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="121" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="125" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="120" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="124" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="119" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="123" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="118" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="122" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="117" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="121" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="116" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="119" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="114" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="118" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="113" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="117" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="112" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="116" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="111" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="115" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="110" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="114" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="109" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="112" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="107" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="111" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="106" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="110" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -46298,67 +46340,67 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="105" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="109" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="108" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="103" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="107" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="102" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="12" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="101" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="105" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="104" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="99" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="8" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="97" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="101" priority="7" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ4:BJ27">
-    <cfRule type="cellIs" dxfId="96" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="6" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BH27">
-    <cfRule type="cellIs" dxfId="95" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="99" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="94" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="98" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ28:BJ32">
-    <cfRule type="cellIs" dxfId="93" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="97" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB28:BH32">
-    <cfRule type="cellIs" dxfId="92" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="91" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="95" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52277,28 +52319,28 @@
     <sortCondition ref="I2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="90" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="88" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="92" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="87" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="91" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="86" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="90" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="89" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53674,19 +53716,19 @@
     <mergeCell ref="AD2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
-    <cfRule type="cellIs" dxfId="84" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="lessThan">
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="86" priority="3" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="81" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="85" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="5" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53700,8 +53742,8 @@
   <dimension ref="A1:GB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="FJ1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FW11" sqref="FW11"/>
+      <pane xSplit="1" topLeftCell="FD1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FU5" sqref="FU5:FU44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53913,6 +53955,9 @@
       <c r="FE3" s="69" t="s">
         <v>177</v>
       </c>
+      <c r="FN3" s="69" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="4" spans="1:184" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
@@ -54762,11 +54807,11 @@
         <v>-0.21120000000000516</v>
       </c>
       <c r="FI5">
-        <f t="shared" ref="FI5:FJ5" si="14">FF5-EJ5</f>
+        <f>FF5-EJ5</f>
         <v>-1.2900000000000023E-2</v>
       </c>
       <c r="FJ5">
-        <f t="shared" si="14"/>
+        <f t="shared" ref="FI5:FJ5" si="14">FG5-EK5</f>
         <v>0</v>
       </c>
       <c r="FK5">
@@ -54777,13 +54822,16 @@
         <f>FI5/EJ5</f>
         <v>-5.1828043390920134E-2</v>
       </c>
+      <c r="FO5">
+        <v>0.21141699999999999</v>
+      </c>
       <c r="FQ5">
         <f>FN5-FE5</f>
         <v>-41.577399999999997</v>
       </c>
       <c r="FR5">
         <f>FO5-FF5</f>
-        <v>-0.23599999999999999</v>
+        <v>-2.4582999999999994E-2</v>
       </c>
       <c r="FS5">
         <f>FP5-FG5</f>
@@ -54793,7 +54841,10 @@
         <f>FS5/FF5</f>
         <v>-2444.9152542372881</v>
       </c>
-      <c r="FU5" s="143"/>
+      <c r="FU5" s="143">
+        <f>FR5+FI5</f>
+        <v>-3.7483000000000016E-2</v>
+      </c>
     </row>
     <row r="6" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
@@ -55189,13 +55240,16 @@
         <f t="shared" ref="FL6:FL18" si="53">FI6/EJ6</f>
         <v>-1.4459350370397969E-2</v>
       </c>
+      <c r="FO6">
+        <v>0.15770000000000001</v>
+      </c>
       <c r="FQ6">
         <f t="shared" ref="FQ6:FQ44" si="54">FN6-FE6</f>
         <v>-45.814</v>
       </c>
       <c r="FR6">
         <f t="shared" ref="FR6:FR44" si="55">FO6-FF6</f>
-        <v>-0.34549999999999997</v>
+        <v>-0.18779999999999997</v>
       </c>
       <c r="FS6">
         <f t="shared" ref="FS6:FS44" si="56">FP6-FG6</f>
@@ -55205,6 +55259,10 @@
         <f t="shared" ref="FT6:FT44" si="57">FS6/FF6</f>
         <v>-1554.2691751085385</v>
       </c>
+      <c r="FU6" s="143">
+        <f t="shared" ref="FU6:FU44" si="58">FR6+FI6</f>
+        <v>-0.19286900000000001</v>
+      </c>
     </row>
     <row r="7" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -55596,13 +55654,16 @@
         <f t="shared" si="53"/>
         <v>-1.1051555506433246E-4</v>
       </c>
+      <c r="FO7">
+        <v>0.30356</v>
+      </c>
       <c r="FQ7">
         <f t="shared" si="54"/>
         <v>-56.337000000000003</v>
       </c>
       <c r="FR7">
         <f t="shared" si="55"/>
-        <v>-0.3619</v>
+        <v>-5.8340000000000003E-2</v>
       </c>
       <c r="FS7">
         <f t="shared" si="56"/>
@@ -55612,6 +55673,10 @@
         <f t="shared" si="57"/>
         <v>-1221.331859629732</v>
       </c>
+      <c r="FU7" s="143">
+        <f t="shared" si="58"/>
+        <v>-5.8379999999999987E-2</v>
+      </c>
     </row>
     <row r="8" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
@@ -55982,13 +56047,16 @@
         <f t="shared" si="53"/>
         <v>0.43249451911161946</v>
       </c>
+      <c r="FO8">
+        <v>0.21293000000000001</v>
+      </c>
       <c r="FQ8">
         <f t="shared" si="54"/>
         <v>-24.486799999999999</v>
       </c>
       <c r="FR8">
         <f t="shared" si="55"/>
-        <v>-0.300566</v>
+        <v>-8.7635999999999992E-2</v>
       </c>
       <c r="FS8">
         <f t="shared" si="56"/>
@@ -55997,6 +56065,10 @@
       <c r="FT8">
         <f t="shared" si="57"/>
         <v>-1134.5261939141487</v>
+      </c>
+      <c r="FU8" s="143">
+        <f t="shared" si="58"/>
+        <v>3.1100000000000017E-3</v>
       </c>
     </row>
     <row r="9" spans="1:184" x14ac:dyDescent="0.35">
@@ -56420,20 +56492,24 @@
         <v>1924</v>
       </c>
       <c r="FQ9">
-        <f t="shared" si="54"/>
-        <v>-5.2012999999999749</v>
+        <f>FN9-DJ9</f>
+        <v>0.13690000000002556</v>
       </c>
       <c r="FR9">
-        <f t="shared" si="55"/>
-        <v>4.3879799999999997E-2</v>
+        <f t="shared" ref="FR9:FS9" si="59">FO9-DK9</f>
+        <v>-6.0499999999991116E-5</v>
       </c>
       <c r="FS9">
-        <f t="shared" si="56"/>
-        <v>310</v>
+        <f t="shared" si="59"/>
+        <v>-2</v>
       </c>
       <c r="FT9">
-        <f t="shared" si="57"/>
-        <v>1569.2229815236649</v>
+        <f>FS9/DK9</f>
+        <v>-8.281906146954972</v>
+      </c>
+      <c r="FU9" s="143">
+        <f t="shared" si="58"/>
+        <v>-6.0499999999991116E-5</v>
       </c>
       <c r="FV9" s="65">
         <v>8.3698180000000004E-7</v>
@@ -56548,15 +56624,15 @@
         <v>1015</v>
       </c>
       <c r="AN10">
-        <f t="shared" ref="AN10:AN13" si="58">AK10-AD10</f>
+        <f t="shared" ref="AN10:AN13" si="60">AK10-AD10</f>
         <v>43.599399999999989</v>
       </c>
       <c r="AO10">
-        <f t="shared" ref="AO10:AO13" si="59">AL10-AE10</f>
+        <f t="shared" ref="AO10:AO13" si="61">AL10-AE10</f>
         <v>0.12449200000000001</v>
       </c>
       <c r="AP10">
-        <f t="shared" ref="AP10:AP13" si="60">AM10-AF10</f>
+        <f t="shared" ref="AP10:AP13" si="62">AM10-AF10</f>
         <v>132</v>
       </c>
       <c r="AQ10">
@@ -56682,7 +56758,7 @@
         <v>0</v>
       </c>
       <c r="CW10">
-        <f t="shared" ref="CW10" si="61">(AU10-CQ10)/AU10</f>
+        <f t="shared" ref="CW10" si="63">(AU10-CQ10)/AU10</f>
         <v>2.167487684729064E-2</v>
       </c>
       <c r="DA10">
@@ -56810,13 +56886,16 @@
         <f t="shared" si="53"/>
         <v>-3.6111657165323476E-2</v>
       </c>
+      <c r="FO10">
+        <v>0.19596</v>
+      </c>
       <c r="FQ10">
         <f t="shared" si="54"/>
         <v>-52.234000000000002</v>
       </c>
       <c r="FR10">
         <f t="shared" si="55"/>
-        <v>-0.24516499999999999</v>
+        <v>-4.9204999999999999E-2</v>
       </c>
       <c r="FS10">
         <f t="shared" si="56"/>
@@ -56825,6 +56904,10 @@
       <c r="FT10">
         <f t="shared" si="57"/>
         <v>-2639.0390145412275</v>
+      </c>
+      <c r="FU10" s="143">
+        <f t="shared" si="58"/>
+        <v>-5.8390000000000025E-2</v>
       </c>
       <c r="FV10" s="65"/>
       <c r="FW10" s="65"/>
@@ -56905,15 +56988,15 @@
         <v>1133</v>
       </c>
       <c r="AN11">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>48.030640000000005</v>
       </c>
       <c r="AO11">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>6.7830000000000015E-2</v>
       </c>
       <c r="AP11">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>145</v>
       </c>
       <c r="AQ11">
@@ -57072,7 +57155,7 @@
         <v>0.29904306220095694</v>
       </c>
       <c r="CW11">
-        <f t="shared" ref="CW11:CW43" si="62">(AU11-CQ11)/AU11</f>
+        <f t="shared" ref="CW11:CW43" si="64">(AU11-CQ11)/AU11</f>
         <v>6.7010309278350513E-2</v>
       </c>
       <c r="DA11">
@@ -57191,13 +57274,16 @@
         <f>FI11/EA11</f>
         <v>0.28222149654786355</v>
       </c>
+      <c r="FO11">
+        <v>0.221111</v>
+      </c>
       <c r="FQ11">
         <f t="shared" si="54"/>
         <v>-31.87</v>
       </c>
       <c r="FR11">
         <f t="shared" si="55"/>
-        <v>-0.27485700000000002</v>
+        <v>-5.3746000000000016E-2</v>
       </c>
       <c r="FS11">
         <f t="shared" si="56"/>
@@ -57207,6 +57293,10 @@
         <f t="shared" si="57"/>
         <v>-1971.9344968474516</v>
       </c>
+      <c r="FU11" s="143">
+        <f t="shared" si="58"/>
+        <v>6.751000000000007E-3</v>
+      </c>
     </row>
     <row r="12" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -57279,15 +57369,15 @@
         <v>1157</v>
       </c>
       <c r="AN12">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>95.403899999999993</v>
       </c>
       <c r="AO12">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>0.29437999999999998</v>
       </c>
       <c r="AP12">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>1157</v>
       </c>
       <c r="AQ12" t="e">
@@ -57431,7 +57521,7 @@
         <v>0</v>
       </c>
       <c r="CW12">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.3967339097022094</v>
       </c>
       <c r="DA12">
@@ -57531,24 +57621,27 @@
         <v>650</v>
       </c>
       <c r="FH12">
-        <f t="shared" ref="FH12:FH17" si="63">FE12-DZ12</f>
+        <f t="shared" ref="FH12:FH17" si="65">FE12-DZ12</f>
         <v>-1.6389099999999956</v>
       </c>
       <c r="FI12">
-        <f t="shared" ref="FI12:FI17" si="64">FF12-EA12</f>
+        <f t="shared" ref="FI12:FI17" si="66">FF12-EA12</f>
         <v>4.5619999999999994E-2</v>
       </c>
       <c r="FJ12">
-        <f t="shared" ref="FJ12:FJ17" si="65">FG12-EB12</f>
+        <f t="shared" ref="FJ12:FJ17" si="67">FG12-EB12</f>
         <v>-100</v>
       </c>
       <c r="FK12">
-        <f t="shared" ref="FK12:FK17" si="66">FJ12/EB12</f>
+        <f t="shared" ref="FK12:FK17" si="68">FJ12/EB12</f>
         <v>-0.13333333333333333</v>
       </c>
       <c r="FL12">
-        <f t="shared" ref="FL12:FL17" si="67">FI12/EA12</f>
+        <f t="shared" ref="FL12:FL17" si="69">FI12/EA12</f>
         <v>0.14745620272803669</v>
+      </c>
+      <c r="FO12">
+        <v>0.31856000000000001</v>
       </c>
       <c r="FQ12">
         <f t="shared" si="54"/>
@@ -57556,7 +57649,7 @@
       </c>
       <c r="FR12">
         <f t="shared" si="55"/>
-        <v>-0.35499999999999998</v>
+        <v>-3.6439999999999972E-2</v>
       </c>
       <c r="FS12">
         <f t="shared" si="56"/>
@@ -57566,6 +57659,10 @@
         <f t="shared" si="57"/>
         <v>-1830.9859154929579</v>
       </c>
+      <c r="FU12" s="143">
+        <f t="shared" si="58"/>
+        <v>9.1800000000000215E-3</v>
+      </c>
     </row>
     <row r="13" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -57648,15 +57745,15 @@
         <v>1375</v>
       </c>
       <c r="AN13">
-        <f t="shared" si="58"/>
+        <f t="shared" si="60"/>
         <v>114.5904</v>
       </c>
       <c r="AO13">
-        <f t="shared" si="59"/>
+        <f t="shared" si="61"/>
         <v>0.16016</v>
       </c>
       <c r="AP13">
-        <f t="shared" si="60"/>
+        <f t="shared" si="62"/>
         <v>1375</v>
       </c>
       <c r="AQ13" t="e">
@@ -57773,7 +57870,7 @@
         <v>0</v>
       </c>
       <c r="CW13">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1.9778481012658229E-2</v>
       </c>
       <c r="DA13">
@@ -57873,24 +57970,27 @@
         <v>852</v>
       </c>
       <c r="FH13">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.19265000000000043</v>
       </c>
       <c r="FI13">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>-1.9830000000000014E-2</v>
       </c>
       <c r="FJ13">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>-387</v>
       </c>
       <c r="FK13">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-0.31234866828087166</v>
       </c>
       <c r="FL13">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>-0.10132856412876859</v>
+      </c>
+      <c r="FO13">
+        <v>0.18617</v>
       </c>
       <c r="FQ13">
         <f t="shared" si="54"/>
@@ -57898,7 +57998,7 @@
       </c>
       <c r="FR13">
         <f t="shared" si="55"/>
-        <v>-0.17587</v>
+        <v>1.0300000000000004E-2</v>
       </c>
       <c r="FS13">
         <f t="shared" si="56"/>
@@ -57908,6 +58008,10 @@
         <f t="shared" si="57"/>
         <v>-4844.4874054699494</v>
       </c>
+      <c r="FU13" s="143">
+        <f t="shared" si="58"/>
+        <v>-9.5300000000000107E-3</v>
+      </c>
     </row>
     <row r="14" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
@@ -57980,15 +58084,15 @@
         <v>1154</v>
       </c>
       <c r="AN14">
-        <f t="shared" ref="AN14:AN43" si="68">AK14-AD14</f>
+        <f t="shared" ref="AN14:AN43" si="70">AK14-AD14</f>
         <v>53.567700000000002</v>
       </c>
       <c r="AO14">
-        <f t="shared" ref="AO14:AO43" si="69">AL14-AE14</f>
+        <f t="shared" ref="AO14:AO43" si="71">AL14-AE14</f>
         <v>2.8599999999999987E-2</v>
       </c>
       <c r="AP14">
-        <f t="shared" ref="AP14:AP43" si="70">AM14-AF14</f>
+        <f t="shared" ref="AP14:AP43" si="72">AM14-AF14</f>
         <v>90</v>
       </c>
       <c r="AQ14">
@@ -58150,7 +58254,7 @@
         <v>0.17982456140350878</v>
       </c>
       <c r="CW14">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>8.191126279863481E-2</v>
       </c>
       <c r="DA14">
@@ -58250,24 +58354,27 @@
         <v>310</v>
       </c>
       <c r="FH14">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>-5.8879900000000021</v>
       </c>
       <c r="FI14">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>0.10228700000000002</v>
       </c>
       <c r="FJ14">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>-267</v>
       </c>
       <c r="FK14">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-0.46273830155979201</v>
       </c>
       <c r="FL14">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>0.44929127701910287</v>
+      </c>
+      <c r="FO14">
+        <v>0.24979999999999999</v>
       </c>
       <c r="FQ14">
         <f t="shared" si="54"/>
@@ -58275,7 +58382,7 @@
       </c>
       <c r="FR14">
         <f t="shared" si="55"/>
-        <v>-0.32995000000000002</v>
+        <v>-8.0150000000000027E-2</v>
       </c>
       <c r="FS14">
         <f t="shared" si="56"/>
@@ -58285,6 +58392,10 @@
         <f t="shared" si="57"/>
         <v>-939.53629337778443</v>
       </c>
+      <c r="FU14" s="143">
+        <f t="shared" si="58"/>
+        <v>2.213699999999999E-2</v>
+      </c>
     </row>
     <row r="15" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -58357,15 +58468,15 @@
         <v>1656</v>
       </c>
       <c r="AN15">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>90.829400000000007</v>
       </c>
       <c r="AO15">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.1797</v>
       </c>
       <c r="AP15">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1656</v>
       </c>
       <c r="AQ15" t="e">
@@ -58506,7 +58617,7 @@
         <v>0.297427652733119</v>
       </c>
       <c r="CW15">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>0.10333333333333333</v>
       </c>
       <c r="DA15">
@@ -58606,24 +58717,27 @@
         <v>374</v>
       </c>
       <c r="FH15">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>-1.3086999999999946</v>
       </c>
       <c r="FI15">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>0.12693500000000002</v>
       </c>
       <c r="FJ15">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>-374</v>
       </c>
       <c r="FK15">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-0.5</v>
       </c>
       <c r="FL15">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>0.47708266776915426</v>
+      </c>
+      <c r="FO15">
+        <v>0.24629999999999999</v>
       </c>
       <c r="FQ15">
         <f t="shared" si="54"/>
@@ -58631,7 +58745,7 @@
       </c>
       <c r="FR15">
         <f t="shared" si="55"/>
-        <v>-0.39300000000000002</v>
+        <v>-0.14670000000000002</v>
       </c>
       <c r="FS15">
         <f t="shared" si="56"/>
@@ -58641,6 +58755,10 @@
         <f t="shared" si="57"/>
         <v>-951.65394402035622</v>
       </c>
+      <c r="FU15" s="143">
+        <f t="shared" si="58"/>
+        <v>-1.9765000000000005E-2</v>
+      </c>
     </row>
     <row r="16" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
@@ -58704,15 +58822,15 @@
         <v>1396</v>
       </c>
       <c r="AN16">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>240.0746</v>
       </c>
       <c r="AO16">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>8.5360000000000005E-2</v>
       </c>
       <c r="AP16">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1396</v>
       </c>
       <c r="AQ16" t="e">
@@ -58853,7 +58971,7 @@
         <v>-1</v>
       </c>
       <c r="CW16">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA16">
@@ -58953,24 +59071,27 @@
         <v>660</v>
       </c>
       <c r="FH16">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>0.22479999999998768</v>
       </c>
       <c r="FI16">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>-7.5920000000000015E-3</v>
       </c>
       <c r="FJ16">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>-185</v>
       </c>
       <c r="FK16">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-0.21893491124260356</v>
       </c>
       <c r="FL16">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>-7.5969380097063111E-2</v>
+      </c>
+      <c r="FO16">
+        <v>9.7199999999999995E-2</v>
       </c>
       <c r="FQ16">
         <f t="shared" si="54"/>
@@ -58978,7 +59099,7 @@
       </c>
       <c r="FR16">
         <f t="shared" si="55"/>
-        <v>-9.2342999999999995E-2</v>
+        <v>4.8570000000000002E-3</v>
       </c>
       <c r="FS16">
         <f t="shared" si="56"/>
@@ -58988,8 +59109,12 @@
         <f t="shared" si="57"/>
         <v>-7147.2661706897115</v>
       </c>
-    </row>
-    <row r="17" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU16" s="143">
+        <f t="shared" si="58"/>
+        <v>-2.7350000000000013E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -59069,15 +59194,15 @@
         <v>527</v>
       </c>
       <c r="AN17">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>151.08240000000001</v>
       </c>
       <c r="AO17">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.36549999999999999</v>
       </c>
       <c r="AP17">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>527</v>
       </c>
       <c r="AQ17" t="e">
@@ -59209,7 +59334,7 @@
         <v>-1</v>
       </c>
       <c r="CW17">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA17">
@@ -59309,24 +59434,27 @@
         <v>171</v>
       </c>
       <c r="FH17">
-        <f t="shared" si="63"/>
+        <f t="shared" si="65"/>
         <v>-20.450800000000001</v>
       </c>
       <c r="FI17">
-        <f t="shared" si="64"/>
+        <f t="shared" si="66"/>
         <v>0.2616</v>
       </c>
       <c r="FJ17">
-        <f t="shared" si="65"/>
+        <f t="shared" si="67"/>
         <v>-199</v>
       </c>
       <c r="FK17">
-        <f t="shared" si="66"/>
+        <f t="shared" si="68"/>
         <v>-0.53783783783783778</v>
       </c>
       <c r="FL17">
-        <f t="shared" si="67"/>
+        <f t="shared" si="69"/>
         <v>0.70417227456258413</v>
+      </c>
+      <c r="FO17">
+        <v>0.36530000000000001</v>
       </c>
       <c r="FQ17">
         <f t="shared" si="54"/>
@@ -59334,7 +59462,7 @@
       </c>
       <c r="FR17">
         <f t="shared" si="55"/>
-        <v>-0.6331</v>
+        <v>-0.26779999999999998</v>
       </c>
       <c r="FS17">
         <f t="shared" si="56"/>
@@ -59344,8 +59472,12 @@
         <f t="shared" si="57"/>
         <v>-270.09951034591694</v>
       </c>
-    </row>
-    <row r="18" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU17" s="143">
+        <f t="shared" si="58"/>
+        <v>-6.1999999999999833E-3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -59408,11 +59540,11 @@
         <v>0</v>
       </c>
       <c r="AH18">
-        <f t="shared" ref="AH18" si="71">AE18-BI18</f>
+        <f t="shared" ref="AH18" si="73">AE18-BI18</f>
         <v>0</v>
       </c>
       <c r="AI18">
-        <f t="shared" ref="AI18" si="72">AF18-BJ18</f>
+        <f t="shared" ref="AI18" si="74">AF18-BJ18</f>
         <v>0</v>
       </c>
       <c r="AK18">
@@ -59425,15 +59557,15 @@
         <v>947</v>
       </c>
       <c r="AN18">
-        <f t="shared" ref="AN18" si="73">AK18-AD18</f>
+        <f t="shared" ref="AN18" si="75">AK18-AD18</f>
         <v>76.399000000000001</v>
       </c>
       <c r="AO18">
-        <f t="shared" ref="AO18" si="74">AL18-AE18</f>
+        <f t="shared" ref="AO18" si="76">AL18-AE18</f>
         <v>0.15029999999999999</v>
       </c>
       <c r="AP18">
-        <f t="shared" ref="AP18" si="75">AM18-AF18</f>
+        <f t="shared" ref="AP18" si="77">AM18-AF18</f>
         <v>947</v>
       </c>
       <c r="AQ18" t="e">
@@ -59450,11 +59582,11 @@
         <v>477</v>
       </c>
       <c r="AV18">
-        <f t="shared" ref="AV18" si="76">AS18-AK18</f>
+        <f t="shared" ref="AV18" si="78">AS18-AK18</f>
         <v>-18.928600000000003</v>
       </c>
       <c r="AW18">
-        <f t="shared" ref="AW18" si="77">AT18-AL18</f>
+        <f t="shared" ref="AW18" si="79">AT18-AL18</f>
         <v>0.1784</v>
       </c>
       <c r="AX18">
@@ -59565,7 +59697,7 @@
         <v>0.21787709497206703</v>
       </c>
       <c r="CW18">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>8.5953878406708595E-2</v>
       </c>
       <c r="DA18">
@@ -59693,13 +59825,16 @@
         <f t="shared" si="53"/>
         <v>6.7520752990391494E-2</v>
       </c>
+      <c r="FO18">
+        <v>0.29303000000000001</v>
+      </c>
       <c r="FQ18">
         <f t="shared" si="54"/>
         <v>-27</v>
       </c>
       <c r="FR18">
         <f t="shared" si="55"/>
-        <v>-0.4083</v>
+        <v>-0.11526999999999998</v>
       </c>
       <c r="FS18">
         <f t="shared" si="56"/>
@@ -59709,8 +59844,12 @@
         <f t="shared" si="57"/>
         <v>-600.04898359049719</v>
       </c>
-    </row>
-    <row r="19" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU18" s="143">
+        <f t="shared" si="58"/>
+        <v>-8.9444999999999997E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -59782,15 +59921,15 @@
         <v>734</v>
       </c>
       <c r="AN19">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>80.852900000000005</v>
       </c>
       <c r="AO19">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.24697</v>
       </c>
       <c r="AP19">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>734</v>
       </c>
       <c r="AQ19" t="e">
@@ -59910,7 +60049,7 @@
         <v>-1</v>
       </c>
       <c r="CW19">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA19">
@@ -60010,32 +60149,35 @@
         <v>537</v>
       </c>
       <c r="FH19">
-        <f t="shared" ref="FH19:FH43" si="78">FE19-DZ19</f>
+        <f t="shared" ref="FH19:FH43" si="80">FE19-DZ19</f>
         <v>1.9275900000000021</v>
       </c>
       <c r="FI19">
-        <f t="shared" ref="FI19:FI43" si="79">FF19-EA19</f>
+        <f t="shared" ref="FI19:FI43" si="81">FF19-EA19</f>
         <v>3.2999999999999696E-4</v>
       </c>
       <c r="FJ19">
-        <f t="shared" ref="FJ19:FJ43" si="80">FG19-EB19</f>
+        <f t="shared" ref="FJ19:FJ43" si="82">FG19-EB19</f>
         <v>-52</v>
       </c>
       <c r="FK19">
-        <f t="shared" ref="FK19:FK43" si="81">FJ19/EB19</f>
+        <f t="shared" ref="FK19:FK43" si="83">FJ19/EB19</f>
         <v>-8.8285229202037352E-2</v>
       </c>
       <c r="FL19">
-        <f t="shared" ref="FL19:FL43" si="82">FI19/EA19</f>
+        <f t="shared" ref="FL19:FL43" si="84">FI19/EA19</f>
         <v>1.2015292190059965E-3</v>
+      </c>
+      <c r="FO19">
+        <v>0.28610000000000002</v>
       </c>
       <c r="FQ19">
         <f t="shared" si="54"/>
         <v>-59.324590000000001</v>
       </c>
       <c r="FR19">
-        <f t="shared" si="55"/>
-        <v>-0.27498</v>
+        <f>FO26-FF19</f>
+        <v>-7.8779999999999989E-2</v>
       </c>
       <c r="FS19">
         <f t="shared" si="56"/>
@@ -60045,8 +60187,12 @@
         <f t="shared" si="57"/>
         <v>-1952.8692995854244</v>
       </c>
-    </row>
-    <row r="20" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU19" s="143">
+        <f t="shared" si="58"/>
+        <v>-7.8449999999999992E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -60108,15 +60254,15 @@
         <v>651</v>
       </c>
       <c r="AN20">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>225.16650000000001</v>
       </c>
       <c r="AO20">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.1212</v>
       </c>
       <c r="AP20">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>651</v>
       </c>
       <c r="AQ20" t="e">
@@ -60245,7 +60391,7 @@
         <v>-1</v>
       </c>
       <c r="CW20">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA20">
@@ -60345,24 +60491,27 @@
         <v>205</v>
       </c>
       <c r="FH20">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>18.446499999999986</v>
       </c>
       <c r="FI20">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>-6.5759999999999999E-2</v>
       </c>
       <c r="FJ20">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-167</v>
       </c>
       <c r="FK20">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.44892473118279569</v>
       </c>
       <c r="FL20">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-0.5204178537511871</v>
+      </c>
+      <c r="FO20">
+        <v>0.15090000000000001</v>
       </c>
       <c r="FQ20">
         <f t="shared" si="54"/>
@@ -60370,7 +60519,7 @@
       </c>
       <c r="FR20">
         <f t="shared" si="55"/>
-        <v>-6.0600000000000001E-2</v>
+        <v>9.0300000000000005E-2</v>
       </c>
       <c r="FS20">
         <f t="shared" si="56"/>
@@ -60380,8 +60529,12 @@
         <f t="shared" si="57"/>
         <v>-3382.8382838283828</v>
       </c>
-    </row>
-    <row r="21" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU20" s="143">
+        <f t="shared" si="58"/>
+        <v>2.4540000000000006E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -60464,15 +60617,15 @@
         <v>1742</v>
       </c>
       <c r="AN21">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>48.740499999999997</v>
       </c>
       <c r="AO21">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.1769</v>
       </c>
       <c r="AP21">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1742</v>
       </c>
       <c r="AQ21" t="e">
@@ -60568,7 +60721,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW21">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA21">
@@ -60668,24 +60821,27 @@
         <v>754</v>
       </c>
       <c r="FH21">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>0.28910000000000124</v>
       </c>
       <c r="FI21">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>4.3480000000000019E-2</v>
       </c>
       <c r="FJ21">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-365</v>
       </c>
       <c r="FK21">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.32618409294012513</v>
       </c>
       <c r="FL21">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.19559154295996409</v>
+      </c>
+      <c r="FO21">
+        <v>0.2276</v>
       </c>
       <c r="FQ21">
         <f t="shared" si="54"/>
@@ -60693,7 +60849,7 @@
       </c>
       <c r="FR21">
         <f t="shared" si="55"/>
-        <v>-0.26578000000000002</v>
+        <v>-3.8180000000000019E-2</v>
       </c>
       <c r="FS21">
         <f t="shared" si="56"/>
@@ -60703,8 +60859,12 @@
         <f t="shared" si="57"/>
         <v>-2836.932801565204</v>
       </c>
-    </row>
-    <row r="22" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU21" s="143">
+        <f t="shared" si="58"/>
+        <v>5.2999999999999992E-3</v>
+      </c>
+    </row>
+    <row r="22" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -60775,15 +60935,15 @@
         <v>963</v>
       </c>
       <c r="AN22">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>56.912999999999997</v>
       </c>
       <c r="AO22">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.26650000000000001</v>
       </c>
       <c r="AP22">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>963</v>
       </c>
       <c r="AQ22" t="e">
@@ -60906,7 +61066,7 @@
         <v>-1</v>
       </c>
       <c r="CW22">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA22">
@@ -61006,24 +61166,27 @@
         <v>139</v>
       </c>
       <c r="FH22">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-7.5488</v>
       </c>
       <c r="FI22">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.29722299999999996</v>
       </c>
       <c r="FJ22">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-233</v>
       </c>
       <c r="FK22">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.62634408602150538</v>
       </c>
       <c r="FL22">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.82935846887495557</v>
+      </c>
+      <c r="FO22">
+        <v>0.35930000000000001</v>
       </c>
       <c r="FQ22">
         <f t="shared" si="54"/>
@@ -61031,7 +61194,7 @@
       </c>
       <c r="FR22">
         <f t="shared" si="55"/>
-        <v>-0.65559999999999996</v>
+        <v>-0.29629999999999995</v>
       </c>
       <c r="FS22">
         <f t="shared" si="56"/>
@@ -61041,8 +61204,12 @@
         <f t="shared" si="57"/>
         <v>-212.01952410006103</v>
       </c>
-    </row>
-    <row r="23" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU22" s="143">
+        <f t="shared" si="58"/>
+        <v>9.2300000000000715E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -61092,15 +61259,15 @@
         <v>579</v>
       </c>
       <c r="AN23">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>74.535600000000002</v>
       </c>
       <c r="AO23">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.13339999999999999</v>
       </c>
       <c r="AP23">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>579</v>
       </c>
       <c r="AQ23" t="e">
@@ -61232,7 +61399,7 @@
         <v>-1</v>
       </c>
       <c r="CW23">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA23">
@@ -61332,24 +61499,27 @@
         <v>222</v>
       </c>
       <c r="FH23">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-0.11174999999999358</v>
       </c>
       <c r="FI23">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.17060999999999998</v>
       </c>
       <c r="FJ23">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-187</v>
       </c>
       <c r="FK23">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.45721271393643031</v>
       </c>
       <c r="FL23">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>1.6843716062790006</v>
+      </c>
+      <c r="FO23">
+        <v>0.1381</v>
       </c>
       <c r="FQ23">
         <f t="shared" si="54"/>
@@ -61357,7 +61527,7 @@
       </c>
       <c r="FR23">
         <f t="shared" si="55"/>
-        <v>-0.27189999999999998</v>
+        <v>-0.13379999999999997</v>
       </c>
       <c r="FS23">
         <f t="shared" si="56"/>
@@ -61367,8 +61537,12 @@
         <f t="shared" si="57"/>
         <v>-816.47664582567131</v>
       </c>
-    </row>
-    <row r="24" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU23" s="143">
+        <f t="shared" si="58"/>
+        <v>3.6810000000000009E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -61418,15 +61592,15 @@
         <v>462</v>
       </c>
       <c r="AN24">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>121.116</v>
       </c>
       <c r="AO24">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.2165</v>
       </c>
       <c r="AP24">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>462</v>
       </c>
       <c r="AQ24" t="e">
@@ -61555,7 +61729,7 @@
         <v>-1</v>
       </c>
       <c r="CW24">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA24">
@@ -61655,24 +61829,27 @@
         <v>205</v>
       </c>
       <c r="FH24">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>1.2230999999999952</v>
       </c>
       <c r="FI24">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>8.611000000000002E-2</v>
       </c>
       <c r="FJ24">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-170</v>
       </c>
       <c r="FK24">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.45333333333333331</v>
       </c>
       <c r="FL24">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.29310051397256554</v>
+      </c>
+      <c r="FO24">
+        <v>0.33239999999999997</v>
       </c>
       <c r="FQ24">
         <f t="shared" si="54"/>
@@ -61680,7 +61857,7 @@
       </c>
       <c r="FR24">
         <f t="shared" si="55"/>
-        <v>-0.37990000000000002</v>
+        <v>-4.7500000000000042E-2</v>
       </c>
       <c r="FS24">
         <f t="shared" si="56"/>
@@ -61690,8 +61867,12 @@
         <f t="shared" si="57"/>
         <v>-539.61568833903652</v>
       </c>
-    </row>
-    <row r="25" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU24" s="143">
+        <f t="shared" si="58"/>
+        <v>3.8609999999999978E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -61760,15 +61941,15 @@
         <v>599</v>
       </c>
       <c r="AN25">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>98.161590000000004</v>
       </c>
       <c r="AO25">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.26608999999999999</v>
       </c>
       <c r="AP25">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>599</v>
       </c>
       <c r="AQ25" t="e">
@@ -61891,7 +62072,7 @@
         <v>-1</v>
       </c>
       <c r="CW25">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA25">
@@ -61991,24 +62172,27 @@
         <v>208</v>
       </c>
       <c r="FH25">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>2.0383000000000067</v>
       </c>
       <c r="FI25">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>3.0839999999999979E-2</v>
       </c>
       <c r="FJ25">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-124</v>
       </c>
       <c r="FK25">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.37349397590361444</v>
       </c>
       <c r="FL25">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.10777564214572768</v>
+      </c>
+      <c r="FO25">
+        <v>0.27610000000000001</v>
       </c>
       <c r="FQ25">
         <f t="shared" si="54"/>
@@ -62016,7 +62200,7 @@
       </c>
       <c r="FR25">
         <f t="shared" si="55"/>
-        <v>-0.31698999999999999</v>
+        <v>-4.0889999999999982E-2</v>
       </c>
       <c r="FS25">
         <f t="shared" si="56"/>
@@ -62026,8 +62210,12 @@
         <f t="shared" si="57"/>
         <v>-656.17211899429003</v>
       </c>
-    </row>
-    <row r="26" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU25" s="143">
+        <f t="shared" si="58"/>
+        <v>-1.0050000000000003E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -62097,15 +62285,15 @@
         <v>795</v>
       </c>
       <c r="AN26">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>72.231539999999995</v>
       </c>
       <c r="AO26">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.2412</v>
       </c>
       <c r="AP26">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>795</v>
       </c>
       <c r="AQ26" t="e">
@@ -62225,7 +62413,7 @@
         <v>-1</v>
       </c>
       <c r="CW26">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA26">
@@ -62325,32 +62513,35 @@
         <v>242</v>
       </c>
       <c r="FH26">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-7.7189499999999995</v>
       </c>
       <c r="FI26">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.10633000000000004</v>
       </c>
       <c r="FJ26">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-194</v>
       </c>
       <c r="FK26">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.44495412844036697</v>
       </c>
       <c r="FL26">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.47560048307017955</v>
+      </c>
+      <c r="FO26">
+        <v>0.19620000000000001</v>
       </c>
       <c r="FQ26">
         <f t="shared" si="54"/>
         <v>-37.959000000000003</v>
       </c>
       <c r="FR26">
-        <f t="shared" si="55"/>
-        <v>-0.32990000000000003</v>
+        <f>FO26-FF26</f>
+        <v>-0.13370000000000001</v>
       </c>
       <c r="FS26">
         <f t="shared" si="56"/>
@@ -62360,8 +62551,12 @@
         <f t="shared" si="57"/>
         <v>-733.55562291603508</v>
       </c>
-    </row>
-    <row r="27" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU26" s="143">
+        <f t="shared" si="58"/>
+        <v>-2.7369999999999978E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -62430,15 +62625,15 @@
         <v>421</v>
       </c>
       <c r="AN27">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>83.323599999999999</v>
       </c>
       <c r="AO27">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.31533</v>
       </c>
       <c r="AP27">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>421</v>
       </c>
       <c r="AQ27" t="e">
@@ -62558,7 +62753,7 @@
         <v>-1</v>
       </c>
       <c r="CW27">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA27">
@@ -62658,24 +62853,27 @@
         <v>258</v>
       </c>
       <c r="FH27">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-5.7223000000000042</v>
       </c>
       <c r="FI27">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>6.3369999999999982E-2</v>
       </c>
       <c r="FJ27">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-92</v>
       </c>
       <c r="FK27">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.26285714285714284</v>
       </c>
       <c r="FL27">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.20956380832699489</v>
+      </c>
+      <c r="FO27">
+        <v>0.32097999999999999</v>
       </c>
       <c r="FQ27">
         <f t="shared" si="54"/>
@@ -62683,7 +62881,7 @@
       </c>
       <c r="FR27">
         <f t="shared" si="55"/>
-        <v>-0.36575999999999997</v>
+        <v>-4.4779999999999986E-2</v>
       </c>
       <c r="FS27">
         <f t="shared" si="56"/>
@@ -62693,8 +62891,12 @@
         <f t="shared" si="57"/>
         <v>-705.38057742782155</v>
       </c>
-    </row>
-    <row r="28" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU27" s="143">
+        <f t="shared" si="58"/>
+        <v>1.8589999999999995E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -62764,15 +62966,15 @@
         <v>408</v>
       </c>
       <c r="AN28">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>119.6892</v>
       </c>
       <c r="AO28">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.22966</v>
       </c>
       <c r="AP28">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>408</v>
       </c>
       <c r="AQ28" t="e">
@@ -62892,7 +63094,7 @@
         <v>-1</v>
       </c>
       <c r="CW28">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA28">
@@ -62992,24 +63194,27 @@
         <v>130</v>
       </c>
       <c r="FH28">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>5.5594399999999951</v>
       </c>
       <c r="FI28">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.19097999999999998</v>
       </c>
       <c r="FJ28">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-74</v>
       </c>
       <c r="FK28">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.36274509803921567</v>
       </c>
       <c r="FL28">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.67317589002467393</v>
+      </c>
+      <c r="FO28">
+        <v>0.27929999999999999</v>
       </c>
       <c r="FQ28">
         <f t="shared" si="54"/>
@@ -63017,7 +63222,7 @@
       </c>
       <c r="FR28">
         <f t="shared" si="55"/>
-        <v>-0.47467999999999999</v>
+        <v>-0.19538</v>
       </c>
       <c r="FS28">
         <f t="shared" si="56"/>
@@ -63027,8 +63232,12 @@
         <f t="shared" si="57"/>
         <v>-273.8687115530463</v>
       </c>
-    </row>
-    <row r="29" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU28" s="143">
+        <f t="shared" si="58"/>
+        <v>-4.400000000000015E-3</v>
+      </c>
+    </row>
+    <row r="29" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -63098,15 +63307,15 @@
         <v>712</v>
       </c>
       <c r="AN29">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>91.474900000000005</v>
       </c>
       <c r="AO29">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.34320000000000001</v>
       </c>
       <c r="AP29">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>712</v>
       </c>
       <c r="AQ29" t="e">
@@ -63226,7 +63435,7 @@
         <v>-1</v>
       </c>
       <c r="CW29">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA29">
@@ -63326,24 +63535,27 @@
         <v>259</v>
       </c>
       <c r="FH29">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-0.28419999999999845</v>
       </c>
       <c r="FI29">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>-4.8539999999999972E-2</v>
       </c>
       <c r="FJ29">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-166</v>
       </c>
       <c r="FK29">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.39058823529411762</v>
       </c>
       <c r="FL29">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-9.6225517405439637E-2</v>
+      </c>
+      <c r="FO29">
+        <v>0.49230000000000002</v>
       </c>
       <c r="FQ29">
         <f t="shared" si="54"/>
@@ -63351,7 +63563,7 @@
       </c>
       <c r="FR29">
         <f t="shared" si="55"/>
-        <v>-0.45590000000000003</v>
+        <v>3.6399999999999988E-2</v>
       </c>
       <c r="FS29">
         <f t="shared" si="56"/>
@@ -63361,8 +63573,12 @@
         <f t="shared" si="57"/>
         <v>-568.10704101776707</v>
       </c>
-    </row>
-    <row r="30" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU29" s="143">
+        <f t="shared" si="58"/>
+        <v>-1.2139999999999984E-2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -63432,15 +63648,15 @@
         <v>454</v>
       </c>
       <c r="AN30">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>88.2821</v>
       </c>
       <c r="AO30">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>8.9889999999999998E-2</v>
       </c>
       <c r="AP30">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>454</v>
       </c>
       <c r="AQ30" t="e">
@@ -63560,7 +63776,7 @@
         <v>-1</v>
       </c>
       <c r="CW30">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA30">
@@ -63660,24 +63876,27 @@
         <v>197</v>
       </c>
       <c r="FH30">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>7.5137999999999963</v>
       </c>
       <c r="FI30">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>6.8039999999999989E-2</v>
       </c>
       <c r="FJ30">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-116</v>
       </c>
       <c r="FK30">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.37060702875399359</v>
       </c>
       <c r="FL30">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.34450632911392398</v>
+      </c>
+      <c r="FO30">
+        <v>0.19750000000000001</v>
       </c>
       <c r="FQ30">
         <f t="shared" si="54"/>
@@ -63685,7 +63904,7 @@
       </c>
       <c r="FR30">
         <f t="shared" si="55"/>
-        <v>-0.26554</v>
+        <v>-6.8039999999999989E-2</v>
       </c>
       <c r="FS30">
         <f t="shared" si="56"/>
@@ -63695,8 +63914,12 @@
         <f t="shared" si="57"/>
         <v>-741.88446185132182</v>
       </c>
-    </row>
-    <row r="31" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU30" s="143">
+        <f t="shared" si="58"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -63764,15 +63987,15 @@
         <v>327</v>
       </c>
       <c r="AN31">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>67.405699999999996</v>
       </c>
       <c r="AO31">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.19688</v>
       </c>
       <c r="AP31">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>327</v>
       </c>
       <c r="AQ31" t="e">
@@ -63892,7 +64115,7 @@
         <v>-1</v>
       </c>
       <c r="CW31">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA31">
@@ -63992,24 +64215,27 @@
         <v>133</v>
       </c>
       <c r="FH31">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-7.8052999999999955</v>
       </c>
       <c r="FI31">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.16682000000000002</v>
       </c>
       <c r="FJ31">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-73</v>
       </c>
       <c r="FK31">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.35436893203883496</v>
       </c>
       <c r="FL31">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.64265351722012498</v>
+      </c>
+      <c r="FO31">
+        <v>0.29366999999999999</v>
       </c>
       <c r="FQ31">
         <f t="shared" si="54"/>
@@ -64017,7 +64243,7 @@
       </c>
       <c r="FR31">
         <f t="shared" si="55"/>
-        <v>-0.4264</v>
+        <v>-0.13273000000000001</v>
       </c>
       <c r="FS31">
         <f t="shared" si="56"/>
@@ -64027,8 +64253,12 @@
         <f t="shared" si="57"/>
         <v>-311.91369606003752</v>
       </c>
-    </row>
-    <row r="32" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU31" s="143">
+        <f t="shared" si="58"/>
+        <v>3.4090000000000009E-2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -64097,15 +64327,15 @@
         <v>828</v>
       </c>
       <c r="AN32">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>84.632999999999996</v>
       </c>
       <c r="AO32">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.2198</v>
       </c>
       <c r="AP32">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>828</v>
       </c>
       <c r="AQ32" t="e">
@@ -64225,7 +64455,7 @@
         <v>-1</v>
       </c>
       <c r="CW32">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA32">
@@ -64325,24 +64555,27 @@
         <v>269</v>
       </c>
       <c r="FH32">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-1.2205000000000013</v>
       </c>
       <c r="FI32">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.16509999999999997</v>
       </c>
       <c r="FJ32">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-257</v>
       </c>
       <c r="FK32">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.48859315589353614</v>
       </c>
       <c r="FL32">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.51236694286689621</v>
+      </c>
+      <c r="FO32">
+        <v>0.32219999999999999</v>
       </c>
       <c r="FQ32">
         <f t="shared" si="54"/>
@@ -64350,7 +64583,7 @@
       </c>
       <c r="FR32">
         <f t="shared" si="55"/>
-        <v>-0.48732999999999999</v>
+        <v>-0.16513</v>
       </c>
       <c r="FS32">
         <f t="shared" si="56"/>
@@ -64360,8 +64593,12 @@
         <f t="shared" si="57"/>
         <v>-551.98735969466281</v>
       </c>
-    </row>
-    <row r="33" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU32" s="143">
+        <f t="shared" si="58"/>
+        <v>-3.0000000000030003E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -64430,15 +64667,15 @@
         <v>1052</v>
       </c>
       <c r="AN33">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>113.6572</v>
       </c>
       <c r="AO33">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.13764999999999999</v>
       </c>
       <c r="AP33">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>1052</v>
       </c>
       <c r="AQ33" t="e">
@@ -64558,7 +64795,7 @@
         <v>-1</v>
       </c>
       <c r="CW33">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA33">
@@ -64658,24 +64895,27 @@
         <v>549</v>
       </c>
       <c r="FH33">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-1.4206000000000074</v>
       </c>
       <c r="FI33">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>7.8000000000000014E-3</v>
       </c>
       <c r="FJ33">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-180</v>
       </c>
       <c r="FK33">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.24691358024691357</v>
       </c>
       <c r="FL33">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>4.2553191489361715E-2</v>
+      </c>
+      <c r="FO33">
+        <v>0.1744</v>
       </c>
       <c r="FQ33">
         <f t="shared" si="54"/>
@@ -64683,7 +64923,7 @@
       </c>
       <c r="FR33">
         <f t="shared" si="55"/>
-        <v>-0.19109999999999999</v>
+        <v>-1.6699999999999993E-2</v>
       </c>
       <c r="FS33">
         <f t="shared" si="56"/>
@@ -64693,8 +64933,12 @@
         <f t="shared" si="57"/>
         <v>-2872.8414442700159</v>
       </c>
-    </row>
-    <row r="34" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU33" s="143">
+        <f t="shared" si="58"/>
+        <v>-8.8999999999999913E-3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -64744,15 +64988,15 @@
         <v>840</v>
       </c>
       <c r="AN34">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>46.363799999999998</v>
       </c>
       <c r="AO34">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.27146999999999999</v>
       </c>
       <c r="AP34">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>840</v>
       </c>
       <c r="AQ34" t="e">
@@ -64857,7 +65101,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW34">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA34">
@@ -64957,24 +65201,27 @@
         <v>437</v>
       </c>
       <c r="FH34">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-3.5960999999999963</v>
       </c>
       <c r="FI34">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.13230999999999998</v>
       </c>
       <c r="FJ34">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-400</v>
       </c>
       <c r="FK34">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.47789725209080047</v>
       </c>
       <c r="FL34">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.4679067793613183</v>
+      </c>
+      <c r="FO34">
+        <v>0.28294999999999998</v>
       </c>
       <c r="FQ34">
         <f t="shared" si="54"/>
@@ -64982,7 +65229,7 @@
       </c>
       <c r="FR34">
         <f t="shared" si="55"/>
-        <v>-0.41508</v>
+        <v>-0.13213000000000003</v>
       </c>
       <c r="FS34">
         <f t="shared" si="56"/>
@@ -64992,8 +65239,12 @@
         <f t="shared" si="57"/>
         <v>-1052.8090970415342</v>
       </c>
-    </row>
-    <row r="35" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU34" s="143">
+        <f t="shared" si="58"/>
+        <v>1.7999999999995797E-4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -65043,15 +65294,15 @@
         <v>610</v>
       </c>
       <c r="AN35">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>30.443850000000001</v>
       </c>
       <c r="AO35">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.28094999999999998</v>
       </c>
       <c r="AP35">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>610</v>
       </c>
       <c r="AQ35" t="e">
@@ -65156,7 +65407,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW35">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA35">
@@ -65256,24 +65507,27 @@
         <v>362</v>
       </c>
       <c r="FH35">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-3.8239000000000019</v>
       </c>
       <c r="FI35">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.11747000000000002</v>
       </c>
       <c r="FJ35">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-246</v>
       </c>
       <c r="FK35">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.40460526315789475</v>
       </c>
       <c r="FL35">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.41406415227352844</v>
+      </c>
+      <c r="FO35">
+        <v>0.28239999999999998</v>
       </c>
       <c r="FQ35">
         <f t="shared" si="54"/>
@@ -65281,7 +65535,7 @@
       </c>
       <c r="FR35">
         <f t="shared" si="55"/>
-        <v>-0.40117000000000003</v>
+        <v>-0.11877000000000004</v>
       </c>
       <c r="FS35">
         <f t="shared" si="56"/>
@@ -65291,8 +65545,12 @@
         <f t="shared" si="57"/>
         <v>-902.36059525886776</v>
       </c>
-    </row>
-    <row r="36" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU35" s="143">
+        <f t="shared" si="58"/>
+        <v>-1.3000000000000234E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -65360,15 +65618,15 @@
         <v>307</v>
       </c>
       <c r="AN36">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>66.238900000000001</v>
       </c>
       <c r="AO36">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.42817</v>
       </c>
       <c r="AP36">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>307</v>
       </c>
       <c r="AQ36" t="e">
@@ -65488,7 +65746,7 @@
         <v>-1</v>
       </c>
       <c r="CW36">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA36">
@@ -65588,24 +65846,27 @@
         <v>138</v>
       </c>
       <c r="FH36">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-6.1620599999999968</v>
       </c>
       <c r="FI36">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.14058999999999999</v>
       </c>
       <c r="FJ36">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-36</v>
       </c>
       <c r="FK36">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.20689655172413793</v>
       </c>
       <c r="FL36">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.31645883041462208</v>
+      </c>
+      <c r="FO36">
+        <v>0.45629999999999998</v>
       </c>
       <c r="FQ36">
         <f t="shared" si="54"/>
@@ -65613,7 +65874,7 @@
       </c>
       <c r="FR36">
         <f t="shared" si="55"/>
-        <v>-0.58484999999999998</v>
+        <v>-0.12855</v>
       </c>
       <c r="FS36">
         <f t="shared" si="56"/>
@@ -65623,8 +65884,12 @@
         <f t="shared" si="57"/>
         <v>-235.9579379328033</v>
       </c>
-    </row>
-    <row r="37" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU36" s="143">
+        <f t="shared" si="58"/>
+        <v>1.2039999999999995E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -65692,15 +65957,15 @@
         <v>464</v>
       </c>
       <c r="AN37">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>157.17169999999999</v>
       </c>
       <c r="AO37">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>9.6170000000000005E-2</v>
       </c>
       <c r="AP37">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>464</v>
       </c>
       <c r="AQ37" t="e">
@@ -65820,7 +66085,7 @@
         <v>-1</v>
       </c>
       <c r="CW37">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA37">
@@ -65920,24 +66185,27 @@
         <v>278</v>
       </c>
       <c r="FH37">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-6.5512700000000024</v>
       </c>
       <c r="FI37">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>3.6769999999999997E-2</v>
       </c>
       <c r="FJ37">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-151</v>
       </c>
       <c r="FK37">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.351981351981352</v>
       </c>
       <c r="FL37">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.36769999999999997</v>
+      </c>
+      <c r="FO37">
+        <v>9.8400000000000001E-2</v>
       </c>
       <c r="FQ37">
         <f t="shared" si="54"/>
@@ -65945,7 +66213,7 @@
       </c>
       <c r="FR37">
         <f t="shared" si="55"/>
-        <v>-0.13677</v>
+        <v>-3.8370000000000001E-2</v>
       </c>
       <c r="FS37">
         <f t="shared" si="56"/>
@@ -65955,8 +66223,12 @@
         <f t="shared" si="57"/>
         <v>-2032.6094903853184</v>
       </c>
-    </row>
-    <row r="38" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU37" s="143">
+        <f t="shared" si="58"/>
+        <v>-1.6000000000000042E-3</v>
+      </c>
+    </row>
+    <row r="38" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -66026,15 +66298,15 @@
         <v>508</v>
       </c>
       <c r="AN38">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>98.72</v>
       </c>
       <c r="AO38">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.21548</v>
       </c>
       <c r="AP38">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>508</v>
       </c>
       <c r="AQ38" t="e">
@@ -66154,7 +66426,7 @@
         <v>-1</v>
       </c>
       <c r="CW38">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA38">
@@ -66254,24 +66526,27 @@
         <v>217</v>
       </c>
       <c r="FH38">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-5.3609999999999971</v>
       </c>
       <c r="FI38">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>-6.970000000000004E-2</v>
       </c>
       <c r="FJ38">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-103</v>
       </c>
       <c r="FK38">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.32187500000000002</v>
       </c>
       <c r="FL38">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-0.16450318621666282</v>
+      </c>
+      <c r="FO38">
+        <v>0.45200000000000001</v>
       </c>
       <c r="FQ38">
         <f t="shared" si="54"/>
@@ -66279,7 +66554,7 @@
       </c>
       <c r="FR38">
         <f t="shared" si="55"/>
-        <v>-0.35399999999999998</v>
+        <v>9.8000000000000032E-2</v>
       </c>
       <c r="FS38">
         <f t="shared" si="56"/>
@@ -66289,8 +66564,12 @@
         <f t="shared" si="57"/>
         <v>-612.99435028248593</v>
       </c>
-    </row>
-    <row r="39" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU38" s="143">
+        <f t="shared" si="58"/>
+        <v>2.8299999999999992E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -66358,15 +66637,15 @@
         <v>230</v>
       </c>
       <c r="AN39">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>102.0086</v>
       </c>
       <c r="AO39">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>7.3599999999999999E-2</v>
       </c>
       <c r="AP39">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>230</v>
       </c>
       <c r="AQ39" t="e">
@@ -66446,7 +66725,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW39">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA39">
@@ -66546,24 +66825,27 @@
         <v>163</v>
       </c>
       <c r="FH39">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-1.588000000000001</v>
       </c>
       <c r="FI39">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>-2.4589999999999973E-2</v>
       </c>
       <c r="FJ39">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-8</v>
       </c>
       <c r="FK39">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-4.6783625730994149E-2</v>
       </c>
       <c r="FL39">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-0.12540160130552286</v>
+      </c>
+      <c r="FO39">
+        <v>0.16239999999999999</v>
       </c>
       <c r="FQ39">
         <f t="shared" si="54"/>
@@ -66571,7 +66853,7 @@
       </c>
       <c r="FR39">
         <f t="shared" si="55"/>
-        <v>-0.17150000000000001</v>
+        <v>-9.1000000000000247E-3</v>
       </c>
       <c r="FS39">
         <f t="shared" si="56"/>
@@ -66581,8 +66863,12 @@
         <f t="shared" si="57"/>
         <v>-950.43731778425649</v>
       </c>
-    </row>
-    <row r="40" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU39" s="143">
+        <f t="shared" si="58"/>
+        <v>-3.3689999999999998E-2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -66632,15 +66918,15 @@
         <v>301</v>
       </c>
       <c r="AN40">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>90.071899999999999</v>
       </c>
       <c r="AO40">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.2913</v>
       </c>
       <c r="AP40">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>301</v>
       </c>
       <c r="AQ40" t="e">
@@ -66745,7 +67031,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW40">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA40">
@@ -66845,24 +67131,27 @@
         <v>134</v>
       </c>
       <c r="FH40">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-5.8590000000000018</v>
       </c>
       <c r="FI40">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.15972150000000007</v>
       </c>
       <c r="FJ40">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-101</v>
       </c>
       <c r="FK40">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.4297872340425532</v>
       </c>
       <c r="FL40">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.35120723605007731</v>
+      </c>
+      <c r="FO40">
+        <v>0.45600000000000002</v>
       </c>
       <c r="FQ40">
         <f t="shared" si="54"/>
@@ -66870,7 +67159,7 @@
       </c>
       <c r="FR40">
         <f t="shared" si="55"/>
-        <v>-0.61450000000000005</v>
+        <v>-0.15850000000000003</v>
       </c>
       <c r="FS40">
         <f t="shared" si="56"/>
@@ -66880,8 +67169,12 @@
         <f t="shared" si="57"/>
         <v>-218.06346623270952</v>
       </c>
-    </row>
-    <row r="41" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU40" s="143">
+        <f t="shared" si="58"/>
+        <v>1.221500000000042E-3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -66931,15 +67224,15 @@
         <v>404</v>
       </c>
       <c r="AN41">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>46.406399999999998</v>
       </c>
       <c r="AO41">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.15325</v>
       </c>
       <c r="AP41">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>404</v>
       </c>
       <c r="AQ41" t="e">
@@ -67044,7 +67337,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW41">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA41">
@@ -67144,24 +67437,27 @@
         <v>193</v>
       </c>
       <c r="FH41">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-5.1404999999999994</v>
       </c>
       <c r="FI41">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.12720199999999998</v>
       </c>
       <c r="FJ41">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-131</v>
       </c>
       <c r="FK41">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.40432098765432101</v>
       </c>
       <c r="FL41">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.67456832548470569</v>
+      </c>
+      <c r="FO41">
+        <v>0.20880000000000001</v>
       </c>
       <c r="FQ41">
         <f t="shared" si="54"/>
@@ -67169,7 +67465,7 @@
       </c>
       <c r="FR41">
         <f t="shared" si="55"/>
-        <v>-0.31577</v>
+        <v>-0.10696999999999998</v>
       </c>
       <c r="FS41">
         <f t="shared" si="56"/>
@@ -67179,8 +67475,12 @@
         <f t="shared" si="57"/>
         <v>-611.20435760205214</v>
       </c>
-    </row>
-    <row r="42" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU41" s="143">
+        <f t="shared" si="58"/>
+        <v>2.0232E-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -67230,15 +67530,15 @@
         <v>212</v>
       </c>
       <c r="AN42">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>83.256900000000002</v>
       </c>
       <c r="AO42">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.30740000000000001</v>
       </c>
       <c r="AP42">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>212</v>
       </c>
       <c r="AQ42" t="e">
@@ -67343,7 +67643,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW42">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA42">
@@ -67434,32 +67734,35 @@
         <v>159</v>
       </c>
       <c r="FH42">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-24.643999999999998</v>
       </c>
       <c r="FI42">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>-0.47758699999999998</v>
       </c>
       <c r="FJ42">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-159</v>
       </c>
       <c r="FK42">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-1</v>
       </c>
       <c r="FL42">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>-1</v>
+      </c>
+      <c r="FO42">
+        <v>0.35949999999999999</v>
       </c>
       <c r="FQ42">
         <f t="shared" si="54"/>
         <v>0</v>
       </c>
       <c r="FR42">
-        <f t="shared" si="55"/>
-        <v>0</v>
+        <f>FO42-FB42</f>
+        <v>-0.118087</v>
       </c>
       <c r="FS42">
         <f t="shared" si="56"/>
@@ -67469,8 +67772,12 @@
         <f t="shared" si="57"/>
         <v>#DIV/0!</v>
       </c>
-    </row>
-    <row r="43" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU42" s="143">
+        <f t="shared" si="58"/>
+        <v>-0.59567400000000004</v>
+      </c>
+    </row>
+    <row r="43" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -67520,15 +67827,15 @@
         <v>202</v>
       </c>
       <c r="AN43">
-        <f t="shared" si="68"/>
+        <f t="shared" si="70"/>
         <v>215.42920000000001</v>
       </c>
       <c r="AO43">
-        <f t="shared" si="69"/>
+        <f t="shared" si="71"/>
         <v>0.25890000000000002</v>
       </c>
       <c r="AP43">
-        <f t="shared" si="70"/>
+        <f t="shared" si="72"/>
         <v>202</v>
       </c>
       <c r="AQ43" t="e">
@@ -67617,7 +67924,7 @@
         <v>#DIV/0!</v>
       </c>
       <c r="CW43">
-        <f t="shared" si="62"/>
+        <f t="shared" si="64"/>
         <v>1</v>
       </c>
       <c r="DA43">
@@ -67717,24 +68024,27 @@
         <v>106</v>
       </c>
       <c r="FH43">
-        <f t="shared" si="78"/>
+        <f t="shared" si="80"/>
         <v>-1.6260500000000064</v>
       </c>
       <c r="FI43">
-        <f t="shared" si="79"/>
+        <f t="shared" si="81"/>
         <v>0.13549999999999998</v>
       </c>
       <c r="FJ43">
-        <f t="shared" si="80"/>
+        <f t="shared" si="82"/>
         <v>-46</v>
       </c>
       <c r="FK43">
-        <f t="shared" si="81"/>
+        <f t="shared" si="83"/>
         <v>-0.30263157894736842</v>
       </c>
       <c r="FL43">
-        <f t="shared" si="82"/>
+        <f t="shared" si="84"/>
         <v>0.59691629955947123</v>
+      </c>
+      <c r="FO43">
+        <v>0.2203</v>
       </c>
       <c r="FQ43">
         <f t="shared" si="54"/>
@@ -67742,7 +68052,7 @@
       </c>
       <c r="FR43">
         <f t="shared" si="55"/>
-        <v>-0.36249999999999999</v>
+        <v>-0.14219999999999999</v>
       </c>
       <c r="FS43">
         <f t="shared" si="56"/>
@@ -67752,8 +68062,12 @@
         <f t="shared" si="57"/>
         <v>-292.41379310344831</v>
       </c>
-    </row>
-    <row r="44" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU43" s="143">
+        <f t="shared" si="58"/>
+        <v>-6.7000000000000115E-3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:177" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -67765,6 +68079,9 @@
       </c>
       <c r="FG44">
         <v>268</v>
+      </c>
+      <c r="FO44">
+        <v>0.35449999999999998</v>
       </c>
       <c r="FQ44">
         <f t="shared" si="54"/>
@@ -67772,7 +68089,7 @@
       </c>
       <c r="FR44">
         <f t="shared" si="55"/>
-        <v>-0.35270000000000001</v>
+        <v>1.7999999999999683E-3</v>
       </c>
       <c r="FS44">
         <f t="shared" si="56"/>
@@ -67782,8 +68099,12 @@
         <f t="shared" si="57"/>
         <v>-759.85256592004532</v>
       </c>
-    </row>
-    <row r="45" spans="1:176" x14ac:dyDescent="0.35">
+      <c r="FU44" s="143">
+        <f t="shared" si="58"/>
+        <v>1.7999999999999683E-3</v>
+      </c>
+    </row>
+    <row r="45" spans="1:177" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -67826,7 +68147,7 @@
         <v>0.15523900000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:177" x14ac:dyDescent="0.35">
       <c r="CC46" t="s">
         <v>240</v>
       </c>
@@ -67834,7 +68155,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="47" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:177" x14ac:dyDescent="0.35">
       <c r="CC47" t="s">
         <v>241</v>
       </c>
@@ -67842,7 +68163,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:176" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:177" x14ac:dyDescent="0.35">
       <c r="CC48" t="s">
         <v>242</v>
       </c>
@@ -67863,105 +68184,115 @@
     <mergeCell ref="N3:O3"/>
   </mergeCells>
   <conditionalFormatting sqref="Z5:Z43 BS5:BS43">
-    <cfRule type="cellIs" dxfId="79" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA45:AB45 AA5:AB43 BT5:BU43">
-    <cfRule type="cellIs" dxfId="78" priority="28" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45">
-    <cfRule type="cellIs" dxfId="77" priority="27" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AB46">
-    <cfRule type="cellIs" dxfId="76" priority="24" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46">
-    <cfRule type="cellIs" dxfId="75" priority="23" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS45:BT45">
-    <cfRule type="cellIs" dxfId="74" priority="19" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU1:BU3">
-    <cfRule type="cellIs" dxfId="73" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CA1048576">
-    <cfRule type="cellIs" dxfId="72" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="76" priority="17" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="18" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ED1:ED3 ED5:ED1048576">
-    <cfRule type="cellIs" dxfId="70" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="74" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ED1:ED1048576">
-    <cfRule type="cellIs" dxfId="69" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="73" priority="14" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM5:EM43">
-    <cfRule type="cellIs" dxfId="68" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM4:EM43">
-    <cfRule type="cellIs" dxfId="67" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="12" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ER6:EY6">
-    <cfRule type="cellIs" dxfId="66" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="70" priority="11" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ER5:EY5">
-    <cfRule type="cellIs" dxfId="65" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ET6">
-    <cfRule type="cellIs" dxfId="64" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI4">
-    <cfRule type="cellIs" dxfId="63" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="7" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI5:FI43">
-    <cfRule type="cellIs" dxfId="62" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="5" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI5:FI43">
-    <cfRule type="cellIs" dxfId="61" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FR5:FR44">
-    <cfRule type="cellIs" dxfId="60" priority="1" operator="lessThan">
+  <conditionalFormatting sqref="FR5:FR8 FR10:FR44">
+    <cfRule type="cellIs" dxfId="64" priority="3" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="FR5:FR44">
-    <cfRule type="cellIs" dxfId="59" priority="2" operator="greaterThan">
+  <conditionalFormatting sqref="FR5:FR8 FR10:FR44">
+    <cfRule type="cellIs" dxfId="63" priority="4" operator="greaterThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FR9">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+      <formula>-0.001</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="FR9">
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Specified dplyr::select() due to unused argument when library(EnvCpt) was added
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3606" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="317">
   <si>
     <t>Species</t>
   </si>
@@ -979,6 +979,30 @@
   </si>
   <si>
     <t>Adding Surface temp</t>
+  </si>
+  <si>
+    <t>LocalAbundance</t>
+  </si>
+  <si>
+    <t>SpringTemp</t>
+  </si>
+  <si>
+    <t>TotalCopepods</t>
+  </si>
+  <si>
+    <t>LocalSurfaceTemp</t>
+  </si>
+  <si>
+    <t>WinterTemp</t>
+  </si>
+  <si>
+    <t>FallBloomDuration</t>
+  </si>
+  <si>
+    <t>FallTemp</t>
+  </si>
+  <si>
+    <t>StomachFullness</t>
   </si>
 </sst>
 </file>
@@ -2208,7 +2232,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="144">
+  <cellXfs count="145">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" readingOrder="1"/>
@@ -2512,6 +2536,7 @@
     <xf numFmtId="0" fontId="0" fillId="42" borderId="49" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2560,7 +2585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2606,49 +2631,7 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="217">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B0F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="215">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -3068,6 +3051,27 @@
       <fill>
         <patternFill>
           <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
         </patternFill>
       </fill>
     </dxf>
@@ -5141,30 +5145,30 @@
     </filterColumn>
   </autoFilter>
   <conditionalFormatting sqref="B5:C41">
-    <cfRule type="containsBlanks" dxfId="216" priority="5">
+    <cfRule type="containsBlanks" dxfId="214" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="213" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="214" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="212" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="213" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="211" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H43">
-    <cfRule type="containsBlanks" dxfId="212" priority="1">
+    <cfRule type="containsBlanks" dxfId="210" priority="1">
       <formula>LEN(TRIM(G5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(G5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="211" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="209" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="210" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="208" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6993,16 +6997,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:AF7 F9:AF43 F8:P8 R8:AF8">
-    <cfRule type="containsBlanks" dxfId="62" priority="1">
+    <cfRule type="containsBlanks" dxfId="58" priority="1">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="57" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="60" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="56" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9029,16 +9033,16 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="F5:Z43">
-    <cfRule type="containsBlanks" dxfId="59" priority="1">
+    <cfRule type="containsBlanks" dxfId="55" priority="1">
       <formula>LEN(TRIM(F5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="58" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="53" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="56" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="52" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9438,16 +9442,16 @@
     <sortCondition ref="B5:B41"/>
   </sortState>
   <conditionalFormatting sqref="B5:C41">
-    <cfRule type="containsBlanks" dxfId="55" priority="1">
+    <cfRule type="containsBlanks" dxfId="51" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="50" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="49" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="48" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -9695,16 +9699,16 @@
     <sortCondition ref="C5:C27"/>
   </sortState>
   <conditionalFormatting sqref="B5:C27">
-    <cfRule type="containsBlanks" dxfId="51" priority="1">
+    <cfRule type="containsBlanks" dxfId="47" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="46" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="45" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10230,16 +10234,16 @@
     <sortCondition ref="E5:E42"/>
   </sortState>
   <conditionalFormatting sqref="B5:E43">
-    <cfRule type="containsBlanks" dxfId="48" priority="1">
+    <cfRule type="containsBlanks" dxfId="44" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="43" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="42" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="41" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10882,30 +10886,30 @@
     <sortCondition ref="C5:C28"/>
   </sortState>
   <conditionalFormatting sqref="B5:E28">
-    <cfRule type="containsBlanks" dxfId="44" priority="5">
+    <cfRule type="containsBlanks" dxfId="40" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="39" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="38" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="37" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5:K43">
-    <cfRule type="containsBlanks" dxfId="40" priority="1">
+    <cfRule type="containsBlanks" dxfId="36" priority="1">
       <formula>LEN(TRIM(H5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(H5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="35" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="34" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11202,16 +11206,16 @@
     <sortCondition ref="E5:E31"/>
   </sortState>
   <conditionalFormatting sqref="B5:E31">
-    <cfRule type="containsBlanks" dxfId="37" priority="1">
+    <cfRule type="containsBlanks" dxfId="33" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="32" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="31" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11885,16 +11889,16 @@
     <sortCondition ref="G5:G31"/>
   </sortState>
   <conditionalFormatting sqref="B5:G31 J5:M31">
-    <cfRule type="containsBlanks" dxfId="34" priority="5">
+    <cfRule type="containsBlanks" dxfId="30" priority="5">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="29" priority="6" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="32" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="28" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="27" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12395,16 +12399,16 @@
     <sortCondition ref="L5:L37"/>
   </sortState>
   <conditionalFormatting sqref="B5:L37">
-    <cfRule type="containsBlanks" dxfId="30" priority="1">
+    <cfRule type="containsBlanks" dxfId="26" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="28" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -12806,16 +12810,16 @@
     <sortCondition ref="C6:C43"/>
   </sortState>
   <conditionalFormatting sqref="B5:C41">
-    <cfRule type="containsBlanks" dxfId="27" priority="1">
+    <cfRule type="containsBlanks" dxfId="23" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="25" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="21" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="24" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="20" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25478,44 +25482,44 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D1:D118 D120:D1048576">
-    <cfRule type="cellIs" dxfId="209" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="207" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:B118 B120:B1048576">
-    <cfRule type="cellIs" dxfId="208" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="206" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="207" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="205" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K1:K1048576">
-    <cfRule type="cellIs" dxfId="206" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="204" priority="7" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I85 I119:I1048576 I87:I117">
-    <cfRule type="cellIs" dxfId="205" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="203" priority="5" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="204" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="202" priority="6" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I118">
-    <cfRule type="cellIs" dxfId="203" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="201" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="202" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="200" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I86">
-    <cfRule type="cellIs" dxfId="201" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="199" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="198" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25703,16 +25707,16 @@
     <sortCondition ref="C5:C43"/>
   </sortState>
   <conditionalFormatting sqref="B5:C21">
-    <cfRule type="containsBlanks" dxfId="23" priority="1">
+    <cfRule type="containsBlanks" dxfId="19" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="22" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="21" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -25938,16 +25942,16 @@
     <sortCondition ref="E5:E22"/>
   </sortState>
   <conditionalFormatting sqref="B5:C15 E5:E17 C16:C17">
-    <cfRule type="containsBlanks" dxfId="20" priority="1">
+    <cfRule type="containsBlanks" dxfId="16" priority="1">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="19" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="15" priority="2" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="18" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="14" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="17" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="13" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26657,28 +26661,28 @@
     <sortCondition descending="1" ref="F5:F43"/>
   </sortState>
   <conditionalFormatting sqref="B5:B43">
-    <cfRule type="containsBlanks" dxfId="16" priority="4">
+    <cfRule type="containsBlanks" dxfId="12" priority="4">
       <formula>LEN(TRIM(B5))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="15" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="11" priority="5" operator="equal">
       <formula>" "</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="14" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="10" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="13" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="9" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5:F43">
-    <cfRule type="cellIs" dxfId="12" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="8" priority="1" operator="greaterThan">
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="2" operator="between">
+    <cfRule type="cellIs" dxfId="7" priority="2" operator="between">
       <formula>0.25</formula>
       <formula>0.5</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="10" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
       <formula>0.25</formula>
     </cfRule>
   </conditionalFormatting>
@@ -26997,16 +27001,16 @@
     <sortCondition ref="B3:B41"/>
   </sortState>
   <conditionalFormatting sqref="B3:B41">
-    <cfRule type="containsBlanks" dxfId="9" priority="1">
+    <cfRule type="containsBlanks" dxfId="5" priority="1">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
     <cfRule type="containsBlanks" priority="2">
       <formula>LEN(TRIM(B3))=0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="4" priority="3" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="3" priority="4" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -29303,15 +29307,15 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D1048576">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="lessThan">
       <formula>0</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="1" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E40">
-    <cfRule type="cellIs" dxfId="4" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -31896,145 +31900,145 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 E2:E17 C19:C26 E19:E26 C28 C30:C119 E28 E30 AC26:AC31 AC2:AC7 AA2:AA7 AC9 AA9 AC11:AC18 AA11:AA18 AC20:AC21 AC24 AA20:AA21 AA24:AA31">
-    <cfRule type="cellIs" dxfId="199" priority="42" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="197" priority="42" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 D2:D17 B19:B26 D19:D26 B28 B30:B119 D28 D30 AB26:AB31 AB2:AB7 Z2:Z7 AB9 Z9 AB11:AB18 Z11:Z18 AB20:AB21 AB24 Z20:Z21 Z24:Z31">
-    <cfRule type="cellIs" dxfId="198" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="196" priority="40" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="41" operator="lessThan">
+    <cfRule type="cellIs" dxfId="195" priority="41" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="196" priority="36" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="194" priority="36" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="195" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="193" priority="34" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="35" operator="lessThan">
+    <cfRule type="cellIs" dxfId="192" priority="35" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="193" priority="33" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="191" priority="33" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="192" priority="31" operator="lessThan">
+    <cfRule type="cellIs" dxfId="190" priority="31" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="32" operator="lessThan">
+    <cfRule type="cellIs" dxfId="189" priority="32" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31">
-    <cfRule type="cellIs" dxfId="190" priority="30" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="188" priority="30" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2:J31">
-    <cfRule type="cellIs" dxfId="189" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="187" priority="28" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="29" operator="lessThan">
+    <cfRule type="cellIs" dxfId="186" priority="29" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31">
-    <cfRule type="cellIs" dxfId="187" priority="27" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="185" priority="27" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L31">
-    <cfRule type="cellIs" dxfId="186" priority="25" operator="lessThan">
+    <cfRule type="cellIs" dxfId="184" priority="25" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="26" operator="lessThan">
+    <cfRule type="cellIs" dxfId="183" priority="26" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="184" priority="24" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="182" priority="24" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="183" priority="22" operator="lessThan">
+    <cfRule type="cellIs" dxfId="181" priority="22" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="23" operator="lessThan">
+    <cfRule type="cellIs" dxfId="180" priority="23" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q31">
-    <cfRule type="cellIs" dxfId="181" priority="21" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="179" priority="21" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P31">
-    <cfRule type="cellIs" dxfId="180" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="178" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="177" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S31">
-    <cfRule type="cellIs" dxfId="178" priority="18" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="176" priority="18" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2:R31">
-    <cfRule type="cellIs" dxfId="177" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="175" priority="16" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="174" priority="17" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U2:U31">
-    <cfRule type="cellIs" dxfId="175" priority="15" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="173" priority="15" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T2:T31">
-    <cfRule type="cellIs" dxfId="174" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="172" priority="13" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="171" priority="14" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="W2:W31">
-    <cfRule type="cellIs" dxfId="172" priority="12" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="170" priority="12" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="V2:V31">
-    <cfRule type="cellIs" dxfId="171" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="169" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="168" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y2:Y31">
-    <cfRule type="cellIs" dxfId="169" priority="9" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="167" priority="9" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="X2:X31">
-    <cfRule type="cellIs" dxfId="168" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="166" priority="7" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="165" priority="8" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -33857,168 +33861,168 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="W26:W31 W2:W7 U2:U7 W9 U9 W11:W18 U11:U18 W20:W21 W24 U20:U21 U24:U31">
-    <cfRule type="cellIs" dxfId="166" priority="50" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="164" priority="50" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B121:B1048576 B2:B17 B19:B26 B30 B28 D30 V26:V31 V2:V7 T2:T7 V9 T9 V11:V18 T11:T18 V20:V21 V24 T20:T21 T24:T31 D28 D19:D26 D2:D17 B38:B119">
-    <cfRule type="cellIs" dxfId="165" priority="48" operator="lessThan">
+    <cfRule type="cellIs" dxfId="163" priority="48" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="49" operator="lessThan">
+    <cfRule type="cellIs" dxfId="162" priority="49" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F2:F31">
-    <cfRule type="cellIs" dxfId="163" priority="45" operator="lessThan">
+    <cfRule type="cellIs" dxfId="161" priority="45" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="46" operator="lessThan">
+    <cfRule type="cellIs" dxfId="160" priority="46" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H2:H31">
-    <cfRule type="cellIs" dxfId="161" priority="42" operator="lessThan">
+    <cfRule type="cellIs" dxfId="159" priority="42" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="160" priority="43" operator="lessThan">
+    <cfRule type="cellIs" dxfId="158" priority="43" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J2 J5 J10 J14 J17:J18 J21:J22 J24:J25 J27:J29">
-    <cfRule type="cellIs" dxfId="159" priority="39" operator="lessThan">
+    <cfRule type="cellIs" dxfId="157" priority="39" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="40" operator="lessThan">
+    <cfRule type="cellIs" dxfId="156" priority="40" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M2:M31 L5 L10 L14 L17:L18 L21:L22 L27:L29 L24:L25">
-    <cfRule type="cellIs" dxfId="157" priority="38" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="155" priority="38" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L2:L4 L6:L9 L11:L13 L15:L16 L19:L20 L23 L30:L31 L26">
-    <cfRule type="cellIs" dxfId="156" priority="36" operator="lessThan">
+    <cfRule type="cellIs" dxfId="154" priority="36" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="37" operator="lessThan">
+    <cfRule type="cellIs" dxfId="153" priority="37" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O2:O31">
-    <cfRule type="cellIs" dxfId="154" priority="35" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="152" priority="35" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N2:N31">
-    <cfRule type="cellIs" dxfId="153" priority="33" operator="lessThan">
+    <cfRule type="cellIs" dxfId="151" priority="33" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="34" operator="lessThan">
+    <cfRule type="cellIs" dxfId="150" priority="34" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q2:Q16 Q30:Q31 Q18:Q26 P4:P9 P11 P13:P15 P19:P21 P24 P30">
-    <cfRule type="cellIs" dxfId="151" priority="29" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="149" priority="29" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P2:P3 P31 P18 P10 P12 P16 P22:P23 P25:P26">
-    <cfRule type="cellIs" dxfId="150" priority="27" operator="lessThan">
+    <cfRule type="cellIs" dxfId="148" priority="27" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="28" operator="lessThan">
+    <cfRule type="cellIs" dxfId="147" priority="28" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S14:S15">
-    <cfRule type="cellIs" dxfId="148" priority="17" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="146" priority="17" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R14:R15">
-    <cfRule type="cellIs" dxfId="147" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="145" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="144" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S2:S4 S16:S31 S6:S13 R10 R12 R16:R18 R22:R23 R25:R29 R31 R3">
-    <cfRule type="cellIs" dxfId="145" priority="20" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="143" priority="20" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R2 R19:R21 R6:R9 R11 R13 R24 R30 R4">
-    <cfRule type="cellIs" dxfId="144" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="142" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="141" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q27:Q29">
-    <cfRule type="cellIs" dxfId="142" priority="14" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="140" priority="14" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P27:P29">
-    <cfRule type="cellIs" dxfId="141" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="139" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="138" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Q17">
-    <cfRule type="cellIs" dxfId="139" priority="11" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="137" priority="11" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P17">
-    <cfRule type="cellIs" dxfId="138" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="136" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="135" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="S5">
-    <cfRule type="cellIs" dxfId="136" priority="8" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="134" priority="8" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="R5">
-    <cfRule type="cellIs" dxfId="135" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="133" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="132" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C121:C1048576 C1:C17 C19:C26 C28 C30:C119 B31:B37">
-    <cfRule type="cellIs" dxfId="133" priority="5" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="131" priority="5" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2:E17 E19:E26 E28 E30">
-    <cfRule type="cellIs" dxfId="132" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="130" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G2:G31">
-    <cfRule type="cellIs" dxfId="131" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="129" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I2:I31">
-    <cfRule type="cellIs" dxfId="130" priority="2" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="128" priority="2" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K2:K31 J3:J4 J6:J9 J11:J13 J15:J16 J19:J20 J23 J26 J30:J31">
-    <cfRule type="cellIs" dxfId="129" priority="1" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="127" priority="1" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42237,87 +42241,87 @@
     <sortCondition ref="R164"/>
   </sortState>
   <conditionalFormatting sqref="I1:I53 I78:I80 I105:I108 I133:I135 I160:I163 I188:I1048576 V164:V171 V174:V178 V180:V182 V184:V185 V187:V192 S164:S171 S174:S178 S180:S182 S184:S185 S187:S192">
-    <cfRule type="cellIs" dxfId="128" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="126" priority="21" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1:G1048576">
-    <cfRule type="cellIs" dxfId="127" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="125" priority="19" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="126" priority="20" operator="lessThan">
+    <cfRule type="cellIs" dxfId="124" priority="20" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L55:L77">
-    <cfRule type="cellIs" dxfId="125" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="123" priority="18" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H55:H77">
-    <cfRule type="cellIs" dxfId="124" priority="17" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="122" priority="17" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H81:H104">
-    <cfRule type="cellIs" dxfId="123" priority="15" operator="lessThan">
+    <cfRule type="cellIs" dxfId="121" priority="15" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="16" operator="lessThan">
+    <cfRule type="cellIs" dxfId="120" priority="16" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J81:J104">
-    <cfRule type="cellIs" dxfId="121" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="119" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H109:H132">
-    <cfRule type="cellIs" dxfId="120" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="118" priority="12" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="13" operator="lessThan">
+    <cfRule type="cellIs" dxfId="117" priority="13" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J109:J132">
-    <cfRule type="cellIs" dxfId="118" priority="11" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="116" priority="11" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J136:J159">
-    <cfRule type="cellIs" dxfId="117" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="115" priority="8" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H136:H159">
-    <cfRule type="cellIs" dxfId="116" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="114" priority="9" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="115" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="113" priority="10" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J164:J187">
-    <cfRule type="cellIs" dxfId="114" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="112" priority="5" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H164:H187">
-    <cfRule type="cellIs" dxfId="113" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="111" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="112" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="110" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Y164:Y192">
-    <cfRule type="cellIs" dxfId="111" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="109" priority="3" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="T164:T192">
-    <cfRule type="cellIs" dxfId="110" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="108" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -42354,35 +42358,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="127" t="s">
+      <c r="B2" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="128"/>
-      <c r="D2" s="128"/>
-      <c r="E2" s="128"/>
-      <c r="F2" s="128"/>
-      <c r="G2" s="128"/>
-      <c r="H2" s="128"/>
-      <c r="I2" s="128"/>
-      <c r="J2" s="128"/>
-      <c r="K2" s="128"/>
-      <c r="L2" s="128"/>
-      <c r="M2" s="129"/>
+      <c r="C2" s="129"/>
+      <c r="D2" s="129"/>
+      <c r="E2" s="129"/>
+      <c r="F2" s="129"/>
+      <c r="G2" s="129"/>
+      <c r="H2" s="129"/>
+      <c r="I2" s="129"/>
+      <c r="J2" s="129"/>
+      <c r="K2" s="129"/>
+      <c r="L2" s="129"/>
+      <c r="M2" s="130"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="127" t="s">
+      <c r="R2" s="128" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="128"/>
-      <c r="T2" s="128"/>
-      <c r="U2" s="128"/>
-      <c r="V2" s="128"/>
-      <c r="W2" s="128"/>
-      <c r="X2" s="128"/>
-      <c r="Y2" s="128"/>
-      <c r="Z2" s="128"/>
-      <c r="AA2" s="129"/>
+      <c r="S2" s="129"/>
+      <c r="T2" s="129"/>
+      <c r="U2" s="129"/>
+      <c r="V2" s="129"/>
+      <c r="W2" s="129"/>
+      <c r="X2" s="129"/>
+      <c r="Y2" s="129"/>
+      <c r="Z2" s="129"/>
+      <c r="AA2" s="130"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -42395,50 +42399,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="133" t="s">
+      <c r="C3" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="135" t="s">
+      <c r="D3" s="136" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="133" t="s">
+      <c r="E3" s="134" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="130" t="s">
+      <c r="F3" s="131" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="131"/>
-      <c r="H3" s="130" t="s">
+      <c r="G3" s="132"/>
+      <c r="H3" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="132"/>
-      <c r="J3" s="131"/>
-      <c r="K3" s="130" t="s">
+      <c r="I3" s="133"/>
+      <c r="J3" s="132"/>
+      <c r="K3" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="132"/>
-      <c r="M3" s="131"/>
+      <c r="L3" s="133"/>
+      <c r="M3" s="132"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="133" t="s">
+      <c r="S3" s="134" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="130" t="s">
+      <c r="T3" s="131" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="131"/>
-      <c r="V3" s="130" t="s">
+      <c r="U3" s="132"/>
+      <c r="V3" s="131" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="132"/>
-      <c r="X3" s="131"/>
-      <c r="Y3" s="130" t="s">
+      <c r="W3" s="133"/>
+      <c r="X3" s="132"/>
+      <c r="Y3" s="131" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="132"/>
-      <c r="AA3" s="131"/>
+      <c r="Z3" s="133"/>
+      <c r="AA3" s="132"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -42452,9 +42456,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="134"/>
-      <c r="D4" s="136"/>
-      <c r="E4" s="134"/>
+      <c r="C4" s="135"/>
+      <c r="D4" s="137"/>
+      <c r="E4" s="135"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -42489,7 +42493,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="134"/>
+      <c r="S4" s="135"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -46340,67 +46344,67 @@
     <mergeCell ref="C3:C4"/>
   </mergeCells>
   <conditionalFormatting sqref="B1:M1048576">
-    <cfRule type="cellIs" dxfId="109" priority="18" operator="lessThan">
+    <cfRule type="cellIs" dxfId="107" priority="18" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="108" priority="19" operator="lessThan">
+    <cfRule type="cellIs" dxfId="106" priority="19" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O1:O1048576">
-    <cfRule type="cellIs" dxfId="107" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="105" priority="14" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AX4:AX27">
-    <cfRule type="cellIs" dxfId="106" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="12" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AQ4:AV27">
-    <cfRule type="cellIs" dxfId="105" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="103" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="102" priority="11" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AF4:AI27">
-    <cfRule type="cellIs" dxfId="103" priority="8" operator="lessThan">
+    <cfRule type="cellIs" dxfId="101" priority="8" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="102" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="100" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AK4:AK27">
-    <cfRule type="cellIs" dxfId="101" priority="7" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="99" priority="7" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ4:BJ27">
-    <cfRule type="cellIs" dxfId="100" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="6" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB4:BH27">
-    <cfRule type="cellIs" dxfId="99" priority="4" operator="lessThan">
+    <cfRule type="cellIs" dxfId="97" priority="4" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="96" priority="5" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BJ28:BJ32">
-    <cfRule type="cellIs" dxfId="97" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="95" priority="3" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BB28:BH32">
-    <cfRule type="cellIs" dxfId="96" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="94" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="93" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52319,28 +52323,28 @@
     <sortCondition ref="I2"/>
   </sortState>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="94" priority="6" operator="lessThan">
+    <cfRule type="cellIs" dxfId="92" priority="6" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="93" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="91" priority="7" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="D1:D1048576">
-    <cfRule type="cellIs" dxfId="92" priority="4" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="90" priority="4" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L1:L1048576">
-    <cfRule type="cellIs" dxfId="91" priority="3" operator="greaterThanOrEqual">
+    <cfRule type="cellIs" dxfId="89" priority="3" operator="greaterThanOrEqual">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J1:J1048576">
-    <cfRule type="cellIs" dxfId="90" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="1" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="87" priority="2" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
@@ -52501,30 +52505,30 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="138" t="s">
+      <c r="W2" s="139" t="s">
         <v>178</v>
       </c>
-      <c r="X2" s="139"/>
-      <c r="Y2" s="137" t="s">
+      <c r="X2" s="140"/>
+      <c r="Y2" s="138" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="137"/>
-      <c r="AA2" s="137"/>
-      <c r="AB2" s="137"/>
+      <c r="Z2" s="138"/>
+      <c r="AA2" s="138"/>
+      <c r="AB2" s="138"/>
       <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="137" t="s">
+      <c r="AD2" s="138" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" s="137"/>
-      <c r="AF2" s="137"/>
-      <c r="AG2" s="137"/>
-      <c r="AH2" s="137"/>
-      <c r="AI2" s="137" t="s">
+      <c r="AE2" s="138"/>
+      <c r="AF2" s="138"/>
+      <c r="AG2" s="138"/>
+      <c r="AH2" s="138"/>
+      <c r="AI2" s="138" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="137"/>
+      <c r="AJ2" s="138"/>
       <c r="AK2" s="63" t="s">
         <v>183</v>
       </c>
@@ -53716,19 +53720,19 @@
     <mergeCell ref="AD2:AH2"/>
   </mergeCells>
   <conditionalFormatting sqref="B2:T20">
-    <cfRule type="cellIs" dxfId="88" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="86" priority="1" operator="lessThan">
       <formula>-0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="87" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="85" priority="2" operator="lessThan">
       <formula>-0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="3" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="84" priority="3" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="85" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="83" priority="4" operator="greaterThan">
       <formula>0.1</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="84" priority="5" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="82" priority="5" operator="greaterThan">
       <formula>0.3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -53742,8 +53746,8 @@
   <dimension ref="A1:GB49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="FD1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FU5" sqref="FU5:FU44"/>
+      <pane xSplit="1" topLeftCell="FN1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="FV16" sqref="FV16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53888,30 +53892,30 @@
       </c>
     </row>
     <row r="3" spans="1:184" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="140" t="s">
+      <c r="B3" s="141" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="141"/>
-      <c r="D3" s="142" t="s">
+      <c r="C3" s="142"/>
+      <c r="D3" s="143" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="142"/>
-      <c r="F3" s="142"/>
-      <c r="G3" s="142"/>
+      <c r="E3" s="143"/>
+      <c r="F3" s="143"/>
+      <c r="G3" s="143"/>
       <c r="H3" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="142" t="s">
+      <c r="I3" s="143" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="142"/>
-      <c r="K3" s="142"/>
-      <c r="L3" s="142"/>
-      <c r="M3" s="142"/>
-      <c r="N3" s="142" t="s">
+      <c r="J3" s="143"/>
+      <c r="K3" s="143"/>
+      <c r="L3" s="143"/>
+      <c r="M3" s="143"/>
+      <c r="N3" s="143" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="142"/>
+      <c r="O3" s="143"/>
       <c r="P3" s="70" t="s">
         <v>183</v>
       </c>
@@ -54811,7 +54815,7 @@
         <v>-1.2900000000000023E-2</v>
       </c>
       <c r="FJ5">
-        <f t="shared" ref="FI5:FJ5" si="14">FG5-EK5</f>
+        <f t="shared" ref="FJ5" si="14">FG5-EK5</f>
         <v>0</v>
       </c>
       <c r="FK5">
@@ -54841,7 +54845,7 @@
         <f>FS5/FF5</f>
         <v>-2444.9152542372881</v>
       </c>
-      <c r="FU5" s="143">
+      <c r="FU5" s="127">
         <f>FR5+FI5</f>
         <v>-3.7483000000000016E-2</v>
       </c>
@@ -55259,7 +55263,7 @@
         <f t="shared" ref="FT6:FT44" si="57">FS6/FF6</f>
         <v>-1554.2691751085385</v>
       </c>
-      <c r="FU6" s="143">
+      <c r="FU6" s="127">
         <f t="shared" ref="FU6:FU44" si="58">FR6+FI6</f>
         <v>-0.19286900000000001</v>
       </c>
@@ -55673,7 +55677,7 @@
         <f t="shared" si="57"/>
         <v>-1221.331859629732</v>
       </c>
-      <c r="FU7" s="143">
+      <c r="FU7" s="127">
         <f t="shared" si="58"/>
         <v>-5.8379999999999987E-2</v>
       </c>
@@ -56066,7 +56070,7 @@
         <f t="shared" si="57"/>
         <v>-1134.5261939141487</v>
       </c>
-      <c r="FU8" s="143">
+      <c r="FU8" s="127">
         <f t="shared" si="58"/>
         <v>3.1100000000000017E-3</v>
       </c>
@@ -56496,18 +56500,18 @@
         <v>0.13690000000002556</v>
       </c>
       <c r="FR9">
-        <f t="shared" ref="FR9:FS9" si="59">FO9-DK9</f>
+        <f>FO9-DK9</f>
         <v>-6.0499999999991116E-5</v>
       </c>
       <c r="FS9">
-        <f t="shared" si="59"/>
+        <f t="shared" ref="FR9:FS9" si="59">FP9-DL9</f>
         <v>-2</v>
       </c>
       <c r="FT9">
         <f>FS9/DK9</f>
         <v>-8.281906146954972</v>
       </c>
-      <c r="FU9" s="143">
+      <c r="FU9" s="127">
         <f t="shared" si="58"/>
         <v>-6.0499999999991116E-5</v>
       </c>
@@ -56905,7 +56909,7 @@
         <f t="shared" si="57"/>
         <v>-2639.0390145412275</v>
       </c>
-      <c r="FU10" s="143">
+      <c r="FU10" s="127">
         <f t="shared" si="58"/>
         <v>-5.8390000000000025E-2</v>
       </c>
@@ -57293,7 +57297,7 @@
         <f t="shared" si="57"/>
         <v>-1971.9344968474516</v>
       </c>
-      <c r="FU11" s="143">
+      <c r="FU11" s="127">
         <f t="shared" si="58"/>
         <v>6.751000000000007E-3</v>
       </c>
@@ -57659,9 +57663,30 @@
         <f t="shared" si="57"/>
         <v>-1830.9859154929579</v>
       </c>
-      <c r="FU12" s="143">
+      <c r="FU12" s="127">
         <f t="shared" si="58"/>
         <v>9.1800000000000215E-3</v>
+      </c>
+      <c r="FV12" t="s">
+        <v>299</v>
+      </c>
+      <c r="FW12" t="s">
+        <v>309</v>
+      </c>
+      <c r="FX12" t="s">
+        <v>310</v>
+      </c>
+      <c r="FY12" t="s">
+        <v>302</v>
+      </c>
+      <c r="FZ12" t="s">
+        <v>311</v>
+      </c>
+      <c r="GA12" t="s">
+        <v>185</v>
+      </c>
+      <c r="GB12" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="13" spans="1:184" x14ac:dyDescent="0.35">
@@ -58008,9 +58033,30 @@
         <f t="shared" si="57"/>
         <v>-4844.4874054699494</v>
       </c>
-      <c r="FU13" s="143">
+      <c r="FU13" s="127">
         <f t="shared" si="58"/>
         <v>-9.5300000000000107E-3</v>
+      </c>
+      <c r="FV13">
+        <v>2.7339489299999999E-2</v>
+      </c>
+      <c r="FW13">
+        <v>1.5401050600000001E-2</v>
+      </c>
+      <c r="FX13">
+        <v>3.3246948999999999E-3</v>
+      </c>
+      <c r="FY13">
+        <v>6.1490739999999996E-4</v>
+      </c>
+      <c r="FZ13">
+        <v>3.2438230000000001E-4</v>
+      </c>
+      <c r="GA13">
+        <v>0</v>
+      </c>
+      <c r="GB13">
+        <v>3.41424491E-2</v>
       </c>
     </row>
     <row r="14" spans="1:184" x14ac:dyDescent="0.35">
@@ -58392,7 +58438,7 @@
         <f t="shared" si="57"/>
         <v>-939.53629337778443</v>
       </c>
-      <c r="FU14" s="143">
+      <c r="FU14" s="127">
         <f t="shared" si="58"/>
         <v>2.213699999999999E-2</v>
       </c>
@@ -58755,9 +58801,30 @@
         <f t="shared" si="57"/>
         <v>-951.65394402035622</v>
       </c>
-      <c r="FU15" s="143">
+      <c r="FU15" s="127">
         <f t="shared" si="58"/>
         <v>-1.9765000000000005E-2</v>
+      </c>
+      <c r="FV15" s="66" t="s">
+        <v>312</v>
+      </c>
+      <c r="FW15" t="s">
+        <v>309</v>
+      </c>
+      <c r="FX15" t="s">
+        <v>313</v>
+      </c>
+      <c r="FY15" t="s">
+        <v>302</v>
+      </c>
+      <c r="FZ15" t="s">
+        <v>314</v>
+      </c>
+      <c r="GA15" t="s">
+        <v>185</v>
+      </c>
+      <c r="GB15" t="s">
+        <v>304</v>
       </c>
     </row>
     <row r="16" spans="1:184" x14ac:dyDescent="0.35">
@@ -59109,12 +59176,33 @@
         <f t="shared" si="57"/>
         <v>-7147.2661706897115</v>
       </c>
-      <c r="FU16" s="143">
+      <c r="FU16" s="127">
         <f t="shared" si="58"/>
         <v>-2.7350000000000013E-3</v>
       </c>
-    </row>
-    <row r="17" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV16" s="65">
+        <v>0.1768942</v>
+      </c>
+      <c r="FW16" s="65">
+        <v>0.16088659999999999</v>
+      </c>
+      <c r="FX16" s="65">
+        <v>2.5501010000000001E-2</v>
+      </c>
+      <c r="FY16" s="65">
+        <v>0.77796560000000003</v>
+      </c>
+      <c r="FZ16" s="65">
+        <v>4.1073030000000003E-2</v>
+      </c>
+      <c r="GA16" s="65">
+        <v>9.7949679999999997E-2</v>
+      </c>
+      <c r="GB16" s="65">
+        <v>7.8434610000000004E-5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>27</v>
       </c>
@@ -59472,12 +59560,12 @@
         <f t="shared" si="57"/>
         <v>-270.09951034591694</v>
       </c>
-      <c r="FU17" s="143">
+      <c r="FU17" s="127">
         <f t="shared" si="58"/>
         <v>-6.1999999999999833E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>7</v>
       </c>
@@ -59844,12 +59932,12 @@
         <f t="shared" si="57"/>
         <v>-600.04898359049719</v>
       </c>
-      <c r="FU18" s="143">
+      <c r="FU18" s="127">
         <f t="shared" si="58"/>
         <v>-8.9444999999999997E-2</v>
       </c>
     </row>
-    <row r="19" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>8</v>
       </c>
@@ -60187,12 +60275,33 @@
         <f t="shared" si="57"/>
         <v>-1952.8692995854244</v>
       </c>
-      <c r="FU19" s="143">
+      <c r="FU19" s="127">
         <f t="shared" si="58"/>
         <v>-7.8449999999999992E-2</v>
       </c>
-    </row>
-    <row r="20" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV19" s="66" t="s">
+        <v>312</v>
+      </c>
+      <c r="FW19" t="s">
+        <v>309</v>
+      </c>
+      <c r="FX19" t="s">
+        <v>315</v>
+      </c>
+      <c r="FY19" t="s">
+        <v>302</v>
+      </c>
+      <c r="FZ19" t="s">
+        <v>314</v>
+      </c>
+      <c r="GA19" t="s">
+        <v>185</v>
+      </c>
+      <c r="GB19" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="20" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -60529,12 +60638,33 @@
         <f t="shared" si="57"/>
         <v>-3382.8382838283828</v>
       </c>
-      <c r="FU20" s="143">
+      <c r="FU20" s="127">
         <f t="shared" si="58"/>
         <v>2.4540000000000006E-2</v>
       </c>
-    </row>
-    <row r="21" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV20">
+        <v>0.238661277</v>
+      </c>
+      <c r="FW20">
+        <v>0.42666700800000001</v>
+      </c>
+      <c r="FX20">
+        <v>0.18070791899999999</v>
+      </c>
+      <c r="FY20">
+        <v>0.33082874699999998</v>
+      </c>
+      <c r="FZ20">
+        <v>3.471427E-3</v>
+      </c>
+      <c r="GA20">
+        <v>0.16415397900000001</v>
+      </c>
+      <c r="GB20">
+        <v>2.982887E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>18</v>
       </c>
@@ -60859,12 +60989,12 @@
         <f t="shared" si="57"/>
         <v>-2836.932801565204</v>
       </c>
-      <c r="FU21" s="143">
+      <c r="FU21" s="127">
         <f t="shared" si="58"/>
         <v>5.2999999999999992E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>19</v>
       </c>
@@ -61204,12 +61334,12 @@
         <f t="shared" si="57"/>
         <v>-212.01952410006103</v>
       </c>
-      <c r="FU22" s="143">
+      <c r="FU22" s="127">
         <f t="shared" si="58"/>
         <v>9.2300000000000715E-4</v>
       </c>
     </row>
-    <row r="23" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>12</v>
       </c>
@@ -61537,12 +61667,12 @@
         <f t="shared" si="57"/>
         <v>-816.47664582567131</v>
       </c>
-      <c r="FU23" s="143">
+      <c r="FU23" s="127">
         <f t="shared" si="58"/>
         <v>3.6810000000000009E-2</v>
       </c>
     </row>
-    <row r="24" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>191</v>
       </c>
@@ -61867,12 +61997,12 @@
         <f t="shared" si="57"/>
         <v>-539.61568833903652</v>
       </c>
-      <c r="FU24" s="143">
+      <c r="FU24" s="127">
         <f t="shared" si="58"/>
         <v>3.8609999999999978E-2</v>
       </c>
     </row>
-    <row r="25" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -62210,12 +62340,12 @@
         <f t="shared" si="57"/>
         <v>-656.17211899429003</v>
       </c>
-      <c r="FU25" s="143">
+      <c r="FU25" s="127">
         <f t="shared" si="58"/>
         <v>-1.0050000000000003E-2</v>
       </c>
     </row>
-    <row r="26" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>15</v>
       </c>
@@ -62551,12 +62681,12 @@
         <f t="shared" si="57"/>
         <v>-733.55562291603508</v>
       </c>
-      <c r="FU26" s="143">
+      <c r="FU26" s="127">
         <f t="shared" si="58"/>
         <v>-2.7369999999999978E-2</v>
       </c>
     </row>
-    <row r="27" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>22</v>
       </c>
@@ -62891,12 +63021,12 @@
         <f t="shared" si="57"/>
         <v>-705.38057742782155</v>
       </c>
-      <c r="FU27" s="143">
+      <c r="FU27" s="127">
         <f t="shared" si="58"/>
         <v>1.8589999999999995E-2</v>
       </c>
     </row>
-    <row r="28" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -63232,12 +63362,33 @@
         <f t="shared" si="57"/>
         <v>-273.8687115530463</v>
       </c>
-      <c r="FU28" s="143">
+      <c r="FU28" s="127">
         <f t="shared" si="58"/>
         <v>-4.400000000000015E-3</v>
       </c>
-    </row>
-    <row r="29" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV28" s="66" t="s">
+        <v>312</v>
+      </c>
+      <c r="FW28" t="s">
+        <v>300</v>
+      </c>
+      <c r="FX28" t="s">
+        <v>301</v>
+      </c>
+      <c r="FY28" t="s">
+        <v>302</v>
+      </c>
+      <c r="FZ28" t="s">
+        <v>311</v>
+      </c>
+      <c r="GA28" t="s">
+        <v>185</v>
+      </c>
+      <c r="GB28" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="29" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>17</v>
       </c>
@@ -63573,12 +63724,33 @@
         <f t="shared" si="57"/>
         <v>-568.10704101776707</v>
       </c>
-      <c r="FU29" s="143">
+      <c r="FU29" s="127">
         <f t="shared" si="58"/>
         <v>-1.2139999999999984E-2</v>
       </c>
-    </row>
-    <row r="30" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV29">
+        <v>0.83212224189999995</v>
+      </c>
+      <c r="FW29">
+        <v>8.3979781700000006E-2</v>
+      </c>
+      <c r="FX29">
+        <v>0</v>
+      </c>
+      <c r="FY29">
+        <v>2.4143950000000001E-4</v>
+      </c>
+      <c r="FZ29">
+        <v>1.4792706799999999E-2</v>
+      </c>
+      <c r="GA29">
+        <v>3.5331441999999998E-3</v>
+      </c>
+      <c r="GB29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>26</v>
       </c>
@@ -63914,12 +64086,12 @@
         <f t="shared" si="57"/>
         <v>-741.88446185132182</v>
       </c>
-      <c r="FU30" s="143">
+      <c r="FU30" s="127">
         <f t="shared" si="58"/>
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>14</v>
       </c>
@@ -64253,12 +64425,12 @@
         <f t="shared" si="57"/>
         <v>-311.91369606003752</v>
       </c>
-      <c r="FU31" s="143">
+      <c r="FU31" s="127">
         <f t="shared" si="58"/>
         <v>3.4090000000000009E-2</v>
       </c>
     </row>
-    <row r="32" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -64593,12 +64765,12 @@
         <f t="shared" si="57"/>
         <v>-551.98735969466281</v>
       </c>
-      <c r="FU32" s="143">
+      <c r="FU32" s="127">
         <f t="shared" si="58"/>
         <v>-3.0000000000030003E-5</v>
       </c>
     </row>
-    <row r="33" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>25</v>
       </c>
@@ -64933,12 +65105,12 @@
         <f t="shared" si="57"/>
         <v>-2872.8414442700159</v>
       </c>
-      <c r="FU33" s="143">
+      <c r="FU33" s="127">
         <f t="shared" si="58"/>
         <v>-8.8999999999999913E-3</v>
       </c>
     </row>
-    <row r="34" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>38</v>
       </c>
@@ -65239,12 +65411,12 @@
         <f t="shared" si="57"/>
         <v>-1052.8090970415342</v>
       </c>
-      <c r="FU34" s="143">
+      <c r="FU34" s="127">
         <f t="shared" si="58"/>
         <v>1.7999999999995797E-4</v>
       </c>
     </row>
-    <row r="35" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>190</v>
       </c>
@@ -65545,12 +65717,12 @@
         <f t="shared" si="57"/>
         <v>-902.36059525886776</v>
       </c>
-      <c r="FU35" s="143">
+      <c r="FU35" s="127">
         <f t="shared" si="58"/>
         <v>-1.3000000000000234E-3</v>
       </c>
     </row>
-    <row r="36" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>158</v>
       </c>
@@ -65884,12 +66056,12 @@
         <f t="shared" si="57"/>
         <v>-235.9579379328033</v>
       </c>
-      <c r="FU36" s="143">
+      <c r="FU36" s="127">
         <f t="shared" si="58"/>
         <v>1.2039999999999995E-2</v>
       </c>
     </row>
-    <row r="37" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>157</v>
       </c>
@@ -66223,12 +66395,33 @@
         <f t="shared" si="57"/>
         <v>-2032.6094903853184</v>
       </c>
-      <c r="FU37" s="143">
+      <c r="FU37" s="127">
         <f t="shared" si="58"/>
         <v>-1.6000000000000042E-3</v>
       </c>
-    </row>
-    <row r="38" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV37" t="s">
+        <v>299</v>
+      </c>
+      <c r="FW37" t="s">
+        <v>309</v>
+      </c>
+      <c r="FX37" t="s">
+        <v>315</v>
+      </c>
+      <c r="FY37" t="s">
+        <v>302</v>
+      </c>
+      <c r="FZ37" t="s">
+        <v>303</v>
+      </c>
+      <c r="GA37" t="s">
+        <v>185</v>
+      </c>
+      <c r="GB37" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="38" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>159</v>
       </c>
@@ -66564,12 +66757,33 @@
         <f t="shared" si="57"/>
         <v>-612.99435028248593</v>
       </c>
-      <c r="FU38" s="143">
+      <c r="FU38" s="127">
         <f t="shared" si="58"/>
         <v>2.8299999999999992E-2</v>
       </c>
-    </row>
-    <row r="39" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV38" s="65">
+        <v>0.14611270000000001</v>
+      </c>
+      <c r="FW38" s="65">
+        <v>6.5028539999999996E-2</v>
+      </c>
+      <c r="FX38" s="65">
+        <v>4.2204769999999997E-5</v>
+      </c>
+      <c r="FY38" s="65">
+        <v>1.4821890000000001E-3</v>
+      </c>
+      <c r="FZ38" s="65">
+        <v>1.238988E-6</v>
+      </c>
+      <c r="GA38" s="65">
+        <v>2.28335E-3</v>
+      </c>
+      <c r="GB38" s="65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>160</v>
       </c>
@@ -66863,12 +67077,12 @@
         <f t="shared" si="57"/>
         <v>-950.43731778425649</v>
       </c>
-      <c r="FU39" s="143">
+      <c r="FU39" s="127">
         <f t="shared" si="58"/>
         <v>-3.3689999999999998E-2</v>
       </c>
     </row>
-    <row r="40" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
         <v>187</v>
       </c>
@@ -67169,12 +67383,12 @@
         <f t="shared" si="57"/>
         <v>-218.06346623270952</v>
       </c>
-      <c r="FU40" s="143">
+      <c r="FU40" s="127">
         <f t="shared" si="58"/>
         <v>1.221500000000042E-3</v>
       </c>
     </row>
-    <row r="41" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
         <v>188</v>
       </c>
@@ -67475,12 +67689,12 @@
         <f t="shared" si="57"/>
         <v>-611.20435760205214</v>
       </c>
-      <c r="FU41" s="143">
+      <c r="FU41" s="127">
         <f t="shared" si="58"/>
         <v>2.0232E-2</v>
       </c>
     </row>
-    <row r="42" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
         <v>192</v>
       </c>
@@ -67772,12 +67986,12 @@
         <f t="shared" si="57"/>
         <v>#DIV/0!</v>
       </c>
-      <c r="FU42" s="143">
+      <c r="FU42" s="127">
         <f t="shared" si="58"/>
         <v>-0.59567400000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
         <v>186</v>
       </c>
@@ -68062,12 +68276,33 @@
         <f t="shared" si="57"/>
         <v>-292.41379310344831</v>
       </c>
-      <c r="FU43" s="143">
+      <c r="FU43" s="127">
         <f t="shared" si="58"/>
         <v>-6.7000000000000115E-3</v>
       </c>
-    </row>
-    <row r="44" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV43" s="66" t="s">
+        <v>312</v>
+      </c>
+      <c r="FW43" t="s">
+        <v>300</v>
+      </c>
+      <c r="FX43" t="s">
+        <v>310</v>
+      </c>
+      <c r="FY43" t="s">
+        <v>302</v>
+      </c>
+      <c r="FZ43" t="s">
+        <v>316</v>
+      </c>
+      <c r="GA43" t="s">
+        <v>185</v>
+      </c>
+      <c r="GB43" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="44" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
         <v>6</v>
       </c>
@@ -68099,12 +68334,33 @@
         <f t="shared" si="57"/>
         <v>-759.85256592004532</v>
       </c>
-      <c r="FU44" s="143">
+      <c r="FU44" s="127">
         <f t="shared" si="58"/>
         <v>1.7999999999999683E-3</v>
       </c>
-    </row>
-    <row r="45" spans="1:177" x14ac:dyDescent="0.35">
+      <c r="FV44" s="144">
+        <v>1.374798E-3</v>
+      </c>
+      <c r="FW44" s="65">
+        <v>7.3757379999999997E-2</v>
+      </c>
+      <c r="FX44" s="65">
+        <v>0</v>
+      </c>
+      <c r="FY44" s="65">
+        <v>1.3894790000000001E-4</v>
+      </c>
+      <c r="FZ44" s="65">
+        <v>4.3813270000000001E-4</v>
+      </c>
+      <c r="GA44" s="65">
+        <v>0.2091163</v>
+      </c>
+      <c r="GB44" s="65">
+        <v>6.5188939999999998E-5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:184" x14ac:dyDescent="0.35">
       <c r="Z45">
         <f>SUM(Z5,Z9:Z10,Z13,Z17:Z18,Z21,Z25:Z33,Z36:Z39)</f>
         <v>20.418899999999997</v>
@@ -68147,7 +68403,7 @@
         <v>0.15523900000000007</v>
       </c>
     </row>
-    <row r="46" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:184" x14ac:dyDescent="0.35">
       <c r="CC46" t="s">
         <v>240</v>
       </c>
@@ -68155,7 +68411,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="47" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:184" x14ac:dyDescent="0.35">
       <c r="CC47" t="s">
         <v>241</v>
       </c>
@@ -68163,7 +68419,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="48" spans="1:177" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:184" x14ac:dyDescent="0.35">
       <c r="CC48" t="s">
         <v>242</v>
       </c>
@@ -68184,115 +68440,115 @@
     <mergeCell ref="N3:O3"/>
   </mergeCells>
   <conditionalFormatting sqref="Z5:Z43 BS5:BS43">
-    <cfRule type="cellIs" dxfId="83" priority="31" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="81" priority="31" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA45:AB45 AA5:AB43 BT5:BU43">
-    <cfRule type="cellIs" dxfId="82" priority="30" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="80" priority="30" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z45">
-    <cfRule type="cellIs" dxfId="81" priority="29" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="79" priority="29" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="AA46:AB46">
-    <cfRule type="cellIs" dxfId="80" priority="26" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="78" priority="26" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="Z46">
-    <cfRule type="cellIs" dxfId="79" priority="25" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="77" priority="25" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BS45:BT45">
-    <cfRule type="cellIs" dxfId="78" priority="21" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="76" priority="21" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="BU1:BU3">
-    <cfRule type="cellIs" dxfId="77" priority="20" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="75" priority="20" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="CA1:CA1048576">
-    <cfRule type="cellIs" dxfId="76" priority="17" operator="lessThan">
+    <cfRule type="cellIs" dxfId="74" priority="17" operator="lessThan">
       <formula>-0.05</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="75" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="73" priority="18" operator="greaterThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ED1:ED3 ED5:ED1048576">
-    <cfRule type="cellIs" dxfId="74" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="72" priority="16" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ED1:ED1048576">
-    <cfRule type="cellIs" dxfId="73" priority="14" operator="lessThan">
+    <cfRule type="cellIs" dxfId="71" priority="14" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM5:EM43">
-    <cfRule type="cellIs" dxfId="72" priority="13" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="70" priority="13" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="EM4:EM43">
-    <cfRule type="cellIs" dxfId="71" priority="12" operator="lessThan">
+    <cfRule type="cellIs" dxfId="69" priority="12" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ER6:EY6">
-    <cfRule type="cellIs" dxfId="70" priority="11" operator="lessThan">
+    <cfRule type="cellIs" dxfId="68" priority="11" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ER5:EY5">
-    <cfRule type="cellIs" dxfId="69" priority="10" operator="lessThan">
+    <cfRule type="cellIs" dxfId="67" priority="10" operator="lessThan">
       <formula>0.01</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="ET6">
-    <cfRule type="cellIs" dxfId="68" priority="9" operator="lessThan">
+    <cfRule type="cellIs" dxfId="66" priority="9" operator="lessThan">
       <formula>0.05</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI4">
-    <cfRule type="cellIs" dxfId="67" priority="7" operator="lessThan">
+    <cfRule type="cellIs" dxfId="65" priority="7" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI5:FI43">
-    <cfRule type="cellIs" dxfId="66" priority="5" operator="lessThan">
+    <cfRule type="cellIs" dxfId="64" priority="5" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FI5:FI43">
-    <cfRule type="cellIs" dxfId="65" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="6" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FR5:FR8 FR10:FR44">
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="lessThan">
+    <cfRule type="cellIs" dxfId="62" priority="3" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FR5:FR8 FR10:FR44">
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="4" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FR9">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="lessThan">
+    <cfRule type="cellIs" dxfId="60" priority="1" operator="lessThan">
       <formula>-0.001</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="FR9">
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="2" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Ran regime shift analysis on summer temp and plotted
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3648" uniqueCount="317">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3666" uniqueCount="321">
   <si>
     <t>Species</t>
   </si>
@@ -1003,6 +1003,18 @@
   </si>
   <si>
     <t>StomachFullness</t>
+  </si>
+  <si>
+    <t>Run surftemp with zoopl data by strata instead of EPU</t>
+  </si>
+  <si>
+    <t>by sex</t>
+  </si>
+  <si>
+    <t>regime shift for butterfish</t>
+  </si>
+  <si>
+    <t>regime shift for all species</t>
   </si>
 </sst>
 </file>
@@ -53743,11 +53755,11 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GB49"/>
+  <dimension ref="A1:HE49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="FN1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="FV16" sqref="FV16"/>
+      <pane xSplit="1" topLeftCell="GP1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="GY3" sqref="GY3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53779,9 +53791,11 @@
     <col min="126" max="126" width="9.90625" customWidth="1"/>
     <col min="181" max="181" width="10.7265625" customWidth="1"/>
     <col min="182" max="182" width="9.453125" customWidth="1"/>
+    <col min="197" max="197" width="10.90625" customWidth="1"/>
+    <col min="198" max="198" width="10.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:184" s="73" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:213" s="73" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B1" s="76" t="s">
         <v>216</v>
       </c>
@@ -53841,7 +53855,7 @@
         <v>307</v>
       </c>
     </row>
-    <row r="2" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:213" x14ac:dyDescent="0.35">
       <c r="B2" s="62" t="s">
         <v>210</v>
       </c>
@@ -53890,8 +53904,17 @@
       <c r="FN2" t="s">
         <v>308</v>
       </c>
-    </row>
-    <row r="3" spans="1:184" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="GD2" t="s">
+        <v>317</v>
+      </c>
+      <c r="GT2" t="s">
+        <v>318</v>
+      </c>
+      <c r="HE2" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="3" spans="1:213" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="B3" s="141" t="s">
         <v>178</v>
       </c>
@@ -53962,8 +53985,11 @@
       <c r="FN3" s="69" t="s">
         <v>233</v>
       </c>
-    </row>
-    <row r="4" spans="1:184" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="HE3" s="73" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="4" spans="1:213" s="69" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="71" t="s">
         <v>162</v>
       </c>
@@ -54420,8 +54446,50 @@
       <c r="GB4" s="69" t="s">
         <v>286</v>
       </c>
-    </row>
-    <row r="5" spans="1:184" x14ac:dyDescent="0.35">
+      <c r="GD4" s="69" t="s">
+        <v>4</v>
+      </c>
+      <c r="GE4" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="GF4" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="GG4" s="69" t="s">
+        <v>218</v>
+      </c>
+      <c r="GH4" s="69" t="s">
+        <v>219</v>
+      </c>
+      <c r="GI4" s="69" t="s">
+        <v>225</v>
+      </c>
+      <c r="GJ4" s="69" t="s">
+        <v>264</v>
+      </c>
+      <c r="GL4" s="69" t="s">
+        <v>162</v>
+      </c>
+      <c r="GM4" s="69" t="s">
+        <v>144</v>
+      </c>
+      <c r="GN4" s="69" t="s">
+        <v>165</v>
+      </c>
+      <c r="GO4" s="69" t="s">
+        <v>305</v>
+      </c>
+      <c r="GP4" s="69" t="s">
+        <v>172</v>
+      </c>
+      <c r="GQ4" s="69" t="s">
+        <v>185</v>
+      </c>
+      <c r="GR4" s="69" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="5" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -54850,7 +54918,7 @@
         <v>-3.7483000000000016E-2</v>
       </c>
     </row>
-    <row r="6" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>11</v>
       </c>
@@ -55268,7 +55336,7 @@
         <v>-0.19286900000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>36</v>
       </c>
@@ -55682,7 +55750,7 @@
         <v>-5.8379999999999987E-2</v>
       </c>
     </row>
-    <row r="8" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>20</v>
       </c>
@@ -56075,7 +56143,7 @@
         <v>3.1100000000000017E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>23</v>
       </c>
@@ -56537,7 +56605,7 @@
         <v>1.925668E-6</v>
       </c>
     </row>
-    <row r="10" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>24</v>
       </c>
@@ -56921,7 +56989,7 @@
       <c r="GA10" s="65"/>
       <c r="GB10" s="65"/>
     </row>
-    <row r="11" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -57302,7 +57370,7 @@
         <v>6.751000000000007E-3</v>
       </c>
     </row>
-    <row r="12" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -57689,7 +57757,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="13" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>156</v>
       </c>
@@ -58059,7 +58127,7 @@
         <v>3.41424491E-2</v>
       </c>
     </row>
-    <row r="14" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -58443,7 +58511,7 @@
         <v>2.213699999999999E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>16</v>
       </c>
@@ -58827,7 +58895,7 @@
         <v>304</v>
       </c>
     </row>
-    <row r="16" spans="1:184" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
Added butterfish condition regime shift plots by sex
</commit_message>
<xml_diff>
--- a/GAM_Summary_notes_2020.xlsx
+++ b/GAM_Summary_notes_2020.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="8" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8960" windowHeight="4360" firstSheet="6" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="WFC LocalDensity (2)" sheetId="24" r:id="rId1"/>
@@ -52,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3666" uniqueCount="321">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3680" uniqueCount="327">
   <si>
     <t>Species</t>
   </si>
@@ -1015,6 +1015,24 @@
   </si>
   <si>
     <t>regime shift for all species</t>
+  </si>
+  <si>
+    <t>`</t>
+  </si>
+  <si>
+    <t>CopepodSmallLargeStrataSummer</t>
+  </si>
+  <si>
+    <t>ZooplAbundStrataWinter</t>
+  </si>
+  <si>
+    <t>CopepodSmallLargeStrataWinter</t>
+  </si>
+  <si>
+    <t>ZooplAbundStrataSummer</t>
+  </si>
+  <si>
+    <t>(Haddock)</t>
   </si>
 </sst>
 </file>
@@ -2549,6 +2567,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="45" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="60" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="34" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2597,7 +2616,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="45" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -7032,8 +7050,8 @@
   <dimension ref="A1:Z43"/>
   <sheetViews>
     <sheetView zoomScale="68" workbookViewId="0">
-      <pane ySplit="4" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B43" sqref="B43"/>
+      <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A23" sqref="A23:XFD23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -26707,7 +26725,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:B41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="M9" sqref="M9"/>
     </sheetView>
   </sheetViews>
@@ -27035,8 +27053,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C40"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" workbookViewId="0">
-      <selection sqref="A1:A40"/>
+    <sheetView topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -27497,8 +27515,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="I25" sqref="I25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -27803,6 +27821,9 @@
       </c>
       <c r="F6" s="85" t="s">
         <v>236</v>
+      </c>
+      <c r="H6" t="s">
+        <v>321</v>
       </c>
       <c r="I6" s="88" t="s">
         <v>23</v>
@@ -42370,35 +42391,35 @@
     </row>
     <row r="2" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
-      <c r="B2" s="128" t="s">
+      <c r="B2" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="129"/>
-      <c r="D2" s="129"/>
-      <c r="E2" s="129"/>
-      <c r="F2" s="129"/>
-      <c r="G2" s="129"/>
-      <c r="H2" s="129"/>
-      <c r="I2" s="129"/>
-      <c r="J2" s="129"/>
-      <c r="K2" s="129"/>
-      <c r="L2" s="129"/>
-      <c r="M2" s="130"/>
+      <c r="C2" s="130"/>
+      <c r="D2" s="130"/>
+      <c r="E2" s="130"/>
+      <c r="F2" s="130"/>
+      <c r="G2" s="130"/>
+      <c r="H2" s="130"/>
+      <c r="I2" s="130"/>
+      <c r="J2" s="130"/>
+      <c r="K2" s="130"/>
+      <c r="L2" s="130"/>
+      <c r="M2" s="131"/>
       <c r="N2" s="2"/>
       <c r="O2" s="3"/>
       <c r="Q2" s="1"/>
-      <c r="R2" s="128" t="s">
+      <c r="R2" s="129" t="s">
         <v>107</v>
       </c>
-      <c r="S2" s="129"/>
-      <c r="T2" s="129"/>
-      <c r="U2" s="129"/>
-      <c r="V2" s="129"/>
-      <c r="W2" s="129"/>
-      <c r="X2" s="129"/>
-      <c r="Y2" s="129"/>
-      <c r="Z2" s="129"/>
-      <c r="AA2" s="130"/>
+      <c r="S2" s="130"/>
+      <c r="T2" s="130"/>
+      <c r="U2" s="130"/>
+      <c r="V2" s="130"/>
+      <c r="W2" s="130"/>
+      <c r="X2" s="130"/>
+      <c r="Y2" s="130"/>
+      <c r="Z2" s="130"/>
+      <c r="AA2" s="131"/>
       <c r="AB2" s="2"/>
       <c r="AC2" s="3"/>
       <c r="BA2">
@@ -42411,50 +42432,50 @@
     <row r="3" spans="1:64" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
       <c r="B3" s="4"/>
-      <c r="C3" s="134" t="s">
+      <c r="C3" s="135" t="s">
         <v>111</v>
       </c>
-      <c r="D3" s="136" t="s">
+      <c r="D3" s="137" t="s">
         <v>40</v>
       </c>
-      <c r="E3" s="134" t="s">
+      <c r="E3" s="135" t="s">
         <v>1</v>
       </c>
-      <c r="F3" s="131" t="s">
+      <c r="F3" s="132" t="s">
         <v>108</v>
       </c>
-      <c r="G3" s="132"/>
-      <c r="H3" s="131" t="s">
+      <c r="G3" s="133"/>
+      <c r="H3" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="I3" s="133"/>
-      <c r="J3" s="132"/>
-      <c r="K3" s="131" t="s">
+      <c r="I3" s="134"/>
+      <c r="J3" s="133"/>
+      <c r="K3" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="L3" s="133"/>
-      <c r="M3" s="132"/>
+      <c r="L3" s="134"/>
+      <c r="M3" s="133"/>
       <c r="N3" s="5"/>
       <c r="O3" s="6"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="4"/>
-      <c r="S3" s="134" t="s">
+      <c r="S3" s="135" t="s">
         <v>111</v>
       </c>
-      <c r="T3" s="131" t="s">
+      <c r="T3" s="132" t="s">
         <v>108</v>
       </c>
-      <c r="U3" s="132"/>
-      <c r="V3" s="131" t="s">
+      <c r="U3" s="133"/>
+      <c r="V3" s="132" t="s">
         <v>109</v>
       </c>
-      <c r="W3" s="133"/>
-      <c r="X3" s="132"/>
-      <c r="Y3" s="131" t="s">
+      <c r="W3" s="134"/>
+      <c r="X3" s="133"/>
+      <c r="Y3" s="132" t="s">
         <v>110</v>
       </c>
-      <c r="Z3" s="133"/>
-      <c r="AA3" s="132"/>
+      <c r="Z3" s="134"/>
+      <c r="AA3" s="133"/>
       <c r="AB3" s="5"/>
       <c r="AC3" s="6"/>
       <c r="AE3">
@@ -42468,9 +42489,9 @@
       <c r="B4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="135"/>
-      <c r="D4" s="137"/>
-      <c r="E4" s="135"/>
+      <c r="C4" s="136"/>
+      <c r="D4" s="138"/>
+      <c r="E4" s="136"/>
       <c r="F4" s="10" t="s">
         <v>112</v>
       </c>
@@ -42505,7 +42526,7 @@
       <c r="R4" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="135"/>
+      <c r="S4" s="136"/>
       <c r="T4" s="10" t="s">
         <v>112</v>
       </c>
@@ -52517,30 +52538,30 @@
       <c r="T2">
         <v>-8.5642271706535794E-2</v>
       </c>
-      <c r="W2" s="139" t="s">
+      <c r="W2" s="140" t="s">
         <v>178</v>
       </c>
-      <c r="X2" s="140"/>
-      <c r="Y2" s="138" t="s">
+      <c r="X2" s="141"/>
+      <c r="Y2" s="139" t="s">
         <v>179</v>
       </c>
-      <c r="Z2" s="138"/>
-      <c r="AA2" s="138"/>
-      <c r="AB2" s="138"/>
+      <c r="Z2" s="139"/>
+      <c r="AA2" s="139"/>
+      <c r="AB2" s="139"/>
       <c r="AC2" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="AD2" s="138" t="s">
+      <c r="AD2" s="139" t="s">
         <v>181</v>
       </c>
-      <c r="AE2" s="138"/>
-      <c r="AF2" s="138"/>
-      <c r="AG2" s="138"/>
-      <c r="AH2" s="138"/>
-      <c r="AI2" s="138" t="s">
+      <c r="AE2" s="139"/>
+      <c r="AF2" s="139"/>
+      <c r="AG2" s="139"/>
+      <c r="AH2" s="139"/>
+      <c r="AI2" s="139" t="s">
         <v>108</v>
       </c>
-      <c r="AJ2" s="138"/>
+      <c r="AJ2" s="139"/>
       <c r="AK2" s="63" t="s">
         <v>183</v>
       </c>
@@ -53757,9 +53778,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:HE49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="88" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="GP1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="GY3" sqref="GY3"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="88" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="FO1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="GE15" sqref="GE15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -53915,30 +53936,30 @@
       </c>
     </row>
     <row r="3" spans="1:213" s="69" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="B3" s="141" t="s">
+      <c r="B3" s="142" t="s">
         <v>178</v>
       </c>
-      <c r="C3" s="142"/>
-      <c r="D3" s="143" t="s">
+      <c r="C3" s="143"/>
+      <c r="D3" s="144" t="s">
         <v>179</v>
       </c>
-      <c r="E3" s="143"/>
-      <c r="F3" s="143"/>
-      <c r="G3" s="143"/>
+      <c r="E3" s="144"/>
+      <c r="F3" s="144"/>
+      <c r="G3" s="144"/>
       <c r="H3" s="70" t="s">
         <v>180</v>
       </c>
-      <c r="I3" s="143" t="s">
+      <c r="I3" s="144" t="s">
         <v>181</v>
       </c>
-      <c r="J3" s="143"/>
-      <c r="K3" s="143"/>
-      <c r="L3" s="143"/>
-      <c r="M3" s="143"/>
-      <c r="N3" s="143" t="s">
+      <c r="J3" s="144"/>
+      <c r="K3" s="144"/>
+      <c r="L3" s="144"/>
+      <c r="M3" s="144"/>
+      <c r="N3" s="144" t="s">
         <v>108</v>
       </c>
-      <c r="O3" s="143"/>
+      <c r="O3" s="144"/>
       <c r="P3" s="70" t="s">
         <v>183</v>
       </c>
@@ -56572,7 +56593,7 @@
         <v>-6.0499999999991116E-5</v>
       </c>
       <c r="FS9">
-        <f t="shared" ref="FR9:FS9" si="59">FP9-DL9</f>
+        <f t="shared" ref="FS9" si="59">FP9-DL9</f>
         <v>-2</v>
       </c>
       <c r="FT9">
@@ -57369,6 +57390,27 @@
         <f t="shared" si="58"/>
         <v>6.751000000000007E-3</v>
       </c>
+      <c r="FV11" t="s">
+        <v>299</v>
+      </c>
+      <c r="FW11" t="s">
+        <v>309</v>
+      </c>
+      <c r="FX11" t="s">
+        <v>313</v>
+      </c>
+      <c r="FY11" t="s">
+        <v>324</v>
+      </c>
+      <c r="FZ11" t="s">
+        <v>325</v>
+      </c>
+      <c r="GA11" t="s">
+        <v>304</v>
+      </c>
+      <c r="GC11" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="12" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
@@ -58510,6 +58552,24 @@
         <f t="shared" si="58"/>
         <v>2.213699999999999E-2</v>
       </c>
+      <c r="FV14">
+        <v>1.0896514E-3</v>
+      </c>
+      <c r="FW14">
+        <v>4.1733366600000002E-2</v>
+      </c>
+      <c r="FX14">
+        <v>3.4072209999999999E-4</v>
+      </c>
+      <c r="FY14">
+        <v>2.5403382400000001E-2</v>
+      </c>
+      <c r="FZ14">
+        <v>1.14731329E-2</v>
+      </c>
+      <c r="GA14">
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:213" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -61406,6 +61466,24 @@
         <f t="shared" si="58"/>
         <v>9.2300000000000715E-4</v>
       </c>
+      <c r="FV22" t="s">
+        <v>299</v>
+      </c>
+      <c r="FW22" t="s">
+        <v>300</v>
+      </c>
+      <c r="FX22" t="s">
+        <v>301</v>
+      </c>
+      <c r="FY22" t="s">
+        <v>322</v>
+      </c>
+      <c r="FZ22" t="s">
+        <v>323</v>
+      </c>
+      <c r="GA22" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="23" spans="1:184" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
@@ -61738,6 +61816,24 @@
       <c r="FU23" s="127">
         <f t="shared" si="58"/>
         <v>3.6810000000000009E-2</v>
+      </c>
+      <c r="FV23">
+        <v>2.17170922E-2</v>
+      </c>
+      <c r="FW23">
+        <v>0.1169788786</v>
+      </c>
+      <c r="FX23">
+        <v>6.9906493799999997E-2</v>
+      </c>
+      <c r="FY23">
+        <v>4.1428230000000002E-4</v>
+      </c>
+      <c r="FZ23">
+        <v>1.2385913599999999E-2</v>
+      </c>
+      <c r="GA23">
+        <v>1.1851948500000001E-2</v>
       </c>
     </row>
     <row r="24" spans="1:184" x14ac:dyDescent="0.35">
@@ -68406,7 +68502,7 @@
         <f t="shared" si="58"/>
         <v>1.7999999999999683E-3</v>
       </c>
-      <c r="FV44" s="144">
+      <c r="FV44" s="128">
         <v>1.374798E-3</v>
       </c>
       <c r="FW44" s="65">

</xml_diff>